<commit_message>
add fs and cs reports
</commit_message>
<xml_diff>
--- a/ExcelInputs/Structural.xlsx
+++ b/ExcelInputs/Structural.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\ExcelInputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\Models\AFO\ExcelInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C7354E-7193-4702-B9CE-FDEA19277032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3361026-BDDD-41AF-9EA0-899F32B84F3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="3" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -140,12 +140,14 @@
     <definedName name="i_rev_trait_name" localSheetId="2">StructuralSA!$H$129:$H$136</definedName>
     <definedName name="i_sim_periods_year" localSheetId="3">[2]FeedSupply!$P$28</definedName>
     <definedName name="i_sim_periods_year">Stock!$I$62</definedName>
-    <definedName name="i_store_feedbud" localSheetId="3">'Report Settings'!$Q$18</definedName>
+    <definedName name="i_store_cs_rep" localSheetId="3">'Report Settings'!$K$18</definedName>
+    <definedName name="i_store_feedbud" localSheetId="3">'Report Settings'!$U$18</definedName>
     <definedName name="i_store_ffcfw_rep">'Report Settings'!$G$18</definedName>
+    <definedName name="i_store_fs_rep" localSheetId="3">'Report Settings'!$M$18</definedName>
     <definedName name="i_store_lw_rep">'Report Settings'!$I$18</definedName>
-    <definedName name="i_store_mort" localSheetId="3">'Report Settings'!$O$18</definedName>
-    <definedName name="i_store_nv_rep">'Report Settings'!$K$18</definedName>
-    <definedName name="i_store_on_hand_mort" localSheetId="3">'Report Settings'!$M$18</definedName>
+    <definedName name="i_store_mort" localSheetId="3">'Report Settings'!$S$18</definedName>
+    <definedName name="i_store_nv_rep">'Report Settings'!$O$18</definedName>
+    <definedName name="i_store_on_hand_mort" localSheetId="3">'Report Settings'!$Q$18</definedName>
     <definedName name="i_transfer_exists_tg1">Stock!$K$119:$N$121</definedName>
     <definedName name="i_use_pkl_condensed_start_condition" localSheetId="2">StructuralSA!$M$125</definedName>
     <definedName name="i_w_pos">Stock!$I$56</definedName>
@@ -184,7 +186,7 @@
     <definedName name="ZA.WidthCol" localSheetId="4">Admin!$L$26</definedName>
     <definedName name="ZA.ZoomSheet" localSheetId="4">Admin!$O$26</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -192,7 +194,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2222,7 +2226,7 @@
     <author>John</author>
   </authors>
   <commentList>
-    <comment ref="M16" authorId="0" shapeId="0" xr:uid="{2E84FAC6-A425-42D0-899A-CA98558F543C}">
+    <comment ref="Q16" authorId="0" shapeId="0" xr:uid="{2E84FAC6-A425-42D0-899A-CA98558F543C}">
       <text>
         <r>
           <rPr>
@@ -2251,7 +2255,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="391">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -3533,6 +3537,18 @@
 25Apr21: Moved inputs from Property.xlsx
                    Moved FVP &amp; N inputs from Stock
 1: 1Apr19-Created the version control table</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>FS</t>
+  </si>
+  <si>
+    <t>store fat score</t>
+  </si>
+  <si>
+    <t>store condition score</t>
   </si>
 </sst>
 </file>
@@ -27769,7 +27785,7 @@
   </sheetPr>
   <dimension ref="A1:AB175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="9" ySplit="10" topLeftCell="J33" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
@@ -29479,19 +29495,19 @@
         <v>43485</v>
       </c>
       <c r="S45" s="204">
-        <f>MIN(364,INT((O45 - DATE(YEAR(O45),1,1))))</f>
+        <f t="shared" ref="S45:V47" si="2">MIN(364,INT((O45 - DATE(YEAR(O45),1,1))))</f>
         <v>288</v>
       </c>
       <c r="T45" s="204">
-        <f>MIN(364,INT((P45 - DATE(YEAR(P45),1,1))))</f>
+        <f t="shared" si="2"/>
         <v>319</v>
       </c>
       <c r="U45" s="204">
-        <f>MIN(364,INT((Q45 - DATE(YEAR(Q45),1,1))))</f>
+        <f t="shared" si="2"/>
         <v>113</v>
       </c>
       <c r="V45" s="204">
-        <f>MIN(364,INT((R45 - DATE(YEAR(R45),1,1))))</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="W45" s="2"/>
@@ -29524,11 +29540,11 @@
       <c r="M46" s="211"/>
       <c r="N46" s="211"/>
       <c r="O46" s="203">
-        <f t="shared" ref="O46:O47" si="2">$K46+91+126/2</f>
+        <f t="shared" ref="O46:O47" si="3">$K46+91+126/2</f>
         <v>43788</v>
       </c>
       <c r="P46" s="203">
-        <f t="shared" ref="P46:P47" si="3">O46+126/4</f>
+        <f t="shared" ref="P46:P47" si="4">O46+126/4</f>
         <v>43819.5</v>
       </c>
       <c r="Q46" s="203">
@@ -29536,23 +29552,23 @@
         <v>43613</v>
       </c>
       <c r="R46" s="203">
-        <f t="shared" ref="R46:R47" si="4">$K46-150+35</f>
+        <f t="shared" ref="R46:R47" si="5">$K46-150+35</f>
         <v>43519</v>
       </c>
       <c r="S46" s="204">
-        <f>MIN(364,INT((O46 - DATE(YEAR(O46),1,1))))</f>
+        <f t="shared" si="2"/>
         <v>322</v>
       </c>
       <c r="T46" s="204">
-        <f>MIN(364,INT((P46 - DATE(YEAR(P46),1,1))))</f>
+        <f t="shared" si="2"/>
         <v>353</v>
       </c>
       <c r="U46" s="204">
-        <f>MIN(364,INT((Q46 - DATE(YEAR(Q46),1,1))))</f>
+        <f t="shared" si="2"/>
         <v>147</v>
       </c>
       <c r="V46" s="204">
-        <f>MIN(364,INT((R46 - DATE(YEAR(R46),1,1))))</f>
+        <f t="shared" si="2"/>
         <v>53</v>
       </c>
       <c r="W46" s="2"/>
@@ -29585,11 +29601,11 @@
       <c r="M47" s="211"/>
       <c r="N47" s="211"/>
       <c r="O47" s="203">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43823</v>
       </c>
       <c r="P47" s="203">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43854.5</v>
       </c>
       <c r="Q47" s="203">
@@ -29597,23 +29613,23 @@
         <v>43648</v>
       </c>
       <c r="R47" s="203">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>43554</v>
       </c>
       <c r="S47" s="204">
-        <f>MIN(364,INT((O47 - DATE(YEAR(O47),1,1))))</f>
+        <f t="shared" si="2"/>
         <v>357</v>
       </c>
       <c r="T47" s="204">
-        <f>MIN(364,INT((P47 - DATE(YEAR(P47),1,1))))</f>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="U47" s="204">
-        <f>MIN(364,INT((Q47 - DATE(YEAR(Q47),1,1))))</f>
+        <f t="shared" si="2"/>
         <v>182</v>
       </c>
       <c r="V47" s="204">
-        <f>MIN(364,INT((R47 - DATE(YEAR(R47),1,1))))</f>
+        <f t="shared" si="2"/>
         <v>88</v>
       </c>
       <c r="W47" s="2"/>
@@ -29904,11 +29920,11 @@
         <v>13</v>
       </c>
       <c r="Q54" s="204">
-        <f t="shared" ref="Q54:Q56" si="5">MIN(364,INT((N54 - DATE(YEAR(N54),1,1))))</f>
+        <f t="shared" ref="Q54:Q56" si="6">MIN(364,INT((N54 - DATE(YEAR(N54),1,1))))</f>
         <v>134</v>
       </c>
       <c r="R54" s="204">
-        <f t="shared" ref="R54:R56" si="6">MIN(364,INT((O54 - DATE(YEAR(O54),1,1))))</f>
+        <f t="shared" ref="R54:R56" si="7">MIN(364,INT((O54 - DATE(YEAR(O54),1,1))))</f>
         <v>255</v>
       </c>
       <c r="S54" s="2"/>
@@ -29951,11 +29967,11 @@
         <v>43</v>
       </c>
       <c r="Q55" s="204">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>164</v>
       </c>
       <c r="R55" s="204">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>285</v>
       </c>
       <c r="S55" s="2"/>
@@ -29998,11 +30014,11 @@
         <v>74</v>
       </c>
       <c r="Q56" s="204">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>195</v>
       </c>
       <c r="R56" s="204">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>316</v>
       </c>
       <c r="S56" s="2"/>
@@ -31332,7 +31348,7 @@
       <c r="A91" s="1"/>
       <c r="B91" s="33"/>
       <c r="C91" s="73">
-        <f t="shared" ref="C91:C94" si="7">INT(C$68+3)</f>
+        <f t="shared" ref="C91:C94" si="8">INT(C$68+3)</f>
         <v>4</v>
       </c>
       <c r="D91" s="4"/>
@@ -31381,7 +31397,7 @@
       <c r="A92" s="1"/>
       <c r="B92" s="33"/>
       <c r="C92" s="73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="D92" s="4"/>
@@ -31430,7 +31446,7 @@
       <c r="A93" s="1"/>
       <c r="B93" s="33"/>
       <c r="C93" s="73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="D93" s="4"/>
@@ -31479,7 +31495,7 @@
       <c r="A94" s="1"/>
       <c r="B94" s="33"/>
       <c r="C94" s="73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="D94" s="4"/>
@@ -31696,7 +31712,7 @@
       <c r="A99" s="1"/>
       <c r="B99" s="33"/>
       <c r="C99" s="73">
-        <f t="shared" ref="C99:C102" si="8">INT($C$68)+3</f>
+        <f t="shared" ref="C99:C102" si="9">INT($C$68)+3</f>
         <v>4</v>
       </c>
       <c r="D99" s="4"/>
@@ -31757,7 +31773,7 @@
       <c r="A100" s="1"/>
       <c r="B100" s="33"/>
       <c r="C100" s="73">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="D100" s="4"/>
@@ -31810,7 +31826,7 @@
       <c r="A101" s="1"/>
       <c r="B101" s="33"/>
       <c r="C101" s="73">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="D101" s="4"/>
@@ -31863,7 +31879,7 @@
       <c r="A102" s="1"/>
       <c r="B102" s="33"/>
       <c r="C102" s="73">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="D102" s="4"/>
@@ -33029,7 +33045,7 @@
       <c r="A134" s="1"/>
       <c r="B134" s="33"/>
       <c r="C134" s="73">
-        <f t="shared" ref="C134:C136" si="9">INT(C$112+3)</f>
+        <f t="shared" ref="C134:C136" si="10">INT(C$112+3)</f>
         <v>4</v>
       </c>
       <c r="D134" s="4"/>
@@ -33068,7 +33084,7 @@
       <c r="A135" s="1"/>
       <c r="B135" s="33"/>
       <c r="C135" s="73">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="D135" s="4"/>
@@ -33107,7 +33123,7 @@
       <c r="A136" s="1"/>
       <c r="B136" s="33"/>
       <c r="C136" s="73">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="D136" s="4"/>
@@ -34517,8 +34533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE3626F-D681-4ABD-B02A-5C870438CFCF}">
   <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -34970,24 +34986,27 @@
         <v>249</v>
       </c>
       <c r="K16" s="193" t="s">
+        <v>387</v>
+      </c>
+      <c r="L16" s="192"/>
+      <c r="M16" s="193" t="s">
+        <v>388</v>
+      </c>
+      <c r="O16" s="193" t="s">
         <v>356</v>
       </c>
-      <c r="L16" s="191"/>
-      <c r="M16" s="193" t="s">
+      <c r="P16" s="191"/>
+      <c r="Q16" s="193" t="s">
         <v>357</v>
       </c>
-      <c r="N16" s="191"/>
-      <c r="O16" s="193" t="s">
+      <c r="R16" s="191"/>
+      <c r="S16" s="193" t="s">
         <v>358</v>
       </c>
-      <c r="P16" s="192"/>
-      <c r="Q16" s="193" t="s">
+      <c r="T16" s="192"/>
+      <c r="U16" s="193" t="s">
         <v>363</v>
       </c>
-      <c r="R16" s="192"/>
-      <c r="S16" s="192"/>
-      <c r="T16" s="192"/>
-      <c r="U16" s="192"/>
       <c r="V16" s="190"/>
       <c r="W16" s="176"/>
       <c r="X16" s="168"/>
@@ -35010,24 +35029,27 @@
       </c>
       <c r="J17" s="194"/>
       <c r="K17" s="191" t="s">
+        <v>390</v>
+      </c>
+      <c r="L17" s="192"/>
+      <c r="M17" s="191" t="s">
+        <v>389</v>
+      </c>
+      <c r="O17" s="191" t="s">
         <v>360</v>
       </c>
-      <c r="L17" s="191"/>
-      <c r="M17" s="191" t="s">
+      <c r="P17" s="191"/>
+      <c r="Q17" s="191" t="s">
         <v>361</v>
       </c>
-      <c r="N17" s="191"/>
-      <c r="O17" s="191" t="s">
+      <c r="R17" s="191"/>
+      <c r="S17" s="191" t="s">
         <v>362</v>
       </c>
-      <c r="P17" s="192"/>
-      <c r="Q17" s="191" t="s">
+      <c r="T17" s="192"/>
+      <c r="U17" s="191" t="s">
         <v>364</v>
       </c>
-      <c r="R17" s="192"/>
-      <c r="S17" s="192"/>
-      <c r="T17" s="192"/>
-      <c r="U17" s="192"/>
       <c r="V17" s="190"/>
       <c r="W17" s="176"/>
       <c r="X17" s="168"/>
@@ -35051,22 +35073,25 @@
       <c r="K18" s="195" t="b">
         <v>0</v>
       </c>
-      <c r="L18" s="191"/>
+      <c r="L18" s="192"/>
       <c r="M18" s="195" t="b">
-        <v>0</v>
-      </c>
-      <c r="N18" s="191"/>
+        <v>1</v>
+      </c>
       <c r="O18" s="195" t="b">
         <v>0</v>
       </c>
-      <c r="P18" s="192"/>
+      <c r="P18" s="191"/>
       <c r="Q18" s="195" t="b">
-        <v>1</v>
-      </c>
-      <c r="R18" s="192"/>
-      <c r="S18" s="192"/>
+        <v>0</v>
+      </c>
+      <c r="R18" s="191"/>
+      <c r="S18" s="195" t="b">
+        <v>0</v>
+      </c>
       <c r="T18" s="192"/>
-      <c r="U18" s="192"/>
+      <c r="U18" s="195" t="b">
+        <v>1</v>
+      </c>
       <c r="V18" s="190"/>
       <c r="W18" s="176"/>
       <c r="X18" s="168"/>

</xml_diff>

<commit_message>
make the calculation of hay yield to grain yield occur in AFO so that sensitivities on the r axis work and the sim inputs work if hay included.
</commit_message>
<xml_diff>
--- a/ExcelInputs/Structural.xlsx
+++ b/ExcelInputs/Structural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\Models\AFO\ExcelInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3361026-BDDD-41AF-9EA0-899F32B84F3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D209B64-8C0D-4B3F-8296-6FE455BFBDA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="3" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <definedName name="grazing_int" localSheetId="0">General!$I$49:$L$49</definedName>
     <definedName name="i_a0_pos">Stock!$I$43</definedName>
     <definedName name="i_a1_pos">Stock!$I$44</definedName>
-    <definedName name="i_a2_idx" localSheetId="0">General!$M$80</definedName>
+    <definedName name="i_a2_idx" localSheetId="0">General!$N$80</definedName>
     <definedName name="i_adjp_cfw_initial_w0" localSheetId="2">StructuralSA!$K$99</definedName>
     <definedName name="i_adjp_cfw_initial_w1" localSheetId="2">StructuralSA!$P$99:$P$101</definedName>
     <definedName name="i_adjp_cfw_initial_w3" localSheetId="2">StructuralSA!$U$99:$U$101</definedName>
@@ -83,12 +83,13 @@
     <definedName name="i_fvp_mask_dams">StructuralSA!$N$43:$R$43</definedName>
     <definedName name="i_fvp_mask_offs">StructuralSA!$J$52:$O$52</definedName>
     <definedName name="i_generate_with_t" localSheetId="2">StructuralSA!$P$121</definedName>
-    <definedName name="i_history4_req" localSheetId="0">General!$Q$80:$Q$115</definedName>
+    <definedName name="i_history4_req" localSheetId="0">General!$R$80:$R$115</definedName>
     <definedName name="i_i_pos">Stock!$I$50</definedName>
-    <definedName name="i_idx_k" localSheetId="0">General!$O$80:$O$115</definedName>
+    <definedName name="i_idx_k" localSheetId="0">General!$P$80:$P$115</definedName>
     <definedName name="i_idx_k1" localSheetId="0">General!$I$80:$I$96</definedName>
-    <definedName name="i_idx_k2" localSheetId="0">General!$K$80:$K$98</definedName>
+    <definedName name="i_idx_k2" localSheetId="0">General!$L$80:$L$98</definedName>
     <definedName name="i_initial_b1">Stock!$L$155:$V$155</definedName>
+    <definedName name="i_is_baled_k" localSheetId="0">General!$J$80:$J$96</definedName>
     <definedName name="i_is_dry_b1">Stock!$L$149:$V$149</definedName>
     <definedName name="i_k2_idx_dams">Stock!$L$202:$V$204</definedName>
     <definedName name="i_k2_pos">Stock!$I$51</definedName>
@@ -97,7 +98,7 @@
     <definedName name="i_k5_pos">Stock!$I$53</definedName>
     <definedName name="i_lag_organs">Stock!$I$70</definedName>
     <definedName name="i_lag_wool">Stock!$I$69</definedName>
-    <definedName name="i_landuse_is_dual" localSheetId="0">General!$P$80:$P$115</definedName>
+    <definedName name="i_landuse_is_dual" localSheetId="0">General!$Q$80:$Q$115</definedName>
     <definedName name="i_len_f">StructuralSA!$I$157</definedName>
     <definedName name="i_len_l">Stock!$M$160</definedName>
     <definedName name="i_len_m">Stock!$L$160</definedName>
@@ -401,7 +402,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="M79" authorId="0" shapeId="0" xr:uid="{40DF5727-F08F-40E0-9958-8A507CE17D1A}">
+    <comment ref="J79" authorId="0" shapeId="0" xr:uid="{FDA4D9B5-6EAD-41B3-8D7C-2C4ABEDC1C1E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael Young (21512438):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+is this landuse baled usually (all landuses can be tactically baled but this is to tell AFO which landuses are meant to be baled i.e. which landuses have yields that are entered at baled)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N79" authorId="0" shapeId="0" xr:uid="{40DF5727-F08F-40E0-9958-8A507CE17D1A}">
       <text>
         <r>
           <rPr>
@@ -425,7 +450,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q79" authorId="0" shapeId="0" xr:uid="{88CDE5B0-F826-4C1C-BBBC-47E28308B927}">
+    <comment ref="R79" authorId="0" shapeId="0" xr:uid="{88CDE5B0-F826-4C1C-BBBC-47E28308B927}">
       <text>
         <r>
           <rPr>
@@ -2255,7 +2280,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="392">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -3550,6 +3575,9 @@
   <si>
     <t>store condition score</t>
   </si>
+  <si>
+    <t>is baled</t>
+  </si>
 </sst>
 </file>
 
@@ -3561,7 +3589,7 @@
     <numFmt numFmtId="166" formatCode="0.00_)"/>
     <numFmt numFmtId="167" formatCode="[$-C09]dd\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3780,6 +3808,19 @@
       <color rgb="FF0000CC"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="40">
@@ -7232,12 +7273,12 @@
   </sheetPr>
   <dimension ref="A1:AT128"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J69" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <pane xSplit="9" ySplit="10" topLeftCell="J73" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="M80" sqref="M80"/>
+      <selection pane="bottomRight" activeCell="J80" sqref="J80:J96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -7496,7 +7537,7 @@
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
     </row>
-    <row r="7" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="33"/>
       <c r="C7" s="67">
@@ -7535,7 +7576,7 @@
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
     </row>
-    <row r="8" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="33"/>
       <c r="C8" s="67">
@@ -7568,7 +7609,7 @@
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
     </row>
-    <row r="9" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="33"/>
       <c r="C9" s="67">
@@ -7605,7 +7646,7 @@
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
     </row>
-    <row r="10" spans="1:28" ht="11.45" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="11.45" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="33" t="s">
         <v>20</v>
@@ -7751,7 +7792,7 @@
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
     </row>
-    <row r="14" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="45" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="33"/>
       <c r="C14" s="67">
@@ -7790,7 +7831,7 @@
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
     </row>
-    <row r="15" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="33"/>
       <c r="C15" s="67">
@@ -7825,7 +7866,7 @@
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
     </row>
-    <row r="16" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="33"/>
       <c r="C16" s="67">
@@ -7860,7 +7901,7 @@
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
     </row>
-    <row r="17" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="33"/>
       <c r="C17" s="67">
@@ -7907,7 +7948,7 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
     </row>
-    <row r="18" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="33"/>
       <c r="C18" s="67">
@@ -7944,7 +7985,7 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
     </row>
-    <row r="19" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="33"/>
       <c r="C19" s="67">
@@ -7981,7 +8022,7 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
     </row>
-    <row r="20" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="33"/>
       <c r="C20" s="67">
@@ -8018,7 +8059,7 @@
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
     </row>
-    <row r="21" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="33"/>
       <c r="C21" s="67">
@@ -8055,7 +8096,7 @@
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
     </row>
-    <row r="22" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="33"/>
       <c r="C22" s="67">
@@ -8090,7 +8131,7 @@
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
     </row>
-    <row r="23" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="33"/>
       <c r="C23" s="67">
@@ -10092,25 +10133,27 @@
       <c r="I79" s="161" t="s">
         <v>312</v>
       </c>
-      <c r="J79" s="2"/>
-      <c r="K79" s="161" t="s">
+      <c r="J79" s="161" t="s">
+        <v>391</v>
+      </c>
+      <c r="K79" s="2"/>
+      <c r="L79" s="161" t="s">
         <v>313</v>
       </c>
-      <c r="L79" s="2"/>
-      <c r="M79" s="161" t="s">
+      <c r="M79" s="2"/>
+      <c r="N79" s="161" t="s">
         <v>377</v>
       </c>
-      <c r="N79" s="2"/>
-      <c r="O79" s="161" t="s">
+      <c r="O79" s="2"/>
+      <c r="P79" s="161" t="s">
         <v>314</v>
       </c>
-      <c r="P79" s="161" t="s">
+      <c r="Q79" s="161" t="s">
         <v>375</v>
       </c>
-      <c r="Q79" s="161" t="s">
+      <c r="R79" s="161" t="s">
         <v>376</v>
       </c>
-      <c r="R79" s="2"/>
       <c r="S79" s="2"/>
       <c r="T79" s="2"/>
       <c r="U79" s="2"/>
@@ -10137,26 +10180,28 @@
       <c r="I80" s="162" t="s">
         <v>315</v>
       </c>
-      <c r="J80" s="165"/>
-      <c r="K80" s="162" t="s">
+      <c r="J80" s="162" t="b">
+        <v>0</v>
+      </c>
+      <c r="K80" s="55"/>
+      <c r="L80" s="162" t="s">
         <v>316</v>
       </c>
-      <c r="L80" s="165"/>
-      <c r="M80" s="210" t="s">
+      <c r="M80" s="165"/>
+      <c r="N80" s="210" t="s">
         <v>374</v>
       </c>
-      <c r="N80" s="165"/>
-      <c r="O80" s="162" t="s">
+      <c r="O80" s="165"/>
+      <c r="P80" s="162" t="s">
         <v>316</v>
       </c>
-      <c r="P80" s="162" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q80" s="206" t="str">
-        <f>O80</f>
+      <c r="Q80" s="162" t="b">
+        <v>0</v>
+      </c>
+      <c r="R80" s="206" t="str">
+        <f>P80</f>
         <v>a</v>
       </c>
-      <c r="R80" s="2"/>
       <c r="S80" s="2"/>
       <c r="T80" s="2"/>
       <c r="U80" s="2"/>
@@ -10180,24 +10225,26 @@
       <c r="I81" s="163" t="s">
         <v>317</v>
       </c>
-      <c r="J81" s="165"/>
-      <c r="K81" s="163" t="s">
+      <c r="J81" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="K81" s="55"/>
+      <c r="L81" s="163" t="s">
         <v>318</v>
       </c>
-      <c r="L81" s="165"/>
-      <c r="M81" s="209"/>
-      <c r="N81" s="165"/>
-      <c r="O81" s="163" t="s">
+      <c r="M81" s="165"/>
+      <c r="N81" s="209"/>
+      <c r="O81" s="165"/>
+      <c r="P81" s="163" t="s">
         <v>318</v>
       </c>
-      <c r="P81" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q81" s="207" t="str">
-        <f t="shared" ref="Q81:Q115" si="4">O81</f>
+      <c r="Q81" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R81" s="207" t="str">
+        <f t="shared" ref="R81:R115" si="4">P81</f>
         <v>ar</v>
       </c>
-      <c r="R81" s="2"/>
       <c r="S81" s="2"/>
       <c r="T81" s="2"/>
       <c r="U81" s="2"/>
@@ -10221,24 +10268,26 @@
       <c r="I82" s="163" t="s">
         <v>319</v>
       </c>
-      <c r="J82" s="165"/>
-      <c r="K82" s="163" t="s">
+      <c r="J82" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="K82" s="55"/>
+      <c r="L82" s="163" t="s">
         <v>374</v>
       </c>
-      <c r="L82" s="165"/>
       <c r="M82" s="165"/>
       <c r="N82" s="165"/>
-      <c r="O82" s="163" t="s">
+      <c r="O82" s="165"/>
+      <c r="P82" s="163" t="s">
         <v>374</v>
       </c>
-      <c r="P82" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q82" s="207" t="str">
+      <c r="Q82" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R82" s="207" t="str">
         <f t="shared" si="4"/>
         <v>a2</v>
       </c>
-      <c r="R82" s="2"/>
       <c r="S82" s="2"/>
       <c r="T82" s="2"/>
       <c r="U82" s="2"/>
@@ -10262,24 +10311,26 @@
       <c r="I83" s="163" t="s">
         <v>321</v>
       </c>
-      <c r="J83" s="165"/>
-      <c r="K83" s="163" t="s">
+      <c r="J83" s="163" t="b">
+        <v>1</v>
+      </c>
+      <c r="K83" s="55"/>
+      <c r="L83" s="163" t="s">
         <v>320</v>
       </c>
-      <c r="L83" s="165"/>
       <c r="M83" s="165"/>
       <c r="N83" s="165"/>
-      <c r="O83" s="163" t="s">
+      <c r="O83" s="165"/>
+      <c r="P83" s="163" t="s">
         <v>315</v>
       </c>
-      <c r="P83" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q83" s="207" t="str">
+      <c r="Q83" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R83" s="207" t="str">
         <f t="shared" si="4"/>
         <v>b</v>
       </c>
-      <c r="R83" s="2"/>
       <c r="S83" s="2"/>
       <c r="T83" s="2"/>
       <c r="U83" s="2"/>
@@ -10303,24 +10354,26 @@
       <c r="I84" s="163" t="s">
         <v>323</v>
       </c>
-      <c r="J84" s="165"/>
-      <c r="K84" s="163" t="s">
+      <c r="J84" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="K84" s="55"/>
+      <c r="L84" s="163" t="s">
         <v>322</v>
       </c>
-      <c r="L84" s="165"/>
       <c r="M84" s="165"/>
       <c r="N84" s="165"/>
-      <c r="O84" s="163" t="s">
+      <c r="O84" s="165"/>
+      <c r="P84" s="163" t="s">
         <v>317</v>
       </c>
-      <c r="P84" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q84" s="207" t="str">
+      <c r="Q84" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R84" s="207" t="str">
         <f t="shared" si="4"/>
         <v>bd</v>
       </c>
-      <c r="R84" s="2"/>
       <c r="S84" s="2"/>
       <c r="T84" s="2"/>
       <c r="U84" s="2"/>
@@ -10344,24 +10397,26 @@
       <c r="I85" s="163" t="s">
         <v>325</v>
       </c>
-      <c r="J85" s="165"/>
-      <c r="K85" s="163" t="s">
+      <c r="J85" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="K85" s="55"/>
+      <c r="L85" s="163" t="s">
         <v>324</v>
       </c>
-      <c r="L85" s="165"/>
       <c r="M85" s="165"/>
       <c r="N85" s="165"/>
-      <c r="O85" s="163" t="s">
+      <c r="O85" s="165"/>
+      <c r="P85" s="163" t="s">
         <v>319</v>
       </c>
-      <c r="P85" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q85" s="207" t="str">
+      <c r="Q85" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R85" s="207" t="str">
         <f t="shared" si="4"/>
         <v>f</v>
       </c>
-      <c r="R85" s="2"/>
       <c r="S85" s="2"/>
       <c r="T85" s="2"/>
       <c r="U85" s="2"/>
@@ -10385,24 +10440,26 @@
       <c r="I86" s="163" t="s">
         <v>327</v>
       </c>
-      <c r="J86" s="165"/>
-      <c r="K86" s="163" t="s">
+      <c r="J86" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="K86" s="55"/>
+      <c r="L86" s="163" t="s">
         <v>326</v>
       </c>
-      <c r="L86" s="165"/>
       <c r="M86" s="165"/>
       <c r="N86" s="165"/>
-      <c r="O86" s="163" t="s">
+      <c r="O86" s="165"/>
+      <c r="P86" s="163" t="s">
         <v>321</v>
       </c>
-      <c r="P86" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q86" s="207" t="str">
+      <c r="Q86" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R86" s="207" t="str">
         <f t="shared" si="4"/>
         <v>h</v>
       </c>
-      <c r="R86" s="2"/>
       <c r="S86" s="2"/>
       <c r="T86" s="2"/>
       <c r="U86" s="2"/>
@@ -10426,24 +10483,26 @@
       <c r="I87" s="163" t="s">
         <v>329</v>
       </c>
-      <c r="J87" s="165"/>
-      <c r="K87" s="163" t="s">
+      <c r="J87" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="K87" s="55"/>
+      <c r="L87" s="163" t="s">
         <v>328</v>
       </c>
-      <c r="L87" s="165"/>
       <c r="M87" s="165"/>
       <c r="N87" s="165"/>
-      <c r="O87" s="163" t="s">
+      <c r="O87" s="165"/>
+      <c r="P87" s="163" t="s">
         <v>323</v>
       </c>
-      <c r="P87" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q87" s="207" t="str">
+      <c r="Q87" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R87" s="207" t="str">
         <f t="shared" si="4"/>
         <v>i</v>
       </c>
-      <c r="R87" s="2"/>
       <c r="S87" s="2"/>
       <c r="T87" s="2"/>
       <c r="U87" s="2"/>
@@ -10467,24 +10526,26 @@
       <c r="I88" s="163" t="s">
         <v>331</v>
       </c>
-      <c r="J88" s="165"/>
-      <c r="K88" s="163" t="s">
+      <c r="J88" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="K88" s="55"/>
+      <c r="L88" s="163" t="s">
         <v>366</v>
       </c>
-      <c r="L88" s="165"/>
       <c r="M88" s="165"/>
       <c r="N88" s="165"/>
-      <c r="O88" s="163" t="s">
+      <c r="O88" s="165"/>
+      <c r="P88" s="163" t="s">
         <v>322</v>
       </c>
-      <c r="P88" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q88" s="207" t="str">
+      <c r="Q88" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R88" s="207" t="str">
         <f t="shared" si="4"/>
         <v>j</v>
       </c>
-      <c r="R88" s="2"/>
       <c r="S88" s="2"/>
       <c r="T88" s="2"/>
       <c r="U88" s="2"/>
@@ -10508,24 +10569,26 @@
       <c r="I89" s="163" t="s">
         <v>333</v>
       </c>
-      <c r="J89" s="165"/>
-      <c r="K89" s="163" t="s">
+      <c r="J89" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="K89" s="55"/>
+      <c r="L89" s="163" t="s">
         <v>330</v>
       </c>
-      <c r="L89" s="165"/>
       <c r="M89" s="165"/>
       <c r="N89" s="165"/>
-      <c r="O89" s="163" t="s">
+      <c r="O89" s="165"/>
+      <c r="P89" s="163" t="s">
         <v>324</v>
       </c>
-      <c r="P89" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q89" s="207" t="str">
+      <c r="Q89" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R89" s="207" t="str">
         <f t="shared" si="4"/>
         <v>jc</v>
       </c>
-      <c r="R89" s="2"/>
       <c r="S89" s="2"/>
       <c r="T89" s="2"/>
       <c r="U89" s="2"/>
@@ -10549,24 +10612,26 @@
       <c r="I90" s="163" t="s">
         <v>335</v>
       </c>
-      <c r="J90" s="165"/>
-      <c r="K90" s="163" t="s">
+      <c r="J90" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="K90" s="55"/>
+      <c r="L90" s="163" t="s">
         <v>332</v>
       </c>
-      <c r="L90" s="165"/>
       <c r="M90" s="165"/>
       <c r="N90" s="165"/>
-      <c r="O90" s="163" t="s">
+      <c r="O90" s="165"/>
+      <c r="P90" s="163" t="s">
         <v>326</v>
       </c>
-      <c r="P90" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q90" s="207" t="str">
+      <c r="Q90" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R90" s="207" t="str">
         <f t="shared" si="4"/>
         <v>jr</v>
       </c>
-      <c r="R90" s="2"/>
       <c r="S90" s="2"/>
       <c r="T90" s="2"/>
       <c r="U90" s="2"/>
@@ -10590,24 +10655,26 @@
       <c r="I91" s="163" t="s">
         <v>337</v>
       </c>
-      <c r="J91" s="165"/>
-      <c r="K91" s="163" t="s">
+      <c r="J91" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="K91" s="55"/>
+      <c r="L91" s="163" t="s">
         <v>334</v>
       </c>
-      <c r="L91" s="165"/>
       <c r="M91" s="165"/>
       <c r="N91" s="165"/>
-      <c r="O91" s="163" t="s">
+      <c r="O91" s="165"/>
+      <c r="P91" s="163" t="s">
         <v>325</v>
       </c>
-      <c r="P91" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q91" s="207" t="str">
+      <c r="Q91" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R91" s="207" t="str">
         <f t="shared" si="4"/>
         <v>k</v>
       </c>
-      <c r="R91" s="2"/>
       <c r="S91" s="2"/>
       <c r="T91" s="2"/>
       <c r="U91" s="2"/>
@@ -10631,24 +10698,26 @@
       <c r="I92" s="163" t="s">
         <v>339</v>
       </c>
-      <c r="J92" s="165"/>
-      <c r="K92" s="163" t="s">
+      <c r="J92" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="K92" s="55"/>
+      <c r="L92" s="163" t="s">
         <v>336</v>
       </c>
-      <c r="L92" s="165"/>
       <c r="M92" s="165"/>
       <c r="N92" s="165"/>
-      <c r="O92" s="163" t="s">
+      <c r="O92" s="165"/>
+      <c r="P92" s="163" t="s">
         <v>327</v>
       </c>
-      <c r="P92" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q92" s="207" t="str">
+      <c r="Q92" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R92" s="207" t="str">
         <f t="shared" si="4"/>
         <v>l</v>
       </c>
-      <c r="R92" s="2"/>
       <c r="S92" s="2"/>
       <c r="T92" s="2"/>
       <c r="U92" s="2"/>
@@ -10672,24 +10741,26 @@
       <c r="I93" s="163" t="s">
         <v>341</v>
       </c>
-      <c r="J93" s="165"/>
-      <c r="K93" s="163" t="s">
+      <c r="J93" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="K93" s="55"/>
+      <c r="L93" s="163" t="s">
         <v>338</v>
       </c>
-      <c r="L93" s="165"/>
       <c r="M93" s="165"/>
       <c r="N93" s="165"/>
-      <c r="O93" s="163" t="s">
+      <c r="O93" s="165"/>
+      <c r="P93" s="163" t="s">
         <v>320</v>
       </c>
-      <c r="P93" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q93" s="207" t="str">
+      <c r="Q93" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R93" s="207" t="str">
         <f t="shared" si="4"/>
         <v>m</v>
       </c>
-      <c r="R93" s="2"/>
       <c r="S93" s="2"/>
       <c r="T93" s="2"/>
       <c r="U93" s="2"/>
@@ -10713,24 +10784,26 @@
       <c r="I94" s="163" t="s">
         <v>343</v>
       </c>
-      <c r="J94" s="165"/>
-      <c r="K94" s="163" t="s">
+      <c r="J94" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="K94" s="55"/>
+      <c r="L94" s="163" t="s">
         <v>340</v>
       </c>
-      <c r="L94" s="165"/>
       <c r="M94" s="165"/>
       <c r="N94" s="165"/>
-      <c r="O94" s="163" t="s">
+      <c r="O94" s="165"/>
+      <c r="P94" s="163" t="s">
         <v>329</v>
       </c>
-      <c r="P94" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q94" s="207" t="str">
+      <c r="Q94" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R94" s="207" t="str">
         <f t="shared" si="4"/>
         <v>o</v>
       </c>
-      <c r="R94" s="2"/>
       <c r="S94" s="2"/>
       <c r="T94" s="2"/>
       <c r="U94" s="2"/>
@@ -10754,24 +10827,26 @@
       <c r="I95" s="163" t="s">
         <v>345</v>
       </c>
-      <c r="J95" s="165"/>
-      <c r="K95" s="163" t="s">
+      <c r="J95" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="K95" s="55"/>
+      <c r="L95" s="163" t="s">
         <v>342</v>
       </c>
-      <c r="L95" s="165"/>
       <c r="M95" s="165"/>
       <c r="N95" s="165"/>
-      <c r="O95" s="163" t="s">
+      <c r="O95" s="165"/>
+      <c r="P95" s="163" t="s">
         <v>331</v>
       </c>
-      <c r="P95" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q95" s="207" t="str">
+      <c r="Q95" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R95" s="207" t="str">
         <f t="shared" si="4"/>
         <v>od</v>
       </c>
-      <c r="R95" s="2"/>
       <c r="S95" s="2"/>
       <c r="T95" s="2"/>
       <c r="U95" s="2"/>
@@ -10795,24 +10870,26 @@
       <c r="I96" s="164" t="s">
         <v>347</v>
       </c>
-      <c r="J96" s="165"/>
-      <c r="K96" s="163" t="s">
+      <c r="J96" s="164" t="b">
+        <v>0</v>
+      </c>
+      <c r="K96" s="55"/>
+      <c r="L96" s="163" t="s">
         <v>344</v>
       </c>
-      <c r="L96" s="165"/>
       <c r="M96" s="165"/>
       <c r="N96" s="165"/>
-      <c r="O96" s="163" t="s">
+      <c r="O96" s="165"/>
+      <c r="P96" s="163" t="s">
         <v>333</v>
       </c>
-      <c r="P96" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q96" s="207" t="str">
+      <c r="Q96" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R96" s="207" t="str">
         <f t="shared" si="4"/>
         <v>of</v>
       </c>
-      <c r="R96" s="2"/>
       <c r="S96" s="2"/>
       <c r="T96" s="2"/>
       <c r="U96" s="2"/>
@@ -10834,24 +10911,24 @@
       <c r="G97" s="4"/>
       <c r="H97" s="2"/>
       <c r="I97" s="53"/>
-      <c r="J97" s="2"/>
-      <c r="K97" s="163" t="s">
+      <c r="J97" s="53"/>
+      <c r="K97" s="2"/>
+      <c r="L97" s="163" t="s">
         <v>346</v>
       </c>
-      <c r="L97" s="165"/>
       <c r="M97" s="165"/>
       <c r="N97" s="165"/>
-      <c r="O97" s="163" t="s">
+      <c r="O97" s="165"/>
+      <c r="P97" s="163" t="s">
         <v>335</v>
       </c>
-      <c r="P97" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q97" s="207" t="str">
+      <c r="Q97" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R97" s="207" t="str">
         <f t="shared" si="4"/>
         <v>r</v>
       </c>
-      <c r="R97" s="2"/>
       <c r="S97" s="2"/>
       <c r="T97" s="2"/>
       <c r="U97" s="2"/>
@@ -10874,23 +10951,23 @@
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
       <c r="J98" s="2"/>
-      <c r="K98" s="164" t="s">
+      <c r="K98" s="2"/>
+      <c r="L98" s="164" t="s">
         <v>348</v>
       </c>
-      <c r="L98" s="148"/>
       <c r="M98" s="148"/>
       <c r="N98" s="148"/>
-      <c r="O98" s="163" t="s">
+      <c r="O98" s="148"/>
+      <c r="P98" s="163" t="s">
         <v>337</v>
       </c>
-      <c r="P98" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q98" s="207" t="str">
+      <c r="Q98" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R98" s="207" t="str">
         <f t="shared" si="4"/>
         <v>rd</v>
       </c>
-      <c r="R98" s="2"/>
       <c r="S98" s="2"/>
       <c r="T98" s="2"/>
       <c r="U98" s="2"/>
@@ -10913,21 +10990,21 @@
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
       <c r="J99" s="2"/>
-      <c r="K99" s="53"/>
-      <c r="L99" s="148"/>
+      <c r="K99" s="2"/>
+      <c r="L99" s="53"/>
       <c r="M99" s="148"/>
       <c r="N99" s="148"/>
-      <c r="O99" s="163" t="s">
+      <c r="O99" s="148"/>
+      <c r="P99" s="163" t="s">
         <v>328</v>
       </c>
-      <c r="P99" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q99" s="207" t="str">
+      <c r="Q99" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R99" s="207" t="str">
         <f t="shared" si="4"/>
         <v>s</v>
       </c>
-      <c r="R99" s="2"/>
       <c r="S99" s="2"/>
       <c r="T99" s="2"/>
       <c r="U99" s="2"/>
@@ -10950,21 +11027,21 @@
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
       <c r="J100" s="2"/>
-      <c r="K100" s="53"/>
-      <c r="L100" s="148"/>
+      <c r="K100" s="2"/>
+      <c r="L100" s="53"/>
       <c r="M100" s="148"/>
       <c r="N100" s="148"/>
-      <c r="O100" s="163" t="s">
+      <c r="O100" s="148"/>
+      <c r="P100" s="163" t="s">
         <v>366</v>
       </c>
-      <c r="P100" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q100" s="207" t="str">
+      <c r="Q100" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R100" s="207" t="str">
         <f t="shared" si="4"/>
         <v>sp</v>
       </c>
-      <c r="R100" s="2"/>
       <c r="S100" s="2"/>
       <c r="T100" s="2"/>
       <c r="U100" s="2"/>
@@ -10988,20 +11065,20 @@
       <c r="I101" s="2"/>
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
-      <c r="L101" s="148"/>
+      <c r="L101" s="2"/>
       <c r="M101" s="148"/>
       <c r="N101" s="148"/>
-      <c r="O101" s="163" t="s">
+      <c r="O101" s="148"/>
+      <c r="P101" s="163" t="s">
         <v>330</v>
       </c>
-      <c r="P101" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q101" s="207" t="str">
+      <c r="Q101" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R101" s="207" t="str">
         <f t="shared" si="4"/>
         <v>sr</v>
       </c>
-      <c r="R101" s="2"/>
       <c r="S101" s="2"/>
       <c r="T101" s="2"/>
       <c r="U101" s="2"/>
@@ -11025,20 +11102,20 @@
       <c r="I102" s="2"/>
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
-      <c r="L102" s="148"/>
+      <c r="L102" s="2"/>
       <c r="M102" s="148"/>
       <c r="N102" s="148"/>
-      <c r="O102" s="163" t="s">
+      <c r="O102" s="148"/>
+      <c r="P102" s="163" t="s">
         <v>332</v>
       </c>
-      <c r="P102" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q102" s="207" t="str">
+      <c r="Q102" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R102" s="207" t="str">
         <f t="shared" si="4"/>
         <v>t</v>
       </c>
-      <c r="R102" s="2"/>
       <c r="S102" s="2"/>
       <c r="T102" s="2"/>
       <c r="U102" s="2"/>
@@ -11062,20 +11139,20 @@
       <c r="I103" s="2"/>
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
-      <c r="L103" s="148"/>
+      <c r="L103" s="2"/>
       <c r="M103" s="148"/>
       <c r="N103" s="148"/>
-      <c r="O103" s="163" t="s">
+      <c r="O103" s="148"/>
+      <c r="P103" s="163" t="s">
         <v>334</v>
       </c>
-      <c r="P103" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q103" s="207" t="str">
+      <c r="Q103" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R103" s="207" t="str">
         <f t="shared" si="4"/>
         <v>tc</v>
       </c>
-      <c r="R103" s="2"/>
       <c r="S103" s="2"/>
       <c r="T103" s="2"/>
       <c r="U103" s="2"/>
@@ -11099,20 +11176,20 @@
       <c r="I104" s="2"/>
       <c r="J104" s="2"/>
       <c r="K104" s="2"/>
-      <c r="L104" s="148"/>
+      <c r="L104" s="2"/>
       <c r="M104" s="148"/>
       <c r="N104" s="148"/>
-      <c r="O104" s="163" t="s">
+      <c r="O104" s="148"/>
+      <c r="P104" s="163" t="s">
         <v>336</v>
       </c>
-      <c r="P104" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q104" s="207" t="str">
+      <c r="Q104" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R104" s="207" t="str">
         <f t="shared" si="4"/>
         <v>tr</v>
       </c>
-      <c r="R104" s="2"/>
       <c r="S104" s="2"/>
       <c r="T104" s="2"/>
       <c r="U104" s="2"/>
@@ -11136,20 +11213,20 @@
       <c r="I105" s="2"/>
       <c r="J105" s="2"/>
       <c r="K105" s="2"/>
-      <c r="L105" s="148"/>
+      <c r="L105" s="2"/>
       <c r="M105" s="148"/>
       <c r="N105" s="148"/>
-      <c r="O105" s="163" t="s">
+      <c r="O105" s="148"/>
+      <c r="P105" s="163" t="s">
         <v>338</v>
       </c>
-      <c r="P105" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q105" s="207" t="str">
+      <c r="Q105" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R105" s="207" t="str">
         <f t="shared" si="4"/>
         <v>u</v>
       </c>
-      <c r="R105" s="2"/>
       <c r="S105" s="2"/>
       <c r="T105" s="2"/>
       <c r="U105" s="2"/>
@@ -11173,20 +11250,20 @@
       <c r="I106" s="2"/>
       <c r="J106" s="2"/>
       <c r="K106" s="2"/>
-      <c r="L106" s="148"/>
+      <c r="L106" s="2"/>
       <c r="M106" s="148"/>
       <c r="N106" s="148"/>
-      <c r="O106" s="163" t="s">
+      <c r="O106" s="148"/>
+      <c r="P106" s="163" t="s">
         <v>340</v>
       </c>
-      <c r="P106" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q106" s="207" t="str">
+      <c r="Q106" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R106" s="207" t="str">
         <f t="shared" si="4"/>
         <v>uc</v>
       </c>
-      <c r="R106" s="2"/>
       <c r="S106" s="2"/>
       <c r="T106" s="2"/>
       <c r="U106" s="2"/>
@@ -11210,20 +11287,20 @@
       <c r="I107" s="2"/>
       <c r="J107" s="2"/>
       <c r="K107" s="2"/>
-      <c r="L107" s="148"/>
+      <c r="L107" s="2"/>
       <c r="M107" s="148"/>
       <c r="N107" s="148"/>
-      <c r="O107" s="163" t="s">
+      <c r="O107" s="148"/>
+      <c r="P107" s="163" t="s">
         <v>342</v>
       </c>
-      <c r="P107" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q107" s="207" t="str">
+      <c r="Q107" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R107" s="207" t="str">
         <f t="shared" si="4"/>
         <v>ur</v>
       </c>
-      <c r="R107" s="2"/>
       <c r="S107" s="2"/>
       <c r="T107" s="2"/>
       <c r="U107" s="2"/>
@@ -11247,20 +11324,20 @@
       <c r="I108" s="2"/>
       <c r="J108" s="2"/>
       <c r="K108" s="2"/>
-      <c r="L108" s="148"/>
+      <c r="L108" s="2"/>
       <c r="M108" s="148"/>
       <c r="N108" s="148"/>
-      <c r="O108" s="163" t="s">
+      <c r="O108" s="148"/>
+      <c r="P108" s="163" t="s">
         <v>339</v>
       </c>
-      <c r="P108" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q108" s="207" t="str">
+      <c r="Q108" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R108" s="207" t="str">
         <f t="shared" si="4"/>
         <v>v</v>
       </c>
-      <c r="R108" s="2"/>
       <c r="S108" s="2"/>
       <c r="T108" s="2"/>
       <c r="U108" s="2"/>
@@ -11284,20 +11361,20 @@
       <c r="I109" s="2"/>
       <c r="J109" s="2"/>
       <c r="K109" s="2"/>
-      <c r="L109" s="148"/>
+      <c r="L109" s="2"/>
       <c r="M109" s="148"/>
       <c r="N109" s="148"/>
-      <c r="O109" s="163" t="s">
+      <c r="O109" s="148"/>
+      <c r="P109" s="163" t="s">
         <v>341</v>
       </c>
-      <c r="P109" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q109" s="207" t="str">
+      <c r="Q109" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R109" s="207" t="str">
         <f t="shared" si="4"/>
         <v>w</v>
       </c>
-      <c r="R109" s="2"/>
       <c r="S109" s="2"/>
       <c r="T109" s="2"/>
       <c r="U109" s="2"/>
@@ -11321,20 +11398,20 @@
       <c r="I110" s="2"/>
       <c r="J110" s="2"/>
       <c r="K110" s="2"/>
-      <c r="L110" s="148"/>
+      <c r="L110" s="2"/>
       <c r="M110" s="148"/>
       <c r="N110" s="148"/>
-      <c r="O110" s="163" t="s">
+      <c r="O110" s="148"/>
+      <c r="P110" s="163" t="s">
         <v>343</v>
       </c>
-      <c r="P110" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q110" s="207" t="str">
+      <c r="Q110" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R110" s="207" t="str">
         <f t="shared" si="4"/>
         <v>wd</v>
       </c>
-      <c r="R110" s="2"/>
       <c r="S110" s="2"/>
       <c r="T110" s="2"/>
       <c r="U110" s="2"/>
@@ -11361,20 +11438,20 @@
       <c r="I111" s="2"/>
       <c r="J111" s="2"/>
       <c r="K111" s="2"/>
-      <c r="L111" s="148"/>
+      <c r="L111" s="2"/>
       <c r="M111" s="148"/>
       <c r="N111" s="148"/>
-      <c r="O111" s="163" t="s">
+      <c r="O111" s="148"/>
+      <c r="P111" s="163" t="s">
         <v>344</v>
       </c>
-      <c r="P111" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q111" s="207" t="str">
+      <c r="Q111" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R111" s="207" t="str">
         <f t="shared" si="4"/>
         <v>x</v>
       </c>
-      <c r="R111" s="2"/>
       <c r="S111" s="2"/>
       <c r="T111" s="2"/>
       <c r="U111" s="2"/>
@@ -11401,20 +11478,20 @@
       <c r="I112" s="2"/>
       <c r="J112" s="2"/>
       <c r="K112" s="2"/>
-      <c r="L112" s="148"/>
+      <c r="L112" s="2"/>
       <c r="M112" s="148"/>
       <c r="N112" s="148"/>
-      <c r="O112" s="163" t="s">
+      <c r="O112" s="148"/>
+      <c r="P112" s="163" t="s">
         <v>346</v>
       </c>
-      <c r="P112" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q112" s="207" t="str">
+      <c r="Q112" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R112" s="207" t="str">
         <f t="shared" si="4"/>
         <v>xc</v>
       </c>
-      <c r="R112" s="2"/>
       <c r="S112" s="2"/>
       <c r="T112" s="2"/>
       <c r="U112" s="2"/>
@@ -11441,20 +11518,20 @@
       <c r="I113" s="2"/>
       <c r="J113" s="2"/>
       <c r="K113" s="2"/>
-      <c r="L113" s="148"/>
+      <c r="L113" s="2"/>
       <c r="M113" s="148"/>
       <c r="N113" s="148"/>
-      <c r="O113" s="163" t="s">
+      <c r="O113" s="148"/>
+      <c r="P113" s="163" t="s">
         <v>348</v>
       </c>
-      <c r="P113" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q113" s="207" t="str">
+      <c r="Q113" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R113" s="207" t="str">
         <f t="shared" si="4"/>
         <v>xr</v>
       </c>
-      <c r="R113" s="2"/>
       <c r="S113" s="2"/>
       <c r="T113" s="2"/>
       <c r="U113" s="2"/>
@@ -11481,20 +11558,20 @@
       <c r="I114" s="2"/>
       <c r="J114" s="2"/>
       <c r="K114" s="2"/>
-      <c r="L114" s="148"/>
+      <c r="L114" s="2"/>
       <c r="M114" s="148"/>
       <c r="N114" s="148"/>
-      <c r="O114" s="163" t="s">
+      <c r="O114" s="148"/>
+      <c r="P114" s="163" t="s">
         <v>345</v>
       </c>
-      <c r="P114" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q114" s="207" t="str">
+      <c r="Q114" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R114" s="207" t="str">
         <f t="shared" si="4"/>
         <v>z</v>
       </c>
-      <c r="R114" s="2"/>
       <c r="S114" s="2"/>
       <c r="T114" s="2"/>
       <c r="U114" s="2"/>
@@ -11521,20 +11598,20 @@
       <c r="I115" s="2"/>
       <c r="J115" s="2"/>
       <c r="K115" s="2"/>
-      <c r="L115" s="148"/>
+      <c r="L115" s="2"/>
       <c r="M115" s="148"/>
       <c r="N115" s="148"/>
-      <c r="O115" s="164" t="s">
+      <c r="O115" s="148"/>
+      <c r="P115" s="164" t="s">
         <v>347</v>
       </c>
-      <c r="P115" s="164" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q115" s="208" t="str">
+      <c r="Q115" s="164" t="b">
+        <v>0</v>
+      </c>
+      <c r="R115" s="208" t="str">
         <f t="shared" si="4"/>
         <v>zd</v>
       </c>
-      <c r="R115" s="2"/>
       <c r="S115" s="2"/>
       <c r="T115" s="2"/>
       <c r="U115" s="2"/>
@@ -34533,7 +34610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE3626F-D681-4ABD-B02A-5C870438CFCF}">
   <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
remove unused named ranges
</commit_message>
<xml_diff>
--- a/ExcelInputs/Structural.xlsx
+++ b/ExcelInputs/Structural.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\Models\AFO\ExcelInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D209B64-8C0D-4B3F-8296-6FE455BFBDA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C181A69-6433-40B2-B06A-1EEBCCDC9425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -19,11 +19,6 @@
     <sheet name="Report Settings" sheetId="26" r:id="rId4"/>
     <sheet name="Admin" sheetId="3" state="hidden" r:id="rId5"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId6"/>
-    <externalReference r:id="rId7"/>
-    <externalReference r:id="rId8"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Admin!$E$13:$Y$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">General!$E$10:$W$22</definedName>
@@ -31,13 +26,13 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">StructuralSA!$E$10:$W$22</definedName>
     <definedName name="a_nfoet_b1">Stock!$L$153:$V$153</definedName>
     <definedName name="a_nyatf_b1">Stock!$L$154:$V$154</definedName>
-    <definedName name="dry_groups" localSheetId="0">General!$I$48:$J$48</definedName>
-    <definedName name="foo_levels" localSheetId="0">General!$I$50:$K$50</definedName>
+    <definedName name="dry_groups" localSheetId="0">General!$I$47:$J$47</definedName>
+    <definedName name="foo_levels" localSheetId="0">General!$I$49:$K$49</definedName>
     <definedName name="grain_pools" localSheetId="0">General!$I$44:$J$44</definedName>
-    <definedName name="grazing_int" localSheetId="0">General!$I$49:$L$49</definedName>
+    <definedName name="grazing_int" localSheetId="0">General!$I$48:$L$48</definedName>
     <definedName name="i_a0_pos">Stock!$I$43</definedName>
     <definedName name="i_a1_pos">Stock!$I$44</definedName>
-    <definedName name="i_a2_idx" localSheetId="0">General!$N$80</definedName>
+    <definedName name="i_a2_idx" localSheetId="0">General!$N$79</definedName>
     <definedName name="i_adjp_cfw_initial_w0" localSheetId="2">StructuralSA!$K$99</definedName>
     <definedName name="i_adjp_cfw_initial_w1" localSheetId="2">StructuralSA!$P$99:$P$101</definedName>
     <definedName name="i_adjp_cfw_initial_w3" localSheetId="2">StructuralSA!$U$99:$U$101</definedName>
@@ -54,8 +49,6 @@
     <definedName name="i_age_max_offs">Stock!$I$64</definedName>
     <definedName name="i_b0_pos">Stock!$I$45</definedName>
     <definedName name="i_b1_pos">Stock!$I$46</definedName>
-    <definedName name="i_break">[1]General!$Z$104:$Z$113</definedName>
-    <definedName name="i_break_date">[2]General!$R$104:$R$113</definedName>
     <definedName name="i_btrt_idx_offs">Stock!$L$268:$Q$268</definedName>
     <definedName name="i_chill_adj_b1">Stock!$L$156:$V$156</definedName>
     <definedName name="i_confinement_n0">StructuralSA!$K$87</definedName>
@@ -64,7 +57,6 @@
     <definedName name="i_core_dvp_types_f1" localSheetId="1">Stock!$J$313:$L$313</definedName>
     <definedName name="i_d_pos">Stock!$I$47</definedName>
     <definedName name="i_dams_user_fvp_date_iu">StructuralSA!$S$45:$V$47</definedName>
-    <definedName name="i_date_node_zm">[2]General!$T$104:$V$113</definedName>
     <definedName name="i_density_n0" localSheetId="2">StructuralSA!$L$87</definedName>
     <definedName name="i_density_n1" localSheetId="2">StructuralSA!$O$87:$O$94</definedName>
     <definedName name="i_density_n3" localSheetId="2">StructuralSA!$U$87:$U$94</definedName>
@@ -72,7 +64,7 @@
     <definedName name="i_dvp_mask_f3">StructuralSA!$J$53:$O$53</definedName>
     <definedName name="i_e0_pos">Stock!$I$48</definedName>
     <definedName name="i_e1_pos">Stock!$I$49</definedName>
-    <definedName name="i_enterprises_c0" localSheetId="0">General!$I$56:$J$56</definedName>
+    <definedName name="i_enterprises_c0" localSheetId="0">General!$I$55:$J$55</definedName>
     <definedName name="i_feedsupply_itn_max">Stock!$I$72</definedName>
     <definedName name="i_fixed_dvp_mask_f1">Stock!$J$314:$L$314</definedName>
     <definedName name="i_fixed_fvp_mask_dams">Stock!$J$312:$L$312</definedName>
@@ -83,13 +75,13 @@
     <definedName name="i_fvp_mask_dams">StructuralSA!$N$43:$R$43</definedName>
     <definedName name="i_fvp_mask_offs">StructuralSA!$J$52:$O$52</definedName>
     <definedName name="i_generate_with_t" localSheetId="2">StructuralSA!$P$121</definedName>
-    <definedName name="i_history4_req" localSheetId="0">General!$R$80:$R$115</definedName>
+    <definedName name="i_history4_req" localSheetId="0">General!$R$79:$R$114</definedName>
     <definedName name="i_i_pos">Stock!$I$50</definedName>
-    <definedName name="i_idx_k" localSheetId="0">General!$P$80:$P$115</definedName>
-    <definedName name="i_idx_k1" localSheetId="0">General!$I$80:$I$96</definedName>
-    <definedName name="i_idx_k2" localSheetId="0">General!$L$80:$L$98</definedName>
+    <definedName name="i_idx_k" localSheetId="0">General!$P$79:$P$114</definedName>
+    <definedName name="i_idx_k1" localSheetId="0">General!$I$79:$I$95</definedName>
+    <definedName name="i_idx_k2" localSheetId="0">General!$L$79:$L$97</definedName>
     <definedName name="i_initial_b1">Stock!$L$155:$V$155</definedName>
-    <definedName name="i_is_baled_k" localSheetId="0">General!$J$80:$J$96</definedName>
+    <definedName name="i_is_baled_k" localSheetId="0">General!$J$79:$J$95</definedName>
     <definedName name="i_is_dry_b1">Stock!$L$149:$V$149</definedName>
     <definedName name="i_k2_idx_dams">Stock!$L$202:$V$204</definedName>
     <definedName name="i_k2_pos">Stock!$I$51</definedName>
@@ -98,7 +90,7 @@
     <definedName name="i_k5_pos">Stock!$I$53</definedName>
     <definedName name="i_lag_organs">Stock!$I$70</definedName>
     <definedName name="i_lag_wool">Stock!$I$69</definedName>
-    <definedName name="i_landuse_is_dual" localSheetId="0">General!$Q$80:$Q$115</definedName>
+    <definedName name="i_landuse_is_dual" localSheetId="0">General!$Q$79:$Q$114</definedName>
     <definedName name="i_len_f">StructuralSA!$I$157</definedName>
     <definedName name="i_len_l">Stock!$M$160</definedName>
     <definedName name="i_len_m">Stock!$L$160</definedName>
@@ -131,7 +123,6 @@
     <definedName name="i_nv_upper_p6">StructuralSA!$J$161:$S$161</definedName>
     <definedName name="i_offs_user_fvp_date_iu" localSheetId="2">StructuralSA!$P$54:$R$56</definedName>
     <definedName name="i_p_pos">Stock!$I$55</definedName>
-    <definedName name="i_pasture_stage_p6z">[2]Annual!$K$20:$T$29</definedName>
     <definedName name="i_prejoin_offset">Stock!$I$66</definedName>
     <definedName name="i_progeny_w2_len">StructuralSA!$Q$79</definedName>
     <definedName name="i_r2adjust_inc">StructuralSA!$U$120</definedName>
@@ -139,7 +130,6 @@
     <definedName name="i_rev_number" localSheetId="2">StructuralSA!$I$122</definedName>
     <definedName name="i_rev_trait_inc" localSheetId="2">StructuralSA!$I$129:$I$136</definedName>
     <definedName name="i_rev_trait_name" localSheetId="2">StructuralSA!$H$129:$H$136</definedName>
-    <definedName name="i_sim_periods_year" localSheetId="3">[2]FeedSupply!$P$28</definedName>
     <definedName name="i_sim_periods_year">Stock!$I$62</definedName>
     <definedName name="i_store_cs_rep" localSheetId="3">'Report Settings'!$K$18</definedName>
     <definedName name="i_store_feedbud" localSheetId="3">'Report Settings'!$U$18</definedName>
@@ -168,14 +158,11 @@
     <definedName name="ia_prepost_b1">Stock!$L$152:$V$152</definedName>
     <definedName name="ia_sire_dsegroup">Stock!$L$144</definedName>
     <definedName name="ia_yatf_dsegroup_b1">Stock!$L$146:$V$146</definedName>
-    <definedName name="labour_period_len" localSheetId="0">General!$I$54</definedName>
+    <definedName name="labour_period_len" localSheetId="0">General!$I$53</definedName>
     <definedName name="pastures" localSheetId="0">General!$I$46:$L$46</definedName>
-    <definedName name="pastures_exist" localSheetId="0">General!$I$47:$L$47</definedName>
-    <definedName name="phase_len" localSheetId="0">General!$I$52</definedName>
+    <definedName name="phase_len" localSheetId="0">General!$I$51</definedName>
     <definedName name="rdvp_type_r">Stock!$J$318:$L$318</definedName>
     <definedName name="worker_levels" localSheetId="0">General!$I$42:$K$42</definedName>
-    <definedName name="YieldBySoil.i">[3]Rotation!$J$47:$V$59</definedName>
-    <definedName name="YieldBySoil.n">[3]Rotation!$H$47:$H$59</definedName>
     <definedName name="ZA.Gridlines" localSheetId="4">Admin!$L$29</definedName>
     <definedName name="ZA.Headers" localSheetId="4">Admin!$L$30</definedName>
     <definedName name="ZA.HeightRow" localSheetId="4">Admin!$J$26</definedName>
@@ -278,35 +265,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-annual must be first in the list</t>
+annual must be first in the list. Define which pastures exist in pinp.</t>
         </r>
       </text>
     </comment>
-    <comment ref="H47" authorId="0" shapeId="0" xr:uid="{5C8A94C4-3AA8-470F-98DB-74504D6919F3}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Michael Young (21512438):</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-define which pastures exist (inputs must exist). SA can be used to adjust which pastures included in a given trial (property input).</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H48" authorId="0" shapeId="0" xr:uid="{EE762646-B744-4CD9-A953-31EA528567F4}">
+    <comment ref="H47" authorId="0" shapeId="0" xr:uid="{EE762646-B744-4CD9-A953-31EA528567F4}">
       <text>
         <r>
           <rPr>
@@ -330,7 +293,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H49" authorId="0" shapeId="0" xr:uid="{13AA60DC-F1B5-4C6A-9480-13EBF4BC7B06}">
+    <comment ref="H48" authorId="0" shapeId="0" xr:uid="{13AA60DC-F1B5-4C6A-9480-13EBF4BC7B06}">
       <text>
         <r>
           <rPr>
@@ -354,7 +317,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H50" authorId="0" shapeId="0" xr:uid="{46711F29-44B1-4DAE-8B05-697DCE7A28E8}">
+    <comment ref="H49" authorId="0" shapeId="0" xr:uid="{46711F29-44B1-4DAE-8B05-697DCE7A28E8}">
       <text>
         <r>
           <rPr>
@@ -378,7 +341,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H54" authorId="0" shapeId="0" xr:uid="{A77A1A40-0F21-448B-8603-3590BB2B7FCC}">
+    <comment ref="H53" authorId="0" shapeId="0" xr:uid="{A77A1A40-0F21-448B-8603-3590BB2B7FCC}">
       <text>
         <r>
           <rPr>
@@ -402,7 +365,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J79" authorId="0" shapeId="0" xr:uid="{FDA4D9B5-6EAD-41B3-8D7C-2C4ABEDC1C1E}">
+    <comment ref="J78" authorId="0" shapeId="0" xr:uid="{FDA4D9B5-6EAD-41B3-8D7C-2C4ABEDC1C1E}">
       <text>
         <r>
           <rPr>
@@ -426,7 +389,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N79" authorId="0" shapeId="0" xr:uid="{40DF5727-F08F-40E0-9958-8A507CE17D1A}">
+    <comment ref="N78" authorId="0" shapeId="0" xr:uid="{40DF5727-F08F-40E0-9958-8A507CE17D1A}">
       <text>
         <r>
           <rPr>
@@ -450,7 +413,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R79" authorId="0" shapeId="0" xr:uid="{88CDE5B0-F826-4C1C-BBBC-47E28308B927}">
+    <comment ref="R78" authorId="0" shapeId="0" xr:uid="{88CDE5B0-F826-4C1C-BBBC-47E28308B927}">
       <text>
         <r>
           <rPr>
@@ -2280,7 +2243,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="391">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -3279,9 +3242,6 @@
   </si>
   <si>
     <t>generate with t axis</t>
-  </si>
-  <si>
-    <t>pastures inputs exist</t>
   </si>
   <si>
     <t>Landuses</t>
@@ -5877,1100 +5837,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Home"/>
-      <sheetName val="General"/>
-      <sheetName val="Sup Feed"/>
-      <sheetName val="Crop"/>
-      <sheetName val="CropGrazing"/>
-      <sheetName val="Saltbush"/>
-      <sheetName val="Periods"/>
-      <sheetName val="Labour"/>
-      <sheetName val="Annual"/>
-      <sheetName val="Understory"/>
-      <sheetName val="Sheep"/>
-      <sheetName val="FeedSupply"/>
-      <sheetName val="Mach"/>
-      <sheetName val="CropResidue"/>
-      <sheetName val="Finance"/>
-      <sheetName val="MVEnergy"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="17">
-          <cell r="H17" t="str">
-            <v>b</v>
-          </cell>
-        </row>
-        <row r="105">
-          <cell r="Z105" t="str">
-            <v>Break of season</v>
-          </cell>
-        </row>
-        <row r="107">
-          <cell r="Z107">
-            <v>119</v>
-          </cell>
-        </row>
-        <row r="108">
-          <cell r="Z108">
-            <v>105</v>
-          </cell>
-        </row>
-        <row r="109">
-          <cell r="Z109">
-            <v>105</v>
-          </cell>
-        </row>
-        <row r="110">
-          <cell r="Z110">
-            <v>105</v>
-          </cell>
-        </row>
-        <row r="111">
-          <cell r="Z111">
-            <v>105</v>
-          </cell>
-        </row>
-        <row r="112">
-          <cell r="Z112">
-            <v>126</v>
-          </cell>
-        </row>
-        <row r="113">
-          <cell r="Z113">
-            <v>126</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10">
-        <row r="266">
-          <cell r="I266">
-            <v>2019</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="11">
-        <row r="266">
-          <cell r="I266" t="str">
-            <v>4th cycle</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Home"/>
-      <sheetName val="General"/>
-      <sheetName val="Sup Feed"/>
-      <sheetName val="Crop"/>
-      <sheetName val="CropGrazing"/>
-      <sheetName val="Saltbush"/>
-      <sheetName val="Periods"/>
-      <sheetName val="Labour"/>
-      <sheetName val="Annual"/>
-      <sheetName val="Understory"/>
-      <sheetName val="Sheep"/>
-      <sheetName val="FeedSupply"/>
-      <sheetName val="Mach"/>
-      <sheetName val="CropResidue"/>
-      <sheetName val="Finance"/>
-      <sheetName val="MVEnergy"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="104">
-          <cell r="R104">
-            <v>43595</v>
-          </cell>
-          <cell r="T104">
-            <v>105</v>
-          </cell>
-          <cell r="U104">
-            <v>217</v>
-          </cell>
-          <cell r="V104">
-            <v>287</v>
-          </cell>
-        </row>
-        <row r="105">
-          <cell r="R105">
-            <v>43572</v>
-          </cell>
-          <cell r="T105">
-            <v>105</v>
-          </cell>
-          <cell r="U105">
-            <v>217</v>
-          </cell>
-          <cell r="V105">
-            <v>287</v>
-          </cell>
-        </row>
-        <row r="106">
-          <cell r="R106">
-            <v>43572</v>
-          </cell>
-          <cell r="T106" t="str">
-            <v>Early brk</v>
-          </cell>
-          <cell r="U106" t="str">
-            <v>Med brk</v>
-          </cell>
-          <cell r="V106" t="str">
-            <v>Spring</v>
-          </cell>
-        </row>
-        <row r="107">
-          <cell r="R107">
-            <v>43595</v>
-          </cell>
-          <cell r="T107">
-            <v>105</v>
-          </cell>
-          <cell r="U107">
-            <v>217</v>
-          </cell>
-          <cell r="V107">
-            <v>287</v>
-          </cell>
-        </row>
-        <row r="108">
-          <cell r="R108">
-            <v>43572</v>
-          </cell>
-          <cell r="T108">
-            <v>105</v>
-          </cell>
-          <cell r="U108">
-            <v>217</v>
-          </cell>
-          <cell r="V108">
-            <v>287</v>
-          </cell>
-        </row>
-        <row r="109">
-          <cell r="R109">
-            <v>43572</v>
-          </cell>
-          <cell r="T109">
-            <v>105</v>
-          </cell>
-          <cell r="U109">
-            <v>217</v>
-          </cell>
-          <cell r="V109">
-            <v>287</v>
-          </cell>
-        </row>
-        <row r="110">
-          <cell r="R110">
-            <v>43572</v>
-          </cell>
-          <cell r="T110">
-            <v>105</v>
-          </cell>
-          <cell r="U110">
-            <v>217</v>
-          </cell>
-          <cell r="V110">
-            <v>287</v>
-          </cell>
-        </row>
-        <row r="111">
-          <cell r="R111">
-            <v>43593</v>
-          </cell>
-          <cell r="T111">
-            <v>105</v>
-          </cell>
-          <cell r="U111">
-            <v>217</v>
-          </cell>
-          <cell r="V111">
-            <v>287</v>
-          </cell>
-        </row>
-        <row r="112">
-          <cell r="R112">
-            <v>43593</v>
-          </cell>
-          <cell r="T112">
-            <v>105</v>
-          </cell>
-          <cell r="U112">
-            <v>217</v>
-          </cell>
-          <cell r="V112">
-            <v>287</v>
-          </cell>
-        </row>
-        <row r="113">
-          <cell r="R113">
-            <v>43593</v>
-          </cell>
-          <cell r="T113">
-            <v>105</v>
-          </cell>
-          <cell r="U113">
-            <v>217</v>
-          </cell>
-          <cell r="V113">
-            <v>287</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8">
-        <row r="20">
-          <cell r="K20">
-            <v>0</v>
-          </cell>
-          <cell r="L20">
-            <v>0</v>
-          </cell>
-          <cell r="M20">
-            <v>0</v>
-          </cell>
-          <cell r="N20">
-            <v>0</v>
-          </cell>
-          <cell r="O20">
-            <v>0</v>
-          </cell>
-          <cell r="P20">
-            <v>0</v>
-          </cell>
-          <cell r="Q20">
-            <v>0</v>
-          </cell>
-          <cell r="R20">
-            <v>0</v>
-          </cell>
-          <cell r="S20">
-            <v>0</v>
-          </cell>
-          <cell r="T20">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="K21">
-            <v>0</v>
-          </cell>
-          <cell r="L21">
-            <v>0</v>
-          </cell>
-          <cell r="M21">
-            <v>0</v>
-          </cell>
-          <cell r="N21">
-            <v>0</v>
-          </cell>
-          <cell r="O21">
-            <v>0</v>
-          </cell>
-          <cell r="P21">
-            <v>0</v>
-          </cell>
-          <cell r="Q21">
-            <v>0</v>
-          </cell>
-          <cell r="R21">
-            <v>0</v>
-          </cell>
-          <cell r="S21">
-            <v>0</v>
-          </cell>
-          <cell r="T21">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="K22">
-            <v>1</v>
-          </cell>
-          <cell r="L22">
-            <v>1</v>
-          </cell>
-          <cell r="M22">
-            <v>1</v>
-          </cell>
-          <cell r="N22">
-            <v>1</v>
-          </cell>
-          <cell r="O22">
-            <v>1</v>
-          </cell>
-          <cell r="P22">
-            <v>1</v>
-          </cell>
-          <cell r="Q22">
-            <v>1</v>
-          </cell>
-          <cell r="R22">
-            <v>1</v>
-          </cell>
-          <cell r="S22">
-            <v>1</v>
-          </cell>
-          <cell r="T22">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="K23">
-            <v>1</v>
-          </cell>
-          <cell r="L23">
-            <v>1</v>
-          </cell>
-          <cell r="M23">
-            <v>1</v>
-          </cell>
-          <cell r="N23">
-            <v>1</v>
-          </cell>
-          <cell r="O23">
-            <v>1</v>
-          </cell>
-          <cell r="P23">
-            <v>1</v>
-          </cell>
-          <cell r="Q23">
-            <v>1</v>
-          </cell>
-          <cell r="R23">
-            <v>1</v>
-          </cell>
-          <cell r="S23">
-            <v>1</v>
-          </cell>
-          <cell r="T23">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="K24">
-            <v>1</v>
-          </cell>
-          <cell r="L24">
-            <v>1</v>
-          </cell>
-          <cell r="M24">
-            <v>1</v>
-          </cell>
-          <cell r="N24">
-            <v>1</v>
-          </cell>
-          <cell r="O24">
-            <v>1</v>
-          </cell>
-          <cell r="P24">
-            <v>1</v>
-          </cell>
-          <cell r="Q24">
-            <v>1</v>
-          </cell>
-          <cell r="R24">
-            <v>1</v>
-          </cell>
-          <cell r="S24">
-            <v>1</v>
-          </cell>
-          <cell r="T24">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="K25">
-            <v>1</v>
-          </cell>
-          <cell r="L25">
-            <v>1</v>
-          </cell>
-          <cell r="M25">
-            <v>1</v>
-          </cell>
-          <cell r="N25">
-            <v>1</v>
-          </cell>
-          <cell r="O25">
-            <v>1</v>
-          </cell>
-          <cell r="P25">
-            <v>1</v>
-          </cell>
-          <cell r="Q25">
-            <v>1</v>
-          </cell>
-          <cell r="R25">
-            <v>1</v>
-          </cell>
-          <cell r="S25">
-            <v>1</v>
-          </cell>
-          <cell r="T25">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="K26">
-            <v>1</v>
-          </cell>
-          <cell r="L26">
-            <v>1</v>
-          </cell>
-          <cell r="M26">
-            <v>1</v>
-          </cell>
-          <cell r="N26">
-            <v>1</v>
-          </cell>
-          <cell r="O26">
-            <v>1</v>
-          </cell>
-          <cell r="P26">
-            <v>1</v>
-          </cell>
-          <cell r="Q26">
-            <v>1</v>
-          </cell>
-          <cell r="R26">
-            <v>1</v>
-          </cell>
-          <cell r="S26">
-            <v>1</v>
-          </cell>
-          <cell r="T26">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="K27">
-            <v>1</v>
-          </cell>
-          <cell r="L27">
-            <v>1</v>
-          </cell>
-          <cell r="M27">
-            <v>1</v>
-          </cell>
-          <cell r="N27">
-            <v>1</v>
-          </cell>
-          <cell r="O27">
-            <v>1</v>
-          </cell>
-          <cell r="P27">
-            <v>1</v>
-          </cell>
-          <cell r="Q27">
-            <v>1</v>
-          </cell>
-          <cell r="R27">
-            <v>1</v>
-          </cell>
-          <cell r="S27">
-            <v>1</v>
-          </cell>
-          <cell r="T27">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="K28">
-            <v>1</v>
-          </cell>
-          <cell r="L28">
-            <v>1</v>
-          </cell>
-          <cell r="M28">
-            <v>1</v>
-          </cell>
-          <cell r="N28">
-            <v>1</v>
-          </cell>
-          <cell r="O28">
-            <v>1</v>
-          </cell>
-          <cell r="P28">
-            <v>1</v>
-          </cell>
-          <cell r="Q28">
-            <v>1</v>
-          </cell>
-          <cell r="R28">
-            <v>1</v>
-          </cell>
-          <cell r="S28">
-            <v>1</v>
-          </cell>
-          <cell r="T28">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="K29">
-            <v>1</v>
-          </cell>
-          <cell r="L29">
-            <v>1</v>
-          </cell>
-          <cell r="M29">
-            <v>1</v>
-          </cell>
-          <cell r="N29">
-            <v>1</v>
-          </cell>
-          <cell r="O29">
-            <v>1</v>
-          </cell>
-          <cell r="P29">
-            <v>1</v>
-          </cell>
-          <cell r="Q29">
-            <v>1</v>
-          </cell>
-          <cell r="R29">
-            <v>1</v>
-          </cell>
-          <cell r="S29">
-            <v>1</v>
-          </cell>
-          <cell r="T29">
-            <v>1</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11">
-        <row r="28">
-          <cell r="P28">
-            <v>52</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Controls"/>
-      <sheetName val="Gloss"/>
-      <sheetName val="MPS"/>
-      <sheetName val="FullRepStd"/>
-      <sheetName val="Names"/>
-      <sheetName val="GenData"/>
-      <sheetName val="Mach"/>
-      <sheetName val="Rotation"/>
-      <sheetName val="FullRep callibration"/>
-      <sheetName val="MRY callibration"/>
-      <sheetName val="Table Fill"/>
-      <sheetName val="Summ-MRY (2)"/>
-      <sheetName val="Sum-MRY"/>
-      <sheetName val="EL-Std"/>
-      <sheetName val="Summ-Std"/>
-      <sheetName val="Sheep"/>
-      <sheetName val="Grazingcrop"/>
-      <sheetName val="LabourSheep"/>
-      <sheetName val="Labour"/>
-      <sheetName val="LabourCrop"/>
-      <sheetName val="Emissions"/>
-      <sheetName val="EmPast1"/>
-      <sheetName val="Annual"/>
-      <sheetName val="Lucerne"/>
-      <sheetName val="TederaP"/>
-      <sheetName val="TederaM"/>
-      <sheetName val="Stubble"/>
-      <sheetName val="ChaffPiles"/>
-      <sheetName val="FodCrop"/>
-      <sheetName val="Saltbush"/>
-      <sheetName val="Sheep$"/>
-      <sheetName val="Luc Structural"/>
-      <sheetName val="LucRotnData"/>
-      <sheetName val="Luc Rotn Inputs"/>
-      <sheetName val="LucFertMPS"/>
-      <sheetName val="Blank"/>
-      <sheetName val="Starter"/>
-      <sheetName val="MinROE"/>
-      <sheetName val="MVEnergy"/>
-      <sheetName val="ExpLib"/>
-      <sheetName val="Chart2"/>
-      <sheetName val="Rep-MVP"/>
-      <sheetName val="RepLib"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7">
-        <row r="47">
-          <cell r="H47"/>
-          <cell r="J47"/>
-          <cell r="K47"/>
-          <cell r="L47"/>
-          <cell r="M47"/>
-          <cell r="N47"/>
-          <cell r="O47"/>
-          <cell r="P47"/>
-          <cell r="Q47"/>
-          <cell r="R47"/>
-          <cell r="S47"/>
-          <cell r="T47"/>
-          <cell r="U47"/>
-          <cell r="V47"/>
-        </row>
-        <row r="48">
-          <cell r="H48" t="str">
-            <v>T</v>
-          </cell>
-          <cell r="J48">
-            <v>0.54</v>
-          </cell>
-          <cell r="K48">
-            <v>0.68</v>
-          </cell>
-          <cell r="L48">
-            <v>0.78</v>
-          </cell>
-          <cell r="M48">
-            <v>1</v>
-          </cell>
-          <cell r="N48">
-            <v>0</v>
-          </cell>
-          <cell r="O48">
-            <v>0</v>
-          </cell>
-          <cell r="P48">
-            <v>0</v>
-          </cell>
-          <cell r="Q48"/>
-          <cell r="R48"/>
-          <cell r="S48"/>
-          <cell r="T48"/>
-          <cell r="U48"/>
-          <cell r="V48"/>
-        </row>
-        <row r="49">
-          <cell r="H49" t="str">
-            <v>R</v>
-          </cell>
-          <cell r="J49">
-            <v>0</v>
-          </cell>
-          <cell r="K49">
-            <v>0</v>
-          </cell>
-          <cell r="L49">
-            <v>0</v>
-          </cell>
-          <cell r="M49">
-            <v>1</v>
-          </cell>
-          <cell r="N49">
-            <v>0</v>
-          </cell>
-          <cell r="O49">
-            <v>0</v>
-          </cell>
-          <cell r="P49">
-            <v>0</v>
-          </cell>
-          <cell r="Q49"/>
-          <cell r="R49"/>
-          <cell r="S49"/>
-          <cell r="T49"/>
-          <cell r="U49"/>
-          <cell r="V49"/>
-        </row>
-        <row r="50">
-          <cell r="H50" t="str">
-            <v>W</v>
-          </cell>
-          <cell r="J50">
-            <v>0.67</v>
-          </cell>
-          <cell r="K50">
-            <v>0.77</v>
-          </cell>
-          <cell r="L50">
-            <v>0.85</v>
-          </cell>
-          <cell r="M50">
-            <v>1</v>
-          </cell>
-          <cell r="N50">
-            <v>0</v>
-          </cell>
-          <cell r="O50">
-            <v>0</v>
-          </cell>
-          <cell r="P50">
-            <v>0</v>
-          </cell>
-          <cell r="Q50"/>
-          <cell r="R50"/>
-          <cell r="S50"/>
-          <cell r="T50"/>
-          <cell r="U50"/>
-          <cell r="V50"/>
-        </row>
-        <row r="51">
-          <cell r="H51" t="str">
-            <v>F</v>
-          </cell>
-          <cell r="J51">
-            <v>0</v>
-          </cell>
-          <cell r="K51">
-            <v>0</v>
-          </cell>
-          <cell r="L51">
-            <v>0</v>
-          </cell>
-          <cell r="M51">
-            <v>0</v>
-          </cell>
-          <cell r="N51">
-            <v>0</v>
-          </cell>
-          <cell r="O51">
-            <v>0</v>
-          </cell>
-          <cell r="P51">
-            <v>0</v>
-          </cell>
-          <cell r="Q51"/>
-          <cell r="R51"/>
-          <cell r="S51"/>
-          <cell r="T51"/>
-          <cell r="U51"/>
-          <cell r="V51"/>
-        </row>
-        <row r="52">
-          <cell r="H52" t="str">
-            <v>O</v>
-          </cell>
-          <cell r="J52">
-            <v>0.7</v>
-          </cell>
-          <cell r="K52">
-            <v>0.8</v>
-          </cell>
-          <cell r="L52">
-            <v>0.87</v>
-          </cell>
-          <cell r="M52">
-            <v>1</v>
-          </cell>
-          <cell r="N52">
-            <v>0</v>
-          </cell>
-          <cell r="O52">
-            <v>0</v>
-          </cell>
-          <cell r="P52">
-            <v>0</v>
-          </cell>
-          <cell r="Q52"/>
-          <cell r="R52"/>
-          <cell r="S52"/>
-          <cell r="T52"/>
-          <cell r="U52"/>
-          <cell r="V52"/>
-        </row>
-        <row r="53">
-          <cell r="H53" t="str">
-            <v>B</v>
-          </cell>
-          <cell r="J53">
-            <v>0.63</v>
-          </cell>
-          <cell r="K53">
-            <v>0.75</v>
-          </cell>
-          <cell r="L53">
-            <v>0.83</v>
-          </cell>
-          <cell r="M53">
-            <v>1</v>
-          </cell>
-          <cell r="N53">
-            <v>0</v>
-          </cell>
-          <cell r="O53">
-            <v>0</v>
-          </cell>
-          <cell r="P53">
-            <v>0</v>
-          </cell>
-          <cell r="Q53"/>
-          <cell r="R53"/>
-          <cell r="S53"/>
-          <cell r="T53"/>
-          <cell r="U53"/>
-          <cell r="V53"/>
-        </row>
-        <row r="54">
-          <cell r="H54" t="str">
-            <v>L</v>
-          </cell>
-          <cell r="J54">
-            <v>0</v>
-          </cell>
-          <cell r="K54">
-            <v>0.31</v>
-          </cell>
-          <cell r="L54">
-            <v>0.55000000000000004</v>
-          </cell>
-          <cell r="M54">
-            <v>1</v>
-          </cell>
-          <cell r="N54">
-            <v>0</v>
-          </cell>
-          <cell r="O54">
-            <v>0</v>
-          </cell>
-          <cell r="P54">
-            <v>0</v>
-          </cell>
-          <cell r="Q54"/>
-          <cell r="R54"/>
-          <cell r="S54"/>
-          <cell r="T54"/>
-          <cell r="U54"/>
-          <cell r="V54"/>
-        </row>
-        <row r="55">
-          <cell r="H55" t="str">
-            <v>H</v>
-          </cell>
-          <cell r="J55">
-            <v>0.86</v>
-          </cell>
-          <cell r="K55">
-            <v>0.9</v>
-          </cell>
-          <cell r="L55">
-            <v>0.94</v>
-          </cell>
-          <cell r="M55">
-            <v>1</v>
-          </cell>
-          <cell r="N55">
-            <v>0</v>
-          </cell>
-          <cell r="O55">
-            <v>0</v>
-          </cell>
-          <cell r="P55">
-            <v>0</v>
-          </cell>
-          <cell r="Q55"/>
-          <cell r="R55"/>
-          <cell r="S55"/>
-          <cell r="T55"/>
-          <cell r="U55"/>
-          <cell r="V55"/>
-        </row>
-        <row r="56">
-          <cell r="H56" t="str">
-            <v>D</v>
-          </cell>
-          <cell r="J56">
-            <v>0</v>
-          </cell>
-          <cell r="K56">
-            <v>0</v>
-          </cell>
-          <cell r="L56">
-            <v>0</v>
-          </cell>
-          <cell r="M56">
-            <v>0</v>
-          </cell>
-          <cell r="N56">
-            <v>0</v>
-          </cell>
-          <cell r="O56">
-            <v>0</v>
-          </cell>
-          <cell r="P56">
-            <v>0</v>
-          </cell>
-          <cell r="Q56"/>
-          <cell r="R56"/>
-          <cell r="S56"/>
-          <cell r="T56"/>
-          <cell r="U56"/>
-          <cell r="V56"/>
-        </row>
-        <row r="57">
-          <cell r="H57" t="str">
-            <v>Z</v>
-          </cell>
-          <cell r="J57">
-            <v>0</v>
-          </cell>
-          <cell r="K57">
-            <v>0</v>
-          </cell>
-          <cell r="L57">
-            <v>0</v>
-          </cell>
-          <cell r="M57">
-            <v>0</v>
-          </cell>
-          <cell r="N57">
-            <v>0</v>
-          </cell>
-          <cell r="O57">
-            <v>0</v>
-          </cell>
-          <cell r="P57">
-            <v>0</v>
-          </cell>
-          <cell r="Q57"/>
-          <cell r="R57"/>
-          <cell r="S57"/>
-          <cell r="T57"/>
-          <cell r="U57"/>
-          <cell r="V57"/>
-        </row>
-        <row r="58">
-          <cell r="H58" t="str">
-            <v>A</v>
-          </cell>
-          <cell r="J58">
-            <v>0</v>
-          </cell>
-          <cell r="K58">
-            <v>0</v>
-          </cell>
-          <cell r="L58">
-            <v>0</v>
-          </cell>
-          <cell r="M58">
-            <v>0</v>
-          </cell>
-          <cell r="N58">
-            <v>0</v>
-          </cell>
-          <cell r="O58">
-            <v>0</v>
-          </cell>
-          <cell r="P58">
-            <v>0</v>
-          </cell>
-          <cell r="Q58"/>
-          <cell r="R58"/>
-          <cell r="S58"/>
-          <cell r="T58"/>
-          <cell r="U58"/>
-          <cell r="V58"/>
-        </row>
-        <row r="59">
-          <cell r="H59"/>
-          <cell r="J59"/>
-          <cell r="K59"/>
-          <cell r="L59"/>
-          <cell r="M59"/>
-          <cell r="N59"/>
-          <cell r="O59"/>
-          <cell r="P59"/>
-          <cell r="Q59"/>
-          <cell r="R59"/>
-          <cell r="S59"/>
-          <cell r="T59"/>
-          <cell r="U59"/>
-          <cell r="V59"/>
-        </row>
-      </sheetData>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7271,14 +6137,14 @@
   <sheetPr codeName="Sheet2">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AT128"/>
+  <dimension ref="A1:AT127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J73" activePane="bottomRight" state="frozen"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <pane xSplit="9" ySplit="10" topLeftCell="J35" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="J80" sqref="J80:J96"/>
+      <selection pane="bottomRight" activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -7810,7 +6676,7 @@
         <v>44719.411846643503</v>
       </c>
       <c r="J14" s="215" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K14" s="216"/>
       <c r="L14" s="216"/>
@@ -8370,7 +7236,7 @@
       <c r="A30" s="1"/>
       <c r="B30" s="33"/>
       <c r="C30" s="73">
-        <f>INT(MAX($C$41:$C$57))+1</f>
+        <f>INT(MAX($C$41:$C$56))+1</f>
         <v>4</v>
       </c>
       <c r="D30" s="3"/>
@@ -8784,7 +7650,7 @@
       <c r="A42" s="1"/>
       <c r="B42" s="33"/>
       <c r="C42" s="73">
-        <f t="shared" ref="C42:C56" si="1">INT($C$31)+2</f>
+        <f t="shared" ref="C42:C55" si="1">INT($C$31)+2</f>
         <v>3</v>
       </c>
       <c r="D42" s="4"/>
@@ -8950,7 +7816,7 @@
         <v>176</v>
       </c>
       <c r="L46" s="97" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -8981,20 +7847,16 @@
       <c r="F47" s="5"/>
       <c r="G47" s="4"/>
       <c r="H47" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="I47" s="97" t="b">
-        <v>1</v>
-      </c>
-      <c r="J47" s="97" t="b">
-        <v>0</v>
-      </c>
-      <c r="K47" s="97" t="b">
-        <v>0</v>
-      </c>
-      <c r="L47" s="97" t="b">
-        <v>1</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="I47" s="97" t="s">
+        <v>177</v>
+      </c>
+      <c r="J47" s="97" t="s">
+        <v>178</v>
+      </c>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
@@ -9024,16 +7886,20 @@
       <c r="F48" s="5"/>
       <c r="G48" s="4"/>
       <c r="H48" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="I48" s="97" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="J48" s="97" t="s">
-        <v>178</v>
-      </c>
-      <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
+        <v>180</v>
+      </c>
+      <c r="K48" s="97" t="s">
+        <v>266</v>
+      </c>
+      <c r="L48" s="97" t="s">
+        <v>181</v>
+      </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
@@ -9063,20 +7929,18 @@
       <c r="F49" s="5"/>
       <c r="G49" s="4"/>
       <c r="H49" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I49" s="97" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="J49" s="97" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="K49" s="97" t="s">
-        <v>266</v>
-      </c>
-      <c r="L49" s="97" t="s">
-        <v>181</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="L49" s="2"/>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -9105,18 +7969,10 @@
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
       <c r="G50" s="4"/>
-      <c r="H50" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="I50" s="97" t="s">
-        <v>182</v>
-      </c>
-      <c r="J50" s="97" t="s">
-        <v>183</v>
-      </c>
-      <c r="K50" s="97" t="s">
-        <v>184</v>
-      </c>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -9146,8 +8002,12 @@
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
       <c r="G51" s="4"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
+      <c r="H51" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I51" s="97">
+        <v>6</v>
+      </c>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
@@ -9179,12 +8039,8 @@
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
       <c r="G52" s="4"/>
-      <c r="H52" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="I52" s="97">
-        <v>6</v>
-      </c>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
@@ -9216,8 +8072,12 @@
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
       <c r="G53" s="4"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
+      <c r="H53" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="I53" s="97">
+        <v>1</v>
+      </c>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
@@ -9249,12 +8109,8 @@
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
       <c r="G54" s="4"/>
-      <c r="H54" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="I54" s="97">
-        <v>1</v>
-      </c>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
@@ -9286,9 +8142,15 @@
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
       <c r="G55" s="4"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
+      <c r="H55" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="I55" s="97" t="s">
+        <v>304</v>
+      </c>
+      <c r="J55" s="97" t="s">
+        <v>305</v>
+      </c>
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
@@ -9307,62 +8169,58 @@
       <c r="Z55" s="1"/>
       <c r="AA55" s="1"/>
       <c r="AB55" s="1"/>
-    </row>
-    <row r="56" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="AD55" s="2"/>
+      <c r="AE55" s="2"/>
+      <c r="AF55" s="2"/>
+      <c r="AG55" s="2"/>
+      <c r="AH55" s="2"/>
+      <c r="AI55" s="2"/>
+      <c r="AJ55" s="2"/>
+      <c r="AK55" s="2"/>
+      <c r="AL55" s="2"/>
+      <c r="AM55" s="2"/>
+      <c r="AN55" s="2"/>
+      <c r="AO55" s="2"/>
+      <c r="AP55" s="4"/>
+      <c r="AQ55" s="81"/>
+      <c r="AR55" s="1"/>
+      <c r="AS55" s="1"/>
+      <c r="AT55" s="1"/>
+    </row>
+    <row r="56" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="33"/>
       <c r="C56" s="73">
-        <f t="shared" si="1"/>
+        <f>INT($C$31)+2.005</f>
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="4"/>
+      <c r="N56" s="4"/>
+      <c r="O56" s="4"/>
+      <c r="P56" s="4"/>
+      <c r="Q56" s="4"/>
+      <c r="R56" s="4"/>
+      <c r="S56" s="4"/>
+      <c r="T56" s="4"/>
+      <c r="U56" s="4"/>
+      <c r="V56" s="4"/>
+      <c r="W56" s="4"/>
+      <c r="X56" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D56" s="4"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="I56" s="97" t="s">
-        <v>304</v>
-      </c>
-      <c r="J56" s="97" t="s">
-        <v>305</v>
-      </c>
-      <c r="K56" s="2"/>
-      <c r="L56" s="2"/>
-      <c r="M56" s="2"/>
-      <c r="N56" s="2"/>
-      <c r="O56" s="2"/>
-      <c r="P56" s="2"/>
-      <c r="Q56" s="2"/>
-      <c r="R56" s="2"/>
-      <c r="S56" s="2"/>
-      <c r="T56" s="2"/>
-      <c r="U56" s="2"/>
-      <c r="V56" s="2"/>
-      <c r="W56" s="2"/>
-      <c r="X56" s="4"/>
       <c r="Y56" s="16"/>
       <c r="Z56" s="1"/>
       <c r="AA56" s="1"/>
       <c r="AB56" s="1"/>
-      <c r="AD56" s="2"/>
-      <c r="AE56" s="2"/>
-      <c r="AF56" s="2"/>
-      <c r="AG56" s="2"/>
-      <c r="AH56" s="2"/>
-      <c r="AI56" s="2"/>
-      <c r="AJ56" s="2"/>
-      <c r="AK56" s="2"/>
-      <c r="AL56" s="2"/>
-      <c r="AM56" s="2"/>
-      <c r="AN56" s="2"/>
-      <c r="AO56" s="2"/>
-      <c r="AP56" s="4"/>
-      <c r="AQ56" s="81"/>
-      <c r="AR56" s="1"/>
-      <c r="AS56" s="1"/>
-      <c r="AT56" s="1"/>
     </row>
     <row r="57" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
@@ -9391,111 +8249,109 @@
       <c r="U57" s="4"/>
       <c r="V57" s="4"/>
       <c r="W57" s="4"/>
-      <c r="X57" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="X57" s="4"/>
       <c r="Y57" s="16"/>
       <c r="Z57" s="1"/>
       <c r="AA57" s="1"/>
       <c r="AB57" s="1"/>
     </row>
-    <row r="58" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
-      <c r="B58" s="33"/>
-      <c r="C58" s="73">
-        <f>INT($C$31)+2.005</f>
-        <v>3.0049999999999999</v>
-      </c>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
-      <c r="H58" s="4"/>
-      <c r="I58" s="4"/>
-      <c r="J58" s="4"/>
-      <c r="K58" s="4"/>
-      <c r="L58" s="4"/>
-      <c r="M58" s="4"/>
-      <c r="N58" s="4"/>
-      <c r="O58" s="4"/>
-      <c r="P58" s="4"/>
-      <c r="Q58" s="4"/>
-      <c r="R58" s="4"/>
-      <c r="S58" s="4"/>
-      <c r="T58" s="4"/>
-      <c r="U58" s="4"/>
-      <c r="V58" s="4"/>
-      <c r="W58" s="4"/>
-      <c r="X58" s="4"/>
-      <c r="Y58" s="16"/>
+      <c r="B58" s="35"/>
+      <c r="C58" s="76">
+        <f>INT($C$31)+1.005</f>
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="17"/>
+      <c r="I58" s="17"/>
+      <c r="J58" s="17"/>
+      <c r="K58" s="17"/>
+      <c r="L58" s="17"/>
+      <c r="M58" s="17"/>
+      <c r="N58" s="17"/>
+      <c r="O58" s="17"/>
+      <c r="P58" s="17"/>
+      <c r="Q58" s="17"/>
+      <c r="R58" s="17"/>
+      <c r="S58" s="17"/>
+      <c r="T58" s="17"/>
+      <c r="U58" s="17"/>
+      <c r="V58" s="17"/>
+      <c r="W58" s="17"/>
+      <c r="X58" s="17"/>
+      <c r="Y58" s="18" t="s">
+        <v>1</v>
+      </c>
       <c r="Z58" s="1"/>
       <c r="AA58" s="1"/>
       <c r="AB58" s="1"/>
     </row>
-    <row r="59" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:46" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
-      <c r="B59" s="35"/>
-      <c r="C59" s="76">
-        <f>INT($C$31)+1.005</f>
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="17"/>
-      <c r="H59" s="17"/>
-      <c r="I59" s="17"/>
-      <c r="J59" s="17"/>
-      <c r="K59" s="17"/>
-      <c r="L59" s="17"/>
-      <c r="M59" s="17"/>
-      <c r="N59" s="17"/>
-      <c r="O59" s="17"/>
-      <c r="P59" s="17"/>
-      <c r="Q59" s="17"/>
-      <c r="R59" s="17"/>
-      <c r="S59" s="17"/>
-      <c r="T59" s="17"/>
-      <c r="U59" s="17"/>
-      <c r="V59" s="17"/>
-      <c r="W59" s="17"/>
-      <c r="X59" s="17"/>
-      <c r="Y59" s="18" t="s">
-        <v>1</v>
-      </c>
+      <c r="B59" s="19"/>
+      <c r="C59" s="77">
+        <f>INT($C$31)+0.005</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D59" s="19"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="19"/>
+      <c r="G59" s="19"/>
+      <c r="H59" s="19"/>
+      <c r="I59" s="19"/>
+      <c r="J59" s="19"/>
+      <c r="K59" s="19"/>
+      <c r="L59" s="19"/>
+      <c r="M59" s="19"/>
+      <c r="N59" s="19"/>
+      <c r="O59" s="19"/>
+      <c r="P59" s="19"/>
+      <c r="Q59" s="19"/>
+      <c r="R59" s="19"/>
+      <c r="S59" s="19"/>
+      <c r="T59" s="19"/>
+      <c r="U59" s="19"/>
+      <c r="V59" s="19"/>
+      <c r="W59" s="19"/>
+      <c r="X59" s="19"/>
+      <c r="Y59" s="19"/>
       <c r="Z59" s="1"/>
       <c r="AA59" s="1"/>
       <c r="AB59" s="1"/>
     </row>
-    <row r="60" spans="1:46" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
-      <c r="B60" s="19"/>
-      <c r="C60" s="77">
-        <f>INT($C$31)+0.005</f>
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="D60" s="19"/>
-      <c r="E60" s="19"/>
-      <c r="F60" s="19"/>
-      <c r="G60" s="19"/>
-      <c r="H60" s="19"/>
-      <c r="I60" s="19"/>
-      <c r="J60" s="19"/>
-      <c r="K60" s="19"/>
-      <c r="L60" s="19"/>
-      <c r="M60" s="19"/>
-      <c r="N60" s="19"/>
-      <c r="O60" s="19"/>
-      <c r="P60" s="19"/>
-      <c r="Q60" s="19"/>
-      <c r="R60" s="19"/>
-      <c r="S60" s="19"/>
-      <c r="T60" s="19"/>
-      <c r="U60" s="19"/>
-      <c r="V60" s="19"/>
-      <c r="W60" s="19"/>
-      <c r="X60" s="19"/>
-      <c r="Y60" s="19"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="73">
+        <f>INT($C$31)+2</f>
+        <v>3</v>
+      </c>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
+      <c r="R60" s="1"/>
+      <c r="S60" s="1"/>
+      <c r="T60" s="1"/>
+      <c r="U60" s="1"/>
+      <c r="V60" s="1"/>
+      <c r="W60" s="1"/>
+      <c r="X60" s="1"/>
+      <c r="Y60" s="1"/>
       <c r="Z60" s="1"/>
       <c r="AA60" s="1"/>
       <c r="AB60" s="1"/>
@@ -9533,243 +8389,243 @@
       <c r="AA61" s="1"/>
       <c r="AB61" s="1"/>
     </row>
-    <row r="62" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:46" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="73">
-        <f>INT($C$31)+2</f>
-        <v>3</v>
-      </c>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
-      <c r="J62" s="1"/>
-      <c r="K62" s="1"/>
-      <c r="L62" s="1"/>
-      <c r="M62" s="1"/>
-      <c r="N62" s="1"/>
-      <c r="O62" s="1"/>
-      <c r="P62" s="1"/>
-      <c r="Q62" s="1"/>
-      <c r="R62" s="1"/>
-      <c r="S62" s="1"/>
-      <c r="T62" s="1"/>
-      <c r="U62" s="1"/>
-      <c r="V62" s="1"/>
-      <c r="W62" s="1"/>
-      <c r="X62" s="1"/>
-      <c r="Y62" s="1"/>
+      <c r="B62" s="20"/>
+      <c r="C62" s="74">
+        <f>INT($C$31)+0.005</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D62" s="20"/>
+      <c r="E62" s="20"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="20"/>
+      <c r="H62" s="20"/>
+      <c r="I62" s="20"/>
+      <c r="J62" s="20"/>
+      <c r="K62" s="20"/>
+      <c r="L62" s="20"/>
+      <c r="M62" s="20"/>
+      <c r="N62" s="20"/>
+      <c r="O62" s="20"/>
+      <c r="P62" s="20"/>
+      <c r="Q62" s="20"/>
+      <c r="R62" s="20"/>
+      <c r="S62" s="20"/>
+      <c r="T62" s="20"/>
+      <c r="U62" s="20"/>
+      <c r="V62" s="20"/>
+      <c r="W62" s="20"/>
+      <c r="X62" s="20"/>
+      <c r="Y62" s="20"/>
       <c r="Z62" s="1"/>
       <c r="AA62" s="1"/>
       <c r="AB62" s="1"/>
     </row>
-    <row r="63" spans="1:46" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
-      <c r="B63" s="20"/>
-      <c r="C63" s="74">
-        <f>INT($C$31)+0.005</f>
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="D63" s="20"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="20"/>
-      <c r="G63" s="20"/>
-      <c r="H63" s="20"/>
-      <c r="I63" s="20"/>
-      <c r="J63" s="20"/>
-      <c r="K63" s="20"/>
-      <c r="L63" s="20"/>
-      <c r="M63" s="20"/>
-      <c r="N63" s="20"/>
-      <c r="O63" s="20"/>
-      <c r="P63" s="20"/>
-      <c r="Q63" s="20"/>
-      <c r="R63" s="20"/>
-      <c r="S63" s="20"/>
-      <c r="T63" s="20"/>
-      <c r="U63" s="20"/>
-      <c r="V63" s="20"/>
-      <c r="W63" s="20"/>
-      <c r="X63" s="20"/>
-      <c r="Y63" s="20"/>
+      <c r="B63" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C63" s="75">
+        <f>INT($C$31)+1.005</f>
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14"/>
+      <c r="J63" s="14"/>
+      <c r="K63" s="14"/>
+      <c r="L63" s="14"/>
+      <c r="M63" s="14"/>
+      <c r="N63" s="14"/>
+      <c r="O63" s="14"/>
+      <c r="P63" s="14"/>
+      <c r="Q63" s="14"/>
+      <c r="R63" s="14"/>
+      <c r="S63" s="14"/>
+      <c r="T63" s="14"/>
+      <c r="U63" s="14"/>
+      <c r="V63" s="14"/>
+      <c r="W63" s="14"/>
+      <c r="X63" s="14"/>
+      <c r="Y63" s="15"/>
       <c r="Z63" s="1"/>
       <c r="AA63" s="1"/>
       <c r="AB63" s="1"/>
     </row>
-    <row r="64" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:46" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
-      <c r="B64" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="C64" s="75">
-        <f>INT($C$31)+1.005</f>
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="D64" s="14"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="14"/>
-      <c r="G64" s="14"/>
-      <c r="H64" s="14"/>
-      <c r="I64" s="14"/>
-      <c r="J64" s="14"/>
-      <c r="K64" s="14"/>
-      <c r="L64" s="14"/>
-      <c r="M64" s="14"/>
-      <c r="N64" s="14"/>
-      <c r="O64" s="14"/>
-      <c r="P64" s="14"/>
-      <c r="Q64" s="14"/>
-      <c r="R64" s="14"/>
-      <c r="S64" s="14"/>
-      <c r="T64" s="14"/>
-      <c r="U64" s="14"/>
-      <c r="V64" s="14"/>
-      <c r="W64" s="14"/>
-      <c r="X64" s="14"/>
-      <c r="Y64" s="15"/>
+      <c r="B64" s="33"/>
+      <c r="C64" s="73">
+        <f>INT(MAX($C$41:$C$56))+1</f>
+        <v>4</v>
+      </c>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="27"/>
+      <c r="I64" s="27"/>
+      <c r="J64" s="27"/>
+      <c r="K64" s="27"/>
+      <c r="L64" s="27"/>
+      <c r="M64" s="27"/>
+      <c r="N64" s="27"/>
+      <c r="O64" s="27"/>
+      <c r="P64" s="27"/>
+      <c r="Q64" s="27"/>
+      <c r="R64" s="27"/>
+      <c r="S64" s="27"/>
+      <c r="T64" s="27"/>
+      <c r="U64" s="27"/>
+      <c r="V64" s="27"/>
+      <c r="W64" s="27"/>
+      <c r="X64" s="3"/>
+      <c r="Y64" s="16"/>
       <c r="Z64" s="1"/>
       <c r="AA64" s="1"/>
       <c r="AB64" s="1"/>
     </row>
-    <row r="65" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="33"/>
       <c r="C65" s="73">
-        <f>INT(MAX($C$41:$C$57))+1</f>
-        <v>4</v>
-      </c>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
-      <c r="H65" s="27"/>
-      <c r="I65" s="27"/>
-      <c r="J65" s="27"/>
-      <c r="K65" s="27"/>
-      <c r="L65" s="27"/>
-      <c r="M65" s="27"/>
-      <c r="N65" s="27"/>
-      <c r="O65" s="27"/>
-      <c r="P65" s="27"/>
-      <c r="Q65" s="27"/>
-      <c r="R65" s="27"/>
-      <c r="S65" s="27"/>
-      <c r="T65" s="27"/>
-      <c r="U65" s="27"/>
-      <c r="V65" s="27"/>
-      <c r="W65" s="27"/>
-      <c r="X65" s="3"/>
+        <v>1.02</v>
+      </c>
+      <c r="D65" s="21"/>
+      <c r="E65" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F65" s="25"/>
+      <c r="G65" s="12"/>
+      <c r="H65" s="44" t="str">
+        <f>COUNTIFS($B$1:$B65, "«")&amp;" Structural: Landuse sets"</f>
+        <v>3 Structural: Landuse sets</v>
+      </c>
+      <c r="I65" s="6"/>
+      <c r="J65" s="6"/>
+      <c r="K65" s="6"/>
+      <c r="L65" s="6"/>
+      <c r="M65" s="6"/>
+      <c r="N65" s="6"/>
+      <c r="O65" s="6"/>
+      <c r="P65" s="6"/>
+      <c r="Q65" s="6"/>
+      <c r="R65" s="6"/>
+      <c r="S65" s="6"/>
+      <c r="T65" s="6"/>
+      <c r="U65" s="6"/>
+      <c r="V65" s="6"/>
+      <c r="W65" s="6"/>
+      <c r="X65" s="10"/>
       <c r="Y65" s="16"/>
       <c r="Z65" s="1"/>
       <c r="AA65" s="1"/>
       <c r="AB65" s="1"/>
     </row>
-    <row r="66" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="33"/>
       <c r="C66" s="73">
-        <v>1.02</v>
+        <f>INT($C$31)+1.02</f>
+        <v>2.02</v>
       </c>
       <c r="D66" s="21"/>
       <c r="E66" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="F66" s="25"/>
-      <c r="G66" s="12"/>
-      <c r="H66" s="44" t="str">
-        <f>COUNTIFS($B$1:$B66, "«")&amp;" Structural: Landuse sets"</f>
-        <v>3 Structural: Landuse sets</v>
-      </c>
-      <c r="I66" s="6"/>
-      <c r="J66" s="6"/>
-      <c r="K66" s="6"/>
-      <c r="L66" s="6"/>
-      <c r="M66" s="6"/>
-      <c r="N66" s="6"/>
-      <c r="O66" s="6"/>
-      <c r="P66" s="6"/>
-      <c r="Q66" s="6"/>
-      <c r="R66" s="6"/>
-      <c r="S66" s="6"/>
-      <c r="T66" s="6"/>
-      <c r="U66" s="6"/>
-      <c r="V66" s="6"/>
-      <c r="W66" s="6"/>
-      <c r="X66" s="10"/>
+        <v>10</v>
+      </c>
+      <c r="F66" s="28">
+        <v>1</v>
+      </c>
+      <c r="G66" s="13"/>
+      <c r="H66" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="I66" s="7"/>
+      <c r="J66" s="7"/>
+      <c r="K66" s="7"/>
+      <c r="L66" s="7"/>
+      <c r="M66" s="7"/>
+      <c r="N66" s="7"/>
+      <c r="O66" s="7"/>
+      <c r="P66" s="7"/>
+      <c r="Q66" s="7"/>
+      <c r="R66" s="7"/>
+      <c r="S66" s="7"/>
+      <c r="T66" s="7"/>
+      <c r="U66" s="7"/>
+      <c r="V66" s="7"/>
+      <c r="W66" s="7"/>
+      <c r="X66" s="11"/>
       <c r="Y66" s="16"/>
       <c r="Z66" s="1"/>
       <c r="AA66" s="1"/>
       <c r="AB66" s="1"/>
     </row>
-    <row r="67" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="33"/>
       <c r="C67" s="73">
-        <f>INT($C$31)+1.02</f>
-        <v>2.02</v>
-      </c>
-      <c r="D67" s="21"/>
-      <c r="E67" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F67" s="28">
-        <v>1</v>
-      </c>
-      <c r="G67" s="13"/>
-      <c r="H67" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="I67" s="7"/>
-      <c r="J67" s="7"/>
-      <c r="K67" s="7"/>
-      <c r="L67" s="7"/>
-      <c r="M67" s="7"/>
-      <c r="N67" s="7"/>
-      <c r="O67" s="7"/>
-      <c r="P67" s="7"/>
-      <c r="Q67" s="7"/>
-      <c r="R67" s="7"/>
-      <c r="S67" s="7"/>
-      <c r="T67" s="7"/>
-      <c r="U67" s="7"/>
-      <c r="V67" s="7"/>
-      <c r="W67" s="7"/>
-      <c r="X67" s="11"/>
+        <f>INT($C$31)+2.005</f>
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="3"/>
+      <c r="L67" s="3"/>
+      <c r="M67" s="3"/>
+      <c r="N67" s="3"/>
+      <c r="O67" s="3"/>
+      <c r="P67" s="3"/>
+      <c r="Q67" s="3"/>
+      <c r="R67" s="3"/>
+      <c r="S67" s="3"/>
+      <c r="T67" s="3"/>
+      <c r="U67" s="3"/>
+      <c r="V67" s="3"/>
+      <c r="W67" s="3"/>
+      <c r="X67" s="3"/>
       <c r="Y67" s="16"/>
       <c r="Z67" s="1"/>
       <c r="AA67" s="1"/>
       <c r="AB67" s="1"/>
     </row>
-    <row r="68" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="33"/>
       <c r="C68" s="73">
-        <f>INT($C$31)+2.005</f>
-        <v>3.0049999999999999</v>
+        <f>INT($C$31)+3</f>
+        <v>4</v>
       </c>
       <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
       <c r="G68" s="3"/>
-      <c r="H68" s="3"/>
-      <c r="I68" s="3"/>
-      <c r="J68" s="3"/>
-      <c r="K68" s="3"/>
-      <c r="L68" s="3"/>
-      <c r="M68" s="3"/>
-      <c r="N68" s="3"/>
-      <c r="O68" s="3"/>
-      <c r="P68" s="3"/>
-      <c r="Q68" s="3"/>
-      <c r="R68" s="3"/>
-      <c r="S68" s="3"/>
-      <c r="T68" s="3"/>
-      <c r="U68" s="3"/>
-      <c r="V68" s="3"/>
-      <c r="W68" s="3"/>
+      <c r="H68" s="30"/>
+      <c r="I68" s="30"/>
+      <c r="J68" s="30"/>
+      <c r="K68" s="30"/>
+      <c r="L68" s="30"/>
+      <c r="M68" s="30"/>
+      <c r="N68" s="30"/>
+      <c r="O68" s="30"/>
+      <c r="P68" s="30"/>
+      <c r="Q68" s="30"/>
+      <c r="R68" s="30"/>
+      <c r="S68" s="30"/>
+      <c r="T68" s="30"/>
+      <c r="U68" s="30"/>
+      <c r="V68" s="30"/>
+      <c r="W68" s="30"/>
       <c r="X68" s="3"/>
       <c r="Y68" s="16"/>
       <c r="Z68" s="1"/>
@@ -9780,29 +8636,29 @@
       <c r="A69" s="1"/>
       <c r="B69" s="33"/>
       <c r="C69" s="73">
-        <f>INT($C$31)+3</f>
+        <f t="shared" ref="C69:C71" si="2">INT($C$31)+3</f>
         <v>4</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
       <c r="G69" s="3"/>
-      <c r="H69" s="30"/>
-      <c r="I69" s="30"/>
-      <c r="J69" s="30"/>
-      <c r="K69" s="30"/>
-      <c r="L69" s="30"/>
-      <c r="M69" s="30"/>
-      <c r="N69" s="30"/>
-      <c r="O69" s="30"/>
-      <c r="P69" s="30"/>
-      <c r="Q69" s="30"/>
-      <c r="R69" s="30"/>
-      <c r="S69" s="30"/>
-      <c r="T69" s="30"/>
-      <c r="U69" s="30"/>
-      <c r="V69" s="30"/>
-      <c r="W69" s="30"/>
+      <c r="H69" s="29"/>
+      <c r="I69" s="29"/>
+      <c r="J69" s="29"/>
+      <c r="K69" s="29"/>
+      <c r="L69" s="29"/>
+      <c r="M69" s="29"/>
+      <c r="N69" s="29"/>
+      <c r="O69" s="29"/>
+      <c r="P69" s="29"/>
+      <c r="Q69" s="29"/>
+      <c r="R69" s="29"/>
+      <c r="S69" s="29"/>
+      <c r="T69" s="29"/>
+      <c r="U69" s="29"/>
+      <c r="V69" s="29"/>
+      <c r="W69" s="29"/>
       <c r="X69" s="3"/>
       <c r="Y69" s="16"/>
       <c r="Z69" s="1"/>
@@ -9813,7 +8669,7 @@
       <c r="A70" s="1"/>
       <c r="B70" s="33"/>
       <c r="C70" s="73">
-        <f t="shared" ref="C70:C72" si="2">INT($C$31)+3</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="D70" s="3"/>
@@ -9875,16 +8731,18 @@
       <c r="AA71" s="1"/>
       <c r="AB71" s="1"/>
     </row>
-    <row r="72" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:28" ht="11.45" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
-      <c r="B72" s="33"/>
+      <c r="B72" s="33" t="s">
+        <v>20</v>
+      </c>
       <c r="C72" s="73">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f>INT($C$31)+2.01</f>
+        <v>3.01</v>
       </c>
       <c r="D72" s="3"/>
-      <c r="E72" s="5"/>
-      <c r="F72" s="5"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
       <c r="G72" s="3"/>
       <c r="H72" s="29"/>
       <c r="I72" s="29"/>
@@ -9908,36 +8766,34 @@
       <c r="AA72" s="1"/>
       <c r="AB72" s="1"/>
     </row>
-    <row r="73" spans="1:28" ht="11.45" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
-      <c r="B73" s="33" t="s">
-        <v>20</v>
-      </c>
+      <c r="B73" s="33"/>
       <c r="C73" s="73">
-        <f>INT($C$31)+2.01</f>
-        <v>3.01</v>
-      </c>
-      <c r="D73" s="3"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
-      <c r="G73" s="3"/>
-      <c r="H73" s="29"/>
-      <c r="I73" s="29"/>
-      <c r="J73" s="29"/>
-      <c r="K73" s="29"/>
-      <c r="L73" s="29"/>
-      <c r="M73" s="29"/>
-      <c r="N73" s="29"/>
-      <c r="O73" s="29"/>
-      <c r="P73" s="29"/>
-      <c r="Q73" s="29"/>
-      <c r="R73" s="29"/>
-      <c r="S73" s="29"/>
-      <c r="T73" s="29"/>
-      <c r="U73" s="29"/>
-      <c r="V73" s="29"/>
-      <c r="W73" s="29"/>
-      <c r="X73" s="3"/>
+        <f>$C$30</f>
+        <v>4</v>
+      </c>
+      <c r="D73" s="4"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="4"/>
+      <c r="H73" s="5"/>
+      <c r="I73" s="5"/>
+      <c r="J73" s="5"/>
+      <c r="K73" s="5"/>
+      <c r="L73" s="5"/>
+      <c r="M73" s="5"/>
+      <c r="N73" s="5"/>
+      <c r="O73" s="5"/>
+      <c r="P73" s="5"/>
+      <c r="Q73" s="5"/>
+      <c r="R73" s="5"/>
+      <c r="S73" s="5"/>
+      <c r="T73" s="5"/>
+      <c r="U73" s="5"/>
+      <c r="V73" s="5"/>
+      <c r="W73" s="5"/>
+      <c r="X73" s="4"/>
       <c r="Y73" s="16"/>
       <c r="Z73" s="1"/>
       <c r="AA73" s="1"/>
@@ -9945,16 +8801,20 @@
     </row>
     <row r="74" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
-      <c r="B74" s="33"/>
+      <c r="B74" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="C74" s="73">
         <f>$C$30</f>
         <v>4</v>
       </c>
-      <c r="D74" s="4"/>
+      <c r="D74" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
       <c r="G74" s="4"/>
-      <c r="H74" s="5"/>
+      <c r="H74" s="120"/>
       <c r="I74" s="5"/>
       <c r="J74" s="5"/>
       <c r="K74" s="5"/>
@@ -9976,72 +8836,72 @@
       <c r="AA74" s="1"/>
       <c r="AB74" s="1"/>
     </row>
-    <row r="75" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
-      <c r="B75" s="33" t="s">
-        <v>19</v>
-      </c>
+      <c r="B75" s="33"/>
       <c r="C75" s="73">
-        <f>$C$30</f>
-        <v>4</v>
+        <f>INT($C$31)+2.005</f>
+        <v>3.0049999999999999</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E75" s="5"/>
-      <c r="F75" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="E75" s="4"/>
+      <c r="F75" s="4"/>
       <c r="G75" s="4"/>
-      <c r="H75" s="120"/>
-      <c r="I75" s="5"/>
-      <c r="J75" s="5"/>
-      <c r="K75" s="5"/>
-      <c r="L75" s="5"/>
-      <c r="M75" s="5"/>
-      <c r="N75" s="5"/>
-      <c r="O75" s="5"/>
-      <c r="P75" s="5"/>
-      <c r="Q75" s="5"/>
-      <c r="R75" s="5"/>
-      <c r="S75" s="5"/>
-      <c r="T75" s="5"/>
-      <c r="U75" s="5"/>
-      <c r="V75" s="5"/>
-      <c r="W75" s="5"/>
+      <c r="H75" s="58"/>
+      <c r="I75" s="58"/>
+      <c r="J75" s="58"/>
+      <c r="K75" s="58"/>
+      <c r="L75" s="58"/>
+      <c r="M75" s="58"/>
+      <c r="N75" s="58"/>
+      <c r="O75" s="58"/>
+      <c r="P75" s="58"/>
+      <c r="Q75" s="58"/>
+      <c r="R75" s="58"/>
+      <c r="S75" s="58"/>
+      <c r="T75" s="58"/>
+      <c r="U75" s="58"/>
+      <c r="V75" s="58"/>
+      <c r="W75" s="58"/>
       <c r="X75" s="4"/>
       <c r="Y75" s="16"/>
       <c r="Z75" s="1"/>
       <c r="AA75" s="1"/>
       <c r="AB75" s="1"/>
     </row>
-    <row r="76" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="33"/>
       <c r="C76" s="73">
-        <f>INT($C$31)+2.005</f>
-        <v>3.0049999999999999</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E76" s="4"/>
-      <c r="F76" s="4"/>
+        <f t="shared" ref="C76:C114" si="3">INT($C$31)+2</f>
+        <v>3</v>
+      </c>
+      <c r="D76" s="4"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
       <c r="G76" s="4"/>
-      <c r="H76" s="58"/>
-      <c r="I76" s="58"/>
-      <c r="J76" s="58"/>
-      <c r="K76" s="58"/>
-      <c r="L76" s="58"/>
-      <c r="M76" s="58"/>
-      <c r="N76" s="58"/>
-      <c r="O76" s="58"/>
-      <c r="P76" s="58"/>
-      <c r="Q76" s="58"/>
-      <c r="R76" s="58"/>
-      <c r="S76" s="58"/>
-      <c r="T76" s="58"/>
-      <c r="U76" s="58"/>
-      <c r="V76" s="58"/>
-      <c r="W76" s="58"/>
+      <c r="H76" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="I76" s="2"/>
+      <c r="J76" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="K76" s="2"/>
+      <c r="L76" s="2"/>
+      <c r="M76" s="2"/>
+      <c r="N76" s="2"/>
+      <c r="O76" s="2"/>
+      <c r="P76" s="2"/>
+      <c r="Q76" s="2"/>
+      <c r="R76" s="2"/>
+      <c r="S76" s="2"/>
+      <c r="T76" s="2"/>
+      <c r="U76" s="2"/>
+      <c r="V76" s="2"/>
+      <c r="W76" s="2"/>
       <c r="X76" s="4"/>
       <c r="Y76" s="16"/>
       <c r="Z76" s="1"/>
@@ -10052,20 +8912,16 @@
       <c r="A77" s="1"/>
       <c r="B77" s="33"/>
       <c r="C77" s="73">
-        <f t="shared" ref="C77:C115" si="3">INT($C$31)+2</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="5"/>
       <c r="F77" s="5"/>
       <c r="G77" s="4"/>
-      <c r="H77" s="2" t="s">
-        <v>311</v>
-      </c>
+      <c r="H77" s="2"/>
       <c r="I77" s="2"/>
-      <c r="J77" s="2" t="s">
-        <v>349</v>
-      </c>
+      <c r="J77" s="2"/>
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
@@ -10097,16 +8953,30 @@
       <c r="F78" s="5"/>
       <c r="G78" s="4"/>
       <c r="H78" s="2"/>
-      <c r="I78" s="2"/>
-      <c r="J78" s="2"/>
+      <c r="I78" s="161" t="s">
+        <v>311</v>
+      </c>
+      <c r="J78" s="161" t="s">
+        <v>390</v>
+      </c>
       <c r="K78" s="2"/>
-      <c r="L78" s="2"/>
+      <c r="L78" s="161" t="s">
+        <v>312</v>
+      </c>
       <c r="M78" s="2"/>
-      <c r="N78" s="2"/>
+      <c r="N78" s="161" t="s">
+        <v>376</v>
+      </c>
       <c r="O78" s="2"/>
-      <c r="P78" s="2"/>
-      <c r="Q78" s="2"/>
-      <c r="R78" s="2"/>
+      <c r="P78" s="161" t="s">
+        <v>313</v>
+      </c>
+      <c r="Q78" s="161" t="s">
+        <v>374</v>
+      </c>
+      <c r="R78" s="161" t="s">
+        <v>375</v>
+      </c>
       <c r="S78" s="2"/>
       <c r="T78" s="2"/>
       <c r="U78" s="2"/>
@@ -10129,30 +8999,31 @@
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
       <c r="G79" s="4"/>
-      <c r="H79" s="2"/>
-      <c r="I79" s="161" t="s">
-        <v>312</v>
-      </c>
-      <c r="J79" s="161" t="s">
-        <v>391</v>
-      </c>
-      <c r="K79" s="2"/>
-      <c r="L79" s="161" t="s">
-        <v>313</v>
-      </c>
-      <c r="M79" s="2"/>
-      <c r="N79" s="161" t="s">
-        <v>377</v>
-      </c>
-      <c r="O79" s="2"/>
-      <c r="P79" s="161" t="s">
+      <c r="H79" s="148"/>
+      <c r="I79" s="162" t="s">
         <v>314</v>
       </c>
-      <c r="Q79" s="161" t="s">
-        <v>375</v>
-      </c>
-      <c r="R79" s="161" t="s">
-        <v>376</v>
+      <c r="J79" s="162" t="b">
+        <v>0</v>
+      </c>
+      <c r="K79" s="55"/>
+      <c r="L79" s="162" t="s">
+        <v>315</v>
+      </c>
+      <c r="M79" s="165"/>
+      <c r="N79" s="210" t="s">
+        <v>373</v>
+      </c>
+      <c r="O79" s="165"/>
+      <c r="P79" s="162" t="s">
+        <v>315</v>
+      </c>
+      <c r="Q79" s="162" t="b">
+        <v>0</v>
+      </c>
+      <c r="R79" s="206" t="str">
+        <f>P79</f>
+        <v>a</v>
       </c>
       <c r="S79" s="2"/>
       <c r="T79" s="2"/>
@@ -10168,39 +9039,34 @@
     <row r="80" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="33"/>
-      <c r="C80" s="73">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
+      <c r="C80" s="73"/>
       <c r="D80" s="4"/>
       <c r="E80" s="5"/>
       <c r="F80" s="5"/>
       <c r="G80" s="4"/>
       <c r="H80" s="148"/>
-      <c r="I80" s="162" t="s">
-        <v>315</v>
-      </c>
-      <c r="J80" s="162" t="b">
+      <c r="I80" s="163" t="s">
+        <v>316</v>
+      </c>
+      <c r="J80" s="163" t="b">
         <v>0</v>
       </c>
       <c r="K80" s="55"/>
-      <c r="L80" s="162" t="s">
-        <v>316</v>
+      <c r="L80" s="163" t="s">
+        <v>317</v>
       </c>
       <c r="M80" s="165"/>
-      <c r="N80" s="210" t="s">
-        <v>374</v>
-      </c>
+      <c r="N80" s="209"/>
       <c r="O80" s="165"/>
-      <c r="P80" s="162" t="s">
-        <v>316</v>
-      </c>
-      <c r="Q80" s="162" t="b">
-        <v>0</v>
-      </c>
-      <c r="R80" s="206" t="str">
-        <f>P80</f>
-        <v>a</v>
+      <c r="P80" s="163" t="s">
+        <v>317</v>
+      </c>
+      <c r="Q80" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="R80" s="207" t="str">
+        <f t="shared" ref="R80:R114" si="4">P80</f>
+        <v>ar</v>
       </c>
       <c r="S80" s="2"/>
       <c r="T80" s="2"/>
@@ -10223,27 +9089,27 @@
       <c r="G81" s="4"/>
       <c r="H81" s="148"/>
       <c r="I81" s="163" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="J81" s="163" t="b">
         <v>0</v>
       </c>
       <c r="K81" s="55"/>
       <c r="L81" s="163" t="s">
-        <v>318</v>
+        <v>373</v>
       </c>
       <c r="M81" s="165"/>
-      <c r="N81" s="209"/>
+      <c r="N81" s="165"/>
       <c r="O81" s="165"/>
       <c r="P81" s="163" t="s">
-        <v>318</v>
+        <v>373</v>
       </c>
       <c r="Q81" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R81" s="207" t="str">
-        <f t="shared" ref="R81:R115" si="4">P81</f>
-        <v>ar</v>
+        <f t="shared" si="4"/>
+        <v>a2</v>
       </c>
       <c r="S81" s="2"/>
       <c r="T81" s="2"/>
@@ -10266,27 +9132,27 @@
       <c r="G82" s="4"/>
       <c r="H82" s="148"/>
       <c r="I82" s="163" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="J82" s="163" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K82" s="55"/>
       <c r="L82" s="163" t="s">
-        <v>374</v>
+        <v>319</v>
       </c>
       <c r="M82" s="165"/>
       <c r="N82" s="165"/>
       <c r="O82" s="165"/>
       <c r="P82" s="163" t="s">
-        <v>374</v>
+        <v>314</v>
       </c>
       <c r="Q82" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R82" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>a2</v>
+        <v>b</v>
       </c>
       <c r="S82" s="2"/>
       <c r="T82" s="2"/>
@@ -10309,27 +9175,27 @@
       <c r="G83" s="4"/>
       <c r="H83" s="148"/>
       <c r="I83" s="163" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="J83" s="163" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K83" s="55"/>
       <c r="L83" s="163" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="M83" s="165"/>
       <c r="N83" s="165"/>
       <c r="O83" s="165"/>
       <c r="P83" s="163" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="Q83" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R83" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>b</v>
+        <v>bd</v>
       </c>
       <c r="S83" s="2"/>
       <c r="T83" s="2"/>
@@ -10352,27 +9218,27 @@
       <c r="G84" s="4"/>
       <c r="H84" s="148"/>
       <c r="I84" s="163" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="J84" s="163" t="b">
         <v>0</v>
       </c>
       <c r="K84" s="55"/>
       <c r="L84" s="163" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="M84" s="165"/>
       <c r="N84" s="165"/>
       <c r="O84" s="165"/>
       <c r="P84" s="163" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="Q84" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R84" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>bd</v>
+        <v>f</v>
       </c>
       <c r="S84" s="2"/>
       <c r="T84" s="2"/>
@@ -10395,27 +9261,27 @@
       <c r="G85" s="4"/>
       <c r="H85" s="148"/>
       <c r="I85" s="163" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="J85" s="163" t="b">
         <v>0</v>
       </c>
       <c r="K85" s="55"/>
       <c r="L85" s="163" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="M85" s="165"/>
       <c r="N85" s="165"/>
       <c r="O85" s="165"/>
       <c r="P85" s="163" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="Q85" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R85" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>f</v>
+        <v>h</v>
       </c>
       <c r="S85" s="2"/>
       <c r="T85" s="2"/>
@@ -10438,27 +9304,27 @@
       <c r="G86" s="4"/>
       <c r="H86" s="148"/>
       <c r="I86" s="163" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="J86" s="163" t="b">
         <v>0</v>
       </c>
       <c r="K86" s="55"/>
       <c r="L86" s="163" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="M86" s="165"/>
       <c r="N86" s="165"/>
       <c r="O86" s="165"/>
       <c r="P86" s="163" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="Q86" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R86" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>h</v>
+        <v>i</v>
       </c>
       <c r="S86" s="2"/>
       <c r="T86" s="2"/>
@@ -10481,27 +9347,27 @@
       <c r="G87" s="4"/>
       <c r="H87" s="148"/>
       <c r="I87" s="163" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="J87" s="163" t="b">
         <v>0</v>
       </c>
       <c r="K87" s="55"/>
       <c r="L87" s="163" t="s">
-        <v>328</v>
+        <v>365</v>
       </c>
       <c r="M87" s="165"/>
       <c r="N87" s="165"/>
       <c r="O87" s="165"/>
       <c r="P87" s="163" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="Q87" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R87" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>i</v>
+        <v>j</v>
       </c>
       <c r="S87" s="2"/>
       <c r="T87" s="2"/>
@@ -10524,27 +9390,27 @@
       <c r="G88" s="4"/>
       <c r="H88" s="148"/>
       <c r="I88" s="163" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="J88" s="163" t="b">
         <v>0</v>
       </c>
       <c r="K88" s="55"/>
       <c r="L88" s="163" t="s">
-        <v>366</v>
+        <v>329</v>
       </c>
       <c r="M88" s="165"/>
       <c r="N88" s="165"/>
       <c r="O88" s="165"/>
       <c r="P88" s="163" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="Q88" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R88" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>j</v>
+        <v>jc</v>
       </c>
       <c r="S88" s="2"/>
       <c r="T88" s="2"/>
@@ -10567,27 +9433,27 @@
       <c r="G89" s="4"/>
       <c r="H89" s="148"/>
       <c r="I89" s="163" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="J89" s="163" t="b">
         <v>0</v>
       </c>
       <c r="K89" s="55"/>
       <c r="L89" s="163" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="M89" s="165"/>
       <c r="N89" s="165"/>
       <c r="O89" s="165"/>
       <c r="P89" s="163" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="Q89" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R89" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>jc</v>
+        <v>jr</v>
       </c>
       <c r="S89" s="2"/>
       <c r="T89" s="2"/>
@@ -10610,27 +9476,27 @@
       <c r="G90" s="4"/>
       <c r="H90" s="148"/>
       <c r="I90" s="163" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="J90" s="163" t="b">
         <v>0</v>
       </c>
       <c r="K90" s="55"/>
       <c r="L90" s="163" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="M90" s="165"/>
       <c r="N90" s="165"/>
       <c r="O90" s="165"/>
       <c r="P90" s="163" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="Q90" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R90" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>jr</v>
+        <v>k</v>
       </c>
       <c r="S90" s="2"/>
       <c r="T90" s="2"/>
@@ -10653,27 +9519,27 @@
       <c r="G91" s="4"/>
       <c r="H91" s="148"/>
       <c r="I91" s="163" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="J91" s="163" t="b">
         <v>0</v>
       </c>
       <c r="K91" s="55"/>
       <c r="L91" s="163" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="M91" s="165"/>
       <c r="N91" s="165"/>
       <c r="O91" s="165"/>
       <c r="P91" s="163" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="Q91" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R91" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>k</v>
+        <v>l</v>
       </c>
       <c r="S91" s="2"/>
       <c r="T91" s="2"/>
@@ -10696,27 +9562,27 @@
       <c r="G92" s="4"/>
       <c r="H92" s="148"/>
       <c r="I92" s="163" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="J92" s="163" t="b">
         <v>0</v>
       </c>
       <c r="K92" s="55"/>
       <c r="L92" s="163" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="M92" s="165"/>
       <c r="N92" s="165"/>
       <c r="O92" s="165"/>
       <c r="P92" s="163" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="Q92" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R92" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>l</v>
+        <v>m</v>
       </c>
       <c r="S92" s="2"/>
       <c r="T92" s="2"/>
@@ -10739,27 +9605,27 @@
       <c r="G93" s="4"/>
       <c r="H93" s="148"/>
       <c r="I93" s="163" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="J93" s="163" t="b">
         <v>0</v>
       </c>
       <c r="K93" s="55"/>
       <c r="L93" s="163" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="M93" s="165"/>
       <c r="N93" s="165"/>
       <c r="O93" s="165"/>
       <c r="P93" s="163" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="Q93" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R93" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>m</v>
+        <v>o</v>
       </c>
       <c r="S93" s="2"/>
       <c r="T93" s="2"/>
@@ -10782,27 +9648,27 @@
       <c r="G94" s="4"/>
       <c r="H94" s="148"/>
       <c r="I94" s="163" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="J94" s="163" t="b">
         <v>0</v>
       </c>
       <c r="K94" s="55"/>
       <c r="L94" s="163" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="M94" s="165"/>
       <c r="N94" s="165"/>
       <c r="O94" s="165"/>
       <c r="P94" s="163" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="Q94" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R94" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>o</v>
+        <v>od</v>
       </c>
       <c r="S94" s="2"/>
       <c r="T94" s="2"/>
@@ -10824,28 +9690,28 @@
       <c r="F95" s="5"/>
       <c r="G95" s="4"/>
       <c r="H95" s="148"/>
-      <c r="I95" s="163" t="s">
-        <v>345</v>
-      </c>
-      <c r="J95" s="163" t="b">
+      <c r="I95" s="164" t="s">
+        <v>346</v>
+      </c>
+      <c r="J95" s="164" t="b">
         <v>0</v>
       </c>
       <c r="K95" s="55"/>
       <c r="L95" s="163" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="M95" s="165"/>
       <c r="N95" s="165"/>
       <c r="O95" s="165"/>
       <c r="P95" s="163" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="Q95" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R95" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>od</v>
+        <v>of</v>
       </c>
       <c r="S95" s="2"/>
       <c r="T95" s="2"/>
@@ -10866,29 +9732,25 @@
       <c r="E96" s="5"/>
       <c r="F96" s="5"/>
       <c r="G96" s="4"/>
-      <c r="H96" s="148"/>
-      <c r="I96" s="164" t="s">
-        <v>347</v>
-      </c>
-      <c r="J96" s="164" t="b">
-        <v>0</v>
-      </c>
-      <c r="K96" s="55"/>
+      <c r="H96" s="2"/>
+      <c r="I96" s="53"/>
+      <c r="J96" s="53"/>
+      <c r="K96" s="2"/>
       <c r="L96" s="163" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="M96" s="165"/>
       <c r="N96" s="165"/>
       <c r="O96" s="165"/>
       <c r="P96" s="163" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="Q96" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R96" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>of</v>
+        <v>r</v>
       </c>
       <c r="S96" s="2"/>
       <c r="T96" s="2"/>
@@ -10910,24 +9772,24 @@
       <c r="F97" s="5"/>
       <c r="G97" s="4"/>
       <c r="H97" s="2"/>
-      <c r="I97" s="53"/>
-      <c r="J97" s="53"/>
+      <c r="I97" s="2"/>
+      <c r="J97" s="2"/>
       <c r="K97" s="2"/>
-      <c r="L97" s="163" t="s">
-        <v>346</v>
-      </c>
-      <c r="M97" s="165"/>
-      <c r="N97" s="165"/>
-      <c r="O97" s="165"/>
+      <c r="L97" s="164" t="s">
+        <v>347</v>
+      </c>
+      <c r="M97" s="148"/>
+      <c r="N97" s="148"/>
+      <c r="O97" s="148"/>
       <c r="P97" s="163" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="Q97" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R97" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>r</v>
+        <v>rd</v>
       </c>
       <c r="S97" s="2"/>
       <c r="T97" s="2"/>
@@ -10952,21 +9814,19 @@
       <c r="I98" s="2"/>
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
-      <c r="L98" s="164" t="s">
-        <v>348</v>
-      </c>
+      <c r="L98" s="53"/>
       <c r="M98" s="148"/>
       <c r="N98" s="148"/>
       <c r="O98" s="148"/>
       <c r="P98" s="163" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="Q98" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R98" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>rd</v>
+        <v>s</v>
       </c>
       <c r="S98" s="2"/>
       <c r="T98" s="2"/>
@@ -10996,14 +9856,14 @@
       <c r="N99" s="148"/>
       <c r="O99" s="148"/>
       <c r="P99" s="163" t="s">
-        <v>328</v>
+        <v>365</v>
       </c>
       <c r="Q99" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R99" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>s</v>
+        <v>sp</v>
       </c>
       <c r="S99" s="2"/>
       <c r="T99" s="2"/>
@@ -11028,19 +9888,19 @@
       <c r="I100" s="2"/>
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
-      <c r="L100" s="53"/>
+      <c r="L100" s="2"/>
       <c r="M100" s="148"/>
       <c r="N100" s="148"/>
       <c r="O100" s="148"/>
       <c r="P100" s="163" t="s">
-        <v>366</v>
+        <v>329</v>
       </c>
       <c r="Q100" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R100" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>sp</v>
+        <v>sr</v>
       </c>
       <c r="S100" s="2"/>
       <c r="T100" s="2"/>
@@ -11070,14 +9930,14 @@
       <c r="N101" s="148"/>
       <c r="O101" s="148"/>
       <c r="P101" s="163" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="Q101" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R101" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>sr</v>
+        <v>t</v>
       </c>
       <c r="S101" s="2"/>
       <c r="T101" s="2"/>
@@ -11107,14 +9967,14 @@
       <c r="N102" s="148"/>
       <c r="O102" s="148"/>
       <c r="P102" s="163" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="Q102" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R102" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>t</v>
+        <v>tc</v>
       </c>
       <c r="S102" s="2"/>
       <c r="T102" s="2"/>
@@ -11144,14 +10004,14 @@
       <c r="N103" s="148"/>
       <c r="O103" s="148"/>
       <c r="P103" s="163" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="Q103" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R103" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>tc</v>
+        <v>tr</v>
       </c>
       <c r="S103" s="2"/>
       <c r="T103" s="2"/>
@@ -11181,14 +10041,14 @@
       <c r="N104" s="148"/>
       <c r="O104" s="148"/>
       <c r="P104" s="163" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="Q104" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R104" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>tr</v>
+        <v>u</v>
       </c>
       <c r="S104" s="2"/>
       <c r="T104" s="2"/>
@@ -11218,14 +10078,14 @@
       <c r="N105" s="148"/>
       <c r="O105" s="148"/>
       <c r="P105" s="163" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="Q105" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R105" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>u</v>
+        <v>uc</v>
       </c>
       <c r="S105" s="2"/>
       <c r="T105" s="2"/>
@@ -11255,14 +10115,14 @@
       <c r="N106" s="148"/>
       <c r="O106" s="148"/>
       <c r="P106" s="163" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="Q106" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R106" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>uc</v>
+        <v>ur</v>
       </c>
       <c r="S106" s="2"/>
       <c r="T106" s="2"/>
@@ -11292,14 +10152,14 @@
       <c r="N107" s="148"/>
       <c r="O107" s="148"/>
       <c r="P107" s="163" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="Q107" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R107" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>ur</v>
+        <v>v</v>
       </c>
       <c r="S107" s="2"/>
       <c r="T107" s="2"/>
@@ -11329,14 +10189,14 @@
       <c r="N108" s="148"/>
       <c r="O108" s="148"/>
       <c r="P108" s="163" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="Q108" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R108" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>v</v>
+        <v>w</v>
       </c>
       <c r="S108" s="2"/>
       <c r="T108" s="2"/>
@@ -11366,14 +10226,14 @@
       <c r="N109" s="148"/>
       <c r="O109" s="148"/>
       <c r="P109" s="163" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="Q109" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R109" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>w</v>
+        <v>wd</v>
       </c>
       <c r="S109" s="2"/>
       <c r="T109" s="2"/>
@@ -11389,7 +10249,10 @@
     <row r="110" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="33"/>
-      <c r="C110" s="73"/>
+      <c r="C110" s="73">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
       <c r="D110" s="4"/>
       <c r="E110" s="5"/>
       <c r="F110" s="5"/>
@@ -11410,7 +10273,7 @@
       </c>
       <c r="R110" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>wd</v>
+        <v>x</v>
       </c>
       <c r="S110" s="2"/>
       <c r="T110" s="2"/>
@@ -11443,14 +10306,14 @@
       <c r="N111" s="148"/>
       <c r="O111" s="148"/>
       <c r="P111" s="163" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="Q111" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R111" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>x</v>
+        <v>xc</v>
       </c>
       <c r="S111" s="2"/>
       <c r="T111" s="2"/>
@@ -11483,14 +10346,14 @@
       <c r="N112" s="148"/>
       <c r="O112" s="148"/>
       <c r="P112" s="163" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="Q112" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R112" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>xc</v>
+        <v>xr</v>
       </c>
       <c r="S112" s="2"/>
       <c r="T112" s="2"/>
@@ -11523,14 +10386,14 @@
       <c r="N113" s="148"/>
       <c r="O113" s="148"/>
       <c r="P113" s="163" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="Q113" s="163" t="b">
         <v>0</v>
       </c>
       <c r="R113" s="207" t="str">
         <f t="shared" si="4"/>
-        <v>xr</v>
+        <v>z</v>
       </c>
       <c r="S113" s="2"/>
       <c r="T113" s="2"/>
@@ -11562,15 +10425,15 @@
       <c r="M114" s="148"/>
       <c r="N114" s="148"/>
       <c r="O114" s="148"/>
-      <c r="P114" s="163" t="s">
-        <v>345</v>
-      </c>
-      <c r="Q114" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="R114" s="207" t="str">
+      <c r="P114" s="164" t="s">
+        <v>346</v>
+      </c>
+      <c r="Q114" s="164" t="b">
+        <v>0</v>
+      </c>
+      <c r="R114" s="208" t="str">
         <f t="shared" si="4"/>
-        <v>z</v>
+        <v>zd</v>
       </c>
       <c r="S114" s="2"/>
       <c r="T114" s="2"/>
@@ -11582,63 +10445,58 @@
       <c r="Z114" s="1"/>
       <c r="AA114" s="1"/>
       <c r="AB114" s="1"/>
-    </row>
-    <row r="115" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="AD114" s="2"/>
+      <c r="AE114" s="2"/>
+      <c r="AF114" s="2"/>
+      <c r="AG114" s="2"/>
+      <c r="AH114" s="2"/>
+      <c r="AI114" s="2"/>
+      <c r="AJ114" s="2"/>
+      <c r="AK114" s="2"/>
+      <c r="AL114" s="2"/>
+      <c r="AM114" s="2"/>
+      <c r="AN114" s="2"/>
+      <c r="AO114" s="2"/>
+      <c r="AP114" s="4"/>
+      <c r="AQ114" s="81"/>
+      <c r="AR114" s="1"/>
+      <c r="AS114" s="1"/>
+      <c r="AT114" s="1"/>
+    </row>
+    <row r="115" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="33"/>
       <c r="C115" s="73">
-        <f t="shared" si="3"/>
+        <f>INT($C$31)+2.005</f>
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="D115" s="4"/>
+      <c r="E115" s="4"/>
+      <c r="F115" s="4"/>
+      <c r="G115" s="4"/>
+      <c r="H115" s="4"/>
+      <c r="I115" s="4"/>
+      <c r="J115" s="4"/>
+      <c r="K115" s="4"/>
+      <c r="L115" s="4"/>
+      <c r="M115" s="4"/>
+      <c r="N115" s="4"/>
+      <c r="O115" s="4"/>
+      <c r="P115" s="4"/>
+      <c r="Q115" s="4"/>
+      <c r="R115" s="4"/>
+      <c r="S115" s="4"/>
+      <c r="T115" s="4"/>
+      <c r="U115" s="4"/>
+      <c r="V115" s="4"/>
+      <c r="W115" s="4"/>
+      <c r="X115" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D115" s="4"/>
-      <c r="E115" s="5"/>
-      <c r="F115" s="5"/>
-      <c r="G115" s="4"/>
-      <c r="H115" s="2"/>
-      <c r="I115" s="2"/>
-      <c r="J115" s="2"/>
-      <c r="K115" s="2"/>
-      <c r="L115" s="2"/>
-      <c r="M115" s="148"/>
-      <c r="N115" s="148"/>
-      <c r="O115" s="148"/>
-      <c r="P115" s="164" t="s">
-        <v>347</v>
-      </c>
-      <c r="Q115" s="164" t="b">
-        <v>0</v>
-      </c>
-      <c r="R115" s="208" t="str">
-        <f t="shared" si="4"/>
-        <v>zd</v>
-      </c>
-      <c r="S115" s="2"/>
-      <c r="T115" s="2"/>
-      <c r="U115" s="2"/>
-      <c r="V115" s="2"/>
-      <c r="W115" s="2"/>
-      <c r="X115" s="4"/>
       <c r="Y115" s="16"/>
       <c r="Z115" s="1"/>
       <c r="AA115" s="1"/>
       <c r="AB115" s="1"/>
-      <c r="AD115" s="2"/>
-      <c r="AE115" s="2"/>
-      <c r="AF115" s="2"/>
-      <c r="AG115" s="2"/>
-      <c r="AH115" s="2"/>
-      <c r="AI115" s="2"/>
-      <c r="AJ115" s="2"/>
-      <c r="AK115" s="2"/>
-      <c r="AL115" s="2"/>
-      <c r="AM115" s="2"/>
-      <c r="AN115" s="2"/>
-      <c r="AO115" s="2"/>
-      <c r="AP115" s="4"/>
-      <c r="AQ115" s="81"/>
-      <c r="AR115" s="1"/>
-      <c r="AS115" s="1"/>
-      <c r="AT115" s="1"/>
     </row>
     <row r="116" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
@@ -11667,111 +10525,109 @@
       <c r="U116" s="4"/>
       <c r="V116" s="4"/>
       <c r="W116" s="4"/>
-      <c r="X116" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="X116" s="4"/>
       <c r="Y116" s="16"/>
       <c r="Z116" s="1"/>
       <c r="AA116" s="1"/>
       <c r="AB116" s="1"/>
     </row>
-    <row r="117" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
-      <c r="B117" s="33"/>
-      <c r="C117" s="73">
-        <f>INT($C$31)+2.005</f>
-        <v>3.0049999999999999</v>
-      </c>
-      <c r="D117" s="4"/>
-      <c r="E117" s="4"/>
-      <c r="F117" s="4"/>
-      <c r="G117" s="4"/>
-      <c r="H117" s="4"/>
-      <c r="I117" s="4"/>
-      <c r="J117" s="4"/>
-      <c r="K117" s="4"/>
-      <c r="L117" s="4"/>
-      <c r="M117" s="4"/>
-      <c r="N117" s="4"/>
-      <c r="O117" s="4"/>
-      <c r="P117" s="4"/>
-      <c r="Q117" s="4"/>
-      <c r="R117" s="4"/>
-      <c r="S117" s="4"/>
-      <c r="T117" s="4"/>
-      <c r="U117" s="4"/>
-      <c r="V117" s="4"/>
-      <c r="W117" s="4"/>
-      <c r="X117" s="4"/>
-      <c r="Y117" s="16"/>
+      <c r="B117" s="35"/>
+      <c r="C117" s="76">
+        <f>INT($C$31)+1.005</f>
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="D117" s="17"/>
+      <c r="E117" s="17"/>
+      <c r="F117" s="17"/>
+      <c r="G117" s="17"/>
+      <c r="H117" s="17"/>
+      <c r="I117" s="17"/>
+      <c r="J117" s="17"/>
+      <c r="K117" s="17"/>
+      <c r="L117" s="17"/>
+      <c r="M117" s="17"/>
+      <c r="N117" s="17"/>
+      <c r="O117" s="17"/>
+      <c r="P117" s="17"/>
+      <c r="Q117" s="17"/>
+      <c r="R117" s="17"/>
+      <c r="S117" s="17"/>
+      <c r="T117" s="17"/>
+      <c r="U117" s="17"/>
+      <c r="V117" s="17"/>
+      <c r="W117" s="17"/>
+      <c r="X117" s="17"/>
+      <c r="Y117" s="18" t="s">
+        <v>1</v>
+      </c>
       <c r="Z117" s="1"/>
       <c r="AA117" s="1"/>
       <c r="AB117" s="1"/>
     </row>
-    <row r="118" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:46" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
-      <c r="B118" s="35"/>
-      <c r="C118" s="76">
-        <f>INT($C$31)+1.005</f>
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="D118" s="17"/>
-      <c r="E118" s="17"/>
-      <c r="F118" s="17"/>
-      <c r="G118" s="17"/>
-      <c r="H118" s="17"/>
-      <c r="I118" s="17"/>
-      <c r="J118" s="17"/>
-      <c r="K118" s="17"/>
-      <c r="L118" s="17"/>
-      <c r="M118" s="17"/>
-      <c r="N118" s="17"/>
-      <c r="O118" s="17"/>
-      <c r="P118" s="17"/>
-      <c r="Q118" s="17"/>
-      <c r="R118" s="17"/>
-      <c r="S118" s="17"/>
-      <c r="T118" s="17"/>
-      <c r="U118" s="17"/>
-      <c r="V118" s="17"/>
-      <c r="W118" s="17"/>
-      <c r="X118" s="17"/>
-      <c r="Y118" s="18" t="s">
-        <v>1</v>
-      </c>
+      <c r="B118" s="19"/>
+      <c r="C118" s="77">
+        <f>INT($C$31)+0.005</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D118" s="19"/>
+      <c r="E118" s="19"/>
+      <c r="F118" s="19"/>
+      <c r="G118" s="19"/>
+      <c r="H118" s="19"/>
+      <c r="I118" s="19"/>
+      <c r="J118" s="19"/>
+      <c r="K118" s="19"/>
+      <c r="L118" s="19"/>
+      <c r="M118" s="19"/>
+      <c r="N118" s="19"/>
+      <c r="O118" s="19"/>
+      <c r="P118" s="19"/>
+      <c r="Q118" s="19"/>
+      <c r="R118" s="19"/>
+      <c r="S118" s="19"/>
+      <c r="T118" s="19"/>
+      <c r="U118" s="19"/>
+      <c r="V118" s="19"/>
+      <c r="W118" s="19"/>
+      <c r="X118" s="19"/>
+      <c r="Y118" s="19"/>
       <c r="Z118" s="1"/>
       <c r="AA118" s="1"/>
       <c r="AB118" s="1"/>
     </row>
-    <row r="119" spans="1:46" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
-      <c r="B119" s="19"/>
-      <c r="C119" s="77">
-        <f>INT($C$31)+0.005</f>
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="D119" s="19"/>
-      <c r="E119" s="19"/>
-      <c r="F119" s="19"/>
-      <c r="G119" s="19"/>
-      <c r="H119" s="19"/>
-      <c r="I119" s="19"/>
-      <c r="J119" s="19"/>
-      <c r="K119" s="19"/>
-      <c r="L119" s="19"/>
-      <c r="M119" s="19"/>
-      <c r="N119" s="19"/>
-      <c r="O119" s="19"/>
-      <c r="P119" s="19"/>
-      <c r="Q119" s="19"/>
-      <c r="R119" s="19"/>
-      <c r="S119" s="19"/>
-      <c r="T119" s="19"/>
-      <c r="U119" s="19"/>
-      <c r="V119" s="19"/>
-      <c r="W119" s="19"/>
-      <c r="X119" s="19"/>
-      <c r="Y119" s="19"/>
+      <c r="B119" s="1"/>
+      <c r="C119" s="73">
+        <f>INT($C$31)+2</f>
+        <v>3</v>
+      </c>
+      <c r="D119" s="1"/>
+      <c r="E119" s="1"/>
+      <c r="F119" s="1"/>
+      <c r="G119" s="1"/>
+      <c r="H119" s="1"/>
+      <c r="I119" s="1"/>
+      <c r="J119" s="1"/>
+      <c r="K119" s="1"/>
+      <c r="L119" s="1"/>
+      <c r="M119" s="1"/>
+      <c r="N119" s="1"/>
+      <c r="O119" s="1"/>
+      <c r="P119" s="1"/>
+      <c r="Q119" s="1"/>
+      <c r="R119" s="1"/>
+      <c r="S119" s="1"/>
+      <c r="T119" s="1"/>
+      <c r="U119" s="1"/>
+      <c r="V119" s="1"/>
+      <c r="W119" s="1"/>
+      <c r="X119" s="1"/>
+      <c r="Y119" s="1"/>
       <c r="Z119" s="1"/>
       <c r="AA119" s="1"/>
       <c r="AB119" s="1"/>
@@ -11809,13 +10665,10 @@
       <c r="AA120" s="1"/>
       <c r="AB120" s="1"/>
     </row>
-    <row r="121" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
-      <c r="C121" s="73">
-        <f>INT($C$31)+2</f>
-        <v>3</v>
-      </c>
+      <c r="C121" s="66"/>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
@@ -11993,37 +10846,7 @@
       <c r="AB126" s="1"/>
     </row>
     <row r="127" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A127" s="1"/>
-      <c r="B127" s="1"/>
-      <c r="C127" s="66"/>
-      <c r="D127" s="1"/>
-      <c r="E127" s="1"/>
-      <c r="F127" s="1"/>
-      <c r="G127" s="1"/>
-      <c r="H127" s="1"/>
-      <c r="I127" s="1"/>
-      <c r="J127" s="1"/>
-      <c r="K127" s="1"/>
-      <c r="L127" s="1"/>
-      <c r="M127" s="1"/>
-      <c r="N127" s="1"/>
-      <c r="O127" s="1"/>
-      <c r="P127" s="1"/>
-      <c r="Q127" s="1"/>
-      <c r="R127" s="1"/>
-      <c r="S127" s="1"/>
-      <c r="T127" s="1"/>
-      <c r="U127" s="1"/>
-      <c r="V127" s="1"/>
-      <c r="W127" s="1"/>
-      <c r="X127" s="1"/>
-      <c r="Y127" s="1"/>
-      <c r="Z127" s="1"/>
-      <c r="AA127" s="1"/>
-      <c r="AB127" s="1"/>
-    </row>
-    <row r="128" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="C128" s="72" t="s">
+      <c r="C127" s="72" t="s">
         <v>4</v>
       </c>
     </row>
@@ -12046,12 +10869,12 @@
   </sheetPr>
   <dimension ref="A1:AB334"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
       <pane xSplit="9" ySplit="10" topLeftCell="J138" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="N156" sqref="N156"/>
+      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -12544,7 +11367,7 @@
         <v>45049.868338773202</v>
       </c>
       <c r="J13" s="212" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="K13" s="213"/>
       <c r="L13" s="213"/>
@@ -12583,7 +11406,7 @@
         <v>44762.449343865701</v>
       </c>
       <c r="J14" s="215" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K14" s="216"/>
       <c r="L14" s="216"/>
@@ -18159,7 +16982,7 @@
       <c r="F156" s="5"/>
       <c r="G156" s="4"/>
       <c r="H156" s="64" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="I156" s="2"/>
       <c r="J156" s="2"/>
@@ -28365,7 +27188,7 @@
         <v>45076.548888773097</v>
       </c>
       <c r="J13" s="212" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="K13" s="213"/>
       <c r="L13" s="213"/>
@@ -28404,7 +27227,7 @@
         <v>45073.683614236099</v>
       </c>
       <c r="J14" s="215" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K14" s="216"/>
       <c r="L14" s="216"/>
@@ -29156,7 +27979,7 @@
       <c r="M35" s="124"/>
       <c r="N35" s="29"/>
       <c r="O35" s="29" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="P35" s="124" t="s">
         <v>44</v>
@@ -29232,24 +28055,24 @@
       <c r="I37" s="29"/>
       <c r="J37" s="29"/>
       <c r="K37" s="29" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L37" s="29"/>
       <c r="M37" s="156"/>
       <c r="N37" s="156" t="s">
+        <v>379</v>
+      </c>
+      <c r="O37" s="156" t="s">
         <v>380</v>
       </c>
-      <c r="O37" s="156" t="s">
+      <c r="P37" s="156" t="s">
         <v>381</v>
       </c>
-      <c r="P37" s="156" t="s">
+      <c r="Q37" s="156" t="s">
         <v>382</v>
       </c>
-      <c r="Q37" s="156" t="s">
-        <v>383</v>
-      </c>
       <c r="R37" s="156" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="S37" s="29"/>
       <c r="T37" s="29"/>
@@ -29858,7 +28681,7 @@
         <v>208</v>
       </c>
       <c r="O51" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
@@ -31971,7 +30794,7 @@
       <c r="M102" s="2"/>
       <c r="N102" s="2"/>
       <c r="O102" s="26" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="P102" s="2">
         <v>0.8</v>
@@ -32620,7 +31443,7 @@
       <c r="R120" s="2"/>
       <c r="S120" s="2"/>
       <c r="T120" s="26" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="U120" s="31" t="b">
         <v>0</v>
@@ -32649,7 +31472,7 @@
       <c r="J121" s="36"/>
       <c r="K121" s="36"/>
       <c r="L121" s="26" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M121" s="31">
         <v>0</v>
@@ -32731,7 +31554,7 @@
       <c r="J123" s="148"/>
       <c r="K123" s="148"/>
       <c r="L123" s="26" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="M123" s="31">
         <v>0</v>
@@ -32795,7 +31618,7 @@
       <c r="J125" s="205"/>
       <c r="K125" s="205"/>
       <c r="L125" s="26" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M125" s="31" t="b">
         <v>0</v>
@@ -34608,6 +33431,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE3626F-D681-4ABD-B02A-5C870438CFCF}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:Z31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -34744,7 +33568,7 @@
       <c r="E5" s="172"/>
       <c r="F5" s="173"/>
       <c r="G5" s="174" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H5" s="173"/>
       <c r="I5" s="173"/>
@@ -34802,7 +33626,7 @@
       <c r="E7" s="177"/>
       <c r="F7" s="173"/>
       <c r="G7" s="179" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H7" s="173"/>
       <c r="I7" s="173"/>
@@ -35056,33 +33880,33 @@
       <c r="E16" s="177"/>
       <c r="F16" s="185"/>
       <c r="G16" s="193" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H16" s="191"/>
       <c r="I16" s="193" t="s">
         <v>249</v>
       </c>
       <c r="K16" s="193" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L16" s="192"/>
       <c r="M16" s="193" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O16" s="193" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="P16" s="191"/>
       <c r="Q16" s="193" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="R16" s="191"/>
       <c r="S16" s="193" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="T16" s="192"/>
       <c r="U16" s="193" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="V16" s="190"/>
       <c r="W16" s="176"/>
@@ -35098,34 +33922,34 @@
       <c r="E17" s="177"/>
       <c r="F17" s="185"/>
       <c r="G17" s="191" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H17" s="191"/>
       <c r="I17" s="191" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J17" s="194"/>
       <c r="K17" s="191" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="L17" s="192"/>
       <c r="M17" s="191" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="O17" s="191" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="P17" s="191"/>
       <c r="Q17" s="191" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="R17" s="191"/>
       <c r="S17" s="191" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="T17" s="192"/>
       <c r="U17" s="191" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="V17" s="190"/>
       <c r="W17" s="176"/>

</xml_diff>

<commit_message>
Change the ffcfw report to ebw (to remove noise due to gut fill from the graph)
</commit_message>
<xml_diff>
--- a/ExcelInputs/Structural.xlsx
+++ b/ExcelInputs/Structural.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\Models\AFO\ExcelInputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\ExcelInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C181A69-6433-40B2-B06A-1EEBCCDC9425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4DAF90-CD6F-4E63-9AEB-4857997BFD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="678" activeTab="3" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -132,8 +132,8 @@
     <definedName name="i_rev_trait_name" localSheetId="2">StructuralSA!$H$129:$H$136</definedName>
     <definedName name="i_sim_periods_year">Stock!$I$62</definedName>
     <definedName name="i_store_cs_rep" localSheetId="3">'Report Settings'!$K$18</definedName>
+    <definedName name="i_store_ebw_rep">'Report Settings'!$G$18</definedName>
     <definedName name="i_store_feedbud" localSheetId="3">'Report Settings'!$U$18</definedName>
-    <definedName name="i_store_ffcfw_rep">'Report Settings'!$G$18</definedName>
     <definedName name="i_store_fs_rep" localSheetId="3">'Report Settings'!$M$18</definedName>
     <definedName name="i_store_lw_rep">'Report Settings'!$I$18</definedName>
     <definedName name="i_store_mort" localSheetId="3">'Report Settings'!$S$18</definedName>
@@ -182,9 +182,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -373,7 +371,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Michael Young (21512438):</t>
         </r>
@@ -382,7 +380,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 is this landuse baled usually (all landuses can be tactically baled but this is to tell AFO which landuses are meant to be baled i.e. which landuses have yields that are entered at baled)</t>
@@ -2243,7 +2241,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="392">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -3376,9 +3374,6 @@
     <t>Some arrays used for reporting are vary big so the default is not to store them. This is the default settings which can be overwritten using sensitivity values</t>
   </si>
   <si>
-    <t>FFCFW</t>
-  </si>
-  <si>
     <t>NV</t>
   </si>
   <si>
@@ -3465,17 +3460,6 @@
   </si>
   <si>
     <t>TOL</t>
-  </si>
-  <si>
-    <t>3May23: COnvert chill adjustment scalars for GBAL slices to a formula (still needs work on the 11, 22 &amp; 33 slices)
-17Jun22: Add a chill adjustment scalar with a b1 axis (to scale Property.xlsx!i_chill_adj)
-11Jul21: dvp/fvp updates 
-27Apr21: Split fvp inputs
-25Apr21: Deleted range names i_w1_len &amp; w3
-9Apr21: Fix formatting (box) around k2 cluster definition.
-30Mar21: Added inputs for % dry and number dams mated
-2: 17Jul20-Added structural inputs table
-1: 1Apr19-Created the version control table</t>
   </si>
   <si>
     <t>FVP3 / U0</t>
@@ -3538,6 +3522,23 @@
   <si>
     <t>is baled</t>
   </si>
+  <si>
+    <t>3May23: Convert chill adjustment scalars for GBAL slices to a formula (still needs work on the 11, 22 &amp; 33 slices)
+17Jun22: Add a chill adjustment scalar with a b1 axis (to scale Property.xlsx!i_chill_adj)
+11Jul21: dvp/fvp updates 
+27Apr21: Split fvp inputs
+25Apr21: Deleted range names i_w1_len &amp; w3
+9Apr21: Fix formatting (box) around k2 cluster definition.
+30Mar21: Added inputs for % dry and number dams mated
+2: 17Jul20-Added structural inputs table
+1: 1Apr19-Created the version control table</t>
+  </si>
+  <si>
+    <t>EBW</t>
+  </si>
+  <si>
+    <t>store ebw patterns</t>
+  </si>
 </sst>
 </file>
 
@@ -3549,7 +3550,7 @@
     <numFmt numFmtId="166" formatCode="0.00_)"/>
     <numFmt numFmtId="167" formatCode="[$-C09]dd\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3768,19 +3769,6 @@
       <color rgb="FF0000CC"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="40">
@@ -6676,7 +6664,7 @@
         <v>44719.411846643503</v>
       </c>
       <c r="J14" s="215" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="K14" s="216"/>
       <c r="L14" s="216"/>
@@ -7816,7 +7804,7 @@
         <v>176</v>
       </c>
       <c r="L46" s="97" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -8957,7 +8945,7 @@
         <v>311</v>
       </c>
       <c r="J78" s="161" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="K78" s="2"/>
       <c r="L78" s="161" t="s">
@@ -8965,17 +8953,17 @@
       </c>
       <c r="M78" s="2"/>
       <c r="N78" s="161" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="O78" s="2"/>
       <c r="P78" s="161" t="s">
         <v>313</v>
       </c>
       <c r="Q78" s="161" t="s">
+        <v>373</v>
+      </c>
+      <c r="R78" s="161" t="s">
         <v>374</v>
-      </c>
-      <c r="R78" s="161" t="s">
-        <v>375</v>
       </c>
       <c r="S78" s="2"/>
       <c r="T78" s="2"/>
@@ -9012,7 +9000,7 @@
       </c>
       <c r="M79" s="165"/>
       <c r="N79" s="210" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="O79" s="165"/>
       <c r="P79" s="162" t="s">
@@ -9096,13 +9084,13 @@
       </c>
       <c r="K81" s="55"/>
       <c r="L81" s="163" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M81" s="165"/>
       <c r="N81" s="165"/>
       <c r="O81" s="165"/>
       <c r="P81" s="163" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="Q81" s="163" t="b">
         <v>0</v>
@@ -9354,7 +9342,7 @@
       </c>
       <c r="K87" s="55"/>
       <c r="L87" s="163" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="M87" s="165"/>
       <c r="N87" s="165"/>
@@ -9856,7 +9844,7 @@
       <c r="N99" s="148"/>
       <c r="O99" s="148"/>
       <c r="P99" s="163" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="Q99" s="163" t="b">
         <v>0</v>
@@ -10869,12 +10857,12 @@
   </sheetPr>
   <dimension ref="A1:AB334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
       <pane xSplit="9" ySplit="10" topLeftCell="J138" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomRight" activeCell="J13" sqref="J13:T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -11367,7 +11355,7 @@
         <v>45049.868338773202</v>
       </c>
       <c r="J13" s="212" t="s">
-        <v>378</v>
+        <v>389</v>
       </c>
       <c r="K13" s="213"/>
       <c r="L13" s="213"/>
@@ -11406,7 +11394,7 @@
         <v>44762.449343865701</v>
       </c>
       <c r="J14" s="215" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="K14" s="216"/>
       <c r="L14" s="216"/>
@@ -16982,7 +16970,7 @@
       <c r="F156" s="5"/>
       <c r="G156" s="4"/>
       <c r="H156" s="64" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="I156" s="2"/>
       <c r="J156" s="2"/>
@@ -26686,11 +26674,11 @@
   <dimension ref="A1:AB175"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="10" topLeftCell="J75" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="J13" sqref="J13:T13"/>
+      <selection pane="bottomRight" activeCell="O99" sqref="O99:O101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -27188,7 +27176,7 @@
         <v>45076.548888773097</v>
       </c>
       <c r="J13" s="212" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="K13" s="213"/>
       <c r="L13" s="213"/>
@@ -27227,7 +27215,7 @@
         <v>45073.683614236099</v>
       </c>
       <c r="J14" s="215" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="K14" s="216"/>
       <c r="L14" s="216"/>
@@ -27979,7 +27967,7 @@
       <c r="M35" s="124"/>
       <c r="N35" s="29"/>
       <c r="O35" s="29" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="P35" s="124" t="s">
         <v>44</v>
@@ -28055,24 +28043,24 @@
       <c r="I37" s="29"/>
       <c r="J37" s="29"/>
       <c r="K37" s="29" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="L37" s="29"/>
       <c r="M37" s="156"/>
       <c r="N37" s="156" t="s">
+        <v>377</v>
+      </c>
+      <c r="O37" s="156" t="s">
+        <v>378</v>
+      </c>
+      <c r="P37" s="156" t="s">
         <v>379</v>
       </c>
-      <c r="O37" s="156" t="s">
+      <c r="Q37" s="156" t="s">
         <v>380</v>
       </c>
-      <c r="P37" s="156" t="s">
-        <v>381</v>
-      </c>
-      <c r="Q37" s="156" t="s">
+      <c r="R37" s="156" t="s">
         <v>382</v>
-      </c>
-      <c r="R37" s="156" t="s">
-        <v>384</v>
       </c>
       <c r="S37" s="29"/>
       <c r="T37" s="29"/>
@@ -28681,7 +28669,7 @@
         <v>208</v>
       </c>
       <c r="O51" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
@@ -30794,7 +30782,7 @@
       <c r="M102" s="2"/>
       <c r="N102" s="2"/>
       <c r="O102" s="26" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="P102" s="2">
         <v>0.8</v>
@@ -31618,7 +31606,7 @@
       <c r="J125" s="205"/>
       <c r="K125" s="205"/>
       <c r="L125" s="26" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="M125" s="31" t="b">
         <v>0</v>
@@ -33434,8 +33422,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -33880,33 +33868,33 @@
       <c r="E16" s="177"/>
       <c r="F16" s="185"/>
       <c r="G16" s="193" t="s">
-        <v>354</v>
+        <v>390</v>
       </c>
       <c r="H16" s="191"/>
       <c r="I16" s="193" t="s">
         <v>249</v>
       </c>
       <c r="K16" s="193" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="L16" s="192"/>
       <c r="M16" s="193" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="O16" s="193" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="P16" s="191"/>
       <c r="Q16" s="193" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="R16" s="191"/>
       <c r="S16" s="193" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="T16" s="192"/>
       <c r="U16" s="193" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="V16" s="190"/>
       <c r="W16" s="176"/>
@@ -33922,34 +33910,34 @@
       <c r="E17" s="177"/>
       <c r="F17" s="185"/>
       <c r="G17" s="191" t="s">
-        <v>358</v>
+        <v>391</v>
       </c>
       <c r="H17" s="191"/>
       <c r="I17" s="191" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="J17" s="194"/>
       <c r="K17" s="191" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="L17" s="192"/>
       <c r="M17" s="191" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="O17" s="191" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="P17" s="191"/>
       <c r="Q17" s="191" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="R17" s="191"/>
       <c r="S17" s="191" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="T17" s="192"/>
       <c r="U17" s="191" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="V17" s="190"/>
       <c r="W17" s="176"/>

</xml_diff>

<commit_message>
Add extra REV variables: fat, muscle, viscera, foetus, milk, intake & SS. Added to functions, function calls, exp.xl and structural.xl No change in profit
</commit_message>
<xml_diff>
--- a/ExcelInputs/Structural.xlsx
+++ b/ExcelInputs/Structural.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\ExcelInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4045A229-DE11-4F79-8576-24430D5323F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8F5405-6A87-479D-8396-3B938CECEE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
@@ -91,7 +91,7 @@
     <definedName name="i_lag_organs">Stock!$I$70</definedName>
     <definedName name="i_lag_wool">Stock!$I$69</definedName>
     <definedName name="i_landuse_is_dual" localSheetId="0">General!$Q$79:$Q$108</definedName>
-    <definedName name="i_len_f">StructuralSA!$I$157</definedName>
+    <definedName name="i_len_f">StructuralSA!$I$164</definedName>
     <definedName name="i_len_l">Stock!$M$160</definedName>
     <definedName name="i_len_m">Stock!$L$160</definedName>
     <definedName name="i_len_s">Stock!$N$160</definedName>
@@ -119,16 +119,16 @@
     <definedName name="i_nut_spread_n0" localSheetId="2">StructuralSA!$J$87</definedName>
     <definedName name="i_nut_spread_n1" localSheetId="2">StructuralSA!$M$87:$M$94</definedName>
     <definedName name="i_nut_spread_n3" localSheetId="2">StructuralSA!$S$87:$S$94</definedName>
-    <definedName name="i_nv_lower_p6">StructuralSA!$J$160:$S$160</definedName>
-    <definedName name="i_nv_upper_p6">StructuralSA!$J$161:$S$161</definedName>
+    <definedName name="i_nv_lower_p6">StructuralSA!$J$167:$S$167</definedName>
+    <definedName name="i_nv_upper_p6">StructuralSA!$J$168:$S$168</definedName>
     <definedName name="i_offs_user_fvp_date_iu" localSheetId="2">StructuralSA!$P$54:$R$56</definedName>
     <definedName name="i_p_pos">Stock!$I$55</definedName>
     <definedName name="i_prejoin_offset">Stock!$I$66</definedName>
     <definedName name="i_progeny_w2_len">StructuralSA!$Q$79</definedName>
     <definedName name="i_r2adjust_inc">StructuralSA!$U$120</definedName>
     <definedName name="i_rev_number" localSheetId="2">StructuralSA!$I$122</definedName>
-    <definedName name="i_rev_trait_name" localSheetId="2">StructuralSA!$H$129:$H$136</definedName>
-    <definedName name="i_rev_trait_scenario" localSheetId="2">StructuralSA!$I$129:$I$136</definedName>
+    <definedName name="i_rev_trait_name" localSheetId="2">StructuralSA!$H$129:$H$143</definedName>
+    <definedName name="i_rev_trait_scenario" localSheetId="2">StructuralSA!$I$129:$I$143</definedName>
     <definedName name="i_rev_update" localSheetId="2">StructuralSA!$I$120</definedName>
     <definedName name="i_sim_periods_year">Stock!$I$62</definedName>
     <definedName name="i_store_cs_rep" localSheetId="3">'Report Settings'!$K$18</definedName>
@@ -2131,7 +2131,79 @@
         </r>
       </text>
     </comment>
-    <comment ref="H133" authorId="0" shapeId="0" xr:uid="{B4758F67-1D7E-4D60-BB06-F13A6FE89F0F}">
+    <comment ref="H131" authorId="1" shapeId="0" xr:uid="{A12E8373-CBF7-4301-8BBE-54FB2CD3F999}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>John:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Only active for the new feeding system (f_lwc_nfs)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H132" authorId="1" shapeId="0" xr:uid="{ADD99B78-258B-4112-BEFE-ACD7C132C257}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>John:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Only active for the new feeding system (f_lwc_nfs)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H133" authorId="1" shapeId="0" xr:uid="{F4A4ECC6-7846-4162-9607-F6E572F33EDF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>John:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Only active for the new feeding system (f_lwc_nfs)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H139" authorId="0" shapeId="0" xr:uid="{658A1575-7B6D-49A0-9205-9DD14E053E41}">
       <text>
         <r>
           <rPr>
@@ -2155,7 +2227,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H157" authorId="1" shapeId="0" xr:uid="{B39EFDC6-7ABB-4808-93B1-2819F2755236}">
+    <comment ref="H164" authorId="1" shapeId="0" xr:uid="{B39EFDC6-7ABB-4808-93B1-2819F2755236}">
       <text>
         <r>
           <rPr>
@@ -2179,7 +2251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H160" authorId="1" shapeId="0" xr:uid="{315CC92D-C01A-4D16-90CA-458397130ECA}">
+    <comment ref="H167" authorId="1" shapeId="0" xr:uid="{315CC92D-C01A-4D16-90CA-458397130ECA}">
       <text>
         <r>
           <rPr>
@@ -2205,7 +2277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H161" authorId="1" shapeId="0" xr:uid="{24292EB5-78CD-4E29-870F-1743067DEF27}">
+    <comment ref="H168" authorId="1" shapeId="0" xr:uid="{24292EB5-78CD-4E29-870F-1743067DEF27}">
       <text>
         <r>
           <rPr>
@@ -2270,7 +2342,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="393">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -3528,7 +3600,29 @@
     <t>REV scenario</t>
   </si>
   <si>
-    <t>22Jan24: Change rev_create to rev_update, and rev_trait_inc to rev_trait_scenario
+    <t>ss</t>
+  </si>
+  <si>
+    <t>intake</t>
+  </si>
+  <si>
+    <t>fat</t>
+  </si>
+  <si>
+    <t>muscle</t>
+  </si>
+  <si>
+    <t>viscera</t>
+  </si>
+  <si>
+    <t>foetus</t>
+  </si>
+  <si>
+    <t>milk</t>
+  </si>
+  <si>
+    <t>23Jan24: Add extra traits for REV (15 in total counting random)
+22Jan24: Change rev_create to rev_update, and rev_trait_inc to rev_trait_scenario
 30May23: Add extra user FVP to represent the preg tox period.
 27May23: Fix the FVP period numbers defining U0 as weaning
 20Jun22: Add extra user defined FVPs
@@ -26642,14 +26736,14 @@
   <sheetPr codeName="Sheet3">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB175"/>
+  <dimension ref="A1:AB182"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J101" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="10" topLeftCell="J110" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="J13" sqref="J13:T13"/>
+      <selection pane="bottomRight" activeCell="H132" sqref="H132:H133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -27144,10 +27238,10 @@
         <v>16</v>
       </c>
       <c r="I13" s="126">
-        <v>45313.7148212963</v>
+        <v>45314.472435879601</v>
       </c>
       <c r="J13" s="212" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="K13" s="213"/>
       <c r="L13" s="213"/>
@@ -31055,7 +31149,7 @@
       <c r="A111" s="1"/>
       <c r="B111" s="33"/>
       <c r="C111" s="73">
-        <f>INT(MAX($C$119:$C$139))+1</f>
+        <f>INT(MAX($C$119:$C$146))+1</f>
         <v>5</v>
       </c>
       <c r="D111" s="3"/>
@@ -31719,7 +31813,7 @@
       <c r="F129" s="5"/>
       <c r="G129" s="4"/>
       <c r="H129" s="31" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="I129" s="31">
         <v>0</v>
@@ -31758,7 +31852,7 @@
       <c r="F130" s="5"/>
       <c r="G130" s="4"/>
       <c r="H130" s="31" t="s">
-        <v>259</v>
+        <v>386</v>
       </c>
       <c r="I130" s="31">
         <v>0</v>
@@ -31797,7 +31891,7 @@
       <c r="F131" s="5"/>
       <c r="G131" s="4"/>
       <c r="H131" s="31" t="s">
-        <v>260</v>
+        <v>387</v>
       </c>
       <c r="I131" s="31">
         <v>0</v>
@@ -31836,7 +31930,7 @@
       <c r="F132" s="5"/>
       <c r="G132" s="4"/>
       <c r="H132" s="31" t="s">
-        <v>261</v>
+        <v>388</v>
       </c>
       <c r="I132" s="31">
         <v>0</v>
@@ -31875,7 +31969,7 @@
       <c r="F133" s="5"/>
       <c r="G133" s="4"/>
       <c r="H133" s="31" t="s">
-        <v>262</v>
+        <v>389</v>
       </c>
       <c r="I133" s="31">
         <v>0</v>
@@ -31904,7 +31998,7 @@
       <c r="A134" s="1"/>
       <c r="B134" s="33"/>
       <c r="C134" s="73">
-        <f t="shared" ref="C134:C136" si="10">INT(C$112+3)</f>
+        <f t="shared" ref="C134:C143" si="10">INT(C$112+3)</f>
         <v>4</v>
       </c>
       <c r="D134" s="4"/>
@@ -31914,7 +32008,7 @@
       <c r="F134" s="5"/>
       <c r="G134" s="4"/>
       <c r="H134" s="31" t="s">
-        <v>263</v>
+        <v>391</v>
       </c>
       <c r="I134" s="31">
         <v>0</v>
@@ -31953,7 +32047,7 @@
       <c r="F135" s="5"/>
       <c r="G135" s="4"/>
       <c r="H135" s="31" t="s">
-        <v>265</v>
+        <v>390</v>
       </c>
       <c r="I135" s="31">
         <v>0</v>
@@ -31992,7 +32086,7 @@
       <c r="F136" s="5"/>
       <c r="G136" s="4"/>
       <c r="H136" s="31" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I136" s="31">
         <v>0</v>
@@ -32021,15 +32115,21 @@
       <c r="A137" s="1"/>
       <c r="B137" s="33"/>
       <c r="C137" s="73">
-        <f>INT(C$112+3)</f>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="D137" s="4"/>
-      <c r="E137" s="5"/>
+      <c r="E137" s="5">
+        <v>8</v>
+      </c>
       <c r="F137" s="5"/>
       <c r="G137" s="4"/>
-      <c r="H137" s="148"/>
-      <c r="I137" s="148"/>
+      <c r="H137" s="31" t="s">
+        <v>260</v>
+      </c>
+      <c r="I137" s="31">
+        <v>0</v>
+      </c>
       <c r="J137" s="148"/>
       <c r="K137" s="148"/>
       <c r="L137" s="148"/>
@@ -32054,15 +32154,21 @@
       <c r="A138" s="1"/>
       <c r="B138" s="33"/>
       <c r="C138" s="73">
-        <f>INT(C$112+3)</f>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="D138" s="4"/>
-      <c r="E138" s="5"/>
+      <c r="E138" s="5">
+        <v>9</v>
+      </c>
       <c r="F138" s="5"/>
       <c r="G138" s="4"/>
-      <c r="H138" s="148"/>
-      <c r="I138" s="148"/>
+      <c r="H138" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="I138" s="31">
+        <v>0</v>
+      </c>
       <c r="J138" s="148"/>
       <c r="K138" s="148"/>
       <c r="L138" s="148"/>
@@ -32083,537 +32189,533 @@
       <c r="AA138" s="1"/>
       <c r="AB138" s="1"/>
     </row>
-    <row r="139" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="33"/>
       <c r="C139" s="73">
-        <f>INT($C$112)+3.005</f>
-        <v>4.0049999999999999</v>
+        <f t="shared" si="10"/>
+        <v>4</v>
       </c>
       <c r="D139" s="4"/>
-      <c r="E139" s="4"/>
-      <c r="F139" s="4"/>
+      <c r="E139" s="5">
+        <v>10</v>
+      </c>
+      <c r="F139" s="5"/>
       <c r="G139" s="4"/>
-      <c r="H139" s="4"/>
-      <c r="I139" s="4"/>
-      <c r="J139" s="4"/>
-      <c r="K139" s="4"/>
-      <c r="L139" s="4"/>
-      <c r="M139" s="4"/>
-      <c r="N139" s="4"/>
-      <c r="O139" s="4"/>
-      <c r="P139" s="4"/>
-      <c r="Q139" s="4"/>
-      <c r="R139" s="4"/>
-      <c r="S139" s="4"/>
-      <c r="T139" s="4"/>
-      <c r="U139" s="4"/>
-      <c r="V139" s="4"/>
-      <c r="W139" s="4"/>
-      <c r="X139" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="H139" s="31" t="s">
+        <v>262</v>
+      </c>
+      <c r="I139" s="31">
+        <v>0</v>
+      </c>
+      <c r="J139" s="148"/>
+      <c r="K139" s="148"/>
+      <c r="L139" s="148"/>
+      <c r="M139" s="148"/>
+      <c r="N139" s="148"/>
+      <c r="O139" s="148"/>
+      <c r="P139" s="148"/>
+      <c r="Q139" s="148"/>
+      <c r="R139" s="148"/>
+      <c r="S139" s="2"/>
+      <c r="T139" s="2"/>
+      <c r="U139" s="2"/>
+      <c r="V139" s="2"/>
+      <c r="W139" s="2"/>
+      <c r="X139" s="4"/>
       <c r="Y139" s="16"/>
       <c r="Z139" s="1"/>
       <c r="AA139" s="1"/>
       <c r="AB139" s="1"/>
     </row>
-    <row r="140" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="33"/>
       <c r="C140" s="73">
-        <f>INT($C$112)+2.005</f>
-        <v>3.0049999999999999</v>
+        <f t="shared" si="10"/>
+        <v>4</v>
       </c>
       <c r="D140" s="4"/>
-      <c r="E140" s="4"/>
-      <c r="F140" s="4"/>
+      <c r="E140" s="5">
+        <v>11</v>
+      </c>
+      <c r="F140" s="5"/>
       <c r="G140" s="4"/>
-      <c r="H140" s="4"/>
-      <c r="I140" s="4"/>
-      <c r="J140" s="4"/>
-      <c r="K140" s="4"/>
-      <c r="L140" s="4"/>
-      <c r="M140" s="4"/>
-      <c r="N140" s="4"/>
-      <c r="O140" s="4"/>
-      <c r="P140" s="4"/>
-      <c r="Q140" s="4"/>
-      <c r="R140" s="4"/>
-      <c r="S140" s="4"/>
-      <c r="T140" s="4"/>
-      <c r="U140" s="4"/>
-      <c r="V140" s="4"/>
-      <c r="W140" s="4"/>
+      <c r="H140" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="I140" s="31">
+        <v>0</v>
+      </c>
+      <c r="J140" s="148"/>
+      <c r="K140" s="148"/>
+      <c r="L140" s="148"/>
+      <c r="M140" s="148"/>
+      <c r="N140" s="148"/>
+      <c r="O140" s="148"/>
+      <c r="P140" s="148"/>
+      <c r="Q140" s="148"/>
+      <c r="R140" s="148"/>
+      <c r="S140" s="2"/>
+      <c r="T140" s="2"/>
+      <c r="U140" s="2"/>
+      <c r="V140" s="2"/>
+      <c r="W140" s="2"/>
       <c r="X140" s="4"/>
       <c r="Y140" s="16"/>
       <c r="Z140" s="1"/>
       <c r="AA140" s="1"/>
       <c r="AB140" s="1"/>
     </row>
-    <row r="141" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
-      <c r="B141" s="35"/>
-      <c r="C141" s="76">
-        <f>INT($C$112)+1.005</f>
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="D141" s="17"/>
-      <c r="E141" s="17"/>
-      <c r="F141" s="17"/>
-      <c r="G141" s="17"/>
-      <c r="H141" s="17"/>
-      <c r="I141" s="17"/>
-      <c r="J141" s="17"/>
-      <c r="K141" s="17"/>
-      <c r="L141" s="17"/>
-      <c r="M141" s="17"/>
-      <c r="N141" s="17"/>
-      <c r="O141" s="17"/>
-      <c r="P141" s="17"/>
-      <c r="Q141" s="17"/>
-      <c r="R141" s="17"/>
-      <c r="S141" s="17"/>
-      <c r="T141" s="17"/>
-      <c r="U141" s="17"/>
-      <c r="V141" s="17"/>
-      <c r="W141" s="17"/>
-      <c r="X141" s="17"/>
-      <c r="Y141" s="18" t="s">
-        <v>1</v>
-      </c>
+      <c r="B141" s="33"/>
+      <c r="C141" s="73">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="D141" s="4"/>
+      <c r="E141" s="5">
+        <v>12</v>
+      </c>
+      <c r="F141" s="5"/>
+      <c r="G141" s="4"/>
+      <c r="H141" s="31" t="s">
+        <v>258</v>
+      </c>
+      <c r="I141" s="31">
+        <v>0</v>
+      </c>
+      <c r="J141" s="148"/>
+      <c r="K141" s="148"/>
+      <c r="L141" s="148"/>
+      <c r="M141" s="148"/>
+      <c r="N141" s="148"/>
+      <c r="O141" s="148"/>
+      <c r="P141" s="148"/>
+      <c r="Q141" s="148"/>
+      <c r="R141" s="148"/>
+      <c r="S141" s="2"/>
+      <c r="T141" s="2"/>
+      <c r="U141" s="2"/>
+      <c r="V141" s="2"/>
+      <c r="W141" s="2"/>
+      <c r="X141" s="4"/>
+      <c r="Y141" s="16"/>
       <c r="Z141" s="1"/>
       <c r="AA141" s="1"/>
       <c r="AB141" s="1"/>
     </row>
-    <row r="142" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
-      <c r="B142" s="19"/>
-      <c r="C142" s="77">
-        <f>INT($C$112)+0.005</f>
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="D142" s="19"/>
-      <c r="E142" s="19"/>
-      <c r="F142" s="19"/>
-      <c r="G142" s="19"/>
-      <c r="H142" s="19"/>
-      <c r="I142" s="19"/>
-      <c r="J142" s="19"/>
-      <c r="K142" s="19"/>
-      <c r="L142" s="19"/>
-      <c r="M142" s="19"/>
-      <c r="N142" s="19"/>
-      <c r="O142" s="19"/>
-      <c r="P142" s="19"/>
-      <c r="Q142" s="19"/>
-      <c r="R142" s="19"/>
-      <c r="S142" s="19"/>
-      <c r="T142" s="19"/>
-      <c r="U142" s="19"/>
-      <c r="V142" s="19"/>
-      <c r="W142" s="19"/>
-      <c r="X142" s="19"/>
-      <c r="Y142" s="19"/>
+      <c r="B142" s="33"/>
+      <c r="C142" s="73">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="D142" s="4"/>
+      <c r="E142" s="5">
+        <v>13</v>
+      </c>
+      <c r="F142" s="5"/>
+      <c r="G142" s="4"/>
+      <c r="H142" s="31" t="s">
+        <v>259</v>
+      </c>
+      <c r="I142" s="31">
+        <v>0</v>
+      </c>
+      <c r="J142" s="148"/>
+      <c r="K142" s="148"/>
+      <c r="L142" s="148"/>
+      <c r="M142" s="148"/>
+      <c r="N142" s="148"/>
+      <c r="O142" s="148"/>
+      <c r="P142" s="148"/>
+      <c r="Q142" s="148"/>
+      <c r="R142" s="148"/>
+      <c r="S142" s="2"/>
+      <c r="T142" s="2"/>
+      <c r="U142" s="2"/>
+      <c r="V142" s="2"/>
+      <c r="W142" s="2"/>
+      <c r="X142" s="4"/>
+      <c r="Y142" s="16"/>
       <c r="Z142" s="1"/>
       <c r="AA142" s="1"/>
       <c r="AB142" s="1"/>
     </row>
-    <row r="143" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
-      <c r="B143" s="1"/>
+      <c r="B143" s="33"/>
       <c r="C143" s="73">
-        <f>INT($C$112)+2</f>
-        <v>3</v>
-      </c>
-      <c r="D143" s="1"/>
-      <c r="E143" s="1"/>
-      <c r="F143" s="1"/>
-      <c r="G143" s="1"/>
-      <c r="H143" s="1"/>
-      <c r="I143" s="1"/>
-      <c r="J143" s="1"/>
-      <c r="K143" s="1"/>
-      <c r="L143" s="1"/>
-      <c r="M143" s="1"/>
-      <c r="N143" s="1"/>
-      <c r="O143" s="1"/>
-      <c r="P143" s="1"/>
-      <c r="Q143" s="1"/>
-      <c r="R143" s="1"/>
-      <c r="S143" s="1"/>
-      <c r="T143" s="1"/>
-      <c r="U143" s="1"/>
-      <c r="V143" s="1"/>
-      <c r="W143" s="1"/>
-      <c r="X143" s="1"/>
-      <c r="Y143" s="1"/>
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="D143" s="4"/>
+      <c r="E143" s="5">
+        <v>14</v>
+      </c>
+      <c r="F143" s="5"/>
+      <c r="G143" s="4"/>
+      <c r="H143" s="31" t="s">
+        <v>385</v>
+      </c>
+      <c r="I143" s="31">
+        <v>0</v>
+      </c>
+      <c r="J143" s="148"/>
+      <c r="K143" s="148"/>
+      <c r="L143" s="148"/>
+      <c r="M143" s="148"/>
+      <c r="N143" s="148"/>
+      <c r="O143" s="148"/>
+      <c r="P143" s="148"/>
+      <c r="Q143" s="148"/>
+      <c r="R143" s="148"/>
+      <c r="S143" s="2"/>
+      <c r="T143" s="2"/>
+      <c r="U143" s="2"/>
+      <c r="V143" s="2"/>
+      <c r="W143" s="2"/>
+      <c r="X143" s="4"/>
+      <c r="Y143" s="16"/>
       <c r="Z143" s="1"/>
       <c r="AA143" s="1"/>
       <c r="AB143" s="1"/>
     </row>
-    <row r="144" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
-      <c r="B144" s="1"/>
+      <c r="B144" s="33"/>
       <c r="C144" s="73">
-        <f>INT($C$148)+2</f>
-        <v>3</v>
-      </c>
-      <c r="D144" s="1"/>
-      <c r="E144" s="1"/>
-      <c r="F144" s="1"/>
-      <c r="G144" s="1"/>
-      <c r="H144" s="1"/>
-      <c r="I144" s="1"/>
-      <c r="J144" s="1"/>
-      <c r="K144" s="1"/>
-      <c r="L144" s="1"/>
-      <c r="M144" s="1"/>
-      <c r="N144" s="1"/>
-      <c r="O144" s="1"/>
-      <c r="P144" s="1"/>
-      <c r="Q144" s="1"/>
-      <c r="R144" s="1"/>
-      <c r="S144" s="1"/>
-      <c r="T144" s="1"/>
-      <c r="U144" s="1"/>
-      <c r="V144" s="1"/>
-      <c r="W144" s="1"/>
-      <c r="X144" s="1"/>
-      <c r="Y144" s="1"/>
+        <f>INT(C$112+3)</f>
+        <v>4</v>
+      </c>
+      <c r="D144" s="4"/>
+      <c r="E144" s="5"/>
+      <c r="F144" s="5"/>
+      <c r="G144" s="4"/>
+      <c r="H144" s="148"/>
+      <c r="I144" s="148"/>
+      <c r="J144" s="148"/>
+      <c r="K144" s="148"/>
+      <c r="L144" s="148"/>
+      <c r="M144" s="148"/>
+      <c r="N144" s="148"/>
+      <c r="O144" s="148"/>
+      <c r="P144" s="148"/>
+      <c r="Q144" s="148"/>
+      <c r="R144" s="148"/>
+      <c r="S144" s="2"/>
+      <c r="T144" s="2"/>
+      <c r="U144" s="2"/>
+      <c r="V144" s="2"/>
+      <c r="W144" s="2"/>
+      <c r="X144" s="4"/>
+      <c r="Y144" s="16"/>
       <c r="Z144" s="1"/>
       <c r="AA144" s="1"/>
       <c r="AB144" s="1"/>
     </row>
-    <row r="145" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
-      <c r="B145" s="20"/>
-      <c r="C145" s="74">
-        <f>INT($C$148)+0.005</f>
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="D145" s="20"/>
-      <c r="E145" s="20"/>
-      <c r="F145" s="20"/>
-      <c r="G145" s="20"/>
-      <c r="H145" s="20"/>
-      <c r="I145" s="20"/>
-      <c r="J145" s="20"/>
-      <c r="K145" s="20"/>
-      <c r="L145" s="20"/>
-      <c r="M145" s="20"/>
-      <c r="N145" s="20"/>
-      <c r="O145" s="20"/>
-      <c r="P145" s="20"/>
-      <c r="Q145" s="20"/>
-      <c r="R145" s="20"/>
-      <c r="S145" s="20"/>
-      <c r="T145" s="20"/>
-      <c r="U145" s="20"/>
-      <c r="V145" s="20"/>
-      <c r="W145" s="20"/>
-      <c r="X145" s="20"/>
-      <c r="Y145" s="20"/>
+      <c r="B145" s="33"/>
+      <c r="C145" s="73">
+        <f>INT(C$112+3)</f>
+        <v>4</v>
+      </c>
+      <c r="D145" s="4"/>
+      <c r="E145" s="5"/>
+      <c r="F145" s="5"/>
+      <c r="G145" s="4"/>
+      <c r="H145" s="148"/>
+      <c r="I145" s="148"/>
+      <c r="J145" s="148"/>
+      <c r="K145" s="148"/>
+      <c r="L145" s="148"/>
+      <c r="M145" s="148"/>
+      <c r="N145" s="148"/>
+      <c r="O145" s="148"/>
+      <c r="P145" s="148"/>
+      <c r="Q145" s="148"/>
+      <c r="R145" s="148"/>
+      <c r="S145" s="2"/>
+      <c r="T145" s="2"/>
+      <c r="U145" s="2"/>
+      <c r="V145" s="2"/>
+      <c r="W145" s="2"/>
+      <c r="X145" s="4"/>
+      <c r="Y145" s="16"/>
       <c r="Z145" s="1"/>
       <c r="AA145" s="1"/>
       <c r="AB145" s="1"/>
     </row>
-    <row r="146" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
-      <c r="B146" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="C146" s="75">
-        <f>INT($C$148)+1.005</f>
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="D146" s="14"/>
-      <c r="E146" s="14"/>
-      <c r="F146" s="14"/>
-      <c r="G146" s="14"/>
-      <c r="H146" s="14"/>
-      <c r="I146" s="14"/>
-      <c r="J146" s="14"/>
-      <c r="K146" s="14"/>
-      <c r="L146" s="14"/>
-      <c r="M146" s="14"/>
-      <c r="N146" s="14"/>
-      <c r="O146" s="14"/>
-      <c r="P146" s="14"/>
-      <c r="Q146" s="14"/>
-      <c r="R146" s="14"/>
-      <c r="S146" s="14"/>
-      <c r="T146" s="14"/>
-      <c r="U146" s="14"/>
-      <c r="V146" s="14"/>
-      <c r="W146" s="14"/>
-      <c r="X146" s="14"/>
-      <c r="Y146" s="15"/>
+      <c r="B146" s="33"/>
+      <c r="C146" s="73">
+        <f>INT($C$112)+3.005</f>
+        <v>4.0049999999999999</v>
+      </c>
+      <c r="D146" s="4"/>
+      <c r="E146" s="4"/>
+      <c r="F146" s="4"/>
+      <c r="G146" s="4"/>
+      <c r="H146" s="4"/>
+      <c r="I146" s="4"/>
+      <c r="J146" s="4"/>
+      <c r="K146" s="4"/>
+      <c r="L146" s="4"/>
+      <c r="M146" s="4"/>
+      <c r="N146" s="4"/>
+      <c r="O146" s="4"/>
+      <c r="P146" s="4"/>
+      <c r="Q146" s="4"/>
+      <c r="R146" s="4"/>
+      <c r="S146" s="4"/>
+      <c r="T146" s="4"/>
+      <c r="U146" s="4"/>
+      <c r="V146" s="4"/>
+      <c r="W146" s="4"/>
+      <c r="X146" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y146" s="16"/>
       <c r="Z146" s="1"/>
       <c r="AA146" s="1"/>
       <c r="AB146" s="1"/>
     </row>
-    <row r="147" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="33"/>
       <c r="C147" s="73">
-        <f>INT(MAX($C$156:$C$164))+1</f>
-        <v>5</v>
-      </c>
-      <c r="D147" s="3"/>
-      <c r="E147" s="3"/>
-      <c r="F147" s="3"/>
-      <c r="G147" s="3"/>
-      <c r="H147" s="27"/>
-      <c r="I147" s="27"/>
-      <c r="J147" s="27"/>
-      <c r="K147" s="27"/>
-      <c r="L147" s="27"/>
-      <c r="M147" s="27"/>
-      <c r="N147" s="27"/>
-      <c r="O147" s="27"/>
-      <c r="P147" s="27"/>
-      <c r="Q147" s="27"/>
-      <c r="R147" s="27"/>
-      <c r="S147" s="27"/>
-      <c r="T147" s="27"/>
-      <c r="U147" s="27"/>
-      <c r="V147" s="27"/>
-      <c r="W147" s="27"/>
-      <c r="X147" s="3"/>
+        <f>INT($C$112)+2.005</f>
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="D147" s="4"/>
+      <c r="E147" s="4"/>
+      <c r="F147" s="4"/>
+      <c r="G147" s="4"/>
+      <c r="H147" s="4"/>
+      <c r="I147" s="4"/>
+      <c r="J147" s="4"/>
+      <c r="K147" s="4"/>
+      <c r="L147" s="4"/>
+      <c r="M147" s="4"/>
+      <c r="N147" s="4"/>
+      <c r="O147" s="4"/>
+      <c r="P147" s="4"/>
+      <c r="Q147" s="4"/>
+      <c r="R147" s="4"/>
+      <c r="S147" s="4"/>
+      <c r="T147" s="4"/>
+      <c r="U147" s="4"/>
+      <c r="V147" s="4"/>
+      <c r="W147" s="4"/>
+      <c r="X147" s="4"/>
       <c r="Y147" s="16"/>
       <c r="Z147" s="1"/>
       <c r="AA147" s="1"/>
       <c r="AB147" s="1"/>
     </row>
-    <row r="148" spans="1:28" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
-      <c r="B148" s="33"/>
-      <c r="C148" s="73">
-        <v>1.02</v>
-      </c>
-      <c r="D148" s="21"/>
-      <c r="E148" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="F148" s="25"/>
-      <c r="G148" s="12"/>
-      <c r="H148" s="147" t="str">
-        <f>COUNTIFS($B$1:$B148, "«")&amp;" Feed Pool definitions"</f>
-        <v>5 Feed Pool definitions</v>
-      </c>
-      <c r="I148" s="6"/>
-      <c r="J148" s="6"/>
-      <c r="K148" s="6"/>
-      <c r="L148" s="6"/>
-      <c r="M148" s="6"/>
-      <c r="N148" s="6"/>
-      <c r="O148" s="6"/>
-      <c r="P148" s="6"/>
-      <c r="Q148" s="6"/>
-      <c r="R148" s="6"/>
-      <c r="S148" s="6"/>
-      <c r="T148" s="6"/>
-      <c r="U148" s="6"/>
-      <c r="V148" s="6"/>
-      <c r="W148" s="6"/>
-      <c r="X148" s="10"/>
-      <c r="Y148" s="16"/>
+      <c r="B148" s="35"/>
+      <c r="C148" s="76">
+        <f>INT($C$112)+1.005</f>
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="D148" s="17"/>
+      <c r="E148" s="17"/>
+      <c r="F148" s="17"/>
+      <c r="G148" s="17"/>
+      <c r="H148" s="17"/>
+      <c r="I148" s="17"/>
+      <c r="J148" s="17"/>
+      <c r="K148" s="17"/>
+      <c r="L148" s="17"/>
+      <c r="M148" s="17"/>
+      <c r="N148" s="17"/>
+      <c r="O148" s="17"/>
+      <c r="P148" s="17"/>
+      <c r="Q148" s="17"/>
+      <c r="R148" s="17"/>
+      <c r="S148" s="17"/>
+      <c r="T148" s="17"/>
+      <c r="U148" s="17"/>
+      <c r="V148" s="17"/>
+      <c r="W148" s="17"/>
+      <c r="X148" s="17"/>
+      <c r="Y148" s="18" t="s">
+        <v>1</v>
+      </c>
       <c r="Z148" s="1"/>
       <c r="AA148" s="1"/>
       <c r="AB148" s="1"/>
     </row>
-    <row r="149" spans="1:28" ht="18.75" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
-      <c r="B149" s="33"/>
-      <c r="C149" s="73">
-        <f>INT($C$148)+1.02</f>
-        <v>2.02</v>
-      </c>
-      <c r="D149" s="21"/>
-      <c r="E149" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F149" s="28">
-        <v>1</v>
-      </c>
-      <c r="G149" s="13"/>
-      <c r="H149" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="I149" s="7"/>
-      <c r="J149" s="7"/>
-      <c r="K149" s="7"/>
-      <c r="L149" s="7"/>
-      <c r="M149" s="7"/>
-      <c r="N149" s="7"/>
-      <c r="O149" s="7"/>
-      <c r="P149" s="7"/>
-      <c r="Q149" s="7"/>
-      <c r="R149" s="7"/>
-      <c r="S149" s="7"/>
-      <c r="T149" s="7"/>
-      <c r="U149" s="7"/>
-      <c r="V149" s="7"/>
-      <c r="W149" s="7"/>
-      <c r="X149" s="11"/>
-      <c r="Y149" s="16"/>
+      <c r="B149" s="19"/>
+      <c r="C149" s="77">
+        <f>INT($C$112)+0.005</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D149" s="19"/>
+      <c r="E149" s="19"/>
+      <c r="F149" s="19"/>
+      <c r="G149" s="19"/>
+      <c r="H149" s="19"/>
+      <c r="I149" s="19"/>
+      <c r="J149" s="19"/>
+      <c r="K149" s="19"/>
+      <c r="L149" s="19"/>
+      <c r="M149" s="19"/>
+      <c r="N149" s="19"/>
+      <c r="O149" s="19"/>
+      <c r="P149" s="19"/>
+      <c r="Q149" s="19"/>
+      <c r="R149" s="19"/>
+      <c r="S149" s="19"/>
+      <c r="T149" s="19"/>
+      <c r="U149" s="19"/>
+      <c r="V149" s="19"/>
+      <c r="W149" s="19"/>
+      <c r="X149" s="19"/>
+      <c r="Y149" s="19"/>
       <c r="Z149" s="1"/>
       <c r="AA149" s="1"/>
       <c r="AB149" s="1"/>
     </row>
-    <row r="150" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
-      <c r="B150" s="33"/>
+      <c r="B150" s="1"/>
       <c r="C150" s="73">
-        <f>INT($C$148)+2.005</f>
-        <v>3.0049999999999999</v>
-      </c>
-      <c r="D150" s="3"/>
-      <c r="E150" s="3"/>
-      <c r="F150" s="3"/>
-      <c r="G150" s="3"/>
-      <c r="H150" s="3"/>
-      <c r="I150" s="3"/>
-      <c r="J150" s="3"/>
-      <c r="K150" s="3"/>
-      <c r="L150" s="3"/>
-      <c r="M150" s="3"/>
-      <c r="N150" s="3"/>
-      <c r="O150" s="3"/>
-      <c r="P150" s="3"/>
-      <c r="Q150" s="3"/>
-      <c r="R150" s="3"/>
-      <c r="S150" s="3"/>
-      <c r="T150" s="3"/>
-      <c r="U150" s="3"/>
-      <c r="V150" s="3"/>
-      <c r="W150" s="3"/>
-      <c r="X150" s="3"/>
-      <c r="Y150" s="16"/>
+        <f>INT($C$112)+2</f>
+        <v>3</v>
+      </c>
+      <c r="D150" s="1"/>
+      <c r="E150" s="1"/>
+      <c r="F150" s="1"/>
+      <c r="G150" s="1"/>
+      <c r="H150" s="1"/>
+      <c r="I150" s="1"/>
+      <c r="J150" s="1"/>
+      <c r="K150" s="1"/>
+      <c r="L150" s="1"/>
+      <c r="M150" s="1"/>
+      <c r="N150" s="1"/>
+      <c r="O150" s="1"/>
+      <c r="P150" s="1"/>
+      <c r="Q150" s="1"/>
+      <c r="R150" s="1"/>
+      <c r="S150" s="1"/>
+      <c r="T150" s="1"/>
+      <c r="U150" s="1"/>
+      <c r="V150" s="1"/>
+      <c r="W150" s="1"/>
+      <c r="X150" s="1"/>
+      <c r="Y150" s="1"/>
       <c r="Z150" s="1"/>
       <c r="AA150" s="1"/>
       <c r="AB150" s="1"/>
     </row>
     <row r="151" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
-      <c r="B151" s="33"/>
+      <c r="B151" s="1"/>
       <c r="C151" s="73">
-        <f>INT($C$148)+2</f>
+        <f>INT($C$155)+2</f>
         <v>3</v>
       </c>
-      <c r="D151" s="3"/>
-      <c r="E151" s="5"/>
-      <c r="F151" s="5"/>
-      <c r="G151" s="3"/>
-      <c r="H151" s="29"/>
-      <c r="I151" s="29"/>
-      <c r="J151" s="65" t="s">
-        <v>293</v>
-      </c>
-      <c r="K151" s="65"/>
-      <c r="L151" s="65"/>
-      <c r="M151" s="65"/>
-      <c r="N151" s="65"/>
-      <c r="O151" s="65"/>
-      <c r="P151" s="65"/>
-      <c r="Q151" s="65"/>
-      <c r="R151" s="65"/>
-      <c r="S151" s="65"/>
-      <c r="T151" s="29"/>
-      <c r="U151" s="29"/>
-      <c r="V151" s="29"/>
-      <c r="W151" s="29"/>
-      <c r="X151" s="3"/>
-      <c r="Y151" s="16"/>
+      <c r="D151" s="1"/>
+      <c r="E151" s="1"/>
+      <c r="F151" s="1"/>
+      <c r="G151" s="1"/>
+      <c r="H151" s="1"/>
+      <c r="I151" s="1"/>
+      <c r="J151" s="1"/>
+      <c r="K151" s="1"/>
+      <c r="L151" s="1"/>
+      <c r="M151" s="1"/>
+      <c r="N151" s="1"/>
+      <c r="O151" s="1"/>
+      <c r="P151" s="1"/>
+      <c r="Q151" s="1"/>
+      <c r="R151" s="1"/>
+      <c r="S151" s="1"/>
+      <c r="T151" s="1"/>
+      <c r="U151" s="1"/>
+      <c r="V151" s="1"/>
+      <c r="W151" s="1"/>
+      <c r="X151" s="1"/>
+      <c r="Y151" s="1"/>
       <c r="Z151" s="1"/>
       <c r="AA151" s="1"/>
       <c r="AB151" s="1"/>
     </row>
-    <row r="152" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="1"/>
-      <c r="B152" s="33"/>
-      <c r="C152" s="73">
-        <f>INT($C$148)+2</f>
-        <v>3</v>
-      </c>
-      <c r="D152" s="3"/>
-      <c r="E152" s="5"/>
-      <c r="F152" s="5"/>
-      <c r="G152" s="3"/>
-      <c r="H152" s="29"/>
-      <c r="I152" s="29"/>
-      <c r="J152" s="29">
-        <v>0</v>
-      </c>
-      <c r="K152" s="29">
-        <v>1</v>
-      </c>
-      <c r="L152" s="29">
-        <v>2</v>
-      </c>
-      <c r="M152" s="29">
-        <v>3</v>
-      </c>
-      <c r="N152" s="29">
-        <v>4</v>
-      </c>
-      <c r="O152" s="29">
-        <v>5</v>
-      </c>
-      <c r="P152" s="29">
-        <v>6</v>
-      </c>
-      <c r="Q152" s="29">
-        <v>7</v>
-      </c>
-      <c r="R152" s="29">
-        <v>8</v>
-      </c>
-      <c r="S152" s="29">
-        <v>9</v>
-      </c>
-      <c r="T152" s="29"/>
-      <c r="U152" s="29"/>
-      <c r="V152" s="29"/>
-      <c r="W152" s="29"/>
-      <c r="X152" s="3"/>
-      <c r="Y152" s="16"/>
+      <c r="B152" s="20"/>
+      <c r="C152" s="74">
+        <f>INT($C$155)+0.005</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D152" s="20"/>
+      <c r="E152" s="20"/>
+      <c r="F152" s="20"/>
+      <c r="G152" s="20"/>
+      <c r="H152" s="20"/>
+      <c r="I152" s="20"/>
+      <c r="J152" s="20"/>
+      <c r="K152" s="20"/>
+      <c r="L152" s="20"/>
+      <c r="M152" s="20"/>
+      <c r="N152" s="20"/>
+      <c r="O152" s="20"/>
+      <c r="P152" s="20"/>
+      <c r="Q152" s="20"/>
+      <c r="R152" s="20"/>
+      <c r="S152" s="20"/>
+      <c r="T152" s="20"/>
+      <c r="U152" s="20"/>
+      <c r="V152" s="20"/>
+      <c r="W152" s="20"/>
+      <c r="X152" s="20"/>
+      <c r="Y152" s="20"/>
       <c r="Z152" s="1"/>
       <c r="AA152" s="1"/>
       <c r="AB152" s="1"/>
     </row>
-    <row r="153" spans="1:28" ht="9.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
-      <c r="B153" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="C153" s="73">
-        <f>INT($C$148)+2.01</f>
-        <v>3.01</v>
-      </c>
-      <c r="D153" s="3"/>
-      <c r="E153" s="3"/>
-      <c r="F153" s="3"/>
-      <c r="G153" s="3"/>
-      <c r="H153" s="29"/>
-      <c r="I153" s="29"/>
-      <c r="J153" s="29"/>
-      <c r="K153" s="29"/>
-      <c r="L153" s="29"/>
-      <c r="M153" s="29"/>
-      <c r="N153" s="29"/>
-      <c r="O153" s="29"/>
-      <c r="P153" s="29"/>
-      <c r="Q153" s="29"/>
-      <c r="R153" s="29"/>
-      <c r="S153" s="29"/>
-      <c r="T153" s="29"/>
-      <c r="U153" s="29"/>
-      <c r="V153" s="29"/>
-      <c r="W153" s="29"/>
-      <c r="X153" s="3"/>
-      <c r="Y153" s="16"/>
+      <c r="B153" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C153" s="75">
+        <f>INT($C$155)+1.005</f>
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="D153" s="14"/>
+      <c r="E153" s="14"/>
+      <c r="F153" s="14"/>
+      <c r="G153" s="14"/>
+      <c r="H153" s="14"/>
+      <c r="I153" s="14"/>
+      <c r="J153" s="14"/>
+      <c r="K153" s="14"/>
+      <c r="L153" s="14"/>
+      <c r="M153" s="14"/>
+      <c r="N153" s="14"/>
+      <c r="O153" s="14"/>
+      <c r="P153" s="14"/>
+      <c r="Q153" s="14"/>
+      <c r="R153" s="14"/>
+      <c r="S153" s="14"/>
+      <c r="T153" s="14"/>
+      <c r="U153" s="14"/>
+      <c r="V153" s="14"/>
+      <c r="W153" s="14"/>
+      <c r="X153" s="14"/>
+      <c r="Y153" s="15"/>
       <c r="Z153" s="1"/>
       <c r="AA153" s="1"/>
       <c r="AB153" s="1"/>
@@ -32622,174 +32724,174 @@
       <c r="A154" s="1"/>
       <c r="B154" s="33"/>
       <c r="C154" s="73">
-        <f>C$147</f>
+        <f>INT(MAX($C$163:$C$171))+1</f>
         <v>5</v>
       </c>
-      <c r="D154" s="4"/>
-      <c r="E154" s="5"/>
-      <c r="F154" s="5"/>
-      <c r="G154" s="4"/>
-      <c r="H154" s="5"/>
-      <c r="I154" s="5"/>
-      <c r="J154" s="5"/>
-      <c r="K154" s="5"/>
-      <c r="L154" s="5"/>
-      <c r="M154" s="5"/>
-      <c r="N154" s="5"/>
-      <c r="O154" s="5"/>
-      <c r="P154" s="5"/>
-      <c r="Q154" s="5"/>
-      <c r="R154" s="5"/>
-      <c r="S154" s="5"/>
-      <c r="T154" s="5"/>
-      <c r="U154" s="5"/>
-      <c r="V154" s="5"/>
-      <c r="W154" s="5"/>
-      <c r="X154" s="4"/>
+      <c r="D154" s="3"/>
+      <c r="E154" s="3"/>
+      <c r="F154" s="3"/>
+      <c r="G154" s="3"/>
+      <c r="H154" s="27"/>
+      <c r="I154" s="27"/>
+      <c r="J154" s="27"/>
+      <c r="K154" s="27"/>
+      <c r="L154" s="27"/>
+      <c r="M154" s="27"/>
+      <c r="N154" s="27"/>
+      <c r="O154" s="27"/>
+      <c r="P154" s="27"/>
+      <c r="Q154" s="27"/>
+      <c r="R154" s="27"/>
+      <c r="S154" s="27"/>
+      <c r="T154" s="27"/>
+      <c r="U154" s="27"/>
+      <c r="V154" s="27"/>
+      <c r="W154" s="27"/>
+      <c r="X154" s="3"/>
       <c r="Y154" s="16"/>
       <c r="Z154" s="1"/>
       <c r="AA154" s="1"/>
       <c r="AB154" s="1"/>
     </row>
-    <row r="155" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:28" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
-      <c r="B155" s="33" t="s">
-        <v>19</v>
-      </c>
+      <c r="B155" s="33"/>
       <c r="C155" s="73">
-        <f>C$147</f>
-        <v>5</v>
-      </c>
-      <c r="D155" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E155" s="5"/>
-      <c r="F155" s="5"/>
-      <c r="G155" s="4"/>
-      <c r="H155" s="5"/>
-      <c r="I155" s="5"/>
-      <c r="J155" s="5"/>
-      <c r="K155" s="5"/>
-      <c r="L155" s="5"/>
-      <c r="M155" s="5"/>
-      <c r="N155" s="5"/>
-      <c r="O155" s="5"/>
-      <c r="P155" s="5"/>
-      <c r="Q155" s="5"/>
-      <c r="R155" s="5"/>
-      <c r="S155" s="5"/>
-      <c r="T155" s="5"/>
-      <c r="U155" s="5"/>
-      <c r="V155" s="5"/>
-      <c r="W155" s="5"/>
-      <c r="X155" s="4"/>
+        <v>1.02</v>
+      </c>
+      <c r="D155" s="21"/>
+      <c r="E155" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F155" s="25"/>
+      <c r="G155" s="12"/>
+      <c r="H155" s="147" t="str">
+        <f>COUNTIFS($B$1:$B155, "«")&amp;" Feed Pool definitions"</f>
+        <v>5 Feed Pool definitions</v>
+      </c>
+      <c r="I155" s="6"/>
+      <c r="J155" s="6"/>
+      <c r="K155" s="6"/>
+      <c r="L155" s="6"/>
+      <c r="M155" s="6"/>
+      <c r="N155" s="6"/>
+      <c r="O155" s="6"/>
+      <c r="P155" s="6"/>
+      <c r="Q155" s="6"/>
+      <c r="R155" s="6"/>
+      <c r="S155" s="6"/>
+      <c r="T155" s="6"/>
+      <c r="U155" s="6"/>
+      <c r="V155" s="6"/>
+      <c r="W155" s="6"/>
+      <c r="X155" s="10"/>
       <c r="Y155" s="16"/>
       <c r="Z155" s="1"/>
       <c r="AA155" s="1"/>
       <c r="AB155" s="1"/>
     </row>
-    <row r="156" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:28" ht="18.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="33"/>
       <c r="C156" s="73">
-        <f>INT($C$148)+2.005</f>
-        <v>3.0049999999999999</v>
-      </c>
-      <c r="D156" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E156" s="4"/>
-      <c r="F156" s="4"/>
-      <c r="G156" s="4"/>
-      <c r="H156" s="58"/>
-      <c r="I156" s="58"/>
-      <c r="J156" s="58"/>
-      <c r="K156" s="58"/>
-      <c r="L156" s="58"/>
-      <c r="M156" s="58"/>
-      <c r="N156" s="58"/>
-      <c r="O156" s="58"/>
-      <c r="P156" s="58"/>
-      <c r="Q156" s="58"/>
-      <c r="R156" s="58"/>
-      <c r="S156" s="58"/>
-      <c r="T156" s="58"/>
-      <c r="U156" s="58"/>
-      <c r="V156" s="58"/>
-      <c r="W156" s="58"/>
-      <c r="X156" s="4"/>
+        <f>INT($C$155)+1.02</f>
+        <v>2.02</v>
+      </c>
+      <c r="D156" s="21"/>
+      <c r="E156" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F156" s="28">
+        <v>1</v>
+      </c>
+      <c r="G156" s="13"/>
+      <c r="H156" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="I156" s="7"/>
+      <c r="J156" s="7"/>
+      <c r="K156" s="7"/>
+      <c r="L156" s="7"/>
+      <c r="M156" s="7"/>
+      <c r="N156" s="7"/>
+      <c r="O156" s="7"/>
+      <c r="P156" s="7"/>
+      <c r="Q156" s="7"/>
+      <c r="R156" s="7"/>
+      <c r="S156" s="7"/>
+      <c r="T156" s="7"/>
+      <c r="U156" s="7"/>
+      <c r="V156" s="7"/>
+      <c r="W156" s="7"/>
+      <c r="X156" s="11"/>
       <c r="Y156" s="16"/>
       <c r="Z156" s="1"/>
       <c r="AA156" s="1"/>
       <c r="AB156" s="1"/>
     </row>
-    <row r="157" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="33"/>
       <c r="C157" s="73">
-        <f>INT($C$148)+2</f>
-        <v>3</v>
-      </c>
-      <c r="D157" s="4"/>
-      <c r="E157" s="5"/>
-      <c r="F157" s="5"/>
-      <c r="G157" s="4"/>
-      <c r="H157" s="64" t="s">
-        <v>287</v>
-      </c>
-      <c r="I157" s="31">
-        <v>4</v>
-      </c>
-      <c r="J157" s="158" t="s">
-        <v>291</v>
-      </c>
-      <c r="K157" s="2"/>
-      <c r="L157" s="2"/>
-      <c r="M157" s="2"/>
-      <c r="N157" s="2"/>
-      <c r="O157" s="2"/>
-      <c r="P157" s="2"/>
-      <c r="Q157" s="2"/>
-      <c r="R157" s="2"/>
-      <c r="S157" s="2"/>
-      <c r="T157" s="2"/>
-      <c r="U157" s="2"/>
-      <c r="V157" s="2"/>
-      <c r="W157" s="2"/>
-      <c r="X157" s="4"/>
+        <f>INT($C$155)+2.005</f>
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="D157" s="3"/>
+      <c r="E157" s="3"/>
+      <c r="F157" s="3"/>
+      <c r="G157" s="3"/>
+      <c r="H157" s="3"/>
+      <c r="I157" s="3"/>
+      <c r="J157" s="3"/>
+      <c r="K157" s="3"/>
+      <c r="L157" s="3"/>
+      <c r="M157" s="3"/>
+      <c r="N157" s="3"/>
+      <c r="O157" s="3"/>
+      <c r="P157" s="3"/>
+      <c r="Q157" s="3"/>
+      <c r="R157" s="3"/>
+      <c r="S157" s="3"/>
+      <c r="T157" s="3"/>
+      <c r="U157" s="3"/>
+      <c r="V157" s="3"/>
+      <c r="W157" s="3"/>
+      <c r="X157" s="3"/>
       <c r="Y157" s="16"/>
       <c r="Z157" s="1"/>
       <c r="AA157" s="1"/>
       <c r="AB157" s="1"/>
     </row>
-    <row r="158" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="33"/>
       <c r="C158" s="73">
-        <f>INT($C$148)+3</f>
-        <v>4</v>
-      </c>
-      <c r="D158" s="4"/>
+        <f>INT($C$155)+2</f>
+        <v>3</v>
+      </c>
+      <c r="D158" s="3"/>
       <c r="E158" s="5"/>
       <c r="F158" s="5"/>
-      <c r="G158" s="4"/>
-      <c r="H158" s="157"/>
-      <c r="I158" s="2"/>
-      <c r="J158" s="2"/>
-      <c r="K158" s="2"/>
-      <c r="L158" s="2"/>
-      <c r="M158" s="2"/>
-      <c r="N158" s="2"/>
-      <c r="O158" s="2"/>
-      <c r="P158" s="2"/>
-      <c r="Q158" s="2"/>
-      <c r="R158" s="2"/>
-      <c r="S158" s="2"/>
-      <c r="T158" s="2"/>
-      <c r="U158" s="2"/>
-      <c r="V158" s="2"/>
-      <c r="W158" s="2"/>
-      <c r="X158" s="4"/>
+      <c r="G158" s="3"/>
+      <c r="H158" s="29"/>
+      <c r="I158" s="29"/>
+      <c r="J158" s="65" t="s">
+        <v>293</v>
+      </c>
+      <c r="K158" s="65"/>
+      <c r="L158" s="65"/>
+      <c r="M158" s="65"/>
+      <c r="N158" s="65"/>
+      <c r="O158" s="65"/>
+      <c r="P158" s="65"/>
+      <c r="Q158" s="65"/>
+      <c r="R158" s="65"/>
+      <c r="S158" s="65"/>
+      <c r="T158" s="29"/>
+      <c r="U158" s="29"/>
+      <c r="V158" s="29"/>
+      <c r="W158" s="29"/>
+      <c r="X158" s="3"/>
       <c r="Y158" s="16"/>
       <c r="Z158" s="1"/>
       <c r="AA158" s="1"/>
@@ -32799,564 +32901,829 @@
       <c r="A159" s="1"/>
       <c r="B159" s="33"/>
       <c r="C159" s="73">
-        <f>INT($C$148)+2</f>
+        <f>INT($C$155)+2</f>
         <v>3</v>
       </c>
-      <c r="D159" s="4"/>
+      <c r="D159" s="3"/>
       <c r="E159" s="5"/>
       <c r="F159" s="5"/>
-      <c r="G159" s="4"/>
-      <c r="H159" s="64" t="s">
-        <v>292</v>
-      </c>
-      <c r="I159" s="2"/>
-      <c r="J159" s="2"/>
-      <c r="K159" s="2"/>
-      <c r="L159" s="2"/>
-      <c r="M159" s="2"/>
-      <c r="N159" s="2"/>
-      <c r="O159" s="2"/>
-      <c r="P159" s="2"/>
-      <c r="Q159" s="2"/>
-      <c r="R159" s="2"/>
-      <c r="S159" s="2"/>
-      <c r="T159" s="2"/>
-      <c r="U159" s="2"/>
-      <c r="V159" s="2"/>
-      <c r="W159" s="2"/>
-      <c r="X159" s="4"/>
+      <c r="G159" s="3"/>
+      <c r="H159" s="29"/>
+      <c r="I159" s="29"/>
+      <c r="J159" s="29">
+        <v>0</v>
+      </c>
+      <c r="K159" s="29">
+        <v>1</v>
+      </c>
+      <c r="L159" s="29">
+        <v>2</v>
+      </c>
+      <c r="M159" s="29">
+        <v>3</v>
+      </c>
+      <c r="N159" s="29">
+        <v>4</v>
+      </c>
+      <c r="O159" s="29">
+        <v>5</v>
+      </c>
+      <c r="P159" s="29">
+        <v>6</v>
+      </c>
+      <c r="Q159" s="29">
+        <v>7</v>
+      </c>
+      <c r="R159" s="29">
+        <v>8</v>
+      </c>
+      <c r="S159" s="29">
+        <v>9</v>
+      </c>
+      <c r="T159" s="29"/>
+      <c r="U159" s="29"/>
+      <c r="V159" s="29"/>
+      <c r="W159" s="29"/>
+      <c r="X159" s="3"/>
       <c r="Y159" s="16"/>
       <c r="Z159" s="1"/>
       <c r="AA159" s="1"/>
       <c r="AB159" s="1"/>
     </row>
-    <row r="160" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:28" ht="9.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
-      <c r="B160" s="33"/>
+      <c r="B160" s="33" t="s">
+        <v>20</v>
+      </c>
       <c r="C160" s="73">
-        <f>INT($C$148)+3</f>
-        <v>4</v>
-      </c>
-      <c r="D160" s="4"/>
-      <c r="E160" s="5"/>
-      <c r="F160" s="5"/>
-      <c r="G160" s="4"/>
-      <c r="H160" s="159" t="s">
-        <v>298</v>
-      </c>
-      <c r="I160" s="2"/>
-      <c r="J160" s="31">
-        <v>3</v>
-      </c>
-      <c r="K160" s="31">
-        <v>4</v>
-      </c>
-      <c r="L160" s="31">
-        <v>6</v>
-      </c>
-      <c r="M160" s="31">
-        <v>8</v>
-      </c>
-      <c r="N160" s="31">
-        <v>9</v>
-      </c>
-      <c r="O160" s="31">
-        <v>6</v>
-      </c>
-      <c r="P160" s="31">
-        <v>5</v>
-      </c>
-      <c r="Q160" s="31">
-        <v>4</v>
-      </c>
-      <c r="R160" s="31">
-        <v>3.5</v>
-      </c>
-      <c r="S160" s="31">
-        <v>3</v>
-      </c>
-      <c r="T160" s="2"/>
-      <c r="U160" s="2"/>
-      <c r="V160" s="2"/>
-      <c r="W160" s="2"/>
-      <c r="X160" s="4"/>
+        <f>INT($C$155)+2.01</f>
+        <v>3.01</v>
+      </c>
+      <c r="D160" s="3"/>
+      <c r="E160" s="3"/>
+      <c r="F160" s="3"/>
+      <c r="G160" s="3"/>
+      <c r="H160" s="29"/>
+      <c r="I160" s="29"/>
+      <c r="J160" s="29"/>
+      <c r="K160" s="29"/>
+      <c r="L160" s="29"/>
+      <c r="M160" s="29"/>
+      <c r="N160" s="29"/>
+      <c r="O160" s="29"/>
+      <c r="P160" s="29"/>
+      <c r="Q160" s="29"/>
+      <c r="R160" s="29"/>
+      <c r="S160" s="29"/>
+      <c r="T160" s="29"/>
+      <c r="U160" s="29"/>
+      <c r="V160" s="29"/>
+      <c r="W160" s="29"/>
+      <c r="X160" s="3"/>
       <c r="Y160" s="16"/>
       <c r="Z160" s="1"/>
       <c r="AA160" s="1"/>
       <c r="AB160" s="1"/>
     </row>
-    <row r="161" spans="1:28" outlineLevel="3" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="33"/>
       <c r="C161" s="73">
-        <f>INT($C$148)+3</f>
-        <v>4</v>
+        <f>C$154</f>
+        <v>5</v>
       </c>
       <c r="D161" s="4"/>
       <c r="E161" s="5"/>
       <c r="F161" s="5"/>
       <c r="G161" s="4"/>
-      <c r="H161" s="159" t="s">
-        <v>294</v>
-      </c>
-      <c r="I161" s="2"/>
-      <c r="J161" s="31">
-        <v>13.3</v>
-      </c>
-      <c r="K161" s="31">
-        <v>13.3</v>
-      </c>
-      <c r="L161" s="31">
-        <v>13.3</v>
-      </c>
-      <c r="M161" s="31">
-        <v>13.3</v>
-      </c>
-      <c r="N161" s="31">
-        <v>13.3</v>
-      </c>
-      <c r="O161" s="31">
-        <v>13.3</v>
-      </c>
-      <c r="P161" s="31">
-        <v>13.3</v>
-      </c>
-      <c r="Q161" s="31">
-        <v>13.3</v>
-      </c>
-      <c r="R161" s="31">
-        <v>13.3</v>
-      </c>
-      <c r="S161" s="31">
-        <v>13.3</v>
-      </c>
-      <c r="T161" s="2"/>
-      <c r="U161" s="2"/>
-      <c r="V161" s="2"/>
-      <c r="W161" s="2"/>
+      <c r="H161" s="5"/>
+      <c r="I161" s="5"/>
+      <c r="J161" s="5"/>
+      <c r="K161" s="5"/>
+      <c r="L161" s="5"/>
+      <c r="M161" s="5"/>
+      <c r="N161" s="5"/>
+      <c r="O161" s="5"/>
+      <c r="P161" s="5"/>
+      <c r="Q161" s="5"/>
+      <c r="R161" s="5"/>
+      <c r="S161" s="5"/>
+      <c r="T161" s="5"/>
+      <c r="U161" s="5"/>
+      <c r="V161" s="5"/>
+      <c r="W161" s="5"/>
       <c r="X161" s="4"/>
       <c r="Y161" s="16"/>
       <c r="Z161" s="1"/>
       <c r="AA161" s="1"/>
       <c r="AB161" s="1"/>
     </row>
-    <row r="162" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
-      <c r="B162" s="33"/>
+      <c r="B162" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="C162" s="73">
-        <f>INT(C$148+3)</f>
-        <v>4</v>
-      </c>
-      <c r="D162" s="4"/>
+        <f>C$154</f>
+        <v>5</v>
+      </c>
+      <c r="D162" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="E162" s="5"/>
       <c r="F162" s="5"/>
       <c r="G162" s="4"/>
-      <c r="H162" s="148"/>
-      <c r="I162" s="148"/>
-      <c r="J162" s="148"/>
-      <c r="K162" s="148"/>
-      <c r="L162" s="148"/>
-      <c r="M162" s="148"/>
-      <c r="N162" s="148"/>
-      <c r="O162" s="148"/>
-      <c r="P162" s="148"/>
-      <c r="Q162" s="148"/>
-      <c r="R162" s="148"/>
-      <c r="S162" s="148"/>
-      <c r="T162" s="2"/>
-      <c r="U162" s="2"/>
-      <c r="V162" s="2"/>
-      <c r="W162" s="2"/>
+      <c r="H162" s="5"/>
+      <c r="I162" s="5"/>
+      <c r="J162" s="5"/>
+      <c r="K162" s="5"/>
+      <c r="L162" s="5"/>
+      <c r="M162" s="5"/>
+      <c r="N162" s="5"/>
+      <c r="O162" s="5"/>
+      <c r="P162" s="5"/>
+      <c r="Q162" s="5"/>
+      <c r="R162" s="5"/>
+      <c r="S162" s="5"/>
+      <c r="T162" s="5"/>
+      <c r="U162" s="5"/>
+      <c r="V162" s="5"/>
+      <c r="W162" s="5"/>
       <c r="X162" s="4"/>
       <c r="Y162" s="16"/>
       <c r="Z162" s="1"/>
       <c r="AA162" s="1"/>
       <c r="AB162" s="1"/>
     </row>
-    <row r="163" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="33"/>
       <c r="C163" s="73">
-        <f>INT(C$148+3)</f>
-        <v>4</v>
-      </c>
-      <c r="D163" s="4"/>
-      <c r="E163" s="5"/>
-      <c r="F163" s="5"/>
+        <f>INT($C$155)+2.005</f>
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="D163" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E163" s="4"/>
+      <c r="F163" s="4"/>
       <c r="G163" s="4"/>
-      <c r="H163" s="148"/>
-      <c r="I163" s="148"/>
-      <c r="J163" s="148"/>
-      <c r="K163" s="148"/>
-      <c r="L163" s="148"/>
-      <c r="M163" s="148"/>
-      <c r="N163" s="148"/>
-      <c r="O163" s="148"/>
-      <c r="P163" s="148"/>
-      <c r="Q163" s="148"/>
-      <c r="R163" s="148"/>
-      <c r="S163" s="2"/>
-      <c r="T163" s="2"/>
-      <c r="U163" s="2"/>
-      <c r="V163" s="2"/>
-      <c r="W163" s="2"/>
+      <c r="H163" s="58"/>
+      <c r="I163" s="58"/>
+      <c r="J163" s="58"/>
+      <c r="K163" s="58"/>
+      <c r="L163" s="58"/>
+      <c r="M163" s="58"/>
+      <c r="N163" s="58"/>
+      <c r="O163" s="58"/>
+      <c r="P163" s="58"/>
+      <c r="Q163" s="58"/>
+      <c r="R163" s="58"/>
+      <c r="S163" s="58"/>
+      <c r="T163" s="58"/>
+      <c r="U163" s="58"/>
+      <c r="V163" s="58"/>
+      <c r="W163" s="58"/>
       <c r="X163" s="4"/>
       <c r="Y163" s="16"/>
       <c r="Z163" s="1"/>
       <c r="AA163" s="1"/>
       <c r="AB163" s="1"/>
     </row>
-    <row r="164" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="33"/>
       <c r="C164" s="73">
-        <f>INT($C$148)+3.005</f>
-        <v>4.0049999999999999</v>
+        <f>INT($C$155)+2</f>
+        <v>3</v>
       </c>
       <c r="D164" s="4"/>
-      <c r="E164" s="4"/>
-      <c r="F164" s="4"/>
+      <c r="E164" s="5"/>
+      <c r="F164" s="5"/>
       <c r="G164" s="4"/>
-      <c r="H164" s="4"/>
-      <c r="I164" s="4"/>
-      <c r="J164" s="4"/>
-      <c r="K164" s="4"/>
-      <c r="L164" s="4"/>
-      <c r="M164" s="4"/>
-      <c r="N164" s="4"/>
-      <c r="O164" s="4"/>
-      <c r="P164" s="4"/>
-      <c r="Q164" s="4"/>
-      <c r="R164" s="4"/>
-      <c r="S164" s="4"/>
-      <c r="T164" s="4"/>
-      <c r="U164" s="4"/>
-      <c r="V164" s="4"/>
-      <c r="W164" s="4"/>
-      <c r="X164" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="H164" s="64" t="s">
+        <v>287</v>
+      </c>
+      <c r="I164" s="31">
+        <v>4</v>
+      </c>
+      <c r="J164" s="158" t="s">
+        <v>291</v>
+      </c>
+      <c r="K164" s="2"/>
+      <c r="L164" s="2"/>
+      <c r="M164" s="2"/>
+      <c r="N164" s="2"/>
+      <c r="O164" s="2"/>
+      <c r="P164" s="2"/>
+      <c r="Q164" s="2"/>
+      <c r="R164" s="2"/>
+      <c r="S164" s="2"/>
+      <c r="T164" s="2"/>
+      <c r="U164" s="2"/>
+      <c r="V164" s="2"/>
+      <c r="W164" s="2"/>
+      <c r="X164" s="4"/>
       <c r="Y164" s="16"/>
       <c r="Z164" s="1"/>
       <c r="AA164" s="1"/>
       <c r="AB164" s="1"/>
     </row>
-    <row r="165" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="B165" s="33"/>
       <c r="C165" s="73">
-        <f>INT($C$148)+2.005</f>
-        <v>3.0049999999999999</v>
+        <f>INT($C$155)+3</f>
+        <v>4</v>
       </c>
       <c r="D165" s="4"/>
-      <c r="E165" s="4"/>
-      <c r="F165" s="4"/>
+      <c r="E165" s="5"/>
+      <c r="F165" s="5"/>
       <c r="G165" s="4"/>
-      <c r="H165" s="4"/>
-      <c r="I165" s="4"/>
-      <c r="J165" s="4"/>
-      <c r="K165" s="4"/>
-      <c r="L165" s="4"/>
-      <c r="M165" s="4"/>
-      <c r="N165" s="4"/>
-      <c r="O165" s="4"/>
-      <c r="P165" s="4"/>
-      <c r="Q165" s="4"/>
-      <c r="R165" s="4"/>
-      <c r="S165" s="4"/>
-      <c r="T165" s="4"/>
-      <c r="U165" s="4"/>
-      <c r="V165" s="4"/>
-      <c r="W165" s="4"/>
+      <c r="H165" s="157"/>
+      <c r="I165" s="2"/>
+      <c r="J165" s="2"/>
+      <c r="K165" s="2"/>
+      <c r="L165" s="2"/>
+      <c r="M165" s="2"/>
+      <c r="N165" s="2"/>
+      <c r="O165" s="2"/>
+      <c r="P165" s="2"/>
+      <c r="Q165" s="2"/>
+      <c r="R165" s="2"/>
+      <c r="S165" s="2"/>
+      <c r="T165" s="2"/>
+      <c r="U165" s="2"/>
+      <c r="V165" s="2"/>
+      <c r="W165" s="2"/>
       <c r="X165" s="4"/>
       <c r="Y165" s="16"/>
       <c r="Z165" s="1"/>
       <c r="AA165" s="1"/>
       <c r="AB165" s="1"/>
     </row>
-    <row r="166" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
-      <c r="B166" s="35"/>
-      <c r="C166" s="76">
-        <f>INT($C$148)+1.005</f>
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="D166" s="17"/>
-      <c r="E166" s="17"/>
-      <c r="F166" s="17"/>
-      <c r="G166" s="17"/>
-      <c r="H166" s="17"/>
-      <c r="I166" s="17"/>
-      <c r="J166" s="17"/>
-      <c r="K166" s="17"/>
-      <c r="L166" s="17"/>
-      <c r="M166" s="17"/>
-      <c r="N166" s="17"/>
-      <c r="O166" s="17"/>
-      <c r="P166" s="17"/>
-      <c r="Q166" s="17"/>
-      <c r="R166" s="17"/>
-      <c r="S166" s="17"/>
-      <c r="T166" s="17"/>
-      <c r="U166" s="17"/>
-      <c r="V166" s="17"/>
-      <c r="W166" s="17"/>
-      <c r="X166" s="17"/>
-      <c r="Y166" s="18" t="s">
-        <v>1</v>
-      </c>
+      <c r="B166" s="33"/>
+      <c r="C166" s="73">
+        <f>INT($C$155)+2</f>
+        <v>3</v>
+      </c>
+      <c r="D166" s="4"/>
+      <c r="E166" s="5"/>
+      <c r="F166" s="5"/>
+      <c r="G166" s="4"/>
+      <c r="H166" s="64" t="s">
+        <v>292</v>
+      </c>
+      <c r="I166" s="2"/>
+      <c r="J166" s="2"/>
+      <c r="K166" s="2"/>
+      <c r="L166" s="2"/>
+      <c r="M166" s="2"/>
+      <c r="N166" s="2"/>
+      <c r="O166" s="2"/>
+      <c r="P166" s="2"/>
+      <c r="Q166" s="2"/>
+      <c r="R166" s="2"/>
+      <c r="S166" s="2"/>
+      <c r="T166" s="2"/>
+      <c r="U166" s="2"/>
+      <c r="V166" s="2"/>
+      <c r="W166" s="2"/>
+      <c r="X166" s="4"/>
+      <c r="Y166" s="16"/>
       <c r="Z166" s="1"/>
       <c r="AA166" s="1"/>
       <c r="AB166" s="1"/>
     </row>
-    <row r="167" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
-      <c r="B167" s="19"/>
-      <c r="C167" s="77">
-        <f>INT($C$148)+0.005</f>
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="D167" s="19"/>
-      <c r="E167" s="19"/>
-      <c r="F167" s="19"/>
-      <c r="G167" s="19"/>
-      <c r="H167" s="19"/>
-      <c r="I167" s="19"/>
-      <c r="J167" s="19"/>
-      <c r="K167" s="19"/>
-      <c r="L167" s="19"/>
-      <c r="M167" s="19"/>
-      <c r="N167" s="19"/>
-      <c r="O167" s="19"/>
-      <c r="P167" s="19"/>
-      <c r="Q167" s="19"/>
-      <c r="R167" s="19"/>
-      <c r="S167" s="19"/>
-      <c r="T167" s="19"/>
-      <c r="U167" s="19"/>
-      <c r="V167" s="19"/>
-      <c r="W167" s="19"/>
-      <c r="X167" s="19"/>
-      <c r="Y167" s="19"/>
+      <c r="B167" s="33"/>
+      <c r="C167" s="73">
+        <f>INT($C$155)+3</f>
+        <v>4</v>
+      </c>
+      <c r="D167" s="4"/>
+      <c r="E167" s="5"/>
+      <c r="F167" s="5"/>
+      <c r="G167" s="4"/>
+      <c r="H167" s="159" t="s">
+        <v>298</v>
+      </c>
+      <c r="I167" s="2"/>
+      <c r="J167" s="31">
+        <v>3</v>
+      </c>
+      <c r="K167" s="31">
+        <v>4</v>
+      </c>
+      <c r="L167" s="31">
+        <v>6</v>
+      </c>
+      <c r="M167" s="31">
+        <v>8</v>
+      </c>
+      <c r="N167" s="31">
+        <v>9</v>
+      </c>
+      <c r="O167" s="31">
+        <v>6</v>
+      </c>
+      <c r="P167" s="31">
+        <v>5</v>
+      </c>
+      <c r="Q167" s="31">
+        <v>4</v>
+      </c>
+      <c r="R167" s="31">
+        <v>3.5</v>
+      </c>
+      <c r="S167" s="31">
+        <v>3</v>
+      </c>
+      <c r="T167" s="2"/>
+      <c r="U167" s="2"/>
+      <c r="V167" s="2"/>
+      <c r="W167" s="2"/>
+      <c r="X167" s="4"/>
+      <c r="Y167" s="16"/>
       <c r="Z167" s="1"/>
       <c r="AA167" s="1"/>
       <c r="AB167" s="1"/>
     </row>
-    <row r="168" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:28" outlineLevel="3" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
-      <c r="B168" s="1"/>
+      <c r="B168" s="33"/>
       <c r="C168" s="73">
-        <f>INT($C$148)+2</f>
-        <v>3</v>
-      </c>
-      <c r="D168" s="1"/>
-      <c r="E168" s="1"/>
-      <c r="F168" s="1"/>
-      <c r="G168" s="1"/>
-      <c r="H168" s="1"/>
-      <c r="I168" s="1"/>
-      <c r="J168" s="1"/>
-      <c r="K168" s="1"/>
-      <c r="L168" s="1"/>
-      <c r="M168" s="1"/>
-      <c r="N168" s="1"/>
-      <c r="O168" s="1"/>
-      <c r="P168" s="1"/>
-      <c r="Q168" s="1"/>
-      <c r="R168" s="1"/>
-      <c r="S168" s="1"/>
-      <c r="T168" s="1"/>
-      <c r="U168" s="1"/>
-      <c r="V168" s="1"/>
-      <c r="W168" s="1"/>
-      <c r="X168" s="1"/>
-      <c r="Y168" s="1"/>
+        <f>INT($C$155)+3</f>
+        <v>4</v>
+      </c>
+      <c r="D168" s="4"/>
+      <c r="E168" s="5"/>
+      <c r="F168" s="5"/>
+      <c r="G168" s="4"/>
+      <c r="H168" s="159" t="s">
+        <v>294</v>
+      </c>
+      <c r="I168" s="2"/>
+      <c r="J168" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="K168" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="L168" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="M168" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="N168" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="O168" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="P168" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="Q168" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="R168" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="S168" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="T168" s="2"/>
+      <c r="U168" s="2"/>
+      <c r="V168" s="2"/>
+      <c r="W168" s="2"/>
+      <c r="X168" s="4"/>
+      <c r="Y168" s="16"/>
       <c r="Z168" s="1"/>
       <c r="AA168" s="1"/>
       <c r="AB168" s="1"/>
     </row>
-    <row r="169" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
-      <c r="B169" s="1"/>
-      <c r="C169" s="66"/>
-      <c r="D169" s="1"/>
-      <c r="E169" s="1"/>
-      <c r="F169" s="1"/>
-      <c r="G169" s="1"/>
-      <c r="H169" s="1"/>
-      <c r="I169" s="1"/>
-      <c r="J169" s="1"/>
-      <c r="K169" s="1"/>
-      <c r="L169" s="1"/>
-      <c r="M169" s="1"/>
-      <c r="N169" s="1"/>
-      <c r="O169" s="1"/>
-      <c r="P169" s="1"/>
-      <c r="Q169" s="1"/>
-      <c r="R169" s="1"/>
-      <c r="S169" s="1"/>
-      <c r="T169" s="1"/>
-      <c r="U169" s="1"/>
-      <c r="V169" s="1"/>
-      <c r="W169" s="1"/>
-      <c r="X169" s="1"/>
-      <c r="Y169" s="1"/>
+      <c r="B169" s="33"/>
+      <c r="C169" s="73">
+        <f>INT(C$155+3)</f>
+        <v>4</v>
+      </c>
+      <c r="D169" s="4"/>
+      <c r="E169" s="5"/>
+      <c r="F169" s="5"/>
+      <c r="G169" s="4"/>
+      <c r="H169" s="148"/>
+      <c r="I169" s="148"/>
+      <c r="J169" s="148"/>
+      <c r="K169" s="148"/>
+      <c r="L169" s="148"/>
+      <c r="M169" s="148"/>
+      <c r="N169" s="148"/>
+      <c r="O169" s="148"/>
+      <c r="P169" s="148"/>
+      <c r="Q169" s="148"/>
+      <c r="R169" s="148"/>
+      <c r="S169" s="148"/>
+      <c r="T169" s="2"/>
+      <c r="U169" s="2"/>
+      <c r="V169" s="2"/>
+      <c r="W169" s="2"/>
+      <c r="X169" s="4"/>
+      <c r="Y169" s="16"/>
       <c r="Z169" s="1"/>
       <c r="AA169" s="1"/>
       <c r="AB169" s="1"/>
     </row>
-    <row r="170" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
-      <c r="B170" s="1"/>
-      <c r="C170" s="66"/>
-      <c r="D170" s="1"/>
-      <c r="E170" s="1"/>
-      <c r="F170" s="1"/>
-      <c r="G170" s="1"/>
-      <c r="H170" s="1"/>
-      <c r="I170" s="1"/>
-      <c r="J170" s="1"/>
-      <c r="K170" s="1"/>
-      <c r="L170" s="1"/>
-      <c r="M170" s="1"/>
-      <c r="N170" s="1"/>
-      <c r="O170" s="1"/>
-      <c r="P170" s="1"/>
-      <c r="Q170" s="1"/>
-      <c r="R170" s="1"/>
-      <c r="S170" s="1"/>
-      <c r="T170" s="1"/>
-      <c r="U170" s="1"/>
-      <c r="V170" s="1"/>
-      <c r="W170" s="1"/>
-      <c r="X170" s="1"/>
-      <c r="Y170" s="1"/>
+      <c r="B170" s="33"/>
+      <c r="C170" s="73">
+        <f>INT(C$155+3)</f>
+        <v>4</v>
+      </c>
+      <c r="D170" s="4"/>
+      <c r="E170" s="5"/>
+      <c r="F170" s="5"/>
+      <c r="G170" s="4"/>
+      <c r="H170" s="148"/>
+      <c r="I170" s="148"/>
+      <c r="J170" s="148"/>
+      <c r="K170" s="148"/>
+      <c r="L170" s="148"/>
+      <c r="M170" s="148"/>
+      <c r="N170" s="148"/>
+      <c r="O170" s="148"/>
+      <c r="P170" s="148"/>
+      <c r="Q170" s="148"/>
+      <c r="R170" s="148"/>
+      <c r="S170" s="2"/>
+      <c r="T170" s="2"/>
+      <c r="U170" s="2"/>
+      <c r="V170" s="2"/>
+      <c r="W170" s="2"/>
+      <c r="X170" s="4"/>
+      <c r="Y170" s="16"/>
       <c r="Z170" s="1"/>
       <c r="AA170" s="1"/>
       <c r="AB170" s="1"/>
     </row>
-    <row r="171" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
-      <c r="B171" s="1"/>
-      <c r="C171" s="66"/>
-      <c r="D171" s="1"/>
-      <c r="E171" s="1"/>
-      <c r="F171" s="1"/>
-      <c r="G171" s="1"/>
-      <c r="H171" s="1"/>
-      <c r="I171" s="1"/>
-      <c r="J171" s="1"/>
-      <c r="K171" s="1"/>
-      <c r="L171" s="1"/>
-      <c r="M171" s="1"/>
-      <c r="N171" s="1"/>
-      <c r="O171" s="1"/>
-      <c r="P171" s="1"/>
-      <c r="Q171" s="1"/>
-      <c r="R171" s="1"/>
-      <c r="S171" s="1"/>
-      <c r="T171" s="1"/>
-      <c r="U171" s="1"/>
-      <c r="V171" s="1"/>
-      <c r="W171" s="1"/>
-      <c r="X171" s="1"/>
-      <c r="Y171" s="1"/>
+      <c r="B171" s="33"/>
+      <c r="C171" s="73">
+        <f>INT($C$155)+3.005</f>
+        <v>4.0049999999999999</v>
+      </c>
+      <c r="D171" s="4"/>
+      <c r="E171" s="4"/>
+      <c r="F171" s="4"/>
+      <c r="G171" s="4"/>
+      <c r="H171" s="4"/>
+      <c r="I171" s="4"/>
+      <c r="J171" s="4"/>
+      <c r="K171" s="4"/>
+      <c r="L171" s="4"/>
+      <c r="M171" s="4"/>
+      <c r="N171" s="4"/>
+      <c r="O171" s="4"/>
+      <c r="P171" s="4"/>
+      <c r="Q171" s="4"/>
+      <c r="R171" s="4"/>
+      <c r="S171" s="4"/>
+      <c r="T171" s="4"/>
+      <c r="U171" s="4"/>
+      <c r="V171" s="4"/>
+      <c r="W171" s="4"/>
+      <c r="X171" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y171" s="16"/>
       <c r="Z171" s="1"/>
       <c r="AA171" s="1"/>
       <c r="AB171" s="1"/>
     </row>
-    <row r="172" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
-      <c r="B172" s="1"/>
-      <c r="C172" s="66"/>
-      <c r="D172" s="1"/>
-      <c r="E172" s="1"/>
-      <c r="F172" s="1"/>
-      <c r="G172" s="1"/>
-      <c r="H172" s="1"/>
-      <c r="I172" s="1"/>
-      <c r="J172" s="1"/>
-      <c r="K172" s="1"/>
-      <c r="L172" s="1"/>
-      <c r="M172" s="1"/>
-      <c r="N172" s="1"/>
-      <c r="O172" s="1"/>
-      <c r="P172" s="1"/>
-      <c r="Q172" s="1"/>
-      <c r="R172" s="1"/>
-      <c r="S172" s="1"/>
-      <c r="T172" s="1"/>
-      <c r="U172" s="1"/>
-      <c r="V172" s="1"/>
-      <c r="W172" s="1"/>
-      <c r="X172" s="1"/>
-      <c r="Y172" s="1"/>
+      <c r="B172" s="33"/>
+      <c r="C172" s="73">
+        <f>INT($C$155)+2.005</f>
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="D172" s="4"/>
+      <c r="E172" s="4"/>
+      <c r="F172" s="4"/>
+      <c r="G172" s="4"/>
+      <c r="H172" s="4"/>
+      <c r="I172" s="4"/>
+      <c r="J172" s="4"/>
+      <c r="K172" s="4"/>
+      <c r="L172" s="4"/>
+      <c r="M172" s="4"/>
+      <c r="N172" s="4"/>
+      <c r="O172" s="4"/>
+      <c r="P172" s="4"/>
+      <c r="Q172" s="4"/>
+      <c r="R172" s="4"/>
+      <c r="S172" s="4"/>
+      <c r="T172" s="4"/>
+      <c r="U172" s="4"/>
+      <c r="V172" s="4"/>
+      <c r="W172" s="4"/>
+      <c r="X172" s="4"/>
+      <c r="Y172" s="16"/>
       <c r="Z172" s="1"/>
       <c r="AA172" s="1"/>
       <c r="AB172" s="1"/>
     </row>
-    <row r="173" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
-      <c r="B173" s="1"/>
-      <c r="C173" s="66"/>
-      <c r="D173" s="1"/>
-      <c r="E173" s="1"/>
-      <c r="F173" s="1"/>
-      <c r="G173" s="1"/>
-      <c r="H173" s="1"/>
-      <c r="I173" s="1"/>
-      <c r="J173" s="1"/>
-      <c r="K173" s="1"/>
-      <c r="L173" s="1"/>
-      <c r="M173" s="1"/>
-      <c r="N173" s="1"/>
-      <c r="O173" s="1"/>
-      <c r="P173" s="1"/>
-      <c r="Q173" s="1"/>
-      <c r="R173" s="1"/>
-      <c r="S173" s="1"/>
-      <c r="T173" s="1"/>
-      <c r="U173" s="1"/>
-      <c r="V173" s="1"/>
-      <c r="W173" s="1"/>
-      <c r="X173" s="1"/>
-      <c r="Y173" s="1"/>
+      <c r="B173" s="35"/>
+      <c r="C173" s="76">
+        <f>INT($C$155)+1.005</f>
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="D173" s="17"/>
+      <c r="E173" s="17"/>
+      <c r="F173" s="17"/>
+      <c r="G173" s="17"/>
+      <c r="H173" s="17"/>
+      <c r="I173" s="17"/>
+      <c r="J173" s="17"/>
+      <c r="K173" s="17"/>
+      <c r="L173" s="17"/>
+      <c r="M173" s="17"/>
+      <c r="N173" s="17"/>
+      <c r="O173" s="17"/>
+      <c r="P173" s="17"/>
+      <c r="Q173" s="17"/>
+      <c r="R173" s="17"/>
+      <c r="S173" s="17"/>
+      <c r="T173" s="17"/>
+      <c r="U173" s="17"/>
+      <c r="V173" s="17"/>
+      <c r="W173" s="17"/>
+      <c r="X173" s="17"/>
+      <c r="Y173" s="18" t="s">
+        <v>1</v>
+      </c>
       <c r="Z173" s="1"/>
       <c r="AA173" s="1"/>
       <c r="AB173" s="1"/>
     </row>
-    <row r="174" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
-      <c r="B174" s="1"/>
-      <c r="C174" s="66"/>
-      <c r="D174" s="1"/>
-      <c r="E174" s="1"/>
-      <c r="F174" s="1"/>
-      <c r="G174" s="1"/>
-      <c r="H174" s="1"/>
-      <c r="I174" s="1"/>
-      <c r="J174" s="1"/>
-      <c r="K174" s="1"/>
-      <c r="L174" s="1"/>
-      <c r="M174" s="1"/>
-      <c r="N174" s="1"/>
-      <c r="O174" s="1"/>
-      <c r="P174" s="1"/>
-      <c r="Q174" s="1"/>
-      <c r="R174" s="1"/>
-      <c r="S174" s="1"/>
-      <c r="T174" s="1"/>
-      <c r="U174" s="1"/>
-      <c r="V174" s="1"/>
-      <c r="W174" s="1"/>
-      <c r="X174" s="1"/>
-      <c r="Y174" s="1"/>
+      <c r="B174" s="19"/>
+      <c r="C174" s="77">
+        <f>INT($C$155)+0.005</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D174" s="19"/>
+      <c r="E174" s="19"/>
+      <c r="F174" s="19"/>
+      <c r="G174" s="19"/>
+      <c r="H174" s="19"/>
+      <c r="I174" s="19"/>
+      <c r="J174" s="19"/>
+      <c r="K174" s="19"/>
+      <c r="L174" s="19"/>
+      <c r="M174" s="19"/>
+      <c r="N174" s="19"/>
+      <c r="O174" s="19"/>
+      <c r="P174" s="19"/>
+      <c r="Q174" s="19"/>
+      <c r="R174" s="19"/>
+      <c r="S174" s="19"/>
+      <c r="T174" s="19"/>
+      <c r="U174" s="19"/>
+      <c r="V174" s="19"/>
+      <c r="W174" s="19"/>
+      <c r="X174" s="19"/>
+      <c r="Y174" s="19"/>
       <c r="Z174" s="1"/>
       <c r="AA174" s="1"/>
       <c r="AB174" s="1"/>
     </row>
-    <row r="175" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C175" s="72" t="s">
+    <row r="175" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A175" s="1"/>
+      <c r="B175" s="1"/>
+      <c r="C175" s="73">
+        <f>INT($C$155)+2</f>
+        <v>3</v>
+      </c>
+      <c r="D175" s="1"/>
+      <c r="E175" s="1"/>
+      <c r="F175" s="1"/>
+      <c r="G175" s="1"/>
+      <c r="H175" s="1"/>
+      <c r="I175" s="1"/>
+      <c r="J175" s="1"/>
+      <c r="K175" s="1"/>
+      <c r="L175" s="1"/>
+      <c r="M175" s="1"/>
+      <c r="N175" s="1"/>
+      <c r="O175" s="1"/>
+      <c r="P175" s="1"/>
+      <c r="Q175" s="1"/>
+      <c r="R175" s="1"/>
+      <c r="S175" s="1"/>
+      <c r="T175" s="1"/>
+      <c r="U175" s="1"/>
+      <c r="V175" s="1"/>
+      <c r="W175" s="1"/>
+      <c r="X175" s="1"/>
+      <c r="Y175" s="1"/>
+      <c r="Z175" s="1"/>
+      <c r="AA175" s="1"/>
+      <c r="AB175" s="1"/>
+    </row>
+    <row r="176" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A176" s="1"/>
+      <c r="B176" s="1"/>
+      <c r="C176" s="66"/>
+      <c r="D176" s="1"/>
+      <c r="E176" s="1"/>
+      <c r="F176" s="1"/>
+      <c r="G176" s="1"/>
+      <c r="H176" s="1"/>
+      <c r="I176" s="1"/>
+      <c r="J176" s="1"/>
+      <c r="K176" s="1"/>
+      <c r="L176" s="1"/>
+      <c r="M176" s="1"/>
+      <c r="N176" s="1"/>
+      <c r="O176" s="1"/>
+      <c r="P176" s="1"/>
+      <c r="Q176" s="1"/>
+      <c r="R176" s="1"/>
+      <c r="S176" s="1"/>
+      <c r="T176" s="1"/>
+      <c r="U176" s="1"/>
+      <c r="V176" s="1"/>
+      <c r="W176" s="1"/>
+      <c r="X176" s="1"/>
+      <c r="Y176" s="1"/>
+      <c r="Z176" s="1"/>
+      <c r="AA176" s="1"/>
+      <c r="AB176" s="1"/>
+    </row>
+    <row r="177" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A177" s="1"/>
+      <c r="B177" s="1"/>
+      <c r="C177" s="66"/>
+      <c r="D177" s="1"/>
+      <c r="E177" s="1"/>
+      <c r="F177" s="1"/>
+      <c r="G177" s="1"/>
+      <c r="H177" s="1"/>
+      <c r="I177" s="1"/>
+      <c r="J177" s="1"/>
+      <c r="K177" s="1"/>
+      <c r="L177" s="1"/>
+      <c r="M177" s="1"/>
+      <c r="N177" s="1"/>
+      <c r="O177" s="1"/>
+      <c r="P177" s="1"/>
+      <c r="Q177" s="1"/>
+      <c r="R177" s="1"/>
+      <c r="S177" s="1"/>
+      <c r="T177" s="1"/>
+      <c r="U177" s="1"/>
+      <c r="V177" s="1"/>
+      <c r="W177" s="1"/>
+      <c r="X177" s="1"/>
+      <c r="Y177" s="1"/>
+      <c r="Z177" s="1"/>
+      <c r="AA177" s="1"/>
+      <c r="AB177" s="1"/>
+    </row>
+    <row r="178" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A178" s="1"/>
+      <c r="B178" s="1"/>
+      <c r="C178" s="66"/>
+      <c r="D178" s="1"/>
+      <c r="E178" s="1"/>
+      <c r="F178" s="1"/>
+      <c r="G178" s="1"/>
+      <c r="H178" s="1"/>
+      <c r="I178" s="1"/>
+      <c r="J178" s="1"/>
+      <c r="K178" s="1"/>
+      <c r="L178" s="1"/>
+      <c r="M178" s="1"/>
+      <c r="N178" s="1"/>
+      <c r="O178" s="1"/>
+      <c r="P178" s="1"/>
+      <c r="Q178" s="1"/>
+      <c r="R178" s="1"/>
+      <c r="S178" s="1"/>
+      <c r="T178" s="1"/>
+      <c r="U178" s="1"/>
+      <c r="V178" s="1"/>
+      <c r="W178" s="1"/>
+      <c r="X178" s="1"/>
+      <c r="Y178" s="1"/>
+      <c r="Z178" s="1"/>
+      <c r="AA178" s="1"/>
+      <c r="AB178" s="1"/>
+    </row>
+    <row r="179" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A179" s="1"/>
+      <c r="B179" s="1"/>
+      <c r="C179" s="66"/>
+      <c r="D179" s="1"/>
+      <c r="E179" s="1"/>
+      <c r="F179" s="1"/>
+      <c r="G179" s="1"/>
+      <c r="H179" s="1"/>
+      <c r="I179" s="1"/>
+      <c r="J179" s="1"/>
+      <c r="K179" s="1"/>
+      <c r="L179" s="1"/>
+      <c r="M179" s="1"/>
+      <c r="N179" s="1"/>
+      <c r="O179" s="1"/>
+      <c r="P179" s="1"/>
+      <c r="Q179" s="1"/>
+      <c r="R179" s="1"/>
+      <c r="S179" s="1"/>
+      <c r="T179" s="1"/>
+      <c r="U179" s="1"/>
+      <c r="V179" s="1"/>
+      <c r="W179" s="1"/>
+      <c r="X179" s="1"/>
+      <c r="Y179" s="1"/>
+      <c r="Z179" s="1"/>
+      <c r="AA179" s="1"/>
+      <c r="AB179" s="1"/>
+    </row>
+    <row r="180" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A180" s="1"/>
+      <c r="B180" s="1"/>
+      <c r="C180" s="66"/>
+      <c r="D180" s="1"/>
+      <c r="E180" s="1"/>
+      <c r="F180" s="1"/>
+      <c r="G180" s="1"/>
+      <c r="H180" s="1"/>
+      <c r="I180" s="1"/>
+      <c r="J180" s="1"/>
+      <c r="K180" s="1"/>
+      <c r="L180" s="1"/>
+      <c r="M180" s="1"/>
+      <c r="N180" s="1"/>
+      <c r="O180" s="1"/>
+      <c r="P180" s="1"/>
+      <c r="Q180" s="1"/>
+      <c r="R180" s="1"/>
+      <c r="S180" s="1"/>
+      <c r="T180" s="1"/>
+      <c r="U180" s="1"/>
+      <c r="V180" s="1"/>
+      <c r="W180" s="1"/>
+      <c r="X180" s="1"/>
+      <c r="Y180" s="1"/>
+      <c r="Z180" s="1"/>
+      <c r="AA180" s="1"/>
+      <c r="AB180" s="1"/>
+    </row>
+    <row r="181" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A181" s="1"/>
+      <c r="B181" s="1"/>
+      <c r="C181" s="66"/>
+      <c r="D181" s="1"/>
+      <c r="E181" s="1"/>
+      <c r="F181" s="1"/>
+      <c r="G181" s="1"/>
+      <c r="H181" s="1"/>
+      <c r="I181" s="1"/>
+      <c r="J181" s="1"/>
+      <c r="K181" s="1"/>
+      <c r="L181" s="1"/>
+      <c r="M181" s="1"/>
+      <c r="N181" s="1"/>
+      <c r="O181" s="1"/>
+      <c r="P181" s="1"/>
+      <c r="Q181" s="1"/>
+      <c r="R181" s="1"/>
+      <c r="S181" s="1"/>
+      <c r="T181" s="1"/>
+      <c r="U181" s="1"/>
+      <c r="V181" s="1"/>
+      <c r="W181" s="1"/>
+      <c r="X181" s="1"/>
+      <c r="Y181" s="1"/>
+      <c r="Z181" s="1"/>
+      <c r="AA181" s="1"/>
+      <c r="AB181" s="1"/>
+    </row>
+    <row r="182" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C182" s="72" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new sale options for offs (sale evenly spread throughout DVP) profit increase ~25k & make a few minor name fixes
</commit_message>
<xml_diff>
--- a/ExcelInputs/Structural.xlsx
+++ b/ExcelInputs/Structural.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\Work-Uni-Coding\Models\AFO\ExcelInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3B34E5-8430-4DEB-8727-A51785DF120D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6C4748-873C-4A5B-B137-8A598D708135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67080" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="19395" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -122,6 +122,8 @@
     <definedName name="i_nut_spread_n3" localSheetId="2">StructuralSA!$S$115:$S$122</definedName>
     <definedName name="i_nv_lower_p6">StructuralSA!$J$195:$S$195</definedName>
     <definedName name="i_nv_upper_p6">StructuralSA!$J$196:$S$196</definedName>
+    <definedName name="i_offs_sale_method" localSheetId="2">StructuralSA!$I$45</definedName>
+    <definedName name="i_offs_sale_opportunities_per_dvp" localSheetId="2">StructuralSA!$I$46</definedName>
     <definedName name="i_offs_user_fvp_date_iu" localSheetId="2">StructuralSA!$P$82:$R$84</definedName>
     <definedName name="i_p_pos">Stock!$I$55</definedName>
     <definedName name="i_prejoin_offset">Stock!$I$66</definedName>
@@ -1226,6 +1228,54 @@
           </rPr>
           <t xml:space="preserve">
 In the web app this is set to False so that all crops can be wet or dy sown. Which removes the number of landuses required. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H45" authorId="0" shapeId="0" xr:uid="{BB89A993-BB16-406A-945D-1C3F541C2430}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+(i) simply enter a number of sale options per dvp and AFO will make on t slice for each opportunity. The opportunities are evenly space within the dvp. This is the default option. (ii) enter weights and ages that trigger sales (property inputs). This method can be useful to reduce t sices but care must be taken when doing the inputs. This second option is recomended for the DSP model to reduce size.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H46" authorId="0" shapeId="0" xr:uid="{0634BC1B-3FB1-4084-83E3-B16D521CEB1B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is used if the input above is True. The sale opportunities are evenly space within dvp. Each sale opportunity is a t slice.</t>
         </r>
       </text>
     </comment>
@@ -2371,7 +2421,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="396">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -3676,6 +3726,12 @@
   </si>
   <si>
     <t xml:space="preserve">Differentiate wet and dry sown landuses </t>
+  </si>
+  <si>
+    <t>Offs sale opportunities per DVP</t>
+  </si>
+  <si>
+    <t>Offs sale method</t>
   </si>
 </sst>
 </file>
@@ -5028,7 +5084,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="221">
+  <cellXfs count="220">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="3">
@@ -5588,6 +5644,10 @@
     <xf numFmtId="167" fontId="6" fillId="8" borderId="25" xfId="3" applyNumberFormat="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="39" borderId="25" xfId="44" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="38" xfId="12" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -5611,13 +5671,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="39" borderId="25" xfId="44" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -6273,7 +6326,7 @@
   <dimension ref="A1:AT127"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J82" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="10" topLeftCell="J124" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
@@ -6769,19 +6822,19 @@
       <c r="I13" s="126">
         <v>44371.659649305599</v>
       </c>
-      <c r="J13" s="212" t="s">
+      <c r="J13" s="213" t="s">
         <v>296</v>
       </c>
-      <c r="K13" s="213"/>
-      <c r="L13" s="213"/>
-      <c r="M13" s="213"/>
-      <c r="N13" s="213"/>
-      <c r="O13" s="213"/>
-      <c r="P13" s="213"/>
-      <c r="Q13" s="213"/>
-      <c r="R13" s="213"/>
-      <c r="S13" s="213"/>
-      <c r="T13" s="214"/>
+      <c r="K13" s="214"/>
+      <c r="L13" s="214"/>
+      <c r="M13" s="214"/>
+      <c r="N13" s="214"/>
+      <c r="O13" s="214"/>
+      <c r="P13" s="214"/>
+      <c r="Q13" s="214"/>
+      <c r="R13" s="214"/>
+      <c r="S13" s="214"/>
+      <c r="T13" s="215"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
@@ -6808,19 +6861,19 @@
       <c r="I14" s="125">
         <v>44719.411846643503</v>
       </c>
-      <c r="J14" s="215" t="s">
+      <c r="J14" s="216" t="s">
         <v>357</v>
       </c>
-      <c r="K14" s="216"/>
-      <c r="L14" s="216"/>
-      <c r="M14" s="216"/>
-      <c r="N14" s="216"/>
-      <c r="O14" s="216"/>
-      <c r="P14" s="216"/>
-      <c r="Q14" s="216"/>
-      <c r="R14" s="216"/>
-      <c r="S14" s="216"/>
-      <c r="T14" s="216"/>
+      <c r="K14" s="217"/>
+      <c r="L14" s="217"/>
+      <c r="M14" s="217"/>
+      <c r="N14" s="217"/>
+      <c r="O14" s="217"/>
+      <c r="P14" s="217"/>
+      <c r="Q14" s="217"/>
+      <c r="R14" s="217"/>
+      <c r="S14" s="217"/>
+      <c r="T14" s="217"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
@@ -11445,19 +11498,19 @@
       <c r="I13" s="126">
         <v>45049.868338773202</v>
       </c>
-      <c r="J13" s="212" t="s">
+      <c r="J13" s="213" t="s">
         <v>380</v>
       </c>
-      <c r="K13" s="213"/>
-      <c r="L13" s="213"/>
-      <c r="M13" s="213"/>
-      <c r="N13" s="213"/>
-      <c r="O13" s="213"/>
-      <c r="P13" s="213"/>
-      <c r="Q13" s="213"/>
-      <c r="R13" s="213"/>
-      <c r="S13" s="213"/>
-      <c r="T13" s="214"/>
+      <c r="K13" s="214"/>
+      <c r="L13" s="214"/>
+      <c r="M13" s="214"/>
+      <c r="N13" s="214"/>
+      <c r="O13" s="214"/>
+      <c r="P13" s="214"/>
+      <c r="Q13" s="214"/>
+      <c r="R13" s="214"/>
+      <c r="S13" s="214"/>
+      <c r="T13" s="215"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
@@ -11484,19 +11537,19 @@
       <c r="I14" s="125">
         <v>44762.449343865701</v>
       </c>
-      <c r="J14" s="215" t="s">
+      <c r="J14" s="216" t="s">
         <v>362</v>
       </c>
-      <c r="K14" s="216"/>
-      <c r="L14" s="216"/>
-      <c r="M14" s="216"/>
-      <c r="N14" s="216"/>
-      <c r="O14" s="216"/>
-      <c r="P14" s="216"/>
-      <c r="Q14" s="216"/>
-      <c r="R14" s="216"/>
-      <c r="S14" s="216"/>
-      <c r="T14" s="216"/>
+      <c r="K14" s="217"/>
+      <c r="L14" s="217"/>
+      <c r="M14" s="217"/>
+      <c r="N14" s="217"/>
+      <c r="O14" s="217"/>
+      <c r="P14" s="217"/>
+      <c r="Q14" s="217"/>
+      <c r="R14" s="217"/>
+      <c r="S14" s="217"/>
+      <c r="T14" s="217"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
@@ -26765,11 +26818,11 @@
   <dimension ref="A1:AB210"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="10" topLeftCell="J24" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="N47" sqref="N47"/>
+      <selection pane="bottomRight" activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
@@ -27266,19 +27319,19 @@
       <c r="I13" s="126">
         <v>45314.472435879601</v>
       </c>
-      <c r="J13" s="212" t="s">
+      <c r="J13" s="213" t="s">
         <v>392</v>
       </c>
-      <c r="K13" s="213"/>
-      <c r="L13" s="213"/>
-      <c r="M13" s="213"/>
-      <c r="N13" s="213"/>
-      <c r="O13" s="213"/>
-      <c r="P13" s="213"/>
-      <c r="Q13" s="213"/>
-      <c r="R13" s="213"/>
-      <c r="S13" s="213"/>
-      <c r="T13" s="214"/>
+      <c r="K13" s="214"/>
+      <c r="L13" s="214"/>
+      <c r="M13" s="214"/>
+      <c r="N13" s="214"/>
+      <c r="O13" s="214"/>
+      <c r="P13" s="214"/>
+      <c r="Q13" s="214"/>
+      <c r="R13" s="214"/>
+      <c r="S13" s="214"/>
+      <c r="T13" s="215"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
@@ -27305,19 +27358,19 @@
       <c r="I14" s="125">
         <v>45073.683614236099</v>
       </c>
-      <c r="J14" s="215" t="s">
+      <c r="J14" s="216" t="s">
         <v>373</v>
       </c>
-      <c r="K14" s="216"/>
-      <c r="L14" s="216"/>
-      <c r="M14" s="216"/>
-      <c r="N14" s="216"/>
-      <c r="O14" s="216"/>
-      <c r="P14" s="216"/>
-      <c r="Q14" s="216"/>
-      <c r="R14" s="216"/>
-      <c r="S14" s="216"/>
-      <c r="T14" s="216"/>
+      <c r="K14" s="217"/>
+      <c r="L14" s="217"/>
+      <c r="M14" s="217"/>
+      <c r="N14" s="217"/>
+      <c r="O14" s="217"/>
+      <c r="P14" s="217"/>
+      <c r="Q14" s="217"/>
+      <c r="R14" s="217"/>
+      <c r="S14" s="217"/>
+      <c r="T14" s="217"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
@@ -28285,10 +28338,10 @@
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
       <c r="G42" s="4"/>
-      <c r="H42" s="220" t="s">
+      <c r="H42" s="36" t="s">
         <v>393</v>
       </c>
-      <c r="I42" s="219" t="b">
+      <c r="I42" s="212" t="b">
         <v>1</v>
       </c>
       <c r="J42" s="96"/>
@@ -28388,8 +28441,12 @@
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="4"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
+      <c r="H45" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="I45" s="204">
+        <v>1</v>
+      </c>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
@@ -28421,8 +28478,12 @@
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="4"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
+      <c r="H46" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="I46" s="204">
+        <v>4</v>
+      </c>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
@@ -36376,23 +36437,23 @@
       <c r="I18" s="31">
         <v>1</v>
       </c>
-      <c r="J18" s="217" t="s">
+      <c r="J18" s="218" t="s">
         <v>22</v>
       </c>
-      <c r="K18" s="217"/>
-      <c r="L18" s="217"/>
-      <c r="M18" s="217"/>
-      <c r="N18" s="217"/>
-      <c r="O18" s="217"/>
-      <c r="P18" s="217"/>
-      <c r="Q18" s="217"/>
-      <c r="R18" s="217"/>
-      <c r="S18" s="217"/>
-      <c r="T18" s="217"/>
-      <c r="U18" s="217"/>
-      <c r="V18" s="217"/>
-      <c r="W18" s="217"/>
-      <c r="X18" s="217"/>
+      <c r="K18" s="218"/>
+      <c r="L18" s="218"/>
+      <c r="M18" s="218"/>
+      <c r="N18" s="218"/>
+      <c r="O18" s="218"/>
+      <c r="P18" s="218"/>
+      <c r="Q18" s="218"/>
+      <c r="R18" s="218"/>
+      <c r="S18" s="218"/>
+      <c r="T18" s="218"/>
+      <c r="U18" s="218"/>
+      <c r="V18" s="218"/>
+      <c r="W18" s="218"/>
+      <c r="X18" s="218"/>
       <c r="Y18" s="2"/>
       <c r="Z18" s="4"/>
       <c r="AA18" s="16"/>
@@ -36487,23 +36548,23 @@
       <c r="I21" s="23">
         <v>1</v>
       </c>
-      <c r="J21" s="215" t="s">
+      <c r="J21" s="216" t="s">
         <v>34</v>
       </c>
-      <c r="K21" s="216"/>
-      <c r="L21" s="216"/>
-      <c r="M21" s="216"/>
-      <c r="N21" s="216"/>
-      <c r="O21" s="216"/>
-      <c r="P21" s="216"/>
-      <c r="Q21" s="216"/>
-      <c r="R21" s="216"/>
-      <c r="S21" s="216"/>
-      <c r="T21" s="216"/>
-      <c r="U21" s="216"/>
-      <c r="V21" s="216"/>
-      <c r="W21" s="216"/>
-      <c r="X21" s="218"/>
+      <c r="K21" s="217"/>
+      <c r="L21" s="217"/>
+      <c r="M21" s="217"/>
+      <c r="N21" s="217"/>
+      <c r="O21" s="217"/>
+      <c r="P21" s="217"/>
+      <c r="Q21" s="217"/>
+      <c r="R21" s="217"/>
+      <c r="S21" s="217"/>
+      <c r="T21" s="217"/>
+      <c r="U21" s="217"/>
+      <c r="V21" s="217"/>
+      <c r="W21" s="217"/>
+      <c r="X21" s="219"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="4"/>
       <c r="AA21" s="16"/>

</xml_diff>

<commit_message>
Move DSP/SQ controls to structural.xl.
</commit_message>
<xml_diff>
--- a/ExcelInputs/Structural.xlsx
+++ b/ExcelInputs/Structural.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\Work-Uni-Coding\Models\AFO\ExcelInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6886F4-7145-48BD-9CA3-89F6FC886E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FDF07AD-45B4-4EDC-BC44-5A853311D8E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7275" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="678" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="21525" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -81,6 +81,7 @@
     <definedName name="i_idx_k" localSheetId="0">General!$P$79:$P$109</definedName>
     <definedName name="i_idx_k1" localSheetId="0">General!$I$79:$I$96</definedName>
     <definedName name="i_idx_k2" localSheetId="0">General!$L$79:$L$91</definedName>
+    <definedName name="i_inc_node_periods" localSheetId="2">StructuralSA!$M$43</definedName>
     <definedName name="i_initial_b1">Stock!$L$155:$V$155</definedName>
     <definedName name="i_is_baled_k" localSheetId="0">General!$J$79:$J$96</definedName>
     <definedName name="i_is_dry_b1">Stock!$L$149:$V$149</definedName>
@@ -95,6 +96,7 @@
     <definedName name="i_len_f">StructuralSA!$I$193</definedName>
     <definedName name="i_len_l">Stock!$M$160</definedName>
     <definedName name="i_len_m">Stock!$L$160</definedName>
+    <definedName name="i_len_q" localSheetId="2">StructuralSA!$M$44</definedName>
     <definedName name="i_len_s">Stock!$N$160</definedName>
     <definedName name="i_lsln_idx_dams">Stock!$L$202:$V$202</definedName>
     <definedName name="i_mask_b0_b1">Stock!$L$148:$V$148</definedName>
@@ -122,8 +124,8 @@
     <definedName name="i_nut_spread_n3" localSheetId="2">StructuralSA!$S$115:$S$122</definedName>
     <definedName name="i_nv_lower_p6">StructuralSA!$J$196:$S$196</definedName>
     <definedName name="i_nv_upper_p6">StructuralSA!$J$197:$S$197</definedName>
-    <definedName name="i_offs_sale_method" localSheetId="2">StructuralSA!$I$45</definedName>
-    <definedName name="i_offs_sale_opportunities_per_dvp" localSheetId="2">StructuralSA!$I$46</definedName>
+    <definedName name="i_offs_sale_method" localSheetId="2">StructuralSA!$R$42</definedName>
+    <definedName name="i_offs_sale_opportunities_per_dvp" localSheetId="2">StructuralSA!$R$43</definedName>
     <definedName name="i_offs_user_fvp_date_iu" localSheetId="2">StructuralSA!$P$82:$R$84</definedName>
     <definedName name="i_p_pos">Stock!$I$55</definedName>
     <definedName name="i_prejoin_offset">Stock!$I$66</definedName>
@@ -165,6 +167,7 @@
     <definedName name="pastures" localSheetId="0">General!$I$46:$L$46</definedName>
     <definedName name="phase_len" localSheetId="0">General!$I$51</definedName>
     <definedName name="rdvp_type_r">Stock!$J$318:$L$318</definedName>
+    <definedName name="steady_state" localSheetId="2">StructuralSA!$M$42</definedName>
     <definedName name="worker_levels" localSheetId="0">General!$I$42:$K$42</definedName>
     <definedName name="ZA.Gridlines" localSheetId="4">Admin!$L$29</definedName>
     <definedName name="ZA.Headers" localSheetId="4">Admin!$L$30</definedName>
@@ -177,7 +180,7 @@
     <definedName name="ZA.WidthCol" localSheetId="4">Admin!$L$26</definedName>
     <definedName name="ZA.ZoomSheet" localSheetId="4">Admin!$O$26</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1231,7 +1234,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H45" authorId="0" shapeId="0" xr:uid="{BB89A993-BB16-406A-945D-1C3F541C2430}">
+    <comment ref="Q42" authorId="0" shapeId="0" xr:uid="{BB89A993-BB16-406A-945D-1C3F541C2430}">
       <text>
         <r>
           <rPr>
@@ -1255,7 +1258,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="H46" authorId="0" shapeId="0" xr:uid="{0634BC1B-3FB1-4084-83E3-B16D521CEB1B}">
+    <comment ref="L43" authorId="1" shapeId="0" xr:uid="{1C7C64C2-3F12-43F6-8413-0B040031EF4D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young (21512438):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+include nodes as feed periods and dvps. This allows you to include the nodes in the steady state model. In DSP this inputs gets overwritten and essentially set to true.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q43" authorId="0" shapeId="0" xr:uid="{0634BC1B-3FB1-4084-83E3-B16D521CEB1B}">
       <text>
         <r>
           <rPr>
@@ -2445,7 +2472,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="405">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -3764,6 +3791,27 @@
   </si>
   <si>
     <t>ms</t>
+  </si>
+  <si>
+    <t>Steady State Model?</t>
+  </si>
+  <si>
+    <t>include nodes</t>
+  </si>
+  <si>
+    <t>Season sequence len</t>
+  </si>
+  <si>
+    <t>Season Structure</t>
+  </si>
+  <si>
+    <t>Sowing</t>
+  </si>
+  <si>
+    <t>Sheep</t>
+  </si>
+  <si>
+    <t>Multi-period model?</t>
   </si>
 </sst>
 </file>
@@ -5116,7 +5164,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="220">
+  <cellXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="3">
@@ -5702,6 +5750,13 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="32" fillId="39" borderId="22" xfId="44" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="39" borderId="0" xfId="44" applyBorder="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -6357,8 +6412,8 @@
   </sheetPr>
   <dimension ref="A1:AT127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J82" activePane="bottomRight" state="frozen"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <pane xSplit="9" ySplit="10" topLeftCell="J24" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
@@ -26860,12 +26915,12 @@
   </sheetPr>
   <dimension ref="A1:AB211"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J143" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="9" ySplit="10" topLeftCell="J19" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="H164" sqref="H164"/>
+      <selection pane="bottomRight" activeCell="M44" sqref="M44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
@@ -28197,7 +28252,7 @@
       <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
     </row>
-    <row r="37" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:28" ht="28" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="33"/>
       <c r="C37" s="73">
@@ -28209,16 +28264,22 @@
       <c r="F37" s="5"/>
       <c r="G37" s="3"/>
       <c r="H37" s="29"/>
-      <c r="I37" s="29"/>
+      <c r="I37" s="29" t="s">
+        <v>402</v>
+      </c>
       <c r="J37" s="29"/>
       <c r="K37" s="29"/>
       <c r="L37" s="29"/>
-      <c r="M37" s="29"/>
+      <c r="M37" s="29" t="s">
+        <v>401</v>
+      </c>
       <c r="N37" s="29"/>
       <c r="O37" s="29"/>
       <c r="P37" s="29"/>
       <c r="Q37" s="29"/>
-      <c r="R37" s="29"/>
+      <c r="R37" s="29" t="s">
+        <v>403</v>
+      </c>
       <c r="S37" s="29"/>
       <c r="T37" s="29"/>
       <c r="U37" s="29"/>
@@ -28389,13 +28450,21 @@
       </c>
       <c r="J42" s="96"/>
       <c r="K42" s="96"/>
-      <c r="L42" s="96"/>
-      <c r="M42" s="96"/>
+      <c r="L42" s="26" t="s">
+        <v>398</v>
+      </c>
+      <c r="M42" s="220" t="b">
+        <v>1</v>
+      </c>
       <c r="N42" s="96"/>
       <c r="O42" s="96"/>
       <c r="P42" s="96"/>
-      <c r="Q42" s="96"/>
-      <c r="R42" s="96"/>
+      <c r="Q42" s="26" t="s">
+        <v>393</v>
+      </c>
+      <c r="R42" s="204">
+        <v>1</v>
+      </c>
       <c r="S42" s="96"/>
       <c r="T42" s="96"/>
       <c r="U42" s="96"/>
@@ -28422,13 +28491,21 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
+      <c r="L43" s="26" t="s">
+        <v>399</v>
+      </c>
+      <c r="M43" s="220" t="b">
+        <v>0</v>
+      </c>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
-      <c r="Q43" s="2"/>
-      <c r="R43" s="2"/>
+      <c r="Q43" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="R43" s="204">
+        <v>4</v>
+      </c>
       <c r="S43" s="2"/>
       <c r="T43" s="2"/>
       <c r="U43" s="2"/>
@@ -28455,8 +28532,12 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
+      <c r="L44" s="26" t="s">
+        <v>400</v>
+      </c>
+      <c r="M44" s="221">
+        <v>1</v>
+      </c>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
@@ -28484,16 +28565,16 @@
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="4"/>
-      <c r="H45" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="I45" s="204">
-        <v>1</v>
-      </c>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
+      <c r="L45" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="M45" s="220" t="b">
+        <v>0</v>
+      </c>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
@@ -28521,12 +28602,8 @@
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="4"/>
-      <c r="H46" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="I46" s="204">
-        <v>4</v>
-      </c>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>

</xml_diff>

<commit_message>
add input to turn on MP model
</commit_message>
<xml_diff>
--- a/ExcelInputs/Structural.xlsx
+++ b/ExcelInputs/Structural.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\Work-Uni-Coding\Models\AFO\ExcelInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FDF07AD-45B4-4EDC-BC44-5A853311D8E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16540849-E08C-4387-9E42-431B8D779F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21525" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
@@ -164,6 +164,7 @@
     <definedName name="ia_sire_dsegroup">Stock!$L$144</definedName>
     <definedName name="ia_yatf_dsegroup_b1">Stock!$L$146:$V$146</definedName>
     <definedName name="labour_period_len" localSheetId="0">General!$I$53</definedName>
+    <definedName name="model_is_MP" localSheetId="2">StructuralSA!$M$45</definedName>
     <definedName name="pastures" localSheetId="0">General!$I$46:$L$46</definedName>
     <definedName name="phase_len" localSheetId="0">General!$I$51</definedName>
     <definedName name="rdvp_type_r">Stock!$J$318:$L$318</definedName>
@@ -5728,6 +5729,13 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="2" fontId="32" fillId="39" borderId="22" xfId="44" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="39" borderId="0" xfId="44" applyBorder="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="38" xfId="12" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -5750,13 +5758,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="32" fillId="39" borderId="22" xfId="44" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="39" borderId="0" xfId="44" applyBorder="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -6909,19 +6910,19 @@
       <c r="I13" s="126">
         <v>44371.659649305599</v>
       </c>
-      <c r="J13" s="213" t="s">
+      <c r="J13" s="215" t="s">
         <v>296</v>
       </c>
-      <c r="K13" s="214"/>
-      <c r="L13" s="214"/>
-      <c r="M13" s="214"/>
-      <c r="N13" s="214"/>
-      <c r="O13" s="214"/>
-      <c r="P13" s="214"/>
-      <c r="Q13" s="214"/>
-      <c r="R13" s="214"/>
-      <c r="S13" s="214"/>
-      <c r="T13" s="215"/>
+      <c r="K13" s="216"/>
+      <c r="L13" s="216"/>
+      <c r="M13" s="216"/>
+      <c r="N13" s="216"/>
+      <c r="O13" s="216"/>
+      <c r="P13" s="216"/>
+      <c r="Q13" s="216"/>
+      <c r="R13" s="216"/>
+      <c r="S13" s="216"/>
+      <c r="T13" s="217"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
@@ -6948,19 +6949,19 @@
       <c r="I14" s="125">
         <v>44719.411846643503</v>
       </c>
-      <c r="J14" s="216" t="s">
+      <c r="J14" s="218" t="s">
         <v>357</v>
       </c>
-      <c r="K14" s="217"/>
-      <c r="L14" s="217"/>
-      <c r="M14" s="217"/>
-      <c r="N14" s="217"/>
-      <c r="O14" s="217"/>
-      <c r="P14" s="217"/>
-      <c r="Q14" s="217"/>
-      <c r="R14" s="217"/>
-      <c r="S14" s="217"/>
-      <c r="T14" s="217"/>
+      <c r="K14" s="219"/>
+      <c r="L14" s="219"/>
+      <c r="M14" s="219"/>
+      <c r="N14" s="219"/>
+      <c r="O14" s="219"/>
+      <c r="P14" s="219"/>
+      <c r="Q14" s="219"/>
+      <c r="R14" s="219"/>
+      <c r="S14" s="219"/>
+      <c r="T14" s="219"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
@@ -11596,19 +11597,19 @@
       <c r="I13" s="126">
         <v>45049.868338773202</v>
       </c>
-      <c r="J13" s="213" t="s">
+      <c r="J13" s="215" t="s">
         <v>379</v>
       </c>
-      <c r="K13" s="214"/>
-      <c r="L13" s="214"/>
-      <c r="M13" s="214"/>
-      <c r="N13" s="214"/>
-      <c r="O13" s="214"/>
-      <c r="P13" s="214"/>
-      <c r="Q13" s="214"/>
-      <c r="R13" s="214"/>
-      <c r="S13" s="214"/>
-      <c r="T13" s="215"/>
+      <c r="K13" s="216"/>
+      <c r="L13" s="216"/>
+      <c r="M13" s="216"/>
+      <c r="N13" s="216"/>
+      <c r="O13" s="216"/>
+      <c r="P13" s="216"/>
+      <c r="Q13" s="216"/>
+      <c r="R13" s="216"/>
+      <c r="S13" s="216"/>
+      <c r="T13" s="217"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
@@ -11635,19 +11636,19 @@
       <c r="I14" s="125">
         <v>44762.449343865701</v>
       </c>
-      <c r="J14" s="216" t="s">
+      <c r="J14" s="218" t="s">
         <v>362</v>
       </c>
-      <c r="K14" s="217"/>
-      <c r="L14" s="217"/>
-      <c r="M14" s="217"/>
-      <c r="N14" s="217"/>
-      <c r="O14" s="217"/>
-      <c r="P14" s="217"/>
-      <c r="Q14" s="217"/>
-      <c r="R14" s="217"/>
-      <c r="S14" s="217"/>
-      <c r="T14" s="217"/>
+      <c r="K14" s="219"/>
+      <c r="L14" s="219"/>
+      <c r="M14" s="219"/>
+      <c r="N14" s="219"/>
+      <c r="O14" s="219"/>
+      <c r="P14" s="219"/>
+      <c r="Q14" s="219"/>
+      <c r="R14" s="219"/>
+      <c r="S14" s="219"/>
+      <c r="T14" s="219"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
@@ -26920,7 +26921,7 @@
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="M44" sqref="M44"/>
+      <selection pane="bottomRight" activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
@@ -27417,19 +27418,19 @@
       <c r="I13" s="126">
         <v>45441.560548148103</v>
       </c>
-      <c r="J13" s="213" t="s">
+      <c r="J13" s="215" t="s">
         <v>396</v>
       </c>
-      <c r="K13" s="214"/>
-      <c r="L13" s="214"/>
-      <c r="M13" s="214"/>
-      <c r="N13" s="214"/>
-      <c r="O13" s="214"/>
-      <c r="P13" s="214"/>
-      <c r="Q13" s="214"/>
-      <c r="R13" s="214"/>
-      <c r="S13" s="214"/>
-      <c r="T13" s="215"/>
+      <c r="K13" s="216"/>
+      <c r="L13" s="216"/>
+      <c r="M13" s="216"/>
+      <c r="N13" s="216"/>
+      <c r="O13" s="216"/>
+      <c r="P13" s="216"/>
+      <c r="Q13" s="216"/>
+      <c r="R13" s="216"/>
+      <c r="S13" s="216"/>
+      <c r="T13" s="217"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
@@ -27456,19 +27457,19 @@
       <c r="I14" s="125">
         <v>45421.933288078697</v>
       </c>
-      <c r="J14" s="216" t="s">
+      <c r="J14" s="218" t="s">
         <v>394</v>
       </c>
-      <c r="K14" s="217"/>
-      <c r="L14" s="217"/>
-      <c r="M14" s="217"/>
-      <c r="N14" s="217"/>
-      <c r="O14" s="217"/>
-      <c r="P14" s="217"/>
-      <c r="Q14" s="217"/>
-      <c r="R14" s="217"/>
-      <c r="S14" s="217"/>
-      <c r="T14" s="217"/>
+      <c r="K14" s="219"/>
+      <c r="L14" s="219"/>
+      <c r="M14" s="219"/>
+      <c r="N14" s="219"/>
+      <c r="O14" s="219"/>
+      <c r="P14" s="219"/>
+      <c r="Q14" s="219"/>
+      <c r="R14" s="219"/>
+      <c r="S14" s="219"/>
+      <c r="T14" s="219"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
@@ -28453,7 +28454,7 @@
       <c r="L42" s="26" t="s">
         <v>398</v>
       </c>
-      <c r="M42" s="220" t="b">
+      <c r="M42" s="213" t="b">
         <v>1</v>
       </c>
       <c r="N42" s="96"/>
@@ -28494,7 +28495,7 @@
       <c r="L43" s="26" t="s">
         <v>399</v>
       </c>
-      <c r="M43" s="220" t="b">
+      <c r="M43" s="213" t="b">
         <v>0</v>
       </c>
       <c r="N43" s="2"/>
@@ -28535,7 +28536,7 @@
       <c r="L44" s="26" t="s">
         <v>400</v>
       </c>
-      <c r="M44" s="221">
+      <c r="M44" s="214">
         <v>1</v>
       </c>
       <c r="N44" s="2"/>
@@ -28572,7 +28573,7 @@
       <c r="L45" s="26" t="s">
         <v>404</v>
       </c>
-      <c r="M45" s="220" t="b">
+      <c r="M45" s="213" t="b">
         <v>0</v>
       </c>
       <c r="N45" s="2"/>
@@ -36596,23 +36597,23 @@
       <c r="I18" s="31">
         <v>1</v>
       </c>
-      <c r="J18" s="218" t="s">
+      <c r="J18" s="220" t="s">
         <v>22</v>
       </c>
-      <c r="K18" s="218"/>
-      <c r="L18" s="218"/>
-      <c r="M18" s="218"/>
-      <c r="N18" s="218"/>
-      <c r="O18" s="218"/>
-      <c r="P18" s="218"/>
-      <c r="Q18" s="218"/>
-      <c r="R18" s="218"/>
-      <c r="S18" s="218"/>
-      <c r="T18" s="218"/>
-      <c r="U18" s="218"/>
-      <c r="V18" s="218"/>
-      <c r="W18" s="218"/>
-      <c r="X18" s="218"/>
+      <c r="K18" s="220"/>
+      <c r="L18" s="220"/>
+      <c r="M18" s="220"/>
+      <c r="N18" s="220"/>
+      <c r="O18" s="220"/>
+      <c r="P18" s="220"/>
+      <c r="Q18" s="220"/>
+      <c r="R18" s="220"/>
+      <c r="S18" s="220"/>
+      <c r="T18" s="220"/>
+      <c r="U18" s="220"/>
+      <c r="V18" s="220"/>
+      <c r="W18" s="220"/>
+      <c r="X18" s="220"/>
       <c r="Y18" s="2"/>
       <c r="Z18" s="4"/>
       <c r="AA18" s="16"/>
@@ -36707,23 +36708,23 @@
       <c r="I21" s="23">
         <v>1</v>
       </c>
-      <c r="J21" s="216" t="s">
+      <c r="J21" s="218" t="s">
         <v>34</v>
       </c>
-      <c r="K21" s="217"/>
-      <c r="L21" s="217"/>
-      <c r="M21" s="217"/>
-      <c r="N21" s="217"/>
-      <c r="O21" s="217"/>
-      <c r="P21" s="217"/>
-      <c r="Q21" s="217"/>
-      <c r="R21" s="217"/>
-      <c r="S21" s="217"/>
-      <c r="T21" s="217"/>
-      <c r="U21" s="217"/>
-      <c r="V21" s="217"/>
-      <c r="W21" s="217"/>
-      <c r="X21" s="219"/>
+      <c r="K21" s="219"/>
+      <c r="L21" s="219"/>
+      <c r="M21" s="219"/>
+      <c r="N21" s="219"/>
+      <c r="O21" s="219"/>
+      <c r="P21" s="219"/>
+      <c r="Q21" s="219"/>
+      <c r="R21" s="219"/>
+      <c r="S21" s="219"/>
+      <c r="T21" s="219"/>
+      <c r="U21" s="219"/>
+      <c r="V21" s="219"/>
+      <c r="W21" s="219"/>
+      <c r="X21" s="221"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="4"/>
       <c r="AA21" s="16"/>

</xml_diff>

<commit_message>
make it so that lw condensing can occur at season start. This is useful for the MP model so that we can have fvps only at the two nodes. No profit change on base model
</commit_message>
<xml_diff>
--- a/ExcelInputs/Structural.xlsx
+++ b/ExcelInputs/Structural.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\Work-Uni-Coding\Models\AFO\ExcelInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16540849-E08C-4387-9E42-431B8D779F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99B49BF-3401-4328-9C8B-9FB87D5169DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21525" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="-7275" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -54,7 +54,7 @@
     <definedName name="i_confinement_n0">StructuralSA!$K$115</definedName>
     <definedName name="i_confinement_n1">StructuralSA!$N$115:$N$122</definedName>
     <definedName name="i_confinement_n3">StructuralSA!$T$115:$T$122</definedName>
-    <definedName name="i_core_dvp_types_f1" localSheetId="1">Stock!$J$313:$L$313</definedName>
+    <definedName name="i_core_dvp_types_f1" localSheetId="1">Stock!$J$312:$L$312</definedName>
     <definedName name="i_d_pos">Stock!$I$47</definedName>
     <definedName name="i_dams_user_fvp_date_iu">StructuralSA!$S$73:$V$75</definedName>
     <definedName name="i_density_n0" localSheetId="2">StructuralSA!$L$115</definedName>
@@ -67,13 +67,12 @@
     <definedName name="i_e1_pos">Stock!$I$49</definedName>
     <definedName name="i_enterprises_c0" localSheetId="0">General!$I$55:$J$55</definedName>
     <definedName name="i_feedsupply_itn_max">Stock!$I$72</definedName>
-    <definedName name="i_fixed_dvp_mask_f1">Stock!$J$314:$L$314</definedName>
-    <definedName name="i_fixed_fvp_mask_dams">Stock!$J$312:$L$312</definedName>
+    <definedName name="i_fixed_dvp_mask_f1">Stock!$J$313:$L$313</definedName>
     <definedName name="i_fs_create_number" localSheetId="2">StructuralSA!$M$151</definedName>
     <definedName name="i_fs_create_pkl" localSheetId="2">StructuralSA!$M$150</definedName>
     <definedName name="i_fs_use_number">StructuralSA!$M$149</definedName>
     <definedName name="i_fs_use_pkl" localSheetId="2">StructuralSA!$M$148</definedName>
-    <definedName name="i_fvp_mask_dams">StructuralSA!$N$71:$R$71</definedName>
+    <definedName name="i_fvp_mask_dams">StructuralSA!$K$71:$R$71</definedName>
     <definedName name="i_fvp_mask_offs">StructuralSA!$J$80:$O$80</definedName>
     <definedName name="i_generate_with_t" localSheetId="2">StructuralSA!$P$149</definedName>
     <definedName name="i_history4_req" localSheetId="0">General!$R$79:$R$109</definedName>
@@ -167,7 +166,7 @@
     <definedName name="model_is_MP" localSheetId="2">StructuralSA!$M$45</definedName>
     <definedName name="pastures" localSheetId="0">General!$I$46:$L$46</definedName>
     <definedName name="phase_len" localSheetId="0">General!$I$51</definedName>
-    <definedName name="rdvp_type_r">Stock!$J$318:$L$318</definedName>
+    <definedName name="rdvp_type_r">Stock!$J$317:$L$317</definedName>
     <definedName name="steady_state" localSheetId="2">StructuralSA!$M$42</definedName>
     <definedName name="worker_levels" localSheetId="0">General!$I$42:$K$42</definedName>
     <definedName name="ZA.Gridlines" localSheetId="4">Admin!$L$29</definedName>
@@ -181,7 +180,7 @@
     <definedName name="ZA.WidthCol" localSheetId="4">Admin!$L$26</definedName>
     <definedName name="ZA.ZoomSheet" localSheetId="4">Admin!$O$26</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1079,31 +1078,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H312" authorId="0" shapeId="0" xr:uid="{84E02620-105A-49A0-BB13-0F016867D2B6}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Michael Young (21512438):</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-is the fvp being included in the model?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H313" authorId="0" shapeId="0" xr:uid="{DC35C0C4-2368-49C4-B80C-096DB5F5B286}">
+    <comment ref="H312" authorId="0" shapeId="0" xr:uid="{DC35C0C4-2368-49C4-B80C-096DB5F5B286}">
       <text>
         <r>
           <rPr>
@@ -1127,7 +1102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H314" authorId="0" shapeId="0" xr:uid="{40C7893C-45CA-41EE-B47C-3FDA2D2EA429}">
+    <comment ref="H313" authorId="0" shapeId="0" xr:uid="{40C7893C-45CA-41EE-B47C-3FDA2D2EA429}">
       <text>
         <r>
           <rPr>
@@ -1151,7 +1126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J317" authorId="0" shapeId="0" xr:uid="{E1A71694-3808-49CC-84CF-C00DD1A048B7}">
+    <comment ref="J316" authorId="0" shapeId="0" xr:uid="{E1A71694-3808-49CC-84CF-C00DD1A048B7}">
       <text>
         <r>
           <rPr>
@@ -1175,7 +1150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H318" authorId="0" shapeId="0" xr:uid="{D3E0784A-B894-44EF-B048-4F13C34C87DA}">
+    <comment ref="H317" authorId="0" shapeId="0" xr:uid="{D3E0784A-B894-44EF-B048-4F13C34C87DA}">
       <text>
         <r>
           <rPr>
@@ -1429,7 +1404,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K65" authorId="2" shapeId="0" xr:uid="{7A871372-172C-422B-B562-4E4B218F668C}">
+    <comment ref="J65" authorId="2" shapeId="0" xr:uid="{7A871372-172C-422B-B562-4E4B218F668C}">
       <text>
         <r>
           <rPr>
@@ -2473,7 +2448,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="405">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -5864,12 +5839,12 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
       <xdr:row>311</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>313</xdr:row>
+      <xdr:row>312</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -11098,14 +11073,14 @@
   <sheetPr codeName="Sheet1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB334"/>
+  <dimension ref="A1:AB333"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J138" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="10" topLeftCell="J301" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="J13" sqref="J13:T13"/>
+      <selection pane="bottomRight" activeCell="H314" sqref="H314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
@@ -26142,7 +26117,7 @@
       <c r="A312" s="1"/>
       <c r="B312" s="33"/>
       <c r="C312" s="73">
-        <f>INT($C$31)+3</f>
+        <f t="shared" ref="C312:C319" si="72">INT($C$31)+3</f>
         <v>4</v>
       </c>
       <c r="D312" s="4"/>
@@ -26150,17 +26125,17 @@
       <c r="F312" s="5"/>
       <c r="G312" s="4"/>
       <c r="H312" s="2" t="s">
-        <v>299</v>
+        <v>270</v>
       </c>
       <c r="I312" s="2"/>
-      <c r="J312" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="K312" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="L312" s="31" t="b">
-        <v>1</v>
+      <c r="J312" s="109">
+        <v>0</v>
+      </c>
+      <c r="K312" s="109">
+        <v>1</v>
+      </c>
+      <c r="L312" s="109">
+        <v>2</v>
       </c>
       <c r="M312" s="2"/>
       <c r="N312" s="2"/>
@@ -26183,7 +26158,7 @@
       <c r="A313" s="1"/>
       <c r="B313" s="33"/>
       <c r="C313" s="73">
-        <f t="shared" ref="C313:C320" si="72">INT($C$31)+3</f>
+        <f t="shared" si="72"/>
         <v>4</v>
       </c>
       <c r="D313" s="4"/>
@@ -26191,17 +26166,17 @@
       <c r="F313" s="5"/>
       <c r="G313" s="4"/>
       <c r="H313" s="2" t="s">
-        <v>270</v>
+        <v>300</v>
       </c>
       <c r="I313" s="2"/>
-      <c r="J313" s="109">
-        <v>0</v>
-      </c>
-      <c r="K313" s="109">
-        <v>1</v>
-      </c>
-      <c r="L313" s="109">
-        <v>2</v>
+      <c r="J313" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="K313" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="L313" s="31" t="b">
+        <v>1</v>
       </c>
       <c r="M313" s="2"/>
       <c r="N313" s="2"/>
@@ -26231,19 +26206,11 @@
       <c r="E314" s="5"/>
       <c r="F314" s="5"/>
       <c r="G314" s="4"/>
-      <c r="H314" s="2" t="s">
-        <v>300</v>
-      </c>
+      <c r="H314" s="2"/>
       <c r="I314" s="2"/>
-      <c r="J314" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="K314" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="L314" s="31" t="b">
-        <v>1</v>
-      </c>
+      <c r="J314" s="2"/>
+      <c r="K314" s="2"/>
+      <c r="L314" s="2"/>
       <c r="M314" s="2"/>
       <c r="N314" s="2"/>
       <c r="O314" s="2"/>
@@ -26306,10 +26273,16 @@
       <c r="F316" s="5"/>
       <c r="G316" s="4"/>
       <c r="H316" s="2"/>
-      <c r="I316" s="2"/>
-      <c r="J316" s="2"/>
-      <c r="K316" s="2"/>
-      <c r="L316" s="2"/>
+      <c r="I316" s="122"/>
+      <c r="J316" s="123" t="s">
+        <v>219</v>
+      </c>
+      <c r="K316" s="123" t="s">
+        <v>220</v>
+      </c>
+      <c r="L316" s="123" t="s">
+        <v>221</v>
+      </c>
       <c r="M316" s="2"/>
       <c r="N316" s="2"/>
       <c r="O316" s="2"/>
@@ -26338,16 +26311,21 @@
       <c r="E317" s="5"/>
       <c r="F317" s="5"/>
       <c r="G317" s="4"/>
-      <c r="H317" s="2"/>
+      <c r="H317" s="2" t="s">
+        <v>218</v>
+      </c>
       <c r="I317" s="122"/>
-      <c r="J317" s="123" t="s">
-        <v>219</v>
-      </c>
-      <c r="K317" s="123" t="s">
-        <v>220</v>
-      </c>
-      <c r="L317" s="123" t="s">
-        <v>221</v>
+      <c r="J317" s="31">
+        <f>J312</f>
+        <v>0</v>
+      </c>
+      <c r="K317" s="31">
+        <f>K312</f>
+        <v>1</v>
+      </c>
+      <c r="L317" s="31">
+        <f>L312</f>
+        <v>2</v>
       </c>
       <c r="M317" s="2"/>
       <c r="N317" s="2"/>
@@ -26377,22 +26355,11 @@
       <c r="E318" s="5"/>
       <c r="F318" s="5"/>
       <c r="G318" s="4"/>
-      <c r="H318" s="2" t="s">
-        <v>218</v>
-      </c>
+      <c r="H318" s="2"/>
       <c r="I318" s="122"/>
-      <c r="J318" s="31">
-        <f>J313</f>
-        <v>0</v>
-      </c>
-      <c r="K318" s="31">
-        <f>K313</f>
-        <v>1</v>
-      </c>
-      <c r="L318" s="31">
-        <f>L313</f>
-        <v>2</v>
-      </c>
+      <c r="J318" s="123"/>
+      <c r="K318" s="123"/>
+      <c r="L318" s="123"/>
       <c r="M318" s="2"/>
       <c r="N318" s="2"/>
       <c r="O318" s="2"/>
@@ -26447,7 +26414,7 @@
       <c r="A320" s="1"/>
       <c r="B320" s="33"/>
       <c r="C320" s="73">
-        <f t="shared" si="72"/>
+        <f>INT($C$31)+3</f>
         <v>4</v>
       </c>
       <c r="D320" s="4"/>
@@ -26455,10 +26422,10 @@
       <c r="F320" s="5"/>
       <c r="G320" s="4"/>
       <c r="H320" s="2"/>
-      <c r="I320" s="122"/>
-      <c r="J320" s="123"/>
-      <c r="K320" s="123"/>
-      <c r="L320" s="123"/>
+      <c r="I320" s="2"/>
+      <c r="J320" s="2"/>
+      <c r="K320" s="2"/>
+      <c r="L320" s="2"/>
       <c r="M320" s="2"/>
       <c r="N320" s="2"/>
       <c r="O320" s="2"/>
@@ -26476,171 +26443,171 @@
       <c r="AA320" s="1"/>
       <c r="AB320" s="1"/>
     </row>
-    <row r="321" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:28" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A321" s="1"/>
       <c r="B321" s="33"/>
       <c r="C321" s="73">
-        <f>INT($C$31)+3</f>
-        <v>4</v>
+        <f>INT($C$31)+3.005</f>
+        <v>4.0049999999999999</v>
       </c>
       <c r="D321" s="4"/>
-      <c r="E321" s="5"/>
-      <c r="F321" s="5"/>
+      <c r="E321" s="4"/>
+      <c r="F321" s="4"/>
       <c r="G321" s="4"/>
-      <c r="H321" s="2"/>
-      <c r="I321" s="2"/>
-      <c r="J321" s="2"/>
-      <c r="K321" s="2"/>
-      <c r="L321" s="2"/>
-      <c r="M321" s="2"/>
-      <c r="N321" s="2"/>
-      <c r="O321" s="2"/>
-      <c r="P321" s="2"/>
-      <c r="Q321" s="2"/>
-      <c r="R321" s="2"/>
-      <c r="S321" s="2"/>
-      <c r="T321" s="2"/>
-      <c r="U321" s="2"/>
-      <c r="V321" s="2"/>
-      <c r="W321" s="2"/>
-      <c r="X321" s="4"/>
+      <c r="H321" s="82"/>
+      <c r="I321" s="82"/>
+      <c r="J321" s="82"/>
+      <c r="K321" s="82"/>
+      <c r="L321" s="82"/>
+      <c r="M321" s="82"/>
+      <c r="N321" s="82"/>
+      <c r="O321" s="82"/>
+      <c r="P321" s="82"/>
+      <c r="Q321" s="82"/>
+      <c r="R321" s="82"/>
+      <c r="S321" s="82"/>
+      <c r="T321" s="82"/>
+      <c r="U321" s="82"/>
+      <c r="V321" s="82"/>
+      <c r="W321" s="82"/>
+      <c r="X321" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="Y321" s="16"/>
       <c r="Z321" s="1"/>
       <c r="AA321" s="1"/>
       <c r="AB321" s="1"/>
     </row>
-    <row r="322" spans="1:28" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A322" s="1"/>
       <c r="B322" s="33"/>
       <c r="C322" s="73">
-        <f>INT($C$31)+3.005</f>
-        <v>4.0049999999999999</v>
+        <f>INT($C$31)+2.005</f>
+        <v>3.0049999999999999</v>
       </c>
       <c r="D322" s="4"/>
       <c r="E322" s="4"/>
       <c r="F322" s="4"/>
       <c r="G322" s="4"/>
-      <c r="H322" s="82"/>
-      <c r="I322" s="82"/>
-      <c r="J322" s="82"/>
-      <c r="K322" s="82"/>
-      <c r="L322" s="82"/>
-      <c r="M322" s="82"/>
-      <c r="N322" s="82"/>
-      <c r="O322" s="82"/>
-      <c r="P322" s="82"/>
-      <c r="Q322" s="82"/>
-      <c r="R322" s="82"/>
-      <c r="S322" s="82"/>
-      <c r="T322" s="82"/>
-      <c r="U322" s="82"/>
-      <c r="V322" s="82"/>
-      <c r="W322" s="82"/>
-      <c r="X322" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="H322" s="4"/>
+      <c r="I322" s="4"/>
+      <c r="J322" s="4"/>
+      <c r="K322" s="4"/>
+      <c r="L322" s="4"/>
+      <c r="M322" s="4"/>
+      <c r="N322" s="4"/>
+      <c r="O322" s="4"/>
+      <c r="P322" s="4"/>
+      <c r="Q322" s="4"/>
+      <c r="R322" s="4"/>
+      <c r="S322" s="4"/>
+      <c r="T322" s="4"/>
+      <c r="U322" s="4"/>
+      <c r="V322" s="4"/>
+      <c r="W322" s="4"/>
+      <c r="X322" s="4"/>
       <c r="Y322" s="16"/>
       <c r="Z322" s="1"/>
       <c r="AA322" s="1"/>
       <c r="AB322" s="1"/>
     </row>
-    <row r="323" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A323" s="1"/>
-      <c r="B323" s="33"/>
-      <c r="C323" s="73">
-        <f>INT($C$31)+2.005</f>
-        <v>3.0049999999999999</v>
-      </c>
-      <c r="D323" s="4"/>
-      <c r="E323" s="4"/>
-      <c r="F323" s="4"/>
-      <c r="G323" s="4"/>
-      <c r="H323" s="4"/>
-      <c r="I323" s="4"/>
-      <c r="J323" s="4"/>
-      <c r="K323" s="4"/>
-      <c r="L323" s="4"/>
-      <c r="M323" s="4"/>
-      <c r="N323" s="4"/>
-      <c r="O323" s="4"/>
-      <c r="P323" s="4"/>
-      <c r="Q323" s="4"/>
-      <c r="R323" s="4"/>
-      <c r="S323" s="4"/>
-      <c r="T323" s="4"/>
-      <c r="U323" s="4"/>
-      <c r="V323" s="4"/>
-      <c r="W323" s="4"/>
-      <c r="X323" s="4"/>
-      <c r="Y323" s="16"/>
+      <c r="B323" s="35"/>
+      <c r="C323" s="76">
+        <f>INT($C$31)+1.005</f>
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="D323" s="17"/>
+      <c r="E323" s="17"/>
+      <c r="F323" s="17"/>
+      <c r="G323" s="17"/>
+      <c r="H323" s="17"/>
+      <c r="I323" s="17"/>
+      <c r="J323" s="17"/>
+      <c r="K323" s="17"/>
+      <c r="L323" s="17"/>
+      <c r="M323" s="17"/>
+      <c r="N323" s="17"/>
+      <c r="O323" s="17"/>
+      <c r="P323" s="17"/>
+      <c r="Q323" s="17"/>
+      <c r="R323" s="17"/>
+      <c r="S323" s="17"/>
+      <c r="T323" s="17"/>
+      <c r="U323" s="17"/>
+      <c r="V323" s="17"/>
+      <c r="W323" s="17"/>
+      <c r="X323" s="17"/>
+      <c r="Y323" s="18" t="s">
+        <v>1</v>
+      </c>
       <c r="Z323" s="1"/>
       <c r="AA323" s="1"/>
       <c r="AB323" s="1"/>
     </row>
-    <row r="324" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:28" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A324" s="1"/>
-      <c r="B324" s="35"/>
-      <c r="C324" s="76">
-        <f>INT($C$31)+1.005</f>
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="D324" s="17"/>
-      <c r="E324" s="17"/>
-      <c r="F324" s="17"/>
-      <c r="G324" s="17"/>
-      <c r="H324" s="17"/>
-      <c r="I324" s="17"/>
-      <c r="J324" s="17"/>
-      <c r="K324" s="17"/>
-      <c r="L324" s="17"/>
-      <c r="M324" s="17"/>
-      <c r="N324" s="17"/>
-      <c r="O324" s="17"/>
-      <c r="P324" s="17"/>
-      <c r="Q324" s="17"/>
-      <c r="R324" s="17"/>
-      <c r="S324" s="17"/>
-      <c r="T324" s="17"/>
-      <c r="U324" s="17"/>
-      <c r="V324" s="17"/>
-      <c r="W324" s="17"/>
-      <c r="X324" s="17"/>
-      <c r="Y324" s="18" t="s">
-        <v>1</v>
-      </c>
+      <c r="B324" s="19"/>
+      <c r="C324" s="77">
+        <f>INT($C$31)+0.005</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D324" s="19"/>
+      <c r="E324" s="19"/>
+      <c r="F324" s="19"/>
+      <c r="G324" s="19"/>
+      <c r="H324" s="19"/>
+      <c r="I324" s="19"/>
+      <c r="J324" s="19"/>
+      <c r="K324" s="19"/>
+      <c r="L324" s="19"/>
+      <c r="M324" s="19"/>
+      <c r="N324" s="19"/>
+      <c r="O324" s="19"/>
+      <c r="P324" s="19"/>
+      <c r="Q324" s="19"/>
+      <c r="R324" s="19"/>
+      <c r="S324" s="19"/>
+      <c r="T324" s="19"/>
+      <c r="U324" s="19"/>
+      <c r="V324" s="19"/>
+      <c r="W324" s="19"/>
+      <c r="X324" s="19"/>
+      <c r="Y324" s="19"/>
       <c r="Z324" s="1"/>
       <c r="AA324" s="1"/>
       <c r="AB324" s="1"/>
     </row>
-    <row r="325" spans="1:28" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A325" s="1"/>
-      <c r="B325" s="19"/>
-      <c r="C325" s="77">
-        <f>INT($C$31)+0.005</f>
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="D325" s="19"/>
-      <c r="E325" s="19"/>
-      <c r="F325" s="19"/>
-      <c r="G325" s="19"/>
-      <c r="H325" s="19"/>
-      <c r="I325" s="19"/>
-      <c r="J325" s="19"/>
-      <c r="K325" s="19"/>
-      <c r="L325" s="19"/>
-      <c r="M325" s="19"/>
-      <c r="N325" s="19"/>
-      <c r="O325" s="19"/>
-      <c r="P325" s="19"/>
-      <c r="Q325" s="19"/>
-      <c r="R325" s="19"/>
-      <c r="S325" s="19"/>
-      <c r="T325" s="19"/>
-      <c r="U325" s="19"/>
-      <c r="V325" s="19"/>
-      <c r="W325" s="19"/>
-      <c r="X325" s="19"/>
-      <c r="Y325" s="19"/>
+      <c r="B325" s="1"/>
+      <c r="C325" s="73">
+        <f>INT($C$31)+2</f>
+        <v>3</v>
+      </c>
+      <c r="D325" s="1"/>
+      <c r="E325" s="1"/>
+      <c r="F325" s="1"/>
+      <c r="G325" s="1"/>
+      <c r="H325" s="1"/>
+      <c r="I325" s="1"/>
+      <c r="J325" s="1"/>
+      <c r="K325" s="1"/>
+      <c r="L325" s="1"/>
+      <c r="M325" s="1"/>
+      <c r="N325" s="1"/>
+      <c r="O325" s="1"/>
+      <c r="P325" s="1"/>
+      <c r="Q325" s="1"/>
+      <c r="R325" s="1"/>
+      <c r="S325" s="1"/>
+      <c r="T325" s="1"/>
+      <c r="U325" s="1"/>
+      <c r="V325" s="1"/>
+      <c r="W325" s="1"/>
+      <c r="X325" s="1"/>
+      <c r="Y325" s="1"/>
       <c r="Z325" s="1"/>
       <c r="AA325" s="1"/>
       <c r="AB325" s="1"/>
@@ -26649,7 +26616,7 @@
       <c r="A326" s="1"/>
       <c r="B326" s="1"/>
       <c r="C326" s="73">
-        <f>INT($C$31)+2</f>
+        <f>INT($C$132)+2</f>
         <v>3</v>
       </c>
       <c r="D326" s="1"/>
@@ -26678,13 +26645,10 @@
       <c r="AA326" s="1"/>
       <c r="AB326" s="1"/>
     </row>
-    <row r="327" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A327" s="1"/>
       <c r="B327" s="1"/>
-      <c r="C327" s="73">
-        <f>INT($C$132)+2</f>
-        <v>3</v>
-      </c>
+      <c r="C327" s="66"/>
       <c r="D327" s="1"/>
       <c r="E327" s="1"/>
       <c r="F327" s="1"/>
@@ -26862,37 +26826,7 @@
       <c r="AB332" s="1"/>
     </row>
     <row r="333" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A333" s="1"/>
-      <c r="B333" s="1"/>
-      <c r="C333" s="66"/>
-      <c r="D333" s="1"/>
-      <c r="E333" s="1"/>
-      <c r="F333" s="1"/>
-      <c r="G333" s="1"/>
-      <c r="H333" s="1"/>
-      <c r="I333" s="1"/>
-      <c r="J333" s="1"/>
-      <c r="K333" s="1"/>
-      <c r="L333" s="1"/>
-      <c r="M333" s="1"/>
-      <c r="N333" s="1"/>
-      <c r="O333" s="1"/>
-      <c r="P333" s="1"/>
-      <c r="Q333" s="1"/>
-      <c r="R333" s="1"/>
-      <c r="S333" s="1"/>
-      <c r="T333" s="1"/>
-      <c r="U333" s="1"/>
-      <c r="V333" s="1"/>
-      <c r="W333" s="1"/>
-      <c r="X333" s="1"/>
-      <c r="Y333" s="1"/>
-      <c r="Z333" s="1"/>
-      <c r="AA333" s="1"/>
-      <c r="AB333" s="1"/>
-    </row>
-    <row r="334" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="C334" s="72" t="s">
+      <c r="C333" s="72" t="s">
         <v>4</v>
       </c>
     </row>
@@ -26917,11 +26851,11 @@
   <dimension ref="A1:AB211"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="10" topLeftCell="J86" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="M45" sqref="M45"/>
+      <selection pane="bottomRight" activeCell="S108" sqref="S108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
@@ -29222,9 +29156,15 @@
       <c r="H64" s="29"/>
       <c r="I64" s="29"/>
       <c r="J64" s="29"/>
-      <c r="K64" s="29"/>
-      <c r="L64" s="29"/>
-      <c r="M64" s="156"/>
+      <c r="K64" s="156" t="s">
+        <v>209</v>
+      </c>
+      <c r="L64" s="156" t="s">
+        <v>96</v>
+      </c>
+      <c r="M64" s="156" t="s">
+        <v>210</v>
+      </c>
       <c r="N64" s="156" t="s">
         <v>97</v>
       </c>
@@ -29264,12 +29204,18 @@
       <c r="G65" s="3"/>
       <c r="H65" s="29"/>
       <c r="I65" s="29"/>
-      <c r="J65" s="29"/>
-      <c r="K65" s="29" t="s">
+      <c r="J65" s="29" t="s">
         <v>368</v>
       </c>
-      <c r="L65" s="29"/>
-      <c r="M65" s="156"/>
+      <c r="K65" s="156" t="s">
+        <v>202</v>
+      </c>
+      <c r="L65" s="156" t="s">
+        <v>203</v>
+      </c>
+      <c r="M65" s="156" t="s">
+        <v>204</v>
+      </c>
       <c r="N65" s="156" t="s">
         <v>369</v>
       </c>
@@ -29493,9 +29439,15 @@
       </c>
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
-      <c r="K71" s="2"/>
-      <c r="L71" s="2"/>
-      <c r="M71" s="2"/>
+      <c r="K71" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="L71" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="M71" s="31" t="b">
+        <v>1</v>
+      </c>
       <c r="N71" s="31" t="b">
         <v>0</v>
       </c>
@@ -29582,15 +29534,15 @@
         <v>267</v>
       </c>
       <c r="I73" s="2"/>
-      <c r="J73" s="2"/>
-      <c r="K73" s="211">
+      <c r="J73" s="211">
         <v>43600</v>
       </c>
+      <c r="K73" s="211"/>
       <c r="L73" s="211"/>
       <c r="M73" s="211"/>
       <c r="N73" s="211"/>
       <c r="O73" s="203">
-        <f>$K73+91+126/2</f>
+        <f>$J73+91+126/2</f>
         <v>43754</v>
       </c>
       <c r="P73" s="203">
@@ -29598,11 +29550,11 @@
         <v>43785.5</v>
       </c>
       <c r="Q73" s="203">
-        <f>$K73-150+129</f>
+        <f>$J73-150+129</f>
         <v>43579</v>
       </c>
       <c r="R73" s="203">
-        <f>$K73-150+35</f>
+        <f>$J73-150+35</f>
         <v>43485</v>
       </c>
       <c r="S73" s="204">
@@ -29643,27 +29595,27 @@
         <v>268</v>
       </c>
       <c r="I74" s="2"/>
-      <c r="J74" s="2"/>
-      <c r="K74" s="211">
+      <c r="J74" s="211">
         <v>43634</v>
       </c>
+      <c r="K74" s="211"/>
       <c r="L74" s="211"/>
       <c r="M74" s="211"/>
       <c r="N74" s="211"/>
       <c r="O74" s="203">
-        <f t="shared" ref="O74:O75" si="5">$K74+91+126/2</f>
+        <f>$J74+91+126/2</f>
         <v>43788</v>
       </c>
       <c r="P74" s="203">
-        <f t="shared" ref="P74:P75" si="6">O74+126/4</f>
+        <f t="shared" ref="P74:P75" si="5">O74+126/4</f>
         <v>43819.5</v>
       </c>
       <c r="Q74" s="203">
-        <f>$K74-150+129</f>
+        <f>$J74-150+129</f>
         <v>43613</v>
       </c>
       <c r="R74" s="203">
-        <f t="shared" ref="R74:R75" si="7">$K74-150+35</f>
+        <f>$J74-150+35</f>
         <v>43519</v>
       </c>
       <c r="S74" s="204">
@@ -29704,27 +29656,27 @@
         <v>269</v>
       </c>
       <c r="I75" s="2"/>
-      <c r="J75" s="2"/>
-      <c r="K75" s="211">
+      <c r="J75" s="211">
         <v>43669</v>
       </c>
+      <c r="K75" s="211"/>
       <c r="L75" s="211"/>
       <c r="M75" s="211"/>
       <c r="N75" s="211"/>
       <c r="O75" s="203">
+        <f>$J75+91+126/2</f>
+        <v>43823</v>
+      </c>
+      <c r="P75" s="203">
         <f t="shared" si="5"/>
-        <v>43823</v>
-      </c>
-      <c r="P75" s="203">
-        <f t="shared" si="6"/>
         <v>43854.5</v>
       </c>
       <c r="Q75" s="203">
-        <f>$K75-150+129</f>
+        <f>$J75-150+129</f>
         <v>43648</v>
       </c>
       <c r="R75" s="203">
-        <f t="shared" si="7"/>
+        <f>$J75-150+35</f>
         <v>43554</v>
       </c>
       <c r="S75" s="204">
@@ -30031,11 +29983,11 @@
         <v>13</v>
       </c>
       <c r="Q82" s="204">
-        <f t="shared" ref="Q82:Q84" si="8">MIN(364,INT((N82 - DATE(YEAR(N82),1,1))))</f>
+        <f t="shared" ref="Q82:Q84" si="6">MIN(364,INT((N82 - DATE(YEAR(N82),1,1))))</f>
         <v>134</v>
       </c>
       <c r="R82" s="204">
-        <f t="shared" ref="R82:R84" si="9">MIN(364,INT((O82 - DATE(YEAR(O82),1,1))))</f>
+        <f t="shared" ref="R82:R84" si="7">MIN(364,INT((O82 - DATE(YEAR(O82),1,1))))</f>
         <v>255</v>
       </c>
       <c r="S82" s="2"/>
@@ -30078,11 +30030,11 @@
         <v>43</v>
       </c>
       <c r="Q83" s="204">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>164</v>
       </c>
       <c r="R83" s="204">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>285</v>
       </c>
       <c r="S83" s="2"/>
@@ -30125,11 +30077,11 @@
         <v>74</v>
       </c>
       <c r="Q84" s="204">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>195</v>
       </c>
       <c r="R84" s="204">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>316</v>
       </c>
       <c r="S84" s="2"/>
@@ -31067,7 +31019,7 @@
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
       <c r="M110" s="109">
-        <f>COUNTIF(i_fixed_fvp_mask_dams,TRUE)+COUNTIF(i_fvp_mask_dams,TRUE)</f>
+        <f>COUNTIF(i_fvp_mask_dams,TRUE)</f>
         <v>3</v>
       </c>
       <c r="N110" s="2"/>
@@ -31459,7 +31411,7 @@
       <c r="A119" s="1"/>
       <c r="B119" s="33"/>
       <c r="C119" s="73">
-        <f t="shared" ref="C119:C122" si="10">INT(C$96+3)</f>
+        <f t="shared" ref="C119:C122" si="8">INT(C$96+3)</f>
         <v>4</v>
       </c>
       <c r="D119" s="4"/>
@@ -31508,7 +31460,7 @@
       <c r="A120" s="1"/>
       <c r="B120" s="33"/>
       <c r="C120" s="73">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="D120" s="4"/>
@@ -31557,7 +31509,7 @@
       <c r="A121" s="1"/>
       <c r="B121" s="33"/>
       <c r="C121" s="73">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="D121" s="4"/>
@@ -31606,7 +31558,7 @@
       <c r="A122" s="1"/>
       <c r="B122" s="33"/>
       <c r="C122" s="73">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="D122" s="4"/>
@@ -31823,7 +31775,7 @@
       <c r="A127" s="1"/>
       <c r="B127" s="33"/>
       <c r="C127" s="73">
-        <f t="shared" ref="C127:C130" si="11">INT($C$96)+3</f>
+        <f t="shared" ref="C127:C130" si="9">INT($C$96)+3</f>
         <v>4</v>
       </c>
       <c r="D127" s="4"/>
@@ -31884,7 +31836,7 @@
       <c r="A128" s="1"/>
       <c r="B128" s="33"/>
       <c r="C128" s="73">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="D128" s="4"/>
@@ -31937,7 +31889,7 @@
       <c r="A129" s="1"/>
       <c r="B129" s="33"/>
       <c r="C129" s="73">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="D129" s="4"/>
@@ -31990,7 +31942,7 @@
       <c r="A130" s="1"/>
       <c r="B130" s="33"/>
       <c r="C130" s="73">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="D130" s="4"/>
@@ -33156,7 +33108,7 @@
       <c r="A162" s="1"/>
       <c r="B162" s="33"/>
       <c r="C162" s="73">
-        <f t="shared" ref="C162:C172" si="12">INT(C$140+3)</f>
+        <f t="shared" ref="C162:C172" si="10">INT(C$140+3)</f>
         <v>4</v>
       </c>
       <c r="D162" s="4"/>
@@ -33195,7 +33147,7 @@
       <c r="A163" s="1"/>
       <c r="B163" s="33"/>
       <c r="C163" s="73">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="D163" s="4"/>
@@ -33234,7 +33186,7 @@
       <c r="A164" s="1"/>
       <c r="B164" s="33"/>
       <c r="C164" s="73">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="D164" s="4"/>
@@ -33273,7 +33225,7 @@
       <c r="A165" s="1"/>
       <c r="B165" s="33"/>
       <c r="C165" s="73">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="D165" s="4"/>
@@ -33312,7 +33264,7 @@
       <c r="A166" s="1"/>
       <c r="B166" s="33"/>
       <c r="C166" s="73">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="D166" s="4"/>
@@ -33351,7 +33303,7 @@
       <c r="A167" s="1"/>
       <c r="B167" s="33"/>
       <c r="C167" s="73">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="D167" s="4"/>
@@ -33390,7 +33342,7 @@
       <c r="A168" s="1"/>
       <c r="B168" s="33"/>
       <c r="C168" s="73">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="D168" s="4"/>
@@ -33429,7 +33381,7 @@
       <c r="A169" s="1"/>
       <c r="B169" s="33"/>
       <c r="C169" s="73">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="D169" s="4"/>
@@ -33468,7 +33420,7 @@
       <c r="A170" s="1"/>
       <c r="B170" s="33"/>
       <c r="C170" s="73">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="D170" s="4"/>
@@ -33507,7 +33459,7 @@
       <c r="A171" s="1"/>
       <c r="B171" s="33"/>
       <c r="C171" s="73">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="D171" s="4"/>
@@ -33546,7 +33498,7 @@
       <c r="A172" s="1"/>
       <c r="B172" s="33"/>
       <c r="C172" s="73">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="D172" s="4"/>

</xml_diff>

<commit_message>
Add wbec as a REV trait
</commit_message>
<xml_diff>
--- a/ExcelInputs/Structural.xlsx
+++ b/ExcelInputs/Structural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\ExcelInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839ABBC5-9908-4D9A-8776-F762C98D5054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510AB50B-2BD0-4F74-9464-E561BDB06397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="315" windowWidth="25140" windowHeight="15075" tabRatio="678" activeTab="3" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -92,7 +92,7 @@
     <definedName name="i_lag_organs">Stock!$I$70</definedName>
     <definedName name="i_lag_wool">Stock!$I$69</definedName>
     <definedName name="i_landuse_is_dual" localSheetId="0">General!$Q$79:$Q$109</definedName>
-    <definedName name="i_len_f">StructuralSA!$I$193</definedName>
+    <definedName name="i_len_f">StructuralSA!$I$194</definedName>
     <definedName name="i_len_l">Stock!$M$160</definedName>
     <definedName name="i_len_m">Stock!$L$160</definedName>
     <definedName name="i_len_q" localSheetId="2">StructuralSA!$M$44</definedName>
@@ -121,8 +121,8 @@
     <definedName name="i_nut_spread_n0" localSheetId="2">StructuralSA!$J$115</definedName>
     <definedName name="i_nut_spread_n1" localSheetId="2">StructuralSA!$M$115:$M$122</definedName>
     <definedName name="i_nut_spread_n3" localSheetId="2">StructuralSA!$S$115:$S$122</definedName>
-    <definedName name="i_nv_lower_p6">StructuralSA!$J$196:$S$196</definedName>
-    <definedName name="i_nv_upper_p6">StructuralSA!$J$197:$S$197</definedName>
+    <definedName name="i_nv_lower_p6">StructuralSA!$J$197:$S$197</definedName>
+    <definedName name="i_nv_upper_p6">StructuralSA!$J$198:$S$198</definedName>
     <definedName name="i_offs_sale_method" localSheetId="2">StructuralSA!$R$42</definedName>
     <definedName name="i_offs_sale_opportunities_per_dvp" localSheetId="2">StructuralSA!$R$43</definedName>
     <definedName name="i_offs_user_fvp_date_iu" localSheetId="2">StructuralSA!$P$82:$R$84</definedName>
@@ -131,8 +131,8 @@
     <definedName name="i_progeny_w2_len">StructuralSA!$Q$107</definedName>
     <definedName name="i_r2adjust_inc">StructuralSA!$U$148</definedName>
     <definedName name="i_rev_number" localSheetId="2">StructuralSA!$I$150</definedName>
-    <definedName name="i_rev_trait_name" localSheetId="2">StructuralSA!$H$157:$H$172</definedName>
-    <definedName name="i_rev_trait_scenario" localSheetId="2">StructuralSA!$I$157:$I$172</definedName>
+    <definedName name="i_rev_trait_name" localSheetId="2">StructuralSA!$H$157:$H$173</definedName>
+    <definedName name="i_rev_trait_scenario" localSheetId="2">StructuralSA!$I$157:$I$173</definedName>
     <definedName name="i_rev_update" localSheetId="2">StructuralSA!$I$148</definedName>
     <definedName name="i_sim_periods_year">Stock!$I$62</definedName>
     <definedName name="i_store_cs_rep" localSheetId="3">'Report Settings'!$K$18</definedName>
@@ -2236,7 +2236,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H159" authorId="2" shapeId="0" xr:uid="{A12E8373-CBF7-4301-8BBE-54FB2CD3F999}">
+    <comment ref="H160" authorId="2" shapeId="0" xr:uid="{A12E8373-CBF7-4301-8BBE-54FB2CD3F999}">
       <text>
         <r>
           <rPr>
@@ -2260,7 +2260,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H160" authorId="2" shapeId="0" xr:uid="{ADD99B78-258B-4112-BEFE-ACD7C132C257}">
+    <comment ref="H161" authorId="2" shapeId="0" xr:uid="{ADD99B78-258B-4112-BEFE-ACD7C132C257}">
       <text>
         <r>
           <rPr>
@@ -2284,7 +2284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H161" authorId="2" shapeId="0" xr:uid="{F4A4ECC6-7846-4162-9607-F6E572F33EDF}">
+    <comment ref="H162" authorId="2" shapeId="0" xr:uid="{F4A4ECC6-7846-4162-9607-F6E572F33EDF}">
       <text>
         <r>
           <rPr>
@@ -2308,7 +2308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H164" authorId="2" shapeId="0" xr:uid="{4C2B1933-42FC-4263-B576-C6A05675CBF9}">
+    <comment ref="H163" authorId="2" shapeId="0" xr:uid="{4C2B1933-42FC-4263-B576-C6A05675CBF9}">
       <text>
         <r>
           <rPr>
@@ -2332,7 +2332,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H168" authorId="1" shapeId="0" xr:uid="{658A1575-7B6D-49A0-9205-9DD14E053E41}">
+    <comment ref="H169" authorId="1" shapeId="0" xr:uid="{658A1575-7B6D-49A0-9205-9DD14E053E41}">
       <text>
         <r>
           <rPr>
@@ -2356,7 +2356,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H193" authorId="2" shapeId="0" xr:uid="{B39EFDC6-7ABB-4808-93B1-2819F2755236}">
+    <comment ref="H194" authorId="2" shapeId="0" xr:uid="{B39EFDC6-7ABB-4808-93B1-2819F2755236}">
       <text>
         <r>
           <rPr>
@@ -2380,7 +2380,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H196" authorId="2" shapeId="0" xr:uid="{315CC92D-C01A-4D16-90CA-458397130ECA}">
+    <comment ref="H197" authorId="2" shapeId="0" xr:uid="{315CC92D-C01A-4D16-90CA-458397130ECA}">
       <text>
         <r>
           <rPr>
@@ -2406,7 +2406,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H197" authorId="2" shapeId="0" xr:uid="{24292EB5-78CD-4E29-870F-1743067DEF27}">
+    <comment ref="H198" authorId="2" shapeId="0" xr:uid="{24292EB5-78CD-4E29-870F-1743067DEF27}">
       <text>
         <r>
           <rPr>
@@ -2471,7 +2471,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="408">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -3787,7 +3787,17 @@
     <t>FVP3</t>
   </si>
   <si>
-    <t>28Aug24: Improve commenting on the weaning period wrt user defined periods
+    <t>WBE</t>
+  </si>
+  <si>
+    <t>store wbe profile</t>
+  </si>
+  <si>
+    <t>wbec</t>
+  </si>
+  <si>
+    <t>4Sep24: Added wbec as a REV trait (#16)
+28Aug24: Improve commenting on the weaning period wrt user defined periods
 29May24: Add REV[ebg] dictionary
 23Jan24: Add extra traits for REV (15 in total counting random)
 22Jan24: Change rev_create to rev_update, and rev_trait_inc to rev_trait_scenario
@@ -3812,12 +3822,6 @@
 25Apr21: Moved inputs from Property.xlsx
                    Moved FVP &amp; N inputs from Stock
 1: 1Apr19-Created the version control table</t>
-  </si>
-  <si>
-    <t>WBE</t>
-  </si>
-  <si>
-    <t>store wbe profile</t>
   </si>
 </sst>
 </file>
@@ -26878,14 +26882,14 @@
   <sheetPr codeName="Sheet3">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB211"/>
+  <dimension ref="A1:AB212"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J60" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="9" ySplit="10" topLeftCell="J143" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="J13" sqref="J13:T13"/>
+      <selection pane="bottomRight" activeCell="E158" sqref="E158:E173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -27380,10 +27384,10 @@
         <v>16</v>
       </c>
       <c r="I13" s="126">
-        <v>45532.412615856498</v>
+        <v>45539.395936458299</v>
       </c>
       <c r="J13" s="215" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="K13" s="216"/>
       <c r="L13" s="216"/>
@@ -32289,7 +32293,7 @@
       <c r="A139" s="1"/>
       <c r="B139" s="33"/>
       <c r="C139" s="73">
-        <f>INT(MAX($C$147:$C$175))+1</f>
+        <f>INT(MAX($C$147:$C$176))+1</f>
         <v>5</v>
       </c>
       <c r="D139" s="3"/>
@@ -32982,7 +32986,7 @@
       <c r="A158" s="1"/>
       <c r="B158" s="33"/>
       <c r="C158" s="73">
-        <f>INT($C$140)+3</f>
+        <f t="shared" ref="C158:C173" si="10">INT(C$140+3)</f>
         <v>4</v>
       </c>
       <c r="D158" s="4"/>
@@ -32992,7 +32996,7 @@
       <c r="F158" s="5"/>
       <c r="G158" s="4"/>
       <c r="H158" s="31" t="s">
-        <v>380</v>
+        <v>265</v>
       </c>
       <c r="I158" s="31">
         <v>0</v>
@@ -33031,7 +33035,7 @@
       <c r="F159" s="5"/>
       <c r="G159" s="4"/>
       <c r="H159" s="31" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I159" s="31">
         <v>0</v>
@@ -33060,7 +33064,7 @@
       <c r="A160" s="1"/>
       <c r="B160" s="33"/>
       <c r="C160" s="73">
-        <f>INT(C$140+3)</f>
+        <f>INT($C$140)+3</f>
         <v>4</v>
       </c>
       <c r="D160" s="4"/>
@@ -33070,7 +33074,7 @@
       <c r="F160" s="5"/>
       <c r="G160" s="4"/>
       <c r="H160" s="31" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I160" s="31">
         <v>0</v>
@@ -33109,7 +33113,7 @@
       <c r="F161" s="5"/>
       <c r="G161" s="4"/>
       <c r="H161" s="31" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I161" s="31">
         <v>0</v>
@@ -33138,7 +33142,7 @@
       <c r="A162" s="1"/>
       <c r="B162" s="33"/>
       <c r="C162" s="73">
-        <f t="shared" ref="C162:C172" si="10">INT(C$140+3)</f>
+        <f>INT(C$140+3)</f>
         <v>4</v>
       </c>
       <c r="D162" s="4"/>
@@ -33148,7 +33152,7 @@
       <c r="F162" s="5"/>
       <c r="G162" s="4"/>
       <c r="H162" s="31" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I162" s="31">
         <v>0</v>
@@ -33187,7 +33191,7 @@
       <c r="F163" s="5"/>
       <c r="G163" s="4"/>
       <c r="H163" s="31" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="I163" s="31">
         <v>0</v>
@@ -33226,7 +33230,7 @@
       <c r="F164" s="5"/>
       <c r="G164" s="4"/>
       <c r="H164" s="31" t="s">
-        <v>390</v>
+        <v>406</v>
       </c>
       <c r="I164" s="31">
         <v>0</v>
@@ -33265,7 +33269,7 @@
       <c r="F165" s="5"/>
       <c r="G165" s="4"/>
       <c r="H165" s="31" t="s">
-        <v>265</v>
+        <v>384</v>
       </c>
       <c r="I165" s="31">
         <v>0</v>
@@ -33304,7 +33308,7 @@
       <c r="F166" s="5"/>
       <c r="G166" s="4"/>
       <c r="H166" s="31" t="s">
-        <v>260</v>
+        <v>385</v>
       </c>
       <c r="I166" s="31">
         <v>0</v>
@@ -33343,7 +33347,7 @@
       <c r="F167" s="5"/>
       <c r="G167" s="4"/>
       <c r="H167" s="31" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I167" s="31">
         <v>0</v>
@@ -33382,7 +33386,7 @@
       <c r="F168" s="5"/>
       <c r="G168" s="4"/>
       <c r="H168" s="31" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I168" s="31">
         <v>0</v>
@@ -33421,7 +33425,7 @@
       <c r="F169" s="5"/>
       <c r="G169" s="4"/>
       <c r="H169" s="31" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I169" s="31">
         <v>0</v>
@@ -33460,7 +33464,7 @@
       <c r="F170" s="5"/>
       <c r="G170" s="4"/>
       <c r="H170" s="31" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="I170" s="31">
         <v>0</v>
@@ -33499,7 +33503,7 @@
       <c r="F171" s="5"/>
       <c r="G171" s="4"/>
       <c r="H171" s="31" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I171" s="31">
         <v>0</v>
@@ -33538,7 +33542,7 @@
       <c r="F172" s="5"/>
       <c r="G172" s="4"/>
       <c r="H172" s="31" t="s">
-        <v>379</v>
+        <v>259</v>
       </c>
       <c r="I172" s="31">
         <v>0</v>
@@ -33567,15 +33571,21 @@
       <c r="A173" s="1"/>
       <c r="B173" s="33"/>
       <c r="C173" s="73">
-        <f>INT(C$140+3)</f>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="D173" s="4"/>
-      <c r="E173" s="5"/>
+      <c r="E173" s="5">
+        <v>16</v>
+      </c>
       <c r="F173" s="5"/>
       <c r="G173" s="4"/>
-      <c r="H173" s="148"/>
-      <c r="I173" s="148"/>
+      <c r="H173" s="31" t="s">
+        <v>379</v>
+      </c>
+      <c r="I173" s="31">
+        <v>0</v>
+      </c>
       <c r="J173" s="148"/>
       <c r="K173" s="148"/>
       <c r="L173" s="148"/>
@@ -33629,47 +33639,45 @@
       <c r="AA174" s="1"/>
       <c r="AB174" s="1"/>
     </row>
-    <row r="175" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
       <c r="B175" s="33"/>
       <c r="C175" s="73">
-        <f>INT($C$140)+3.005</f>
-        <v>4.0049999999999999</v>
+        <f>INT(C$140+3)</f>
+        <v>4</v>
       </c>
       <c r="D175" s="4"/>
-      <c r="E175" s="4"/>
-      <c r="F175" s="4"/>
+      <c r="E175" s="5"/>
+      <c r="F175" s="5"/>
       <c r="G175" s="4"/>
-      <c r="H175" s="4"/>
-      <c r="I175" s="4"/>
-      <c r="J175" s="4"/>
-      <c r="K175" s="4"/>
-      <c r="L175" s="4"/>
-      <c r="M175" s="4"/>
-      <c r="N175" s="4"/>
-      <c r="O175" s="4"/>
-      <c r="P175" s="4"/>
-      <c r="Q175" s="4"/>
-      <c r="R175" s="4"/>
-      <c r="S175" s="4"/>
-      <c r="T175" s="4"/>
-      <c r="U175" s="4"/>
-      <c r="V175" s="4"/>
-      <c r="W175" s="4"/>
-      <c r="X175" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="H175" s="148"/>
+      <c r="I175" s="148"/>
+      <c r="J175" s="148"/>
+      <c r="K175" s="148"/>
+      <c r="L175" s="148"/>
+      <c r="M175" s="148"/>
+      <c r="N175" s="148"/>
+      <c r="O175" s="148"/>
+      <c r="P175" s="148"/>
+      <c r="Q175" s="148"/>
+      <c r="R175" s="148"/>
+      <c r="S175" s="2"/>
+      <c r="T175" s="2"/>
+      <c r="U175" s="2"/>
+      <c r="V175" s="2"/>
+      <c r="W175" s="2"/>
+      <c r="X175" s="4"/>
       <c r="Y175" s="16"/>
       <c r="Z175" s="1"/>
       <c r="AA175" s="1"/>
       <c r="AB175" s="1"/>
     </row>
-    <row r="176" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="B176" s="33"/>
       <c r="C176" s="73">
-        <f>INT($C$140)+2.005</f>
-        <v>3.0049999999999999</v>
+        <f>INT($C$140)+3.005</f>
+        <v>4.0049999999999999</v>
       </c>
       <c r="D176" s="4"/>
       <c r="E176" s="4"/>
@@ -33691,109 +33699,111 @@
       <c r="U176" s="4"/>
       <c r="V176" s="4"/>
       <c r="W176" s="4"/>
-      <c r="X176" s="4"/>
+      <c r="X176" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="Y176" s="16"/>
       <c r="Z176" s="1"/>
       <c r="AA176" s="1"/>
       <c r="AB176" s="1"/>
     </row>
-    <row r="177" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
-      <c r="B177" s="35"/>
-      <c r="C177" s="76">
-        <f>INT($C$140)+1.005</f>
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="D177" s="17"/>
-      <c r="E177" s="17"/>
-      <c r="F177" s="17"/>
-      <c r="G177" s="17"/>
-      <c r="H177" s="17"/>
-      <c r="I177" s="17"/>
-      <c r="J177" s="17"/>
-      <c r="K177" s="17"/>
-      <c r="L177" s="17"/>
-      <c r="M177" s="17"/>
-      <c r="N177" s="17"/>
-      <c r="O177" s="17"/>
-      <c r="P177" s="17"/>
-      <c r="Q177" s="17"/>
-      <c r="R177" s="17"/>
-      <c r="S177" s="17"/>
-      <c r="T177" s="17"/>
-      <c r="U177" s="17"/>
-      <c r="V177" s="17"/>
-      <c r="W177" s="17"/>
-      <c r="X177" s="17"/>
-      <c r="Y177" s="18" t="s">
-        <v>1</v>
-      </c>
+      <c r="B177" s="33"/>
+      <c r="C177" s="73">
+        <f>INT($C$140)+2.005</f>
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="D177" s="4"/>
+      <c r="E177" s="4"/>
+      <c r="F177" s="4"/>
+      <c r="G177" s="4"/>
+      <c r="H177" s="4"/>
+      <c r="I177" s="4"/>
+      <c r="J177" s="4"/>
+      <c r="K177" s="4"/>
+      <c r="L177" s="4"/>
+      <c r="M177" s="4"/>
+      <c r="N177" s="4"/>
+      <c r="O177" s="4"/>
+      <c r="P177" s="4"/>
+      <c r="Q177" s="4"/>
+      <c r="R177" s="4"/>
+      <c r="S177" s="4"/>
+      <c r="T177" s="4"/>
+      <c r="U177" s="4"/>
+      <c r="V177" s="4"/>
+      <c r="W177" s="4"/>
+      <c r="X177" s="4"/>
+      <c r="Y177" s="16"/>
       <c r="Z177" s="1"/>
       <c r="AA177" s="1"/>
       <c r="AB177" s="1"/>
     </row>
-    <row r="178" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
-      <c r="B178" s="19"/>
-      <c r="C178" s="77">
-        <f>INT($C$140)+0.005</f>
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="D178" s="19"/>
-      <c r="E178" s="19"/>
-      <c r="F178" s="19"/>
-      <c r="G178" s="19"/>
-      <c r="H178" s="19"/>
-      <c r="I178" s="19"/>
-      <c r="J178" s="19"/>
-      <c r="K178" s="19"/>
-      <c r="L178" s="19"/>
-      <c r="M178" s="19"/>
-      <c r="N178" s="19"/>
-      <c r="O178" s="19"/>
-      <c r="P178" s="19"/>
-      <c r="Q178" s="19"/>
-      <c r="R178" s="19"/>
-      <c r="S178" s="19"/>
-      <c r="T178" s="19"/>
-      <c r="U178" s="19"/>
-      <c r="V178" s="19"/>
-      <c r="W178" s="19"/>
-      <c r="X178" s="19"/>
-      <c r="Y178" s="19"/>
+      <c r="B178" s="35"/>
+      <c r="C178" s="76">
+        <f>INT($C$140)+1.005</f>
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="D178" s="17"/>
+      <c r="E178" s="17"/>
+      <c r="F178" s="17"/>
+      <c r="G178" s="17"/>
+      <c r="H178" s="17"/>
+      <c r="I178" s="17"/>
+      <c r="J178" s="17"/>
+      <c r="K178" s="17"/>
+      <c r="L178" s="17"/>
+      <c r="M178" s="17"/>
+      <c r="N178" s="17"/>
+      <c r="O178" s="17"/>
+      <c r="P178" s="17"/>
+      <c r="Q178" s="17"/>
+      <c r="R178" s="17"/>
+      <c r="S178" s="17"/>
+      <c r="T178" s="17"/>
+      <c r="U178" s="17"/>
+      <c r="V178" s="17"/>
+      <c r="W178" s="17"/>
+      <c r="X178" s="17"/>
+      <c r="Y178" s="18" t="s">
+        <v>1</v>
+      </c>
       <c r="Z178" s="1"/>
       <c r="AA178" s="1"/>
       <c r="AB178" s="1"/>
     </row>
-    <row r="179" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
-      <c r="B179" s="1"/>
-      <c r="C179" s="73">
-        <f>INT($C$140)+2</f>
-        <v>3</v>
-      </c>
-      <c r="D179" s="1"/>
-      <c r="E179" s="1"/>
-      <c r="F179" s="1"/>
-      <c r="G179" s="1"/>
-      <c r="H179" s="1"/>
-      <c r="I179" s="1"/>
-      <c r="J179" s="1"/>
-      <c r="K179" s="1"/>
-      <c r="L179" s="1"/>
-      <c r="M179" s="1"/>
-      <c r="N179" s="1"/>
-      <c r="O179" s="1"/>
-      <c r="P179" s="1"/>
-      <c r="Q179" s="1"/>
-      <c r="R179" s="1"/>
-      <c r="S179" s="1"/>
-      <c r="T179" s="1"/>
-      <c r="U179" s="1"/>
-      <c r="V179" s="1"/>
-      <c r="W179" s="1"/>
-      <c r="X179" s="1"/>
-      <c r="Y179" s="1"/>
+      <c r="B179" s="19"/>
+      <c r="C179" s="77">
+        <f>INT($C$140)+0.005</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D179" s="19"/>
+      <c r="E179" s="19"/>
+      <c r="F179" s="19"/>
+      <c r="G179" s="19"/>
+      <c r="H179" s="19"/>
+      <c r="I179" s="19"/>
+      <c r="J179" s="19"/>
+      <c r="K179" s="19"/>
+      <c r="L179" s="19"/>
+      <c r="M179" s="19"/>
+      <c r="N179" s="19"/>
+      <c r="O179" s="19"/>
+      <c r="P179" s="19"/>
+      <c r="Q179" s="19"/>
+      <c r="R179" s="19"/>
+      <c r="S179" s="19"/>
+      <c r="T179" s="19"/>
+      <c r="U179" s="19"/>
+      <c r="V179" s="19"/>
+      <c r="W179" s="19"/>
+      <c r="X179" s="19"/>
+      <c r="Y179" s="19"/>
       <c r="Z179" s="1"/>
       <c r="AA179" s="1"/>
       <c r="AB179" s="1"/>
@@ -33802,7 +33812,7 @@
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="73">
-        <f>INT($C$184)+2</f>
+        <f>INT($C$140)+2</f>
         <v>3</v>
       </c>
       <c r="D180" s="1"/>
@@ -33831,245 +33841,243 @@
       <c r="AA180" s="1"/>
       <c r="AB180" s="1"/>
     </row>
-    <row r="181" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
-      <c r="B181" s="20"/>
-      <c r="C181" s="74">
-        <f>INT($C$184)+0.005</f>
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="D181" s="20"/>
-      <c r="E181" s="20"/>
-      <c r="F181" s="20"/>
-      <c r="G181" s="20"/>
-      <c r="H181" s="20"/>
-      <c r="I181" s="20"/>
-      <c r="J181" s="20"/>
-      <c r="K181" s="20"/>
-      <c r="L181" s="20"/>
-      <c r="M181" s="20"/>
-      <c r="N181" s="20"/>
-      <c r="O181" s="20"/>
-      <c r="P181" s="20"/>
-      <c r="Q181" s="20"/>
-      <c r="R181" s="20"/>
-      <c r="S181" s="20"/>
-      <c r="T181" s="20"/>
-      <c r="U181" s="20"/>
-      <c r="V181" s="20"/>
-      <c r="W181" s="20"/>
-      <c r="X181" s="20"/>
-      <c r="Y181" s="20"/>
+      <c r="B181" s="1"/>
+      <c r="C181" s="73">
+        <f>INT($C$185)+2</f>
+        <v>3</v>
+      </c>
+      <c r="D181" s="1"/>
+      <c r="E181" s="1"/>
+      <c r="F181" s="1"/>
+      <c r="G181" s="1"/>
+      <c r="H181" s="1"/>
+      <c r="I181" s="1"/>
+      <c r="J181" s="1"/>
+      <c r="K181" s="1"/>
+      <c r="L181" s="1"/>
+      <c r="M181" s="1"/>
+      <c r="N181" s="1"/>
+      <c r="O181" s="1"/>
+      <c r="P181" s="1"/>
+      <c r="Q181" s="1"/>
+      <c r="R181" s="1"/>
+      <c r="S181" s="1"/>
+      <c r="T181" s="1"/>
+      <c r="U181" s="1"/>
+      <c r="V181" s="1"/>
+      <c r="W181" s="1"/>
+      <c r="X181" s="1"/>
+      <c r="Y181" s="1"/>
       <c r="Z181" s="1"/>
       <c r="AA181" s="1"/>
       <c r="AB181" s="1"/>
     </row>
-    <row r="182" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="1"/>
-      <c r="B182" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="C182" s="75">
-        <f>INT($C$184)+1.005</f>
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="D182" s="14"/>
-      <c r="E182" s="14"/>
-      <c r="F182" s="14"/>
-      <c r="G182" s="14"/>
-      <c r="H182" s="14"/>
-      <c r="I182" s="14"/>
-      <c r="J182" s="14"/>
-      <c r="K182" s="14"/>
-      <c r="L182" s="14"/>
-      <c r="M182" s="14"/>
-      <c r="N182" s="14"/>
-      <c r="O182" s="14"/>
-      <c r="P182" s="14"/>
-      <c r="Q182" s="14"/>
-      <c r="R182" s="14"/>
-      <c r="S182" s="14"/>
-      <c r="T182" s="14"/>
-      <c r="U182" s="14"/>
-      <c r="V182" s="14"/>
-      <c r="W182" s="14"/>
-      <c r="X182" s="14"/>
-      <c r="Y182" s="15"/>
+      <c r="B182" s="20"/>
+      <c r="C182" s="74">
+        <f>INT($C$185)+0.005</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D182" s="20"/>
+      <c r="E182" s="20"/>
+      <c r="F182" s="20"/>
+      <c r="G182" s="20"/>
+      <c r="H182" s="20"/>
+      <c r="I182" s="20"/>
+      <c r="J182" s="20"/>
+      <c r="K182" s="20"/>
+      <c r="L182" s="20"/>
+      <c r="M182" s="20"/>
+      <c r="N182" s="20"/>
+      <c r="O182" s="20"/>
+      <c r="P182" s="20"/>
+      <c r="Q182" s="20"/>
+      <c r="R182" s="20"/>
+      <c r="S182" s="20"/>
+      <c r="T182" s="20"/>
+      <c r="U182" s="20"/>
+      <c r="V182" s="20"/>
+      <c r="W182" s="20"/>
+      <c r="X182" s="20"/>
+      <c r="Y182" s="20"/>
       <c r="Z182" s="1"/>
       <c r="AA182" s="1"/>
       <c r="AB182" s="1"/>
     </row>
-    <row r="183" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
-      <c r="B183" s="33"/>
-      <c r="C183" s="73">
-        <f>INT(MAX($C$192:$C$200))+1</f>
-        <v>5</v>
-      </c>
-      <c r="D183" s="3"/>
-      <c r="E183" s="3"/>
-      <c r="F183" s="3"/>
-      <c r="G183" s="3"/>
-      <c r="H183" s="27"/>
-      <c r="I183" s="27"/>
-      <c r="J183" s="27"/>
-      <c r="K183" s="27"/>
-      <c r="L183" s="27"/>
-      <c r="M183" s="27"/>
-      <c r="N183" s="27"/>
-      <c r="O183" s="27"/>
-      <c r="P183" s="27"/>
-      <c r="Q183" s="27"/>
-      <c r="R183" s="27"/>
-      <c r="S183" s="27"/>
-      <c r="T183" s="27"/>
-      <c r="U183" s="27"/>
-      <c r="V183" s="27"/>
-      <c r="W183" s="27"/>
-      <c r="X183" s="3"/>
-      <c r="Y183" s="16"/>
+      <c r="B183" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C183" s="75">
+        <f>INT($C$185)+1.005</f>
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="D183" s="14"/>
+      <c r="E183" s="14"/>
+      <c r="F183" s="14"/>
+      <c r="G183" s="14"/>
+      <c r="H183" s="14"/>
+      <c r="I183" s="14"/>
+      <c r="J183" s="14"/>
+      <c r="K183" s="14"/>
+      <c r="L183" s="14"/>
+      <c r="M183" s="14"/>
+      <c r="N183" s="14"/>
+      <c r="O183" s="14"/>
+      <c r="P183" s="14"/>
+      <c r="Q183" s="14"/>
+      <c r="R183" s="14"/>
+      <c r="S183" s="14"/>
+      <c r="T183" s="14"/>
+      <c r="U183" s="14"/>
+      <c r="V183" s="14"/>
+      <c r="W183" s="14"/>
+      <c r="X183" s="14"/>
+      <c r="Y183" s="15"/>
       <c r="Z183" s="1"/>
       <c r="AA183" s="1"/>
       <c r="AB183" s="1"/>
     </row>
-    <row r="184" spans="1:28" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
       <c r="B184" s="33"/>
       <c r="C184" s="73">
-        <v>1.02</v>
-      </c>
-      <c r="D184" s="21"/>
-      <c r="E184" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="F184" s="25"/>
-      <c r="G184" s="12"/>
-      <c r="H184" s="147" t="str">
-        <f>COUNTIFS($B$1:$B184, "«")&amp;" Feed Pool definitions"</f>
-        <v>6 Feed Pool definitions</v>
-      </c>
-      <c r="I184" s="6"/>
-      <c r="J184" s="6"/>
-      <c r="K184" s="6"/>
-      <c r="L184" s="6"/>
-      <c r="M184" s="6"/>
-      <c r="N184" s="6"/>
-      <c r="O184" s="6"/>
-      <c r="P184" s="6"/>
-      <c r="Q184" s="6"/>
-      <c r="R184" s="6"/>
-      <c r="S184" s="6"/>
-      <c r="T184" s="6"/>
-      <c r="U184" s="6"/>
-      <c r="V184" s="6"/>
-      <c r="W184" s="6"/>
-      <c r="X184" s="10"/>
+        <f>INT(MAX($C$193:$C$201))+1</f>
+        <v>5</v>
+      </c>
+      <c r="D184" s="3"/>
+      <c r="E184" s="3"/>
+      <c r="F184" s="3"/>
+      <c r="G184" s="3"/>
+      <c r="H184" s="27"/>
+      <c r="I184" s="27"/>
+      <c r="J184" s="27"/>
+      <c r="K184" s="27"/>
+      <c r="L184" s="27"/>
+      <c r="M184" s="27"/>
+      <c r="N184" s="27"/>
+      <c r="O184" s="27"/>
+      <c r="P184" s="27"/>
+      <c r="Q184" s="27"/>
+      <c r="R184" s="27"/>
+      <c r="S184" s="27"/>
+      <c r="T184" s="27"/>
+      <c r="U184" s="27"/>
+      <c r="V184" s="27"/>
+      <c r="W184" s="27"/>
+      <c r="X184" s="3"/>
       <c r="Y184" s="16"/>
       <c r="Z184" s="1"/>
       <c r="AA184" s="1"/>
       <c r="AB184" s="1"/>
     </row>
-    <row r="185" spans="1:28" ht="18.75" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:28" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="B185" s="33"/>
       <c r="C185" s="73">
-        <f>INT($C$184)+1.02</f>
-        <v>2.02</v>
+        <v>1.02</v>
       </c>
       <c r="D185" s="21"/>
       <c r="E185" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F185" s="28">
-        <v>1</v>
-      </c>
-      <c r="G185" s="13"/>
-      <c r="H185" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="I185" s="7"/>
-      <c r="J185" s="7"/>
-      <c r="K185" s="7"/>
-      <c r="L185" s="7"/>
-      <c r="M185" s="7"/>
-      <c r="N185" s="7"/>
-      <c r="O185" s="7"/>
-      <c r="P185" s="7"/>
-      <c r="Q185" s="7"/>
-      <c r="R185" s="7"/>
-      <c r="S185" s="7"/>
-      <c r="T185" s="7"/>
-      <c r="U185" s="7"/>
-      <c r="V185" s="7"/>
-      <c r="W185" s="7"/>
-      <c r="X185" s="11"/>
+        <v>6</v>
+      </c>
+      <c r="F185" s="25"/>
+      <c r="G185" s="12"/>
+      <c r="H185" s="147" t="str">
+        <f>COUNTIFS($B$1:$B185, "«")&amp;" Feed Pool definitions"</f>
+        <v>6 Feed Pool definitions</v>
+      </c>
+      <c r="I185" s="6"/>
+      <c r="J185" s="6"/>
+      <c r="K185" s="6"/>
+      <c r="L185" s="6"/>
+      <c r="M185" s="6"/>
+      <c r="N185" s="6"/>
+      <c r="O185" s="6"/>
+      <c r="P185" s="6"/>
+      <c r="Q185" s="6"/>
+      <c r="R185" s="6"/>
+      <c r="S185" s="6"/>
+      <c r="T185" s="6"/>
+      <c r="U185" s="6"/>
+      <c r="V185" s="6"/>
+      <c r="W185" s="6"/>
+      <c r="X185" s="10"/>
       <c r="Y185" s="16"/>
       <c r="Z185" s="1"/>
       <c r="AA185" s="1"/>
       <c r="AB185" s="1"/>
     </row>
-    <row r="186" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:28" ht="18.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
       <c r="B186" s="33"/>
       <c r="C186" s="73">
-        <f>INT($C$184)+2.005</f>
-        <v>3.0049999999999999</v>
-      </c>
-      <c r="D186" s="3"/>
-      <c r="E186" s="3"/>
-      <c r="F186" s="3"/>
-      <c r="G186" s="3"/>
-      <c r="H186" s="3"/>
-      <c r="I186" s="3"/>
-      <c r="J186" s="3"/>
-      <c r="K186" s="3"/>
-      <c r="L186" s="3"/>
-      <c r="M186" s="3"/>
-      <c r="N186" s="3"/>
-      <c r="O186" s="3"/>
-      <c r="P186" s="3"/>
-      <c r="Q186" s="3"/>
-      <c r="R186" s="3"/>
-      <c r="S186" s="3"/>
-      <c r="T186" s="3"/>
-      <c r="U186" s="3"/>
-      <c r="V186" s="3"/>
-      <c r="W186" s="3"/>
-      <c r="X186" s="3"/>
+        <f>INT($C$185)+1.02</f>
+        <v>2.02</v>
+      </c>
+      <c r="D186" s="21"/>
+      <c r="E186" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F186" s="28">
+        <v>1</v>
+      </c>
+      <c r="G186" s="13"/>
+      <c r="H186" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="I186" s="7"/>
+      <c r="J186" s="7"/>
+      <c r="K186" s="7"/>
+      <c r="L186" s="7"/>
+      <c r="M186" s="7"/>
+      <c r="N186" s="7"/>
+      <c r="O186" s="7"/>
+      <c r="P186" s="7"/>
+      <c r="Q186" s="7"/>
+      <c r="R186" s="7"/>
+      <c r="S186" s="7"/>
+      <c r="T186" s="7"/>
+      <c r="U186" s="7"/>
+      <c r="V186" s="7"/>
+      <c r="W186" s="7"/>
+      <c r="X186" s="11"/>
       <c r="Y186" s="16"/>
       <c r="Z186" s="1"/>
       <c r="AA186" s="1"/>
       <c r="AB186" s="1"/>
     </row>
-    <row r="187" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
       <c r="B187" s="33"/>
       <c r="C187" s="73">
-        <f>INT($C$184)+2</f>
-        <v>3</v>
+        <f>INT($C$185)+2.005</f>
+        <v>3.0049999999999999</v>
       </c>
       <c r="D187" s="3"/>
-      <c r="E187" s="5"/>
-      <c r="F187" s="5"/>
+      <c r="E187" s="3"/>
+      <c r="F187" s="3"/>
       <c r="G187" s="3"/>
-      <c r="H187" s="29"/>
-      <c r="I187" s="29"/>
-      <c r="J187" s="65" t="s">
-        <v>293</v>
-      </c>
-      <c r="K187" s="65"/>
-      <c r="L187" s="65"/>
-      <c r="M187" s="65"/>
-      <c r="N187" s="65"/>
-      <c r="O187" s="65"/>
-      <c r="P187" s="65"/>
-      <c r="Q187" s="65"/>
-      <c r="R187" s="65"/>
-      <c r="S187" s="65"/>
-      <c r="T187" s="29"/>
-      <c r="U187" s="29"/>
-      <c r="V187" s="29"/>
-      <c r="W187" s="29"/>
+      <c r="H187" s="3"/>
+      <c r="I187" s="3"/>
+      <c r="J187" s="3"/>
+      <c r="K187" s="3"/>
+      <c r="L187" s="3"/>
+      <c r="M187" s="3"/>
+      <c r="N187" s="3"/>
+      <c r="O187" s="3"/>
+      <c r="P187" s="3"/>
+      <c r="Q187" s="3"/>
+      <c r="R187" s="3"/>
+      <c r="S187" s="3"/>
+      <c r="T187" s="3"/>
+      <c r="U187" s="3"/>
+      <c r="V187" s="3"/>
+      <c r="W187" s="3"/>
       <c r="X187" s="3"/>
       <c r="Y187" s="16"/>
       <c r="Z187" s="1"/>
@@ -34080,7 +34088,7 @@
       <c r="A188" s="1"/>
       <c r="B188" s="33"/>
       <c r="C188" s="73">
-        <f>INT($C$184)+2</f>
+        <f>INT($C$185)+2</f>
         <v>3</v>
       </c>
       <c r="D188" s="3"/>
@@ -34089,36 +34097,18 @@
       <c r="G188" s="3"/>
       <c r="H188" s="29"/>
       <c r="I188" s="29"/>
-      <c r="J188" s="29">
-        <v>0</v>
-      </c>
-      <c r="K188" s="29">
-        <v>1</v>
-      </c>
-      <c r="L188" s="29">
-        <v>2</v>
-      </c>
-      <c r="M188" s="29">
-        <v>3</v>
-      </c>
-      <c r="N188" s="29">
-        <v>4</v>
-      </c>
-      <c r="O188" s="29">
-        <v>5</v>
-      </c>
-      <c r="P188" s="29">
-        <v>6</v>
-      </c>
-      <c r="Q188" s="29">
-        <v>7</v>
-      </c>
-      <c r="R188" s="29">
-        <v>8</v>
-      </c>
-      <c r="S188" s="29">
-        <v>9</v>
-      </c>
+      <c r="J188" s="65" t="s">
+        <v>293</v>
+      </c>
+      <c r="K188" s="65"/>
+      <c r="L188" s="65"/>
+      <c r="M188" s="65"/>
+      <c r="N188" s="65"/>
+      <c r="O188" s="65"/>
+      <c r="P188" s="65"/>
+      <c r="Q188" s="65"/>
+      <c r="R188" s="65"/>
+      <c r="S188" s="65"/>
       <c r="T188" s="29"/>
       <c r="U188" s="29"/>
       <c r="V188" s="29"/>
@@ -34129,31 +34119,49 @@
       <c r="AA188" s="1"/>
       <c r="AB188" s="1"/>
     </row>
-    <row r="189" spans="1:28" ht="9.75" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
-      <c r="B189" s="33" t="s">
-        <v>20</v>
-      </c>
+      <c r="B189" s="33"/>
       <c r="C189" s="73">
-        <f>INT($C$184)+2.01</f>
-        <v>3.01</v>
+        <f>INT($C$185)+2</f>
+        <v>3</v>
       </c>
       <c r="D189" s="3"/>
-      <c r="E189" s="3"/>
-      <c r="F189" s="3"/>
+      <c r="E189" s="5"/>
+      <c r="F189" s="5"/>
       <c r="G189" s="3"/>
       <c r="H189" s="29"/>
       <c r="I189" s="29"/>
-      <c r="J189" s="29"/>
-      <c r="K189" s="29"/>
-      <c r="L189" s="29"/>
-      <c r="M189" s="29"/>
-      <c r="N189" s="29"/>
-      <c r="O189" s="29"/>
-      <c r="P189" s="29"/>
-      <c r="Q189" s="29"/>
-      <c r="R189" s="29"/>
-      <c r="S189" s="29"/>
+      <c r="J189" s="29">
+        <v>0</v>
+      </c>
+      <c r="K189" s="29">
+        <v>1</v>
+      </c>
+      <c r="L189" s="29">
+        <v>2</v>
+      </c>
+      <c r="M189" s="29">
+        <v>3</v>
+      </c>
+      <c r="N189" s="29">
+        <v>4</v>
+      </c>
+      <c r="O189" s="29">
+        <v>5</v>
+      </c>
+      <c r="P189" s="29">
+        <v>6</v>
+      </c>
+      <c r="Q189" s="29">
+        <v>7</v>
+      </c>
+      <c r="R189" s="29">
+        <v>8</v>
+      </c>
+      <c r="S189" s="29">
+        <v>9</v>
+      </c>
       <c r="T189" s="29"/>
       <c r="U189" s="29"/>
       <c r="V189" s="29"/>
@@ -34164,34 +34172,36 @@
       <c r="AA189" s="1"/>
       <c r="AB189" s="1"/>
     </row>
-    <row r="190" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:28" ht="9.75" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
-      <c r="B190" s="33"/>
+      <c r="B190" s="33" t="s">
+        <v>20</v>
+      </c>
       <c r="C190" s="73">
-        <f>C$183</f>
-        <v>5</v>
-      </c>
-      <c r="D190" s="4"/>
-      <c r="E190" s="5"/>
-      <c r="F190" s="5"/>
-      <c r="G190" s="4"/>
-      <c r="H190" s="5"/>
-      <c r="I190" s="5"/>
-      <c r="J190" s="5"/>
-      <c r="K190" s="5"/>
-      <c r="L190" s="5"/>
-      <c r="M190" s="5"/>
-      <c r="N190" s="5"/>
-      <c r="O190" s="5"/>
-      <c r="P190" s="5"/>
-      <c r="Q190" s="5"/>
-      <c r="R190" s="5"/>
-      <c r="S190" s="5"/>
-      <c r="T190" s="5"/>
-      <c r="U190" s="5"/>
-      <c r="V190" s="5"/>
-      <c r="W190" s="5"/>
-      <c r="X190" s="4"/>
+        <f>INT($C$185)+2.01</f>
+        <v>3.01</v>
+      </c>
+      <c r="D190" s="3"/>
+      <c r="E190" s="3"/>
+      <c r="F190" s="3"/>
+      <c r="G190" s="3"/>
+      <c r="H190" s="29"/>
+      <c r="I190" s="29"/>
+      <c r="J190" s="29"/>
+      <c r="K190" s="29"/>
+      <c r="L190" s="29"/>
+      <c r="M190" s="29"/>
+      <c r="N190" s="29"/>
+      <c r="O190" s="29"/>
+      <c r="P190" s="29"/>
+      <c r="Q190" s="29"/>
+      <c r="R190" s="29"/>
+      <c r="S190" s="29"/>
+      <c r="T190" s="29"/>
+      <c r="U190" s="29"/>
+      <c r="V190" s="29"/>
+      <c r="W190" s="29"/>
+      <c r="X190" s="3"/>
       <c r="Y190" s="16"/>
       <c r="Z190" s="1"/>
       <c r="AA190" s="1"/>
@@ -34199,16 +34209,12 @@
     </row>
     <row r="191" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
-      <c r="B191" s="33" t="s">
-        <v>19</v>
-      </c>
+      <c r="B191" s="33"/>
       <c r="C191" s="73">
-        <f>C$183</f>
+        <f>C$184</f>
         <v>5</v>
       </c>
-      <c r="D191" s="4" t="s">
-        <v>44</v>
-      </c>
+      <c r="D191" s="4"/>
       <c r="E191" s="5"/>
       <c r="F191" s="5"/>
       <c r="G191" s="4"/>
@@ -34234,94 +34240,98 @@
       <c r="AA191" s="1"/>
       <c r="AB191" s="1"/>
     </row>
-    <row r="192" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
-      <c r="B192" s="33"/>
+      <c r="B192" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="C192" s="73">
-        <f>INT($C$184)+2.005</f>
-        <v>3.0049999999999999</v>
+        <f>C$184</f>
+        <v>5</v>
       </c>
       <c r="D192" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E192" s="4"/>
-      <c r="F192" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="E192" s="5"/>
+      <c r="F192" s="5"/>
       <c r="G192" s="4"/>
-      <c r="H192" s="58"/>
-      <c r="I192" s="58"/>
-      <c r="J192" s="58"/>
-      <c r="K192" s="58"/>
-      <c r="L192" s="58"/>
-      <c r="M192" s="58"/>
-      <c r="N192" s="58"/>
-      <c r="O192" s="58"/>
-      <c r="P192" s="58"/>
-      <c r="Q192" s="58"/>
-      <c r="R192" s="58"/>
-      <c r="S192" s="58"/>
-      <c r="T192" s="58"/>
-      <c r="U192" s="58"/>
-      <c r="V192" s="58"/>
-      <c r="W192" s="58"/>
+      <c r="H192" s="5"/>
+      <c r="I192" s="5"/>
+      <c r="J192" s="5"/>
+      <c r="K192" s="5"/>
+      <c r="L192" s="5"/>
+      <c r="M192" s="5"/>
+      <c r="N192" s="5"/>
+      <c r="O192" s="5"/>
+      <c r="P192" s="5"/>
+      <c r="Q192" s="5"/>
+      <c r="R192" s="5"/>
+      <c r="S192" s="5"/>
+      <c r="T192" s="5"/>
+      <c r="U192" s="5"/>
+      <c r="V192" s="5"/>
+      <c r="W192" s="5"/>
       <c r="X192" s="4"/>
       <c r="Y192" s="16"/>
       <c r="Z192" s="1"/>
       <c r="AA192" s="1"/>
       <c r="AB192" s="1"/>
     </row>
-    <row r="193" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
       <c r="B193" s="33"/>
       <c r="C193" s="73">
-        <f>INT($C$184)+2</f>
-        <v>3</v>
-      </c>
-      <c r="D193" s="4"/>
-      <c r="E193" s="5"/>
-      <c r="F193" s="5"/>
+        <f>INT($C$185)+2.005</f>
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="D193" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E193" s="4"/>
+      <c r="F193" s="4"/>
       <c r="G193" s="4"/>
-      <c r="H193" s="64" t="s">
-        <v>287</v>
-      </c>
-      <c r="I193" s="31">
-        <v>4</v>
-      </c>
-      <c r="J193" s="158" t="s">
-        <v>291</v>
-      </c>
-      <c r="K193" s="2"/>
-      <c r="L193" s="2"/>
-      <c r="M193" s="2"/>
-      <c r="N193" s="2"/>
-      <c r="O193" s="2"/>
-      <c r="P193" s="2"/>
-      <c r="Q193" s="2"/>
-      <c r="R193" s="2"/>
-      <c r="S193" s="2"/>
-      <c r="T193" s="2"/>
-      <c r="U193" s="2"/>
-      <c r="V193" s="2"/>
-      <c r="W193" s="2"/>
+      <c r="H193" s="58"/>
+      <c r="I193" s="58"/>
+      <c r="J193" s="58"/>
+      <c r="K193" s="58"/>
+      <c r="L193" s="58"/>
+      <c r="M193" s="58"/>
+      <c r="N193" s="58"/>
+      <c r="O193" s="58"/>
+      <c r="P193" s="58"/>
+      <c r="Q193" s="58"/>
+      <c r="R193" s="58"/>
+      <c r="S193" s="58"/>
+      <c r="T193" s="58"/>
+      <c r="U193" s="58"/>
+      <c r="V193" s="58"/>
+      <c r="W193" s="58"/>
       <c r="X193" s="4"/>
       <c r="Y193" s="16"/>
       <c r="Z193" s="1"/>
       <c r="AA193" s="1"/>
       <c r="AB193" s="1"/>
     </row>
-    <row r="194" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
       <c r="B194" s="33"/>
       <c r="C194" s="73">
-        <f>INT($C$184)+3</f>
-        <v>4</v>
+        <f>INT($C$185)+2</f>
+        <v>3</v>
       </c>
       <c r="D194" s="4"/>
       <c r="E194" s="5"/>
       <c r="F194" s="5"/>
       <c r="G194" s="4"/>
-      <c r="H194" s="157"/>
-      <c r="I194" s="2"/>
-      <c r="J194" s="2"/>
+      <c r="H194" s="64" t="s">
+        <v>287</v>
+      </c>
+      <c r="I194" s="31">
+        <v>4</v>
+      </c>
+      <c r="J194" s="158" t="s">
+        <v>291</v>
+      </c>
       <c r="K194" s="2"/>
       <c r="L194" s="2"/>
       <c r="M194" s="2"/>
@@ -34341,20 +34351,18 @@
       <c r="AA194" s="1"/>
       <c r="AB194" s="1"/>
     </row>
-    <row r="195" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
       <c r="B195" s="33"/>
       <c r="C195" s="73">
-        <f>INT($C$184)+2</f>
-        <v>3</v>
+        <f>INT($C$185)+3</f>
+        <v>4</v>
       </c>
       <c r="D195" s="4"/>
       <c r="E195" s="5"/>
       <c r="F195" s="5"/>
       <c r="G195" s="4"/>
-      <c r="H195" s="64" t="s">
-        <v>292</v>
-      </c>
+      <c r="H195" s="157"/>
       <c r="I195" s="2"/>
       <c r="J195" s="2"/>
       <c r="K195" s="2"/>
@@ -34376,51 +34384,31 @@
       <c r="AA195" s="1"/>
       <c r="AB195" s="1"/>
     </row>
-    <row r="196" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
       <c r="B196" s="33"/>
       <c r="C196" s="73">
-        <f>INT($C$184)+3</f>
-        <v>4</v>
+        <f>INT($C$185)+2</f>
+        <v>3</v>
       </c>
       <c r="D196" s="4"/>
       <c r="E196" s="5"/>
       <c r="F196" s="5"/>
       <c r="G196" s="4"/>
-      <c r="H196" s="159" t="s">
-        <v>298</v>
+      <c r="H196" s="64" t="s">
+        <v>292</v>
       </c>
       <c r="I196" s="2"/>
-      <c r="J196" s="31">
-        <v>3</v>
-      </c>
-      <c r="K196" s="31">
-        <v>4</v>
-      </c>
-      <c r="L196" s="31">
-        <v>6</v>
-      </c>
-      <c r="M196" s="31">
-        <v>8</v>
-      </c>
-      <c r="N196" s="31">
-        <v>9</v>
-      </c>
-      <c r="O196" s="31">
-        <v>6</v>
-      </c>
-      <c r="P196" s="31">
-        <v>5</v>
-      </c>
-      <c r="Q196" s="31">
-        <v>4</v>
-      </c>
-      <c r="R196" s="31">
-        <v>3.5</v>
-      </c>
-      <c r="S196" s="31">
-        <v>3</v>
-      </c>
+      <c r="J196" s="2"/>
+      <c r="K196" s="2"/>
+      <c r="L196" s="2"/>
+      <c r="M196" s="2"/>
+      <c r="N196" s="2"/>
+      <c r="O196" s="2"/>
+      <c r="P196" s="2"/>
+      <c r="Q196" s="2"/>
+      <c r="R196" s="2"/>
+      <c r="S196" s="2"/>
       <c r="T196" s="2"/>
       <c r="U196" s="2"/>
       <c r="V196" s="2"/>
@@ -34431,11 +34419,11 @@
       <c r="AA196" s="1"/>
       <c r="AB196" s="1"/>
     </row>
-    <row r="197" spans="1:28" outlineLevel="3" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
       <c r="B197" s="33"/>
       <c r="C197" s="73">
-        <f>INT($C$184)+3</f>
+        <f>INT($C$185)+3</f>
         <v>4</v>
       </c>
       <c r="D197" s="4"/>
@@ -34443,38 +34431,38 @@
       <c r="F197" s="5"/>
       <c r="G197" s="4"/>
       <c r="H197" s="159" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="I197" s="2"/>
       <c r="J197" s="31">
-        <v>13.3</v>
+        <v>3</v>
       </c>
       <c r="K197" s="31">
-        <v>13.3</v>
+        <v>4</v>
       </c>
       <c r="L197" s="31">
-        <v>13.3</v>
+        <v>6</v>
       </c>
       <c r="M197" s="31">
-        <v>13.3</v>
+        <v>8</v>
       </c>
       <c r="N197" s="31">
-        <v>13.3</v>
+        <v>9</v>
       </c>
       <c r="O197" s="31">
-        <v>13.3</v>
+        <v>6</v>
       </c>
       <c r="P197" s="31">
-        <v>13.3</v>
+        <v>5</v>
       </c>
       <c r="Q197" s="31">
-        <v>13.3</v>
+        <v>4</v>
       </c>
       <c r="R197" s="31">
-        <v>13.3</v>
+        <v>3.5</v>
       </c>
       <c r="S197" s="31">
-        <v>13.3</v>
+        <v>3</v>
       </c>
       <c r="T197" s="2"/>
       <c r="U197" s="2"/>
@@ -34486,29 +34474,51 @@
       <c r="AA197" s="1"/>
       <c r="AB197" s="1"/>
     </row>
-    <row r="198" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:28" outlineLevel="3" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
       <c r="B198" s="33"/>
       <c r="C198" s="73">
-        <f>INT(C$184+3)</f>
+        <f>INT($C$185)+3</f>
         <v>4</v>
       </c>
       <c r="D198" s="4"/>
       <c r="E198" s="5"/>
       <c r="F198" s="5"/>
       <c r="G198" s="4"/>
-      <c r="H198" s="148"/>
-      <c r="I198" s="148"/>
-      <c r="J198" s="148"/>
-      <c r="K198" s="148"/>
-      <c r="L198" s="148"/>
-      <c r="M198" s="148"/>
-      <c r="N198" s="148"/>
-      <c r="O198" s="148"/>
-      <c r="P198" s="148"/>
-      <c r="Q198" s="148"/>
-      <c r="R198" s="148"/>
-      <c r="S198" s="148"/>
+      <c r="H198" s="159" t="s">
+        <v>294</v>
+      </c>
+      <c r="I198" s="2"/>
+      <c r="J198" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="K198" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="L198" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="M198" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="N198" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="O198" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="P198" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="Q198" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="R198" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="S198" s="31">
+        <v>13.3</v>
+      </c>
       <c r="T198" s="2"/>
       <c r="U198" s="2"/>
       <c r="V198" s="2"/>
@@ -34523,7 +34533,7 @@
       <c r="A199" s="1"/>
       <c r="B199" s="33"/>
       <c r="C199" s="73">
-        <f>INT(C$184+3)</f>
+        <f>INT(C$185+3)</f>
         <v>4</v>
       </c>
       <c r="D199" s="4"/>
@@ -34541,7 +34551,7 @@
       <c r="P199" s="148"/>
       <c r="Q199" s="148"/>
       <c r="R199" s="148"/>
-      <c r="S199" s="2"/>
+      <c r="S199" s="148"/>
       <c r="T199" s="2"/>
       <c r="U199" s="2"/>
       <c r="V199" s="2"/>
@@ -34552,47 +34562,45 @@
       <c r="AA199" s="1"/>
       <c r="AB199" s="1"/>
     </row>
-    <row r="200" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
       <c r="B200" s="33"/>
       <c r="C200" s="73">
-        <f>INT($C$184)+3.005</f>
-        <v>4.0049999999999999</v>
+        <f>INT(C$185+3)</f>
+        <v>4</v>
       </c>
       <c r="D200" s="4"/>
-      <c r="E200" s="4"/>
-      <c r="F200" s="4"/>
+      <c r="E200" s="5"/>
+      <c r="F200" s="5"/>
       <c r="G200" s="4"/>
-      <c r="H200" s="4"/>
-      <c r="I200" s="4"/>
-      <c r="J200" s="4"/>
-      <c r="K200" s="4"/>
-      <c r="L200" s="4"/>
-      <c r="M200" s="4"/>
-      <c r="N200" s="4"/>
-      <c r="O200" s="4"/>
-      <c r="P200" s="4"/>
-      <c r="Q200" s="4"/>
-      <c r="R200" s="4"/>
-      <c r="S200" s="4"/>
-      <c r="T200" s="4"/>
-      <c r="U200" s="4"/>
-      <c r="V200" s="4"/>
-      <c r="W200" s="4"/>
-      <c r="X200" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="H200" s="148"/>
+      <c r="I200" s="148"/>
+      <c r="J200" s="148"/>
+      <c r="K200" s="148"/>
+      <c r="L200" s="148"/>
+      <c r="M200" s="148"/>
+      <c r="N200" s="148"/>
+      <c r="O200" s="148"/>
+      <c r="P200" s="148"/>
+      <c r="Q200" s="148"/>
+      <c r="R200" s="148"/>
+      <c r="S200" s="2"/>
+      <c r="T200" s="2"/>
+      <c r="U200" s="2"/>
+      <c r="V200" s="2"/>
+      <c r="W200" s="2"/>
+      <c r="X200" s="4"/>
       <c r="Y200" s="16"/>
       <c r="Z200" s="1"/>
       <c r="AA200" s="1"/>
       <c r="AB200" s="1"/>
     </row>
-    <row r="201" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A201" s="1"/>
       <c r="B201" s="33"/>
       <c r="C201" s="73">
-        <f>INT($C$184)+2.005</f>
-        <v>3.0049999999999999</v>
+        <f>INT($C$185)+3.005</f>
+        <v>4.0049999999999999</v>
       </c>
       <c r="D201" s="4"/>
       <c r="E201" s="4"/>
@@ -34614,117 +34622,122 @@
       <c r="U201" s="4"/>
       <c r="V201" s="4"/>
       <c r="W201" s="4"/>
-      <c r="X201" s="4"/>
+      <c r="X201" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="Y201" s="16"/>
       <c r="Z201" s="1"/>
       <c r="AA201" s="1"/>
       <c r="AB201" s="1"/>
     </row>
-    <row r="202" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A202" s="1"/>
-      <c r="B202" s="35"/>
-      <c r="C202" s="76">
-        <f>INT($C$184)+1.005</f>
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="D202" s="17"/>
-      <c r="E202" s="17"/>
-      <c r="F202" s="17"/>
-      <c r="G202" s="17"/>
-      <c r="H202" s="17"/>
-      <c r="I202" s="17"/>
-      <c r="J202" s="17"/>
-      <c r="K202" s="17"/>
-      <c r="L202" s="17"/>
-      <c r="M202" s="17"/>
-      <c r="N202" s="17"/>
-      <c r="O202" s="17"/>
-      <c r="P202" s="17"/>
-      <c r="Q202" s="17"/>
-      <c r="R202" s="17"/>
-      <c r="S202" s="17"/>
-      <c r="T202" s="17"/>
-      <c r="U202" s="17"/>
-      <c r="V202" s="17"/>
-      <c r="W202" s="17"/>
-      <c r="X202" s="17"/>
-      <c r="Y202" s="18" t="s">
-        <v>1</v>
-      </c>
+      <c r="B202" s="33"/>
+      <c r="C202" s="73">
+        <f>INT($C$185)+2.005</f>
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="D202" s="4"/>
+      <c r="E202" s="4"/>
+      <c r="F202" s="4"/>
+      <c r="G202" s="4"/>
+      <c r="H202" s="4"/>
+      <c r="I202" s="4"/>
+      <c r="J202" s="4"/>
+      <c r="K202" s="4"/>
+      <c r="L202" s="4"/>
+      <c r="M202" s="4"/>
+      <c r="N202" s="4"/>
+      <c r="O202" s="4"/>
+      <c r="P202" s="4"/>
+      <c r="Q202" s="4"/>
+      <c r="R202" s="4"/>
+      <c r="S202" s="4"/>
+      <c r="T202" s="4"/>
+      <c r="U202" s="4"/>
+      <c r="V202" s="4"/>
+      <c r="W202" s="4"/>
+      <c r="X202" s="4"/>
+      <c r="Y202" s="16"/>
       <c r="Z202" s="1"/>
       <c r="AA202" s="1"/>
       <c r="AB202" s="1"/>
     </row>
-    <row r="203" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A203" s="1"/>
-      <c r="B203" s="19"/>
-      <c r="C203" s="77">
-        <f>INT($C$184)+0.005</f>
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="D203" s="19"/>
-      <c r="E203" s="19"/>
-      <c r="F203" s="19"/>
-      <c r="G203" s="19"/>
-      <c r="H203" s="19"/>
-      <c r="I203" s="19"/>
-      <c r="J203" s="19"/>
-      <c r="K203" s="19"/>
-      <c r="L203" s="19"/>
-      <c r="M203" s="19"/>
-      <c r="N203" s="19"/>
-      <c r="O203" s="19"/>
-      <c r="P203" s="19"/>
-      <c r="Q203" s="19"/>
-      <c r="R203" s="19"/>
-      <c r="S203" s="19"/>
-      <c r="T203" s="19"/>
-      <c r="U203" s="19"/>
-      <c r="V203" s="19"/>
-      <c r="W203" s="19"/>
-      <c r="X203" s="19"/>
-      <c r="Y203" s="19"/>
+      <c r="B203" s="35"/>
+      <c r="C203" s="76">
+        <f>INT($C$185)+1.005</f>
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="D203" s="17"/>
+      <c r="E203" s="17"/>
+      <c r="F203" s="17"/>
+      <c r="G203" s="17"/>
+      <c r="H203" s="17"/>
+      <c r="I203" s="17"/>
+      <c r="J203" s="17"/>
+      <c r="K203" s="17"/>
+      <c r="L203" s="17"/>
+      <c r="M203" s="17"/>
+      <c r="N203" s="17"/>
+      <c r="O203" s="17"/>
+      <c r="P203" s="17"/>
+      <c r="Q203" s="17"/>
+      <c r="R203" s="17"/>
+      <c r="S203" s="17"/>
+      <c r="T203" s="17"/>
+      <c r="U203" s="17"/>
+      <c r="V203" s="17"/>
+      <c r="W203" s="17"/>
+      <c r="X203" s="17"/>
+      <c r="Y203" s="18" t="s">
+        <v>1</v>
+      </c>
       <c r="Z203" s="1"/>
       <c r="AA203" s="1"/>
       <c r="AB203" s="1"/>
     </row>
-    <row r="204" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="1"/>
-      <c r="B204" s="1"/>
-      <c r="C204" s="73">
-        <f>INT($C$184)+2</f>
-        <v>3</v>
-      </c>
-      <c r="D204" s="1"/>
-      <c r="E204" s="1"/>
-      <c r="F204" s="1"/>
-      <c r="G204" s="1"/>
-      <c r="H204" s="1"/>
-      <c r="I204" s="1"/>
-      <c r="J204" s="1"/>
-      <c r="K204" s="1"/>
-      <c r="L204" s="1"/>
-      <c r="M204" s="1"/>
-      <c r="N204" s="1"/>
-      <c r="O204" s="1"/>
-      <c r="P204" s="1"/>
-      <c r="Q204" s="1"/>
-      <c r="R204" s="1"/>
-      <c r="S204" s="1"/>
-      <c r="T204" s="1"/>
-      <c r="U204" s="1"/>
-      <c r="V204" s="1"/>
-      <c r="W204" s="1"/>
-      <c r="X204" s="1"/>
-      <c r="Y204" s="1"/>
+      <c r="B204" s="19"/>
+      <c r="C204" s="77">
+        <f>INT($C$185)+0.005</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D204" s="19"/>
+      <c r="E204" s="19"/>
+      <c r="F204" s="19"/>
+      <c r="G204" s="19"/>
+      <c r="H204" s="19"/>
+      <c r="I204" s="19"/>
+      <c r="J204" s="19"/>
+      <c r="K204" s="19"/>
+      <c r="L204" s="19"/>
+      <c r="M204" s="19"/>
+      <c r="N204" s="19"/>
+      <c r="O204" s="19"/>
+      <c r="P204" s="19"/>
+      <c r="Q204" s="19"/>
+      <c r="R204" s="19"/>
+      <c r="S204" s="19"/>
+      <c r="T204" s="19"/>
+      <c r="U204" s="19"/>
+      <c r="V204" s="19"/>
+      <c r="W204" s="19"/>
+      <c r="X204" s="19"/>
+      <c r="Y204" s="19"/>
       <c r="Z204" s="1"/>
       <c r="AA204" s="1"/>
       <c r="AB204" s="1"/>
     </row>
-    <row r="205" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
-      <c r="C205" s="66"/>
+      <c r="C205" s="73">
+        <f>INT($C$185)+2</f>
+        <v>3</v>
+      </c>
       <c r="D205" s="1"/>
       <c r="E205" s="1"/>
       <c r="F205" s="1"/>
@@ -34902,7 +34915,37 @@
       <c r="AB210" s="1"/>
     </row>
     <row r="211" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C211" s="72" t="s">
+      <c r="A211" s="1"/>
+      <c r="B211" s="1"/>
+      <c r="C211" s="66"/>
+      <c r="D211" s="1"/>
+      <c r="E211" s="1"/>
+      <c r="F211" s="1"/>
+      <c r="G211" s="1"/>
+      <c r="H211" s="1"/>
+      <c r="I211" s="1"/>
+      <c r="J211" s="1"/>
+      <c r="K211" s="1"/>
+      <c r="L211" s="1"/>
+      <c r="M211" s="1"/>
+      <c r="N211" s="1"/>
+      <c r="O211" s="1"/>
+      <c r="P211" s="1"/>
+      <c r="Q211" s="1"/>
+      <c r="R211" s="1"/>
+      <c r="S211" s="1"/>
+      <c r="T211" s="1"/>
+      <c r="U211" s="1"/>
+      <c r="V211" s="1"/>
+      <c r="W211" s="1"/>
+      <c r="X211" s="1"/>
+      <c r="Y211" s="1"/>
+      <c r="Z211" s="1"/>
+      <c r="AA211" s="1"/>
+      <c r="AB211" s="1"/>
+    </row>
+    <row r="212" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C212" s="72" t="s">
         <v>4</v>
       </c>
     </row>
@@ -34939,7 +34982,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
@@ -35568,7 +35611,7 @@
       <c r="E21" s="177"/>
       <c r="F21" s="185"/>
       <c r="G21" s="193" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H21" s="191"/>
       <c r="I21" s="191"/>
@@ -35598,7 +35641,7 @@
       <c r="E22" s="177"/>
       <c r="F22" s="185"/>
       <c r="G22" s="191" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H22" s="191"/>
       <c r="I22" s="191"/>

</xml_diff>

<commit_message>
To Master: Change age range for Yearling genetic stage (425 days) so that a ewe lamb mated at 9mo will be altered by Yearling ERA.
</commit_message>
<xml_diff>
--- a/ExcelInputs/Structural.xlsx
+++ b/ExcelInputs/Structural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\ExcelInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE467B95-AC9E-4C9B-B6E0-1503E9A9D443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881A3E01-523A-4AE0-8398-340D2095183E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2535" yWindow="405" windowWidth="25140" windowHeight="15075" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -3762,15 +3762,6 @@
     <t>Offs sale method</t>
   </si>
   <si>
-    <t>9May24: Change Offs sale method to 0 so that pkl_fs for the NFS would work (temporary change)
-27May23: Alter FVP6 to be beginning of the PregTox period rather than end of joining
-30Sep22: Alter the inputs for the user defined FVP dates, changed to a calculation based on TOL, a 91 day weaning and 126 days from weaning to next joining
-8Jun22: Change the range of the LW for the initial animals.
-18Mar22: Change the default r2_inc to False now that a pickled feed supply is working.
-20May21: Make the extra nut_spread_g1 = 0.1
-1Apr19: Blank worksheet</t>
-  </si>
-  <si>
     <t>evg</t>
   </si>
   <si>
@@ -3970,6 +3961,16 @@
 25Apr21: Moved inputs from Property.xlsx
                    Moved FVP &amp; N inputs from Stock
 1: 1Apr19-Created the version control table</t>
+  </si>
+  <si>
+    <t>22Sep24: Change the yearling End Age to 425 days (so that ewe lambs mated at 9mo can be altered by the yearling ERA)
+9May24: Change Offs sale method to 0 so that pkl_fs for the NFS would work (temporary change)
+27May23: Alter FVP6 to be beginning of the PregTox period rather than end of joining
+30Sep22: Alter the inputs for the user defined FVP dates, changed to a calculation based on TOL, a 91 day weaning and 126 days from weaning to next joining
+8Jun22: Change the range of the LW for the initial animals.
+18Mar22: Change the default r2_inc to False now that a pickled feed supply is working.
+20May21: Make the extra nut_spread_g1 = 0.1
+1Apr19: Blank worksheet</t>
   </si>
 </sst>
 </file>
@@ -9819,7 +9820,7 @@
       <c r="G86" s="4"/>
       <c r="H86" s="148"/>
       <c r="I86" s="163" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="J86" s="163" t="b">
         <v>0</v>
@@ -10047,7 +10048,7 @@
       <c r="N91" s="165"/>
       <c r="O91" s="165"/>
       <c r="P91" s="163" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="Q91" s="163" t="b">
         <v>0</v>
@@ -27121,7 +27122,7 @@
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="J13" sqref="J13:T13"/>
+      <selection pane="bottomRight" activeCell="J14" sqref="J14:T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -27655,7 +27656,7 @@
         <v>45541.344751273202</v>
       </c>
       <c r="J13" s="222" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="K13" s="223"/>
       <c r="L13" s="223"/>
@@ -27694,10 +27695,10 @@
         <v>17</v>
       </c>
       <c r="I14" s="125">
-        <v>45421.933288078697</v>
+        <v>45557.353121412001</v>
       </c>
       <c r="J14" s="225" t="s">
-        <v>389</v>
+        <v>447</v>
       </c>
       <c r="K14" s="226"/>
       <c r="L14" s="226"/>
@@ -28574,20 +28575,20 @@
       <c r="G37" s="3"/>
       <c r="H37" s="29"/>
       <c r="I37" s="29" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J37" s="29"/>
       <c r="K37" s="29"/>
       <c r="L37" s="29"/>
       <c r="M37" s="29" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="N37" s="29"/>
       <c r="O37" s="29"/>
       <c r="P37" s="29"/>
       <c r="Q37" s="29"/>
       <c r="R37" s="29" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="S37" s="29"/>
       <c r="T37" s="29"/>
@@ -28775,7 +28776,7 @@
       <c r="J42" s="96"/>
       <c r="K42" s="96"/>
       <c r="L42" s="26" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="M42" s="213" t="b">
         <v>1</v>
@@ -28819,7 +28820,7 @@
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
       <c r="L43" s="26" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="M43" s="213" t="b">
         <v>0</v>
@@ -28863,7 +28864,7 @@
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
       <c r="L44" s="26" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="M44" s="214">
         <v>1</v>
@@ -28903,7 +28904,7 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
       <c r="L45" s="26" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="M45" s="213" t="b">
         <v>0</v>
@@ -29675,19 +29676,19 @@
         <v>204</v>
       </c>
       <c r="N65" s="156" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="O65" s="156" t="s">
+        <v>398</v>
+      </c>
+      <c r="P65" s="156" t="s">
         <v>399</v>
       </c>
-      <c r="P65" s="156" t="s">
+      <c r="Q65" s="156" t="s">
         <v>400</v>
       </c>
-      <c r="Q65" s="156" t="s">
+      <c r="R65" s="156" t="s">
         <v>401</v>
-      </c>
-      <c r="R65" s="156" t="s">
-        <v>402</v>
       </c>
       <c r="S65" s="29"/>
       <c r="T65" s="29"/>
@@ -33620,43 +33621,43 @@
       <c r="K156" s="148"/>
       <c r="L156" s="148"/>
       <c r="M156" s="148" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="N156" s="36" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="O156" s="56" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="P156" s="56" t="s">
+        <v>419</v>
+      </c>
+      <c r="Q156" s="56" t="s">
         <v>420</v>
       </c>
-      <c r="Q156" s="56" t="s">
+      <c r="R156" s="56" t="s">
         <v>421</v>
       </c>
-      <c r="R156" s="56" t="s">
+      <c r="S156" s="56" t="s">
         <v>422</v>
       </c>
-      <c r="S156" s="56" t="s">
+      <c r="T156" s="36" t="s">
+        <v>425</v>
+      </c>
+      <c r="U156" s="36" t="s">
+        <v>426</v>
+      </c>
+      <c r="V156" s="36" t="s">
+        <v>427</v>
+      </c>
+      <c r="W156" s="36" t="s">
+        <v>428</v>
+      </c>
+      <c r="X156" s="36" t="s">
+        <v>429</v>
+      </c>
+      <c r="Y156" s="36" t="s">
         <v>423</v>
-      </c>
-      <c r="T156" s="36" t="s">
-        <v>426</v>
-      </c>
-      <c r="U156" s="36" t="s">
-        <v>427</v>
-      </c>
-      <c r="V156" s="36" t="s">
-        <v>428</v>
-      </c>
-      <c r="W156" s="36" t="s">
-        <v>429</v>
-      </c>
-      <c r="X156" s="36" t="s">
-        <v>430</v>
-      </c>
-      <c r="Y156" s="36" t="s">
-        <v>424</v>
       </c>
       <c r="Z156" s="36"/>
       <c r="AA156" s="4"/>
@@ -33686,37 +33687,37 @@
         <v>0</v>
       </c>
       <c r="O157" s="56" t="s">
+        <v>435</v>
+      </c>
+      <c r="P157" s="56" t="s">
         <v>436</v>
       </c>
-      <c r="P157" s="56" t="s">
+      <c r="Q157" s="56" t="s">
         <v>437</v>
       </c>
-      <c r="Q157" s="56" t="s">
+      <c r="R157" s="56" t="s">
         <v>438</v>
       </c>
-      <c r="R157" s="56" t="s">
+      <c r="S157" s="56" t="s">
         <v>439</v>
       </c>
-      <c r="S157" s="56" t="s">
+      <c r="T157" s="36" t="s">
         <v>440</v>
       </c>
-      <c r="T157" s="36" t="s">
+      <c r="U157" s="36" t="s">
         <v>441</v>
       </c>
-      <c r="U157" s="36" t="s">
+      <c r="V157" s="36" t="s">
         <v>442</v>
       </c>
-      <c r="V157" s="36" t="s">
+      <c r="W157" s="36" t="s">
         <v>443</v>
       </c>
-      <c r="W157" s="36" t="s">
+      <c r="X157" s="36" t="s">
         <v>444</v>
       </c>
-      <c r="X157" s="36" t="s">
+      <c r="Y157" s="36" t="s">
         <v>445</v>
-      </c>
-      <c r="Y157" s="36" t="s">
-        <v>446</v>
       </c>
       <c r="Z157" s="36">
         <v>12</v>
@@ -33743,42 +33744,42 @@
       <c r="J158" s="148"/>
       <c r="K158" s="148"/>
       <c r="L158" s="26" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="M158" s="52"/>
       <c r="N158" s="36"/>
       <c r="O158" s="56" t="s">
+        <v>409</v>
+      </c>
+      <c r="P158" s="56" t="s">
         <v>410</v>
       </c>
-      <c r="P158" s="56" t="s">
+      <c r="Q158" s="56" t="s">
         <v>411</v>
       </c>
-      <c r="Q158" s="56" t="s">
+      <c r="R158" s="56" t="s">
+        <v>413</v>
+      </c>
+      <c r="S158" s="56" t="s">
         <v>412</v>
       </c>
-      <c r="R158" s="56" t="s">
+      <c r="T158" s="36" t="s">
         <v>414</v>
       </c>
-      <c r="S158" s="56" t="s">
-        <v>413</v>
-      </c>
-      <c r="T158" s="36" t="s">
+      <c r="U158" s="36" t="s">
         <v>415</v>
       </c>
-      <c r="U158" s="36" t="s">
+      <c r="V158" s="36" t="s">
         <v>416</v>
       </c>
-      <c r="V158" s="36" t="s">
+      <c r="W158" s="36" t="s">
         <v>417</v>
       </c>
-      <c r="W158" s="36" t="s">
+      <c r="X158" s="36" t="s">
         <v>418</v>
       </c>
-      <c r="X158" s="36" t="s">
-        <v>419</v>
-      </c>
       <c r="Y158" s="36" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="Z158" s="36"/>
       <c r="AA158" s="4"/>
@@ -33803,10 +33804,10 @@
       <c r="J159" s="148"/>
       <c r="K159" s="148"/>
       <c r="L159" s="151" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="M159" s="151" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="N159" s="31">
         <v>0</v>
@@ -33878,7 +33879,7 @@
       <c r="K160" s="148"/>
       <c r="L160" s="148"/>
       <c r="M160" s="151" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="N160" s="31">
         <v>99999</v>
@@ -33893,7 +33894,7 @@
         <v>183</v>
       </c>
       <c r="R160" s="31">
-        <v>364</v>
+        <v>425</v>
       </c>
       <c r="S160" s="31">
         <f>S159+364</f>
@@ -33994,7 +33995,7 @@
       <c r="L162" s="148"/>
       <c r="M162" s="148"/>
       <c r="N162" s="220" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="O162" s="220"/>
       <c r="P162" s="220"/>
@@ -34038,40 +34039,40 @@
       <c r="L163" s="148"/>
       <c r="M163" s="148"/>
       <c r="N163" s="219" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="O163" s="219" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="P163" s="219" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Q163" s="219" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="R163" s="219" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="S163" s="219" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="T163" s="219" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="U163" s="219" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="V163" s="219" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="W163" s="219" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="X163" s="219" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Y163" s="219" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Z163" s="219"/>
       <c r="AA163" s="4"/>
@@ -34146,7 +34147,7 @@
       <c r="L165" s="148"/>
       <c r="M165" s="148"/>
       <c r="N165" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="O165" s="148"/>
       <c r="P165" s="148"/>
@@ -34190,7 +34191,7 @@
       <c r="L166" s="148"/>
       <c r="M166" s="148"/>
       <c r="N166" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="O166" s="148"/>
       <c r="P166" s="148"/>
@@ -34234,7 +34235,7 @@
       <c r="L167" s="148"/>
       <c r="M167" s="148"/>
       <c r="N167" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="O167" s="148"/>
       <c r="P167" s="148"/>
@@ -34268,7 +34269,7 @@
       <c r="F168" s="5"/>
       <c r="G168" s="4"/>
       <c r="H168" s="31" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I168" s="31">
         <v>0</v>
@@ -34278,7 +34279,7 @@
       <c r="L168" s="148"/>
       <c r="M168" s="148"/>
       <c r="N168" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="O168" s="148"/>
       <c r="P168" s="148"/>
@@ -34312,7 +34313,7 @@
       <c r="F169" s="5"/>
       <c r="G169" s="4"/>
       <c r="H169" s="31" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I169" s="31">
         <v>0</v>
@@ -34322,7 +34323,7 @@
       <c r="L169" s="148"/>
       <c r="M169" s="148"/>
       <c r="N169" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="O169" s="148"/>
       <c r="P169" s="148"/>
@@ -34450,13 +34451,13 @@
       <c r="L172" s="148"/>
       <c r="M172" s="148"/>
       <c r="N172" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="O172" s="148"/>
       <c r="P172" s="148"/>
       <c r="Q172" s="148"/>
       <c r="R172" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="S172" s="148"/>
       <c r="T172" s="2"/>
@@ -34465,7 +34466,7 @@
       <c r="W172" s="2"/>
       <c r="X172" s="2"/>
       <c r="Y172" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Z172" s="2"/>
       <c r="AA172" s="4"/>
@@ -34498,13 +34499,13 @@
       <c r="L173" s="148"/>
       <c r="M173" s="148"/>
       <c r="N173" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="O173" s="148"/>
       <c r="P173" s="148"/>
       <c r="Q173" s="148"/>
       <c r="R173" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="S173" s="148"/>
       <c r="T173" s="2"/>
@@ -34513,7 +34514,7 @@
       <c r="W173" s="2"/>
       <c r="X173" s="2"/>
       <c r="Y173" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Z173" s="2"/>
       <c r="AA173" s="4"/>
@@ -34546,13 +34547,13 @@
       <c r="L174" s="148"/>
       <c r="M174" s="148"/>
       <c r="N174" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="O174" s="148"/>
       <c r="P174" s="148"/>
       <c r="Q174" s="148"/>
       <c r="R174" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="S174" s="148"/>
       <c r="T174" s="2"/>
@@ -34561,7 +34562,7 @@
       <c r="W174" s="2"/>
       <c r="X174" s="2"/>
       <c r="Y174" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Z174" s="2"/>
       <c r="AA174" s="4"/>
@@ -34636,36 +34637,36 @@
       <c r="L176" s="148"/>
       <c r="M176" s="148"/>
       <c r="N176" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="O176" s="148"/>
       <c r="P176" s="148"/>
       <c r="Q176" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="R176" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="S176" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="T176" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="U176" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="V176" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="W176" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="X176" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Y176" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Z176" s="56"/>
       <c r="AA176" s="4"/>
@@ -34698,36 +34699,36 @@
       <c r="L177" s="148"/>
       <c r="M177" s="148"/>
       <c r="N177" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="O177" s="148"/>
       <c r="P177" s="148"/>
       <c r="Q177" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="R177" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="S177" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="T177" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="U177" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="V177" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="W177" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="X177" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Y177" s="56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Z177" s="56"/>
       <c r="AA177" s="4"/>
@@ -34760,36 +34761,36 @@
       <c r="L178" s="148"/>
       <c r="M178" s="148"/>
       <c r="N178" s="218" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="O178" s="217"/>
       <c r="P178" s="217"/>
       <c r="Q178" s="218" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="R178" s="218" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="S178" s="218" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="T178" s="218" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="U178" s="218" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="V178" s="218" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="W178" s="218" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="X178" s="218" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Y178" s="218" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Z178" s="218"/>
       <c r="AA178" s="4"/>
@@ -36917,7 +36918,7 @@
       <c r="E21" s="177"/>
       <c r="F21" s="185"/>
       <c r="G21" s="193" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H21" s="191"/>
       <c r="I21" s="191"/>
@@ -36947,7 +36948,7 @@
       <c r="E22" s="177"/>
       <c r="F22" s="185"/>
       <c r="G22" s="191" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H22" s="191"/>
       <c r="I22" s="191"/>

</xml_diff>

<commit_message>
Add cfat (carcase fat depth) as a REV trait. Change function fs = f(cs)
</commit_message>
<xml_diff>
--- a/ExcelInputs/Structural.xlsx
+++ b/ExcelInputs/Structural.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\ExcelInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881A3E01-523A-4AE0-8398-340D2095183E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881CAD0C-540B-46BD-A1D2-027955337C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
@@ -92,7 +92,7 @@
     <definedName name="i_lag_organs">Stock!$I$70</definedName>
     <definedName name="i_lag_wool">Stock!$I$69</definedName>
     <definedName name="i_landuse_is_dual" localSheetId="0">General!$Q$79:$Q$109</definedName>
-    <definedName name="i_len_f">StructuralSA!$I$199</definedName>
+    <definedName name="i_len_f">StructuralSA!$I$200</definedName>
     <definedName name="i_len_l">Stock!$M$160</definedName>
     <definedName name="i_len_m">Stock!$L$160</definedName>
     <definedName name="i_len_q" localSheetId="2">StructuralSA!$M$44</definedName>
@@ -121,8 +121,8 @@
     <definedName name="i_nut_spread_n0" localSheetId="2">StructuralSA!$J$115</definedName>
     <definedName name="i_nut_spread_n1" localSheetId="2">StructuralSA!$M$115:$M$122</definedName>
     <definedName name="i_nut_spread_n3" localSheetId="2">StructuralSA!$S$115:$S$122</definedName>
-    <definedName name="i_nv_lower_p6">StructuralSA!$J$202:$S$202</definedName>
-    <definedName name="i_nv_upper_p6">StructuralSA!$J$203:$S$203</definedName>
+    <definedName name="i_nv_lower_p6">StructuralSA!$J$203:$S$203</definedName>
+    <definedName name="i_nv_upper_p6">StructuralSA!$J$204:$S$204</definedName>
     <definedName name="i_offs_sale_method" localSheetId="2">StructuralSA!$R$42</definedName>
     <definedName name="i_offs_sale_opportunities_per_dvp" localSheetId="2">StructuralSA!$R$43</definedName>
     <definedName name="i_offs_user_fvp_date_iu" localSheetId="2">StructuralSA!$P$82:$R$84</definedName>
@@ -132,8 +132,8 @@
     <definedName name="i_r2adjust_inc">StructuralSA!$U$148</definedName>
     <definedName name="i_rev_age_stage" localSheetId="2">StructuralSA!$N$159:$Z$160</definedName>
     <definedName name="i_rev_number" localSheetId="2">StructuralSA!$I$150</definedName>
-    <definedName name="i_rev_trait_name" localSheetId="2">StructuralSA!$H$162:$H$178</definedName>
-    <definedName name="i_rev_trait_scenario" localSheetId="2">StructuralSA!$I$162:$I$178</definedName>
+    <definedName name="i_rev_trait_name" localSheetId="2">StructuralSA!$H$162:$H$179</definedName>
+    <definedName name="i_rev_trait_scenario" localSheetId="2">StructuralSA!$I$162:$I$179</definedName>
     <definedName name="i_rev_update" localSheetId="2">StructuralSA!$I$148</definedName>
     <definedName name="i_sim_periods_year">Stock!$I$62</definedName>
     <definedName name="i_store_cs_rep" localSheetId="3">'Report Settings'!$K$18</definedName>
@@ -2382,7 +2382,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="H199" authorId="2" shapeId="0" xr:uid="{B39EFDC6-7ABB-4808-93B1-2819F2755236}">
+    <comment ref="H179" authorId="2" shapeId="0" xr:uid="{7D72CFA0-EF47-40D9-9D6F-9FDC3F1C19F9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>John:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Carcase fat depth</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H200" authorId="2" shapeId="0" xr:uid="{B39EFDC6-7ABB-4808-93B1-2819F2755236}">
       <text>
         <r>
           <rPr>
@@ -2406,7 +2430,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H202" authorId="2" shapeId="0" xr:uid="{315CC92D-C01A-4D16-90CA-458397130ECA}">
+    <comment ref="H203" authorId="2" shapeId="0" xr:uid="{315CC92D-C01A-4D16-90CA-458397130ECA}">
       <text>
         <r>
           <rPr>
@@ -2432,7 +2456,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H203" authorId="2" shapeId="0" xr:uid="{24292EB5-78CD-4E29-870F-1743067DEF27}">
+    <comment ref="H204" authorId="2" shapeId="0" xr:uid="{24292EB5-78CD-4E29-870F-1743067DEF27}">
       <text>
         <r>
           <rPr>
@@ -2497,7 +2521,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="449">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -3933,7 +3957,21 @@
     <t>11 - A</t>
   </si>
   <si>
-    <t>6Sep24: Alter order of age stages so that whole of life is [0] - which is the default in the code.
+    <t>22Sep24: Change the yearling End Age to 425 days (so that ewe lambs mated at 9mo can be altered by the yearling ERA)
+9May24: Change Offs sale method to 0 so that pkl_fs for the NFS would work (temporary change)
+27May23: Alter FVP6 to be beginning of the PregTox period rather than end of joining
+30Sep22: Alter the inputs for the user defined FVP dates, changed to a calculation based on TOL, a 91 day weaning and 126 days from weaning to next joining
+8Jun22: Change the range of the LW for the initial animals.
+18Mar22: Change the default r2_inc to False now that a pickled feed supply is working.
+20May21: Make the extra nut_spread_g1 = 0.1
+1Apr19: Blank worksheet</t>
+  </si>
+  <si>
+    <t>cfat</t>
+  </si>
+  <si>
+    <t>26Sep24: Add cfat (carcase fat depth) trait
+6Sep24: Alter order of age stages so that whole of life is [0] - which is the default in the code.
 5Sep24: Altered descriptions for the age stages to include a value because the stage needs to be defined by a number
 4Sep24: Added wbec as a REV trait (#16). Add age stage information
 28Aug24: Improve commenting on the weaning period wrt user defined periods
@@ -3962,16 +4000,6 @@
                    Moved FVP &amp; N inputs from Stock
 1: 1Apr19-Created the version control table</t>
   </si>
-  <si>
-    <t>22Sep24: Change the yearling End Age to 425 days (so that ewe lambs mated at 9mo can be altered by the yearling ERA)
-9May24: Change Offs sale method to 0 so that pkl_fs for the NFS would work (temporary change)
-27May23: Alter FVP6 to be beginning of the PregTox period rather than end of joining
-30Sep22: Alter the inputs for the user defined FVP dates, changed to a calculation based on TOL, a 91 day weaning and 126 days from weaning to next joining
-8Jun22: Change the range of the LW for the initial animals.
-18Mar22: Change the default r2_inc to False now that a pickled feed supply is working.
-20May21: Make the extra nut_spread_g1 = 0.1
-1Apr19: Blank worksheet</t>
-  </si>
 </sst>
 </file>
 
@@ -3983,7 +4011,7 @@
     <numFmt numFmtId="166" formatCode="0.00_)"/>
     <numFmt numFmtId="167" formatCode="[$-C09]dd\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4202,6 +4230,19 @@
       <color rgb="FF0000CC"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="40">
@@ -27115,14 +27156,14 @@
   <sheetPr codeName="Sheet3">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AE217"/>
+  <dimension ref="A1:AE218"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J151" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="10" topLeftCell="J139" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="J14" sqref="J14:T14"/>
+      <selection pane="bottomRight" activeCell="J13" sqref="J13:T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -27653,10 +27694,10 @@
         <v>16</v>
       </c>
       <c r="I13" s="126">
-        <v>45541.344751273202</v>
+        <v>45561.574224305601</v>
       </c>
       <c r="J13" s="222" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="K13" s="223"/>
       <c r="L13" s="223"/>
@@ -27698,7 +27739,7 @@
         <v>45557.353121412001</v>
       </c>
       <c r="J14" s="225" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="K14" s="226"/>
       <c r="L14" s="226"/>
@@ -32940,7 +32981,7 @@
       <c r="A139" s="1"/>
       <c r="B139" s="33"/>
       <c r="C139" s="73">
-        <f>INT(MAX($C$147:$C$181))+1</f>
+        <f>INT(MAX($C$147:$C$182))+1</f>
         <v>5</v>
       </c>
       <c r="D139" s="3"/>
@@ -34019,7 +34060,7 @@
       <c r="A163" s="1"/>
       <c r="B163" s="33"/>
       <c r="C163" s="73">
-        <f t="shared" ref="C163:C178" si="17">INT(C$140+3)</f>
+        <f t="shared" ref="C163:C179" si="17">INT(C$140+3)</f>
         <v>4</v>
       </c>
       <c r="D163" s="4"/>
@@ -34760,39 +34801,39 @@
       <c r="K178" s="148"/>
       <c r="L178" s="148"/>
       <c r="M178" s="148"/>
-      <c r="N178" s="218" t="s">
+      <c r="N178" s="56" t="s">
         <v>430</v>
       </c>
-      <c r="O178" s="217"/>
-      <c r="P178" s="217"/>
-      <c r="Q178" s="218" t="s">
+      <c r="O178" s="148"/>
+      <c r="P178" s="148"/>
+      <c r="Q178" s="56" t="s">
         <v>430</v>
       </c>
-      <c r="R178" s="218" t="s">
+      <c r="R178" s="56" t="s">
         <v>430</v>
       </c>
-      <c r="S178" s="218" t="s">
+      <c r="S178" s="56" t="s">
         <v>430</v>
       </c>
-      <c r="T178" s="218" t="s">
+      <c r="T178" s="56" t="s">
         <v>430</v>
       </c>
-      <c r="U178" s="218" t="s">
+      <c r="U178" s="56" t="s">
         <v>430</v>
       </c>
-      <c r="V178" s="218" t="s">
+      <c r="V178" s="56" t="s">
         <v>430</v>
       </c>
-      <c r="W178" s="218" t="s">
+      <c r="W178" s="56" t="s">
         <v>430</v>
       </c>
-      <c r="X178" s="218" t="s">
+      <c r="X178" s="56" t="s">
         <v>430</v>
       </c>
-      <c r="Y178" s="218" t="s">
+      <c r="Y178" s="56" t="s">
         <v>430</v>
       </c>
-      <c r="Z178" s="218"/>
+      <c r="Z178" s="56"/>
       <c r="AA178" s="4"/>
       <c r="AB178" s="16"/>
       <c r="AC178" s="1"/>
@@ -34803,32 +34844,58 @@
       <c r="A179" s="1"/>
       <c r="B179" s="33"/>
       <c r="C179" s="73">
-        <f>INT(C$140+3)</f>
+        <f t="shared" si="17"/>
         <v>4</v>
       </c>
       <c r="D179" s="4"/>
-      <c r="E179" s="5"/>
+      <c r="E179" s="5">
+        <v>17</v>
+      </c>
       <c r="F179" s="5"/>
       <c r="G179" s="4"/>
-      <c r="H179" s="148"/>
-      <c r="I179" s="148"/>
+      <c r="H179" s="31" t="s">
+        <v>447</v>
+      </c>
+      <c r="I179" s="31">
+        <v>0</v>
+      </c>
       <c r="J179" s="148"/>
       <c r="K179" s="148"/>
       <c r="L179" s="148"/>
       <c r="M179" s="148"/>
-      <c r="N179" s="216"/>
-      <c r="O179" s="216"/>
-      <c r="P179" s="216"/>
-      <c r="Q179" s="216"/>
-      <c r="R179" s="216"/>
-      <c r="S179" s="53"/>
-      <c r="T179" s="53"/>
-      <c r="U179" s="53"/>
-      <c r="V179" s="53"/>
-      <c r="W179" s="53"/>
-      <c r="X179" s="53"/>
-      <c r="Y179" s="53"/>
-      <c r="Z179" s="53"/>
+      <c r="N179" s="218" t="s">
+        <v>430</v>
+      </c>
+      <c r="O179" s="217"/>
+      <c r="P179" s="217"/>
+      <c r="Q179" s="218" t="s">
+        <v>430</v>
+      </c>
+      <c r="R179" s="218" t="s">
+        <v>430</v>
+      </c>
+      <c r="S179" s="218" t="s">
+        <v>430</v>
+      </c>
+      <c r="T179" s="218" t="s">
+        <v>430</v>
+      </c>
+      <c r="U179" s="218" t="s">
+        <v>430</v>
+      </c>
+      <c r="V179" s="218" t="s">
+        <v>430</v>
+      </c>
+      <c r="W179" s="218" t="s">
+        <v>430</v>
+      </c>
+      <c r="X179" s="218" t="s">
+        <v>430</v>
+      </c>
+      <c r="Y179" s="218" t="s">
+        <v>430</v>
+      </c>
+      <c r="Z179" s="218"/>
       <c r="AA179" s="4"/>
       <c r="AB179" s="16"/>
       <c r="AC179" s="1"/>
@@ -34852,69 +34919,67 @@
       <c r="K180" s="148"/>
       <c r="L180" s="148"/>
       <c r="M180" s="148"/>
-      <c r="N180" s="148"/>
-      <c r="O180" s="148"/>
-      <c r="P180" s="148"/>
-      <c r="Q180" s="148"/>
-      <c r="R180" s="148"/>
-      <c r="S180" s="2"/>
-      <c r="T180" s="2"/>
-      <c r="U180" s="2"/>
-      <c r="V180" s="2"/>
-      <c r="W180" s="2"/>
-      <c r="X180" s="2"/>
-      <c r="Y180" s="2"/>
-      <c r="Z180" s="2"/>
+      <c r="N180" s="216"/>
+      <c r="O180" s="216"/>
+      <c r="P180" s="216"/>
+      <c r="Q180" s="216"/>
+      <c r="R180" s="216"/>
+      <c r="S180" s="53"/>
+      <c r="T180" s="53"/>
+      <c r="U180" s="53"/>
+      <c r="V180" s="53"/>
+      <c r="W180" s="53"/>
+      <c r="X180" s="53"/>
+      <c r="Y180" s="53"/>
+      <c r="Z180" s="53"/>
       <c r="AA180" s="4"/>
       <c r="AB180" s="16"/>
       <c r="AC180" s="1"/>
       <c r="AD180" s="1"/>
       <c r="AE180" s="1"/>
     </row>
-    <row r="181" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:31" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181" s="33"/>
       <c r="C181" s="73">
-        <f>INT($C$140)+3.005</f>
-        <v>4.0049999999999999</v>
+        <f>INT(C$140+3)</f>
+        <v>4</v>
       </c>
       <c r="D181" s="4"/>
-      <c r="E181" s="4"/>
-      <c r="F181" s="4"/>
+      <c r="E181" s="5"/>
+      <c r="F181" s="5"/>
       <c r="G181" s="4"/>
-      <c r="H181" s="4"/>
-      <c r="I181" s="4"/>
-      <c r="J181" s="4"/>
-      <c r="K181" s="4"/>
-      <c r="L181" s="4"/>
-      <c r="M181" s="4"/>
-      <c r="N181" s="4"/>
-      <c r="O181" s="4"/>
-      <c r="P181" s="4"/>
-      <c r="Q181" s="4"/>
-      <c r="R181" s="4"/>
-      <c r="S181" s="4"/>
-      <c r="T181" s="4"/>
-      <c r="U181" s="4"/>
-      <c r="V181" s="4"/>
-      <c r="W181" s="4"/>
-      <c r="X181" s="4"/>
-      <c r="Y181" s="4"/>
-      <c r="Z181" s="4"/>
-      <c r="AA181" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="H181" s="148"/>
+      <c r="I181" s="148"/>
+      <c r="J181" s="148"/>
+      <c r="K181" s="148"/>
+      <c r="L181" s="148"/>
+      <c r="M181" s="148"/>
+      <c r="N181" s="148"/>
+      <c r="O181" s="148"/>
+      <c r="P181" s="148"/>
+      <c r="Q181" s="148"/>
+      <c r="R181" s="148"/>
+      <c r="S181" s="2"/>
+      <c r="T181" s="2"/>
+      <c r="U181" s="2"/>
+      <c r="V181" s="2"/>
+      <c r="W181" s="2"/>
+      <c r="X181" s="2"/>
+      <c r="Y181" s="2"/>
+      <c r="Z181" s="2"/>
+      <c r="AA181" s="4"/>
       <c r="AB181" s="16"/>
       <c r="AC181" s="1"/>
       <c r="AD181" s="1"/>
       <c r="AE181" s="1"/>
     </row>
-    <row r="182" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182" s="33"/>
       <c r="C182" s="73">
-        <f>INT($C$140)+2.005</f>
-        <v>3.0049999999999999</v>
+        <f>INT($C$140)+3.005</f>
+        <v>4.0049999999999999</v>
       </c>
       <c r="D182" s="4"/>
       <c r="E182" s="4"/>
@@ -34939,118 +35004,120 @@
       <c r="X182" s="4"/>
       <c r="Y182" s="4"/>
       <c r="Z182" s="4"/>
-      <c r="AA182" s="4"/>
+      <c r="AA182" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="AB182" s="16"/>
       <c r="AC182" s="1"/>
       <c r="AD182" s="1"/>
       <c r="AE182" s="1"/>
     </row>
-    <row r="183" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
-      <c r="B183" s="35"/>
-      <c r="C183" s="76">
-        <f>INT($C$140)+1.005</f>
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="D183" s="17"/>
-      <c r="E183" s="17"/>
-      <c r="F183" s="17"/>
-      <c r="G183" s="17"/>
-      <c r="H183" s="17"/>
-      <c r="I183" s="17"/>
-      <c r="J183" s="17"/>
-      <c r="K183" s="17"/>
-      <c r="L183" s="17"/>
-      <c r="M183" s="17"/>
-      <c r="N183" s="17"/>
-      <c r="O183" s="17"/>
-      <c r="P183" s="17"/>
-      <c r="Q183" s="17"/>
-      <c r="R183" s="17"/>
-      <c r="S183" s="17"/>
-      <c r="T183" s="17"/>
-      <c r="U183" s="17"/>
-      <c r="V183" s="17"/>
-      <c r="W183" s="17"/>
-      <c r="X183" s="17"/>
-      <c r="Y183" s="17"/>
-      <c r="Z183" s="17"/>
-      <c r="AA183" s="17"/>
-      <c r="AB183" s="18" t="s">
-        <v>1</v>
-      </c>
+      <c r="B183" s="33"/>
+      <c r="C183" s="73">
+        <f>INT($C$140)+2.005</f>
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="D183" s="4"/>
+      <c r="E183" s="4"/>
+      <c r="F183" s="4"/>
+      <c r="G183" s="4"/>
+      <c r="H183" s="4"/>
+      <c r="I183" s="4"/>
+      <c r="J183" s="4"/>
+      <c r="K183" s="4"/>
+      <c r="L183" s="4"/>
+      <c r="M183" s="4"/>
+      <c r="N183" s="4"/>
+      <c r="O183" s="4"/>
+      <c r="P183" s="4"/>
+      <c r="Q183" s="4"/>
+      <c r="R183" s="4"/>
+      <c r="S183" s="4"/>
+      <c r="T183" s="4"/>
+      <c r="U183" s="4"/>
+      <c r="V183" s="4"/>
+      <c r="W183" s="4"/>
+      <c r="X183" s="4"/>
+      <c r="Y183" s="4"/>
+      <c r="Z183" s="4"/>
+      <c r="AA183" s="4"/>
+      <c r="AB183" s="16"/>
       <c r="AC183" s="1"/>
       <c r="AD183" s="1"/>
       <c r="AE183" s="1"/>
     </row>
-    <row r="184" spans="1:31" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
-      <c r="B184" s="19"/>
-      <c r="C184" s="77">
-        <f>INT($C$140)+0.005</f>
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="D184" s="19"/>
-      <c r="E184" s="19"/>
-      <c r="F184" s="19"/>
-      <c r="G184" s="19"/>
-      <c r="H184" s="19"/>
-      <c r="I184" s="19"/>
-      <c r="J184" s="19"/>
-      <c r="K184" s="19"/>
-      <c r="L184" s="19"/>
-      <c r="M184" s="19"/>
-      <c r="N184" s="19"/>
-      <c r="O184" s="19"/>
-      <c r="P184" s="19"/>
-      <c r="Q184" s="19"/>
-      <c r="R184" s="19"/>
-      <c r="S184" s="19"/>
-      <c r="T184" s="19"/>
-      <c r="U184" s="19"/>
-      <c r="V184" s="19"/>
-      <c r="W184" s="19"/>
-      <c r="X184" s="19"/>
-      <c r="Y184" s="19"/>
-      <c r="Z184" s="19"/>
-      <c r="AA184" s="19"/>
-      <c r="AB184" s="19"/>
+      <c r="B184" s="35"/>
+      <c r="C184" s="76">
+        <f>INT($C$140)+1.005</f>
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="D184" s="17"/>
+      <c r="E184" s="17"/>
+      <c r="F184" s="17"/>
+      <c r="G184" s="17"/>
+      <c r="H184" s="17"/>
+      <c r="I184" s="17"/>
+      <c r="J184" s="17"/>
+      <c r="K184" s="17"/>
+      <c r="L184" s="17"/>
+      <c r="M184" s="17"/>
+      <c r="N184" s="17"/>
+      <c r="O184" s="17"/>
+      <c r="P184" s="17"/>
+      <c r="Q184" s="17"/>
+      <c r="R184" s="17"/>
+      <c r="S184" s="17"/>
+      <c r="T184" s="17"/>
+      <c r="U184" s="17"/>
+      <c r="V184" s="17"/>
+      <c r="W184" s="17"/>
+      <c r="X184" s="17"/>
+      <c r="Y184" s="17"/>
+      <c r="Z184" s="17"/>
+      <c r="AA184" s="17"/>
+      <c r="AB184" s="18" t="s">
+        <v>1</v>
+      </c>
       <c r="AC184" s="1"/>
       <c r="AD184" s="1"/>
       <c r="AE184" s="1"/>
     </row>
-    <row r="185" spans="1:31" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:31" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
-      <c r="B185" s="1"/>
-      <c r="C185" s="73">
-        <f>INT($C$140)+2</f>
-        <v>3</v>
-      </c>
-      <c r="D185" s="1"/>
-      <c r="E185" s="1"/>
-      <c r="F185" s="1"/>
-      <c r="G185" s="1"/>
-      <c r="H185" s="1"/>
-      <c r="I185" s="1"/>
-      <c r="J185" s="1"/>
-      <c r="K185" s="1"/>
-      <c r="L185" s="1"/>
-      <c r="M185" s="1"/>
-      <c r="N185" s="1"/>
-      <c r="O185" s="1"/>
-      <c r="P185" s="1"/>
-      <c r="Q185" s="1"/>
-      <c r="R185" s="1"/>
-      <c r="S185" s="1"/>
-      <c r="T185" s="1"/>
-      <c r="U185" s="1"/>
-      <c r="V185" s="1"/>
-      <c r="W185" s="1"/>
-      <c r="X185" s="1"/>
-      <c r="Y185" s="1"/>
-      <c r="Z185" s="1"/>
-      <c r="AA185" s="1"/>
-      <c r="AB185" s="1"/>
+      <c r="B185" s="19"/>
+      <c r="C185" s="77">
+        <f>INT($C$140)+0.005</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D185" s="19"/>
+      <c r="E185" s="19"/>
+      <c r="F185" s="19"/>
+      <c r="G185" s="19"/>
+      <c r="H185" s="19"/>
+      <c r="I185" s="19"/>
+      <c r="J185" s="19"/>
+      <c r="K185" s="19"/>
+      <c r="L185" s="19"/>
+      <c r="M185" s="19"/>
+      <c r="N185" s="19"/>
+      <c r="O185" s="19"/>
+      <c r="P185" s="19"/>
+      <c r="Q185" s="19"/>
+      <c r="R185" s="19"/>
+      <c r="S185" s="19"/>
+      <c r="T185" s="19"/>
+      <c r="U185" s="19"/>
+      <c r="V185" s="19"/>
+      <c r="W185" s="19"/>
+      <c r="X185" s="19"/>
+      <c r="Y185" s="19"/>
+      <c r="Z185" s="19"/>
+      <c r="AA185" s="19"/>
+      <c r="AB185" s="19"/>
       <c r="AC185" s="1"/>
       <c r="AD185" s="1"/>
       <c r="AE185" s="1"/>
@@ -35059,7 +35126,7 @@
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="73">
-        <f>INT($C$190)+2</f>
+        <f>INT($C$140)+2</f>
         <v>3</v>
       </c>
       <c r="D186" s="1"/>
@@ -35091,266 +35158,264 @@
       <c r="AD186" s="1"/>
       <c r="AE186" s="1"/>
     </row>
-    <row r="187" spans="1:31" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:31" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
-      <c r="B187" s="20"/>
-      <c r="C187" s="74">
-        <f>INT($C$190)+0.005</f>
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="D187" s="20"/>
-      <c r="E187" s="20"/>
-      <c r="F187" s="20"/>
-      <c r="G187" s="20"/>
-      <c r="H187" s="20"/>
-      <c r="I187" s="20"/>
-      <c r="J187" s="20"/>
-      <c r="K187" s="20"/>
-      <c r="L187" s="20"/>
-      <c r="M187" s="20"/>
-      <c r="N187" s="20"/>
-      <c r="O187" s="20"/>
-      <c r="P187" s="20"/>
-      <c r="Q187" s="20"/>
-      <c r="R187" s="20"/>
-      <c r="S187" s="20"/>
-      <c r="T187" s="20"/>
-      <c r="U187" s="20"/>
-      <c r="V187" s="20"/>
-      <c r="W187" s="20"/>
-      <c r="X187" s="20"/>
-      <c r="Y187" s="20"/>
-      <c r="Z187" s="20"/>
-      <c r="AA187" s="20"/>
-      <c r="AB187" s="20"/>
+      <c r="B187" s="1"/>
+      <c r="C187" s="73">
+        <f>INT($C$191)+2</f>
+        <v>3</v>
+      </c>
+      <c r="D187" s="1"/>
+      <c r="E187" s="1"/>
+      <c r="F187" s="1"/>
+      <c r="G187" s="1"/>
+      <c r="H187" s="1"/>
+      <c r="I187" s="1"/>
+      <c r="J187" s="1"/>
+      <c r="K187" s="1"/>
+      <c r="L187" s="1"/>
+      <c r="M187" s="1"/>
+      <c r="N187" s="1"/>
+      <c r="O187" s="1"/>
+      <c r="P187" s="1"/>
+      <c r="Q187" s="1"/>
+      <c r="R187" s="1"/>
+      <c r="S187" s="1"/>
+      <c r="T187" s="1"/>
+      <c r="U187" s="1"/>
+      <c r="V187" s="1"/>
+      <c r="W187" s="1"/>
+      <c r="X187" s="1"/>
+      <c r="Y187" s="1"/>
+      <c r="Z187" s="1"/>
+      <c r="AA187" s="1"/>
+      <c r="AB187" s="1"/>
       <c r="AC187" s="1"/>
       <c r="AD187" s="1"/>
       <c r="AE187" s="1"/>
     </row>
-    <row r="188" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:31" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="1"/>
-      <c r="B188" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="C188" s="75">
-        <f>INT($C$190)+1.005</f>
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="D188" s="14"/>
-      <c r="E188" s="14"/>
-      <c r="F188" s="14"/>
-      <c r="G188" s="14"/>
-      <c r="H188" s="14"/>
-      <c r="I188" s="14"/>
-      <c r="J188" s="14"/>
-      <c r="K188" s="14"/>
-      <c r="L188" s="14"/>
-      <c r="M188" s="14"/>
-      <c r="N188" s="14"/>
-      <c r="O188" s="14"/>
-      <c r="P188" s="14"/>
-      <c r="Q188" s="14"/>
-      <c r="R188" s="14"/>
-      <c r="S188" s="14"/>
-      <c r="T188" s="14"/>
-      <c r="U188" s="14"/>
-      <c r="V188" s="14"/>
-      <c r="W188" s="14"/>
-      <c r="X188" s="14"/>
-      <c r="Y188" s="14"/>
-      <c r="Z188" s="14"/>
-      <c r="AA188" s="14"/>
-      <c r="AB188" s="15"/>
+      <c r="B188" s="20"/>
+      <c r="C188" s="74">
+        <f>INT($C$191)+0.005</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D188" s="20"/>
+      <c r="E188" s="20"/>
+      <c r="F188" s="20"/>
+      <c r="G188" s="20"/>
+      <c r="H188" s="20"/>
+      <c r="I188" s="20"/>
+      <c r="J188" s="20"/>
+      <c r="K188" s="20"/>
+      <c r="L188" s="20"/>
+      <c r="M188" s="20"/>
+      <c r="N188" s="20"/>
+      <c r="O188" s="20"/>
+      <c r="P188" s="20"/>
+      <c r="Q188" s="20"/>
+      <c r="R188" s="20"/>
+      <c r="S188" s="20"/>
+      <c r="T188" s="20"/>
+      <c r="U188" s="20"/>
+      <c r="V188" s="20"/>
+      <c r="W188" s="20"/>
+      <c r="X188" s="20"/>
+      <c r="Y188" s="20"/>
+      <c r="Z188" s="20"/>
+      <c r="AA188" s="20"/>
+      <c r="AB188" s="20"/>
       <c r="AC188" s="1"/>
       <c r="AD188" s="1"/>
       <c r="AE188" s="1"/>
     </row>
-    <row r="189" spans="1:31" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
-      <c r="B189" s="33"/>
-      <c r="C189" s="73">
-        <f>INT(MAX($C$198:$C$206))+1</f>
-        <v>5</v>
-      </c>
-      <c r="D189" s="3"/>
-      <c r="E189" s="3"/>
-      <c r="F189" s="3"/>
-      <c r="G189" s="3"/>
-      <c r="H189" s="27"/>
-      <c r="I189" s="27"/>
-      <c r="J189" s="27"/>
-      <c r="K189" s="27"/>
-      <c r="L189" s="27"/>
-      <c r="M189" s="27"/>
-      <c r="N189" s="27"/>
-      <c r="O189" s="27"/>
-      <c r="P189" s="27"/>
-      <c r="Q189" s="27"/>
-      <c r="R189" s="27"/>
-      <c r="S189" s="27"/>
-      <c r="T189" s="27"/>
-      <c r="U189" s="27"/>
-      <c r="V189" s="27"/>
-      <c r="W189" s="27"/>
-      <c r="X189" s="27"/>
-      <c r="Y189" s="27"/>
-      <c r="Z189" s="27"/>
-      <c r="AA189" s="3"/>
-      <c r="AB189" s="16"/>
+      <c r="B189" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C189" s="75">
+        <f>INT($C$191)+1.005</f>
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="D189" s="14"/>
+      <c r="E189" s="14"/>
+      <c r="F189" s="14"/>
+      <c r="G189" s="14"/>
+      <c r="H189" s="14"/>
+      <c r="I189" s="14"/>
+      <c r="J189" s="14"/>
+      <c r="K189" s="14"/>
+      <c r="L189" s="14"/>
+      <c r="M189" s="14"/>
+      <c r="N189" s="14"/>
+      <c r="O189" s="14"/>
+      <c r="P189" s="14"/>
+      <c r="Q189" s="14"/>
+      <c r="R189" s="14"/>
+      <c r="S189" s="14"/>
+      <c r="T189" s="14"/>
+      <c r="U189" s="14"/>
+      <c r="V189" s="14"/>
+      <c r="W189" s="14"/>
+      <c r="X189" s="14"/>
+      <c r="Y189" s="14"/>
+      <c r="Z189" s="14"/>
+      <c r="AA189" s="14"/>
+      <c r="AB189" s="15"/>
       <c r="AC189" s="1"/>
       <c r="AD189" s="1"/>
       <c r="AE189" s="1"/>
     </row>
-    <row r="190" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:31" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
       <c r="B190" s="33"/>
       <c r="C190" s="73">
-        <v>1.02</v>
-      </c>
-      <c r="D190" s="21"/>
-      <c r="E190" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="F190" s="25"/>
-      <c r="G190" s="12"/>
-      <c r="H190" s="147" t="str">
-        <f>COUNTIFS($B$1:$B190, "«")&amp;" Feed Pool definitions"</f>
-        <v>6 Feed Pool definitions</v>
-      </c>
-      <c r="I190" s="6"/>
-      <c r="J190" s="6"/>
-      <c r="K190" s="6"/>
-      <c r="L190" s="6"/>
-      <c r="M190" s="6"/>
-      <c r="N190" s="6"/>
-      <c r="O190" s="6"/>
-      <c r="P190" s="6"/>
-      <c r="Q190" s="6"/>
-      <c r="R190" s="6"/>
-      <c r="S190" s="6"/>
-      <c r="T190" s="6"/>
-      <c r="U190" s="6"/>
-      <c r="V190" s="6"/>
-      <c r="W190" s="6"/>
-      <c r="X190" s="6"/>
-      <c r="Y190" s="6"/>
-      <c r="Z190" s="6"/>
-      <c r="AA190" s="10"/>
+        <f>INT(MAX($C$199:$C$207))+1</f>
+        <v>5</v>
+      </c>
+      <c r="D190" s="3"/>
+      <c r="E190" s="3"/>
+      <c r="F190" s="3"/>
+      <c r="G190" s="3"/>
+      <c r="H190" s="27"/>
+      <c r="I190" s="27"/>
+      <c r="J190" s="27"/>
+      <c r="K190" s="27"/>
+      <c r="L190" s="27"/>
+      <c r="M190" s="27"/>
+      <c r="N190" s="27"/>
+      <c r="O190" s="27"/>
+      <c r="P190" s="27"/>
+      <c r="Q190" s="27"/>
+      <c r="R190" s="27"/>
+      <c r="S190" s="27"/>
+      <c r="T190" s="27"/>
+      <c r="U190" s="27"/>
+      <c r="V190" s="27"/>
+      <c r="W190" s="27"/>
+      <c r="X190" s="27"/>
+      <c r="Y190" s="27"/>
+      <c r="Z190" s="27"/>
+      <c r="AA190" s="3"/>
       <c r="AB190" s="16"/>
       <c r="AC190" s="1"/>
       <c r="AD190" s="1"/>
       <c r="AE190" s="1"/>
     </row>
-    <row r="191" spans="1:31" ht="18.75" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="B191" s="33"/>
       <c r="C191" s="73">
-        <f>INT($C$190)+1.02</f>
-        <v>2.02</v>
+        <v>1.02</v>
       </c>
       <c r="D191" s="21"/>
       <c r="E191" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F191" s="28">
-        <v>1</v>
-      </c>
-      <c r="G191" s="13"/>
-      <c r="H191" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="I191" s="7"/>
-      <c r="J191" s="7"/>
-      <c r="K191" s="7"/>
-      <c r="L191" s="7"/>
-      <c r="M191" s="7"/>
-      <c r="N191" s="7"/>
-      <c r="O191" s="7"/>
-      <c r="P191" s="7"/>
-      <c r="Q191" s="7"/>
-      <c r="R191" s="7"/>
-      <c r="S191" s="7"/>
-      <c r="T191" s="7"/>
-      <c r="U191" s="7"/>
-      <c r="V191" s="7"/>
-      <c r="W191" s="7"/>
-      <c r="X191" s="7"/>
-      <c r="Y191" s="7"/>
-      <c r="Z191" s="7"/>
-      <c r="AA191" s="11"/>
+        <v>6</v>
+      </c>
+      <c r="F191" s="25"/>
+      <c r="G191" s="12"/>
+      <c r="H191" s="147" t="str">
+        <f>COUNTIFS($B$1:$B191, "«")&amp;" Feed Pool definitions"</f>
+        <v>6 Feed Pool definitions</v>
+      </c>
+      <c r="I191" s="6"/>
+      <c r="J191" s="6"/>
+      <c r="K191" s="6"/>
+      <c r="L191" s="6"/>
+      <c r="M191" s="6"/>
+      <c r="N191" s="6"/>
+      <c r="O191" s="6"/>
+      <c r="P191" s="6"/>
+      <c r="Q191" s="6"/>
+      <c r="R191" s="6"/>
+      <c r="S191" s="6"/>
+      <c r="T191" s="6"/>
+      <c r="U191" s="6"/>
+      <c r="V191" s="6"/>
+      <c r="W191" s="6"/>
+      <c r="X191" s="6"/>
+      <c r="Y191" s="6"/>
+      <c r="Z191" s="6"/>
+      <c r="AA191" s="10"/>
       <c r="AB191" s="16"/>
       <c r="AC191" s="1"/>
       <c r="AD191" s="1"/>
       <c r="AE191" s="1"/>
     </row>
-    <row r="192" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:31" ht="18.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
       <c r="B192" s="33"/>
       <c r="C192" s="73">
-        <f>INT($C$190)+2.005</f>
-        <v>3.0049999999999999</v>
-      </c>
-      <c r="D192" s="3"/>
-      <c r="E192" s="3"/>
-      <c r="F192" s="3"/>
-      <c r="G192" s="3"/>
-      <c r="H192" s="3"/>
-      <c r="I192" s="3"/>
-      <c r="J192" s="3"/>
-      <c r="K192" s="3"/>
-      <c r="L192" s="3"/>
-      <c r="M192" s="3"/>
-      <c r="N192" s="3"/>
-      <c r="O192" s="3"/>
-      <c r="P192" s="3"/>
-      <c r="Q192" s="3"/>
-      <c r="R192" s="3"/>
-      <c r="S192" s="3"/>
-      <c r="T192" s="3"/>
-      <c r="U192" s="3"/>
-      <c r="V192" s="3"/>
-      <c r="W192" s="3"/>
-      <c r="X192" s="3"/>
-      <c r="Y192" s="3"/>
-      <c r="Z192" s="3"/>
-      <c r="AA192" s="3"/>
+        <f>INT($C$191)+1.02</f>
+        <v>2.02</v>
+      </c>
+      <c r="D192" s="21"/>
+      <c r="E192" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F192" s="28">
+        <v>1</v>
+      </c>
+      <c r="G192" s="13"/>
+      <c r="H192" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="I192" s="7"/>
+      <c r="J192" s="7"/>
+      <c r="K192" s="7"/>
+      <c r="L192" s="7"/>
+      <c r="M192" s="7"/>
+      <c r="N192" s="7"/>
+      <c r="O192" s="7"/>
+      <c r="P192" s="7"/>
+      <c r="Q192" s="7"/>
+      <c r="R192" s="7"/>
+      <c r="S192" s="7"/>
+      <c r="T192" s="7"/>
+      <c r="U192" s="7"/>
+      <c r="V192" s="7"/>
+      <c r="W192" s="7"/>
+      <c r="X192" s="7"/>
+      <c r="Y192" s="7"/>
+      <c r="Z192" s="7"/>
+      <c r="AA192" s="11"/>
       <c r="AB192" s="16"/>
       <c r="AC192" s="1"/>
       <c r="AD192" s="1"/>
       <c r="AE192" s="1"/>
     </row>
-    <row r="193" spans="1:31" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
       <c r="B193" s="33"/>
       <c r="C193" s="73">
-        <f>INT($C$190)+2</f>
-        <v>3</v>
+        <f>INT($C$191)+2.005</f>
+        <v>3.0049999999999999</v>
       </c>
       <c r="D193" s="3"/>
-      <c r="E193" s="5"/>
-      <c r="F193" s="5"/>
+      <c r="E193" s="3"/>
+      <c r="F193" s="3"/>
       <c r="G193" s="3"/>
-      <c r="H193" s="29"/>
-      <c r="I193" s="29"/>
-      <c r="J193" s="65" t="s">
-        <v>293</v>
-      </c>
-      <c r="K193" s="65"/>
-      <c r="L193" s="65"/>
-      <c r="M193" s="65"/>
-      <c r="N193" s="65"/>
-      <c r="O193" s="65"/>
-      <c r="P193" s="65"/>
-      <c r="Q193" s="65"/>
-      <c r="R193" s="65"/>
-      <c r="S193" s="65"/>
-      <c r="T193" s="29"/>
-      <c r="U193" s="29"/>
-      <c r="V193" s="29"/>
-      <c r="W193" s="29"/>
-      <c r="X193" s="29"/>
-      <c r="Y193" s="29"/>
-      <c r="Z193" s="29"/>
+      <c r="H193" s="3"/>
+      <c r="I193" s="3"/>
+      <c r="J193" s="3"/>
+      <c r="K193" s="3"/>
+      <c r="L193" s="3"/>
+      <c r="M193" s="3"/>
+      <c r="N193" s="3"/>
+      <c r="O193" s="3"/>
+      <c r="P193" s="3"/>
+      <c r="Q193" s="3"/>
+      <c r="R193" s="3"/>
+      <c r="S193" s="3"/>
+      <c r="T193" s="3"/>
+      <c r="U193" s="3"/>
+      <c r="V193" s="3"/>
+      <c r="W193" s="3"/>
+      <c r="X193" s="3"/>
+      <c r="Y193" s="3"/>
+      <c r="Z193" s="3"/>
       <c r="AA193" s="3"/>
       <c r="AB193" s="16"/>
       <c r="AC193" s="1"/>
@@ -35361,7 +35426,7 @@
       <c r="A194" s="1"/>
       <c r="B194" s="33"/>
       <c r="C194" s="73">
-        <f>INT($C$190)+2</f>
+        <f>INT($C$191)+2</f>
         <v>3</v>
       </c>
       <c r="D194" s="3"/>
@@ -35370,36 +35435,18 @@
       <c r="G194" s="3"/>
       <c r="H194" s="29"/>
       <c r="I194" s="29"/>
-      <c r="J194" s="29">
-        <v>0</v>
-      </c>
-      <c r="K194" s="29">
-        <v>1</v>
-      </c>
-      <c r="L194" s="29">
-        <v>2</v>
-      </c>
-      <c r="M194" s="29">
-        <v>3</v>
-      </c>
-      <c r="N194" s="29">
-        <v>4</v>
-      </c>
-      <c r="O194" s="29">
-        <v>5</v>
-      </c>
-      <c r="P194" s="29">
-        <v>6</v>
-      </c>
-      <c r="Q194" s="29">
-        <v>7</v>
-      </c>
-      <c r="R194" s="29">
-        <v>8</v>
-      </c>
-      <c r="S194" s="29">
-        <v>9</v>
-      </c>
+      <c r="J194" s="65" t="s">
+        <v>293</v>
+      </c>
+      <c r="K194" s="65"/>
+      <c r="L194" s="65"/>
+      <c r="M194" s="65"/>
+      <c r="N194" s="65"/>
+      <c r="O194" s="65"/>
+      <c r="P194" s="65"/>
+      <c r="Q194" s="65"/>
+      <c r="R194" s="65"/>
+      <c r="S194" s="65"/>
       <c r="T194" s="29"/>
       <c r="U194" s="29"/>
       <c r="V194" s="29"/>
@@ -35413,31 +35460,49 @@
       <c r="AD194" s="1"/>
       <c r="AE194" s="1"/>
     </row>
-    <row r="195" spans="1:31" ht="9.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:31" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
-      <c r="B195" s="33" t="s">
-        <v>20</v>
-      </c>
+      <c r="B195" s="33"/>
       <c r="C195" s="73">
-        <f>INT($C$190)+2.01</f>
-        <v>3.01</v>
+        <f>INT($C$191)+2</f>
+        <v>3</v>
       </c>
       <c r="D195" s="3"/>
-      <c r="E195" s="3"/>
-      <c r="F195" s="3"/>
+      <c r="E195" s="5"/>
+      <c r="F195" s="5"/>
       <c r="G195" s="3"/>
       <c r="H195" s="29"/>
       <c r="I195" s="29"/>
-      <c r="J195" s="29"/>
-      <c r="K195" s="29"/>
-      <c r="L195" s="29"/>
-      <c r="M195" s="29"/>
-      <c r="N195" s="29"/>
-      <c r="O195" s="29"/>
-      <c r="P195" s="29"/>
-      <c r="Q195" s="29"/>
-      <c r="R195" s="29"/>
-      <c r="S195" s="29"/>
+      <c r="J195" s="29">
+        <v>0</v>
+      </c>
+      <c r="K195" s="29">
+        <v>1</v>
+      </c>
+      <c r="L195" s="29">
+        <v>2</v>
+      </c>
+      <c r="M195" s="29">
+        <v>3</v>
+      </c>
+      <c r="N195" s="29">
+        <v>4</v>
+      </c>
+      <c r="O195" s="29">
+        <v>5</v>
+      </c>
+      <c r="P195" s="29">
+        <v>6</v>
+      </c>
+      <c r="Q195" s="29">
+        <v>7</v>
+      </c>
+      <c r="R195" s="29">
+        <v>8</v>
+      </c>
+      <c r="S195" s="29">
+        <v>9</v>
+      </c>
       <c r="T195" s="29"/>
       <c r="U195" s="29"/>
       <c r="V195" s="29"/>
@@ -35451,37 +35516,39 @@
       <c r="AD195" s="1"/>
       <c r="AE195" s="1"/>
     </row>
-    <row r="196" spans="1:31" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:31" ht="9.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
-      <c r="B196" s="33"/>
+      <c r="B196" s="33" t="s">
+        <v>20</v>
+      </c>
       <c r="C196" s="73">
-        <f>C$189</f>
-        <v>5</v>
-      </c>
-      <c r="D196" s="4"/>
-      <c r="E196" s="5"/>
-      <c r="F196" s="5"/>
-      <c r="G196" s="4"/>
-      <c r="H196" s="5"/>
-      <c r="I196" s="5"/>
-      <c r="J196" s="5"/>
-      <c r="K196" s="5"/>
-      <c r="L196" s="5"/>
-      <c r="M196" s="5"/>
-      <c r="N196" s="5"/>
-      <c r="O196" s="5"/>
-      <c r="P196" s="5"/>
-      <c r="Q196" s="5"/>
-      <c r="R196" s="5"/>
-      <c r="S196" s="5"/>
-      <c r="T196" s="5"/>
-      <c r="U196" s="5"/>
-      <c r="V196" s="5"/>
-      <c r="W196" s="5"/>
-      <c r="X196" s="5"/>
-      <c r="Y196" s="5"/>
-      <c r="Z196" s="5"/>
-      <c r="AA196" s="4"/>
+        <f>INT($C$191)+2.01</f>
+        <v>3.01</v>
+      </c>
+      <c r="D196" s="3"/>
+      <c r="E196" s="3"/>
+      <c r="F196" s="3"/>
+      <c r="G196" s="3"/>
+      <c r="H196" s="29"/>
+      <c r="I196" s="29"/>
+      <c r="J196" s="29"/>
+      <c r="K196" s="29"/>
+      <c r="L196" s="29"/>
+      <c r="M196" s="29"/>
+      <c r="N196" s="29"/>
+      <c r="O196" s="29"/>
+      <c r="P196" s="29"/>
+      <c r="Q196" s="29"/>
+      <c r="R196" s="29"/>
+      <c r="S196" s="29"/>
+      <c r="T196" s="29"/>
+      <c r="U196" s="29"/>
+      <c r="V196" s="29"/>
+      <c r="W196" s="29"/>
+      <c r="X196" s="29"/>
+      <c r="Y196" s="29"/>
+      <c r="Z196" s="29"/>
+      <c r="AA196" s="3"/>
       <c r="AB196" s="16"/>
       <c r="AC196" s="1"/>
       <c r="AD196" s="1"/>
@@ -35489,16 +35556,12 @@
     </row>
     <row r="197" spans="1:31" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
-      <c r="B197" s="33" t="s">
-        <v>19</v>
-      </c>
+      <c r="B197" s="33"/>
       <c r="C197" s="73">
-        <f>C$189</f>
+        <f>C$190</f>
         <v>5</v>
       </c>
-      <c r="D197" s="4" t="s">
-        <v>44</v>
-      </c>
+      <c r="D197" s="4"/>
       <c r="E197" s="5"/>
       <c r="F197" s="5"/>
       <c r="G197" s="4"/>
@@ -35527,100 +35590,104 @@
       <c r="AD197" s="1"/>
       <c r="AE197" s="1"/>
     </row>
-    <row r="198" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:31" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
-      <c r="B198" s="33"/>
+      <c r="B198" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="C198" s="73">
-        <f>INT($C$190)+2.005</f>
-        <v>3.0049999999999999</v>
+        <f>C$190</f>
+        <v>5</v>
       </c>
       <c r="D198" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E198" s="4"/>
-      <c r="F198" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="E198" s="5"/>
+      <c r="F198" s="5"/>
       <c r="G198" s="4"/>
-      <c r="H198" s="58"/>
-      <c r="I198" s="58"/>
-      <c r="J198" s="58"/>
-      <c r="K198" s="58"/>
-      <c r="L198" s="58"/>
-      <c r="M198" s="58"/>
-      <c r="N198" s="58"/>
-      <c r="O198" s="58"/>
-      <c r="P198" s="58"/>
-      <c r="Q198" s="58"/>
-      <c r="R198" s="58"/>
-      <c r="S198" s="58"/>
-      <c r="T198" s="58"/>
-      <c r="U198" s="58"/>
-      <c r="V198" s="58"/>
-      <c r="W198" s="58"/>
-      <c r="X198" s="82"/>
-      <c r="Y198" s="82"/>
-      <c r="Z198" s="82"/>
+      <c r="H198" s="5"/>
+      <c r="I198" s="5"/>
+      <c r="J198" s="5"/>
+      <c r="K198" s="5"/>
+      <c r="L198" s="5"/>
+      <c r="M198" s="5"/>
+      <c r="N198" s="5"/>
+      <c r="O198" s="5"/>
+      <c r="P198" s="5"/>
+      <c r="Q198" s="5"/>
+      <c r="R198" s="5"/>
+      <c r="S198" s="5"/>
+      <c r="T198" s="5"/>
+      <c r="U198" s="5"/>
+      <c r="V198" s="5"/>
+      <c r="W198" s="5"/>
+      <c r="X198" s="5"/>
+      <c r="Y198" s="5"/>
+      <c r="Z198" s="5"/>
       <c r="AA198" s="4"/>
       <c r="AB198" s="16"/>
       <c r="AC198" s="1"/>
       <c r="AD198" s="1"/>
       <c r="AE198" s="1"/>
     </row>
-    <row r="199" spans="1:31" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
       <c r="B199" s="33"/>
       <c r="C199" s="73">
-        <f>INT($C$190)+2</f>
-        <v>3</v>
-      </c>
-      <c r="D199" s="4"/>
-      <c r="E199" s="5"/>
-      <c r="F199" s="5"/>
+        <f>INT($C$191)+2.005</f>
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="D199" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E199" s="4"/>
+      <c r="F199" s="4"/>
       <c r="G199" s="4"/>
-      <c r="H199" s="64" t="s">
-        <v>287</v>
-      </c>
-      <c r="I199" s="31">
-        <v>4</v>
-      </c>
-      <c r="J199" s="158" t="s">
-        <v>291</v>
-      </c>
-      <c r="K199" s="2"/>
-      <c r="L199" s="2"/>
-      <c r="M199" s="2"/>
-      <c r="N199" s="2"/>
-      <c r="O199" s="2"/>
-      <c r="P199" s="2"/>
-      <c r="Q199" s="2"/>
-      <c r="R199" s="2"/>
-      <c r="S199" s="2"/>
-      <c r="T199" s="2"/>
-      <c r="U199" s="2"/>
-      <c r="V199" s="2"/>
-      <c r="W199" s="2"/>
-      <c r="X199" s="2"/>
-      <c r="Y199" s="2"/>
-      <c r="Z199" s="2"/>
+      <c r="H199" s="58"/>
+      <c r="I199" s="58"/>
+      <c r="J199" s="58"/>
+      <c r="K199" s="58"/>
+      <c r="L199" s="58"/>
+      <c r="M199" s="58"/>
+      <c r="N199" s="58"/>
+      <c r="O199" s="58"/>
+      <c r="P199" s="58"/>
+      <c r="Q199" s="58"/>
+      <c r="R199" s="58"/>
+      <c r="S199" s="58"/>
+      <c r="T199" s="58"/>
+      <c r="U199" s="58"/>
+      <c r="V199" s="58"/>
+      <c r="W199" s="58"/>
+      <c r="X199" s="82"/>
+      <c r="Y199" s="82"/>
+      <c r="Z199" s="82"/>
       <c r="AA199" s="4"/>
       <c r="AB199" s="16"/>
       <c r="AC199" s="1"/>
       <c r="AD199" s="1"/>
       <c r="AE199" s="1"/>
     </row>
-    <row r="200" spans="1:31" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:31" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
       <c r="B200" s="33"/>
       <c r="C200" s="73">
-        <f>INT($C$190)+3</f>
-        <v>4</v>
+        <f>INT($C$191)+2</f>
+        <v>3</v>
       </c>
       <c r="D200" s="4"/>
       <c r="E200" s="5"/>
       <c r="F200" s="5"/>
       <c r="G200" s="4"/>
-      <c r="H200" s="157"/>
-      <c r="I200" s="2"/>
-      <c r="J200" s="2"/>
+      <c r="H200" s="64" t="s">
+        <v>287</v>
+      </c>
+      <c r="I200" s="31">
+        <v>4</v>
+      </c>
+      <c r="J200" s="158" t="s">
+        <v>291</v>
+      </c>
       <c r="K200" s="2"/>
       <c r="L200" s="2"/>
       <c r="M200" s="2"/>
@@ -35643,20 +35710,18 @@
       <c r="AD200" s="1"/>
       <c r="AE200" s="1"/>
     </row>
-    <row r="201" spans="1:31" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:31" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A201" s="1"/>
       <c r="B201" s="33"/>
       <c r="C201" s="73">
-        <f>INT($C$190)+2</f>
-        <v>3</v>
+        <f>INT($C$191)+3</f>
+        <v>4</v>
       </c>
       <c r="D201" s="4"/>
       <c r="E201" s="5"/>
       <c r="F201" s="5"/>
       <c r="G201" s="4"/>
-      <c r="H201" s="64" t="s">
-        <v>292</v>
-      </c>
+      <c r="H201" s="157"/>
       <c r="I201" s="2"/>
       <c r="J201" s="2"/>
       <c r="K201" s="2"/>
@@ -35681,51 +35746,31 @@
       <c r="AD201" s="1"/>
       <c r="AE201" s="1"/>
     </row>
-    <row r="202" spans="1:31" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:31" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A202" s="1"/>
       <c r="B202" s="33"/>
       <c r="C202" s="73">
-        <f>INT($C$190)+3</f>
-        <v>4</v>
+        <f>INT($C$191)+2</f>
+        <v>3</v>
       </c>
       <c r="D202" s="4"/>
       <c r="E202" s="5"/>
       <c r="F202" s="5"/>
       <c r="G202" s="4"/>
-      <c r="H202" s="159" t="s">
-        <v>298</v>
+      <c r="H202" s="64" t="s">
+        <v>292</v>
       </c>
       <c r="I202" s="2"/>
-      <c r="J202" s="31">
-        <v>3</v>
-      </c>
-      <c r="K202" s="31">
-        <v>4</v>
-      </c>
-      <c r="L202" s="31">
-        <v>6</v>
-      </c>
-      <c r="M202" s="31">
-        <v>8</v>
-      </c>
-      <c r="N202" s="31">
-        <v>9</v>
-      </c>
-      <c r="O202" s="31">
-        <v>6</v>
-      </c>
-      <c r="P202" s="31">
-        <v>5</v>
-      </c>
-      <c r="Q202" s="31">
-        <v>4</v>
-      </c>
-      <c r="R202" s="31">
-        <v>3.5</v>
-      </c>
-      <c r="S202" s="31">
-        <v>3</v>
-      </c>
+      <c r="J202" s="2"/>
+      <c r="K202" s="2"/>
+      <c r="L202" s="2"/>
+      <c r="M202" s="2"/>
+      <c r="N202" s="2"/>
+      <c r="O202" s="2"/>
+      <c r="P202" s="2"/>
+      <c r="Q202" s="2"/>
+      <c r="R202" s="2"/>
+      <c r="S202" s="2"/>
       <c r="T202" s="2"/>
       <c r="U202" s="2"/>
       <c r="V202" s="2"/>
@@ -35739,11 +35784,11 @@
       <c r="AD202" s="1"/>
       <c r="AE202" s="1"/>
     </row>
-    <row r="203" spans="1:31" outlineLevel="3" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:31" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A203" s="1"/>
       <c r="B203" s="33"/>
       <c r="C203" s="73">
-        <f>INT($C$190)+3</f>
+        <f>INT($C$191)+3</f>
         <v>4</v>
       </c>
       <c r="D203" s="4"/>
@@ -35751,38 +35796,38 @@
       <c r="F203" s="5"/>
       <c r="G203" s="4"/>
       <c r="H203" s="159" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="I203" s="2"/>
       <c r="J203" s="31">
-        <v>13.3</v>
+        <v>3</v>
       </c>
       <c r="K203" s="31">
-        <v>13.3</v>
+        <v>4</v>
       </c>
       <c r="L203" s="31">
-        <v>13.3</v>
+        <v>6</v>
       </c>
       <c r="M203" s="31">
-        <v>13.3</v>
+        <v>8</v>
       </c>
       <c r="N203" s="31">
-        <v>13.3</v>
+        <v>9</v>
       </c>
       <c r="O203" s="31">
-        <v>13.3</v>
+        <v>6</v>
       </c>
       <c r="P203" s="31">
-        <v>13.3</v>
+        <v>5</v>
       </c>
       <c r="Q203" s="31">
-        <v>13.3</v>
+        <v>4</v>
       </c>
       <c r="R203" s="31">
-        <v>13.3</v>
+        <v>3.5</v>
       </c>
       <c r="S203" s="31">
-        <v>13.3</v>
+        <v>3</v>
       </c>
       <c r="T203" s="2"/>
       <c r="U203" s="2"/>
@@ -35797,29 +35842,51 @@
       <c r="AD203" s="1"/>
       <c r="AE203" s="1"/>
     </row>
-    <row r="204" spans="1:31" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:31" outlineLevel="3" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A204" s="1"/>
       <c r="B204" s="33"/>
       <c r="C204" s="73">
-        <f>INT(C$190+3)</f>
+        <f>INT($C$191)+3</f>
         <v>4</v>
       </c>
       <c r="D204" s="4"/>
       <c r="E204" s="5"/>
       <c r="F204" s="5"/>
       <c r="G204" s="4"/>
-      <c r="H204" s="148"/>
-      <c r="I204" s="148"/>
-      <c r="J204" s="148"/>
-      <c r="K204" s="148"/>
-      <c r="L204" s="148"/>
-      <c r="M204" s="148"/>
-      <c r="N204" s="148"/>
-      <c r="O204" s="148"/>
-      <c r="P204" s="148"/>
-      <c r="Q204" s="148"/>
-      <c r="R204" s="148"/>
-      <c r="S204" s="148"/>
+      <c r="H204" s="159" t="s">
+        <v>294</v>
+      </c>
+      <c r="I204" s="2"/>
+      <c r="J204" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="K204" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="L204" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="M204" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="N204" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="O204" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="P204" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="Q204" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="R204" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="S204" s="31">
+        <v>13.3</v>
+      </c>
       <c r="T204" s="2"/>
       <c r="U204" s="2"/>
       <c r="V204" s="2"/>
@@ -35837,7 +35904,7 @@
       <c r="A205" s="1"/>
       <c r="B205" s="33"/>
       <c r="C205" s="73">
-        <f>INT(C$190+3)</f>
+        <f>INT(C$191+3)</f>
         <v>4</v>
       </c>
       <c r="D205" s="4"/>
@@ -35855,7 +35922,7 @@
       <c r="P205" s="148"/>
       <c r="Q205" s="148"/>
       <c r="R205" s="148"/>
-      <c r="S205" s="2"/>
+      <c r="S205" s="148"/>
       <c r="T205" s="2"/>
       <c r="U205" s="2"/>
       <c r="V205" s="2"/>
@@ -35869,50 +35936,48 @@
       <c r="AD205" s="1"/>
       <c r="AE205" s="1"/>
     </row>
-    <row r="206" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:31" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A206" s="1"/>
       <c r="B206" s="33"/>
       <c r="C206" s="73">
-        <f>INT($C$190)+3.005</f>
-        <v>4.0049999999999999</v>
+        <f>INT(C$191+3)</f>
+        <v>4</v>
       </c>
       <c r="D206" s="4"/>
-      <c r="E206" s="4"/>
-      <c r="F206" s="4"/>
+      <c r="E206" s="5"/>
+      <c r="F206" s="5"/>
       <c r="G206" s="4"/>
-      <c r="H206" s="4"/>
-      <c r="I206" s="4"/>
-      <c r="J206" s="4"/>
-      <c r="K206" s="4"/>
-      <c r="L206" s="4"/>
-      <c r="M206" s="4"/>
-      <c r="N206" s="4"/>
-      <c r="O206" s="4"/>
-      <c r="P206" s="4"/>
-      <c r="Q206" s="4"/>
-      <c r="R206" s="4"/>
-      <c r="S206" s="4"/>
-      <c r="T206" s="4"/>
-      <c r="U206" s="4"/>
-      <c r="V206" s="4"/>
-      <c r="W206" s="4"/>
-      <c r="X206" s="4"/>
-      <c r="Y206" s="4"/>
-      <c r="Z206" s="4"/>
-      <c r="AA206" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="H206" s="148"/>
+      <c r="I206" s="148"/>
+      <c r="J206" s="148"/>
+      <c r="K206" s="148"/>
+      <c r="L206" s="148"/>
+      <c r="M206" s="148"/>
+      <c r="N206" s="148"/>
+      <c r="O206" s="148"/>
+      <c r="P206" s="148"/>
+      <c r="Q206" s="148"/>
+      <c r="R206" s="148"/>
+      <c r="S206" s="2"/>
+      <c r="T206" s="2"/>
+      <c r="U206" s="2"/>
+      <c r="V206" s="2"/>
+      <c r="W206" s="2"/>
+      <c r="X206" s="2"/>
+      <c r="Y206" s="2"/>
+      <c r="Z206" s="2"/>
+      <c r="AA206" s="4"/>
       <c r="AB206" s="16"/>
       <c r="AC206" s="1"/>
       <c r="AD206" s="1"/>
       <c r="AE206" s="1"/>
     </row>
-    <row r="207" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A207" s="1"/>
       <c r="B207" s="33"/>
       <c r="C207" s="73">
-        <f>INT($C$190)+2.005</f>
-        <v>3.0049999999999999</v>
+        <f>INT($C$191)+3.005</f>
+        <v>4.0049999999999999</v>
       </c>
       <c r="D207" s="4"/>
       <c r="E207" s="4"/>
@@ -35937,126 +36002,131 @@
       <c r="X207" s="4"/>
       <c r="Y207" s="4"/>
       <c r="Z207" s="4"/>
-      <c r="AA207" s="4"/>
+      <c r="AA207" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="AB207" s="16"/>
       <c r="AC207" s="1"/>
       <c r="AD207" s="1"/>
       <c r="AE207" s="1"/>
     </row>
-    <row r="208" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A208" s="1"/>
-      <c r="B208" s="35"/>
-      <c r="C208" s="76">
-        <f>INT($C$190)+1.005</f>
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="D208" s="17"/>
-      <c r="E208" s="17"/>
-      <c r="F208" s="17"/>
-      <c r="G208" s="17"/>
-      <c r="H208" s="17"/>
-      <c r="I208" s="17"/>
-      <c r="J208" s="17"/>
-      <c r="K208" s="17"/>
-      <c r="L208" s="17"/>
-      <c r="M208" s="17"/>
-      <c r="N208" s="17"/>
-      <c r="O208" s="17"/>
-      <c r="P208" s="17"/>
-      <c r="Q208" s="17"/>
-      <c r="R208" s="17"/>
-      <c r="S208" s="17"/>
-      <c r="T208" s="17"/>
-      <c r="U208" s="17"/>
-      <c r="V208" s="17"/>
-      <c r="W208" s="17"/>
-      <c r="X208" s="17"/>
-      <c r="Y208" s="17"/>
-      <c r="Z208" s="17"/>
-      <c r="AA208" s="17"/>
-      <c r="AB208" s="18" t="s">
-        <v>1</v>
-      </c>
+      <c r="B208" s="33"/>
+      <c r="C208" s="73">
+        <f>INT($C$191)+2.005</f>
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="D208" s="4"/>
+      <c r="E208" s="4"/>
+      <c r="F208" s="4"/>
+      <c r="G208" s="4"/>
+      <c r="H208" s="4"/>
+      <c r="I208" s="4"/>
+      <c r="J208" s="4"/>
+      <c r="K208" s="4"/>
+      <c r="L208" s="4"/>
+      <c r="M208" s="4"/>
+      <c r="N208" s="4"/>
+      <c r="O208" s="4"/>
+      <c r="P208" s="4"/>
+      <c r="Q208" s="4"/>
+      <c r="R208" s="4"/>
+      <c r="S208" s="4"/>
+      <c r="T208" s="4"/>
+      <c r="U208" s="4"/>
+      <c r="V208" s="4"/>
+      <c r="W208" s="4"/>
+      <c r="X208" s="4"/>
+      <c r="Y208" s="4"/>
+      <c r="Z208" s="4"/>
+      <c r="AA208" s="4"/>
+      <c r="AB208" s="16"/>
       <c r="AC208" s="1"/>
       <c r="AD208" s="1"/>
       <c r="AE208" s="1"/>
     </row>
-    <row r="209" spans="1:31" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A209" s="1"/>
-      <c r="B209" s="19"/>
-      <c r="C209" s="77">
-        <f>INT($C$190)+0.005</f>
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="D209" s="19"/>
-      <c r="E209" s="19"/>
-      <c r="F209" s="19"/>
-      <c r="G209" s="19"/>
-      <c r="H209" s="19"/>
-      <c r="I209" s="19"/>
-      <c r="J209" s="19"/>
-      <c r="K209" s="19"/>
-      <c r="L209" s="19"/>
-      <c r="M209" s="19"/>
-      <c r="N209" s="19"/>
-      <c r="O209" s="19"/>
-      <c r="P209" s="19"/>
-      <c r="Q209" s="19"/>
-      <c r="R209" s="19"/>
-      <c r="S209" s="19"/>
-      <c r="T209" s="19"/>
-      <c r="U209" s="19"/>
-      <c r="V209" s="19"/>
-      <c r="W209" s="19"/>
-      <c r="X209" s="19"/>
-      <c r="Y209" s="19"/>
-      <c r="Z209" s="19"/>
-      <c r="AA209" s="19"/>
-      <c r="AB209" s="19"/>
+      <c r="B209" s="35"/>
+      <c r="C209" s="76">
+        <f>INT($C$191)+1.005</f>
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="D209" s="17"/>
+      <c r="E209" s="17"/>
+      <c r="F209" s="17"/>
+      <c r="G209" s="17"/>
+      <c r="H209" s="17"/>
+      <c r="I209" s="17"/>
+      <c r="J209" s="17"/>
+      <c r="K209" s="17"/>
+      <c r="L209" s="17"/>
+      <c r="M209" s="17"/>
+      <c r="N209" s="17"/>
+      <c r="O209" s="17"/>
+      <c r="P209" s="17"/>
+      <c r="Q209" s="17"/>
+      <c r="R209" s="17"/>
+      <c r="S209" s="17"/>
+      <c r="T209" s="17"/>
+      <c r="U209" s="17"/>
+      <c r="V209" s="17"/>
+      <c r="W209" s="17"/>
+      <c r="X209" s="17"/>
+      <c r="Y209" s="17"/>
+      <c r="Z209" s="17"/>
+      <c r="AA209" s="17"/>
+      <c r="AB209" s="18" t="s">
+        <v>1</v>
+      </c>
       <c r="AC209" s="1"/>
       <c r="AD209" s="1"/>
       <c r="AE209" s="1"/>
     </row>
-    <row r="210" spans="1:31" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:31" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="1"/>
-      <c r="B210" s="1"/>
-      <c r="C210" s="73">
-        <f>INT($C$190)+2</f>
-        <v>3</v>
-      </c>
-      <c r="D210" s="1"/>
-      <c r="E210" s="1"/>
-      <c r="F210" s="1"/>
-      <c r="G210" s="1"/>
-      <c r="H210" s="1"/>
-      <c r="I210" s="1"/>
-      <c r="J210" s="1"/>
-      <c r="K210" s="1"/>
-      <c r="L210" s="1"/>
-      <c r="M210" s="1"/>
-      <c r="N210" s="1"/>
-      <c r="O210" s="1"/>
-      <c r="P210" s="1"/>
-      <c r="Q210" s="1"/>
-      <c r="R210" s="1"/>
-      <c r="S210" s="1"/>
-      <c r="T210" s="1"/>
-      <c r="U210" s="1"/>
-      <c r="V210" s="1"/>
-      <c r="W210" s="1"/>
-      <c r="X210" s="1"/>
-      <c r="Y210" s="1"/>
-      <c r="Z210" s="1"/>
-      <c r="AA210" s="1"/>
-      <c r="AB210" s="1"/>
+      <c r="B210" s="19"/>
+      <c r="C210" s="77">
+        <f>INT($C$191)+0.005</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D210" s="19"/>
+      <c r="E210" s="19"/>
+      <c r="F210" s="19"/>
+      <c r="G210" s="19"/>
+      <c r="H210" s="19"/>
+      <c r="I210" s="19"/>
+      <c r="J210" s="19"/>
+      <c r="K210" s="19"/>
+      <c r="L210" s="19"/>
+      <c r="M210" s="19"/>
+      <c r="N210" s="19"/>
+      <c r="O210" s="19"/>
+      <c r="P210" s="19"/>
+      <c r="Q210" s="19"/>
+      <c r="R210" s="19"/>
+      <c r="S210" s="19"/>
+      <c r="T210" s="19"/>
+      <c r="U210" s="19"/>
+      <c r="V210" s="19"/>
+      <c r="W210" s="19"/>
+      <c r="X210" s="19"/>
+      <c r="Y210" s="19"/>
+      <c r="Z210" s="19"/>
+      <c r="AA210" s="19"/>
+      <c r="AB210" s="19"/>
       <c r="AC210" s="1"/>
       <c r="AD210" s="1"/>
       <c r="AE210" s="1"/>
     </row>
-    <row r="211" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:31" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A211" s="1"/>
       <c r="B211" s="1"/>
-      <c r="C211" s="66"/>
+      <c r="C211" s="73">
+        <f>INT($C$191)+2</f>
+        <v>3</v>
+      </c>
       <c r="D211" s="1"/>
       <c r="E211" s="1"/>
       <c r="F211" s="1"/>
@@ -36252,7 +36322,40 @@
       <c r="AE216" s="1"/>
     </row>
     <row r="217" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="C217" s="72" t="s">
+      <c r="A217" s="1"/>
+      <c r="B217" s="1"/>
+      <c r="C217" s="66"/>
+      <c r="D217" s="1"/>
+      <c r="E217" s="1"/>
+      <c r="F217" s="1"/>
+      <c r="G217" s="1"/>
+      <c r="H217" s="1"/>
+      <c r="I217" s="1"/>
+      <c r="J217" s="1"/>
+      <c r="K217" s="1"/>
+      <c r="L217" s="1"/>
+      <c r="M217" s="1"/>
+      <c r="N217" s="1"/>
+      <c r="O217" s="1"/>
+      <c r="P217" s="1"/>
+      <c r="Q217" s="1"/>
+      <c r="R217" s="1"/>
+      <c r="S217" s="1"/>
+      <c r="T217" s="1"/>
+      <c r="U217" s="1"/>
+      <c r="V217" s="1"/>
+      <c r="W217" s="1"/>
+      <c r="X217" s="1"/>
+      <c r="Y217" s="1"/>
+      <c r="Z217" s="1"/>
+      <c r="AA217" s="1"/>
+      <c r="AB217" s="1"/>
+      <c r="AC217" s="1"/>
+      <c r="AD217" s="1"/>
+      <c r="AE217" s="1"/>
+    </row>
+    <row r="218" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="C218" s="72" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
From Master: Add cfat (carcase fat depth) as a REV trait. Change function fs = f(cs)
(cherry picked from commit bb6c7afd9bcd72ccbdc108654903fc0a7c6ab404)
</commit_message>
<xml_diff>
--- a/ExcelInputs/Structural.xlsx
+++ b/ExcelInputs/Structural.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\ExcelInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881A3E01-523A-4AE0-8398-340D2095183E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881CAD0C-540B-46BD-A1D2-027955337C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
@@ -92,7 +92,7 @@
     <definedName name="i_lag_organs">Stock!$I$70</definedName>
     <definedName name="i_lag_wool">Stock!$I$69</definedName>
     <definedName name="i_landuse_is_dual" localSheetId="0">General!$Q$79:$Q$109</definedName>
-    <definedName name="i_len_f">StructuralSA!$I$199</definedName>
+    <definedName name="i_len_f">StructuralSA!$I$200</definedName>
     <definedName name="i_len_l">Stock!$M$160</definedName>
     <definedName name="i_len_m">Stock!$L$160</definedName>
     <definedName name="i_len_q" localSheetId="2">StructuralSA!$M$44</definedName>
@@ -121,8 +121,8 @@
     <definedName name="i_nut_spread_n0" localSheetId="2">StructuralSA!$J$115</definedName>
     <definedName name="i_nut_spread_n1" localSheetId="2">StructuralSA!$M$115:$M$122</definedName>
     <definedName name="i_nut_spread_n3" localSheetId="2">StructuralSA!$S$115:$S$122</definedName>
-    <definedName name="i_nv_lower_p6">StructuralSA!$J$202:$S$202</definedName>
-    <definedName name="i_nv_upper_p6">StructuralSA!$J$203:$S$203</definedName>
+    <definedName name="i_nv_lower_p6">StructuralSA!$J$203:$S$203</definedName>
+    <definedName name="i_nv_upper_p6">StructuralSA!$J$204:$S$204</definedName>
     <definedName name="i_offs_sale_method" localSheetId="2">StructuralSA!$R$42</definedName>
     <definedName name="i_offs_sale_opportunities_per_dvp" localSheetId="2">StructuralSA!$R$43</definedName>
     <definedName name="i_offs_user_fvp_date_iu" localSheetId="2">StructuralSA!$P$82:$R$84</definedName>
@@ -132,8 +132,8 @@
     <definedName name="i_r2adjust_inc">StructuralSA!$U$148</definedName>
     <definedName name="i_rev_age_stage" localSheetId="2">StructuralSA!$N$159:$Z$160</definedName>
     <definedName name="i_rev_number" localSheetId="2">StructuralSA!$I$150</definedName>
-    <definedName name="i_rev_trait_name" localSheetId="2">StructuralSA!$H$162:$H$178</definedName>
-    <definedName name="i_rev_trait_scenario" localSheetId="2">StructuralSA!$I$162:$I$178</definedName>
+    <definedName name="i_rev_trait_name" localSheetId="2">StructuralSA!$H$162:$H$179</definedName>
+    <definedName name="i_rev_trait_scenario" localSheetId="2">StructuralSA!$I$162:$I$179</definedName>
     <definedName name="i_rev_update" localSheetId="2">StructuralSA!$I$148</definedName>
     <definedName name="i_sim_periods_year">Stock!$I$62</definedName>
     <definedName name="i_store_cs_rep" localSheetId="3">'Report Settings'!$K$18</definedName>
@@ -2382,7 +2382,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="H199" authorId="2" shapeId="0" xr:uid="{B39EFDC6-7ABB-4808-93B1-2819F2755236}">
+    <comment ref="H179" authorId="2" shapeId="0" xr:uid="{7D72CFA0-EF47-40D9-9D6F-9FDC3F1C19F9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>John:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Carcase fat depth</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H200" authorId="2" shapeId="0" xr:uid="{B39EFDC6-7ABB-4808-93B1-2819F2755236}">
       <text>
         <r>
           <rPr>
@@ -2406,7 +2430,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H202" authorId="2" shapeId="0" xr:uid="{315CC92D-C01A-4D16-90CA-458397130ECA}">
+    <comment ref="H203" authorId="2" shapeId="0" xr:uid="{315CC92D-C01A-4D16-90CA-458397130ECA}">
       <text>
         <r>
           <rPr>
@@ -2432,7 +2456,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H203" authorId="2" shapeId="0" xr:uid="{24292EB5-78CD-4E29-870F-1743067DEF27}">
+    <comment ref="H204" authorId="2" shapeId="0" xr:uid="{24292EB5-78CD-4E29-870F-1743067DEF27}">
       <text>
         <r>
           <rPr>
@@ -2497,7 +2521,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="449">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -3933,7 +3957,21 @@
     <t>11 - A</t>
   </si>
   <si>
-    <t>6Sep24: Alter order of age stages so that whole of life is [0] - which is the default in the code.
+    <t>22Sep24: Change the yearling End Age to 425 days (so that ewe lambs mated at 9mo can be altered by the yearling ERA)
+9May24: Change Offs sale method to 0 so that pkl_fs for the NFS would work (temporary change)
+27May23: Alter FVP6 to be beginning of the PregTox period rather than end of joining
+30Sep22: Alter the inputs for the user defined FVP dates, changed to a calculation based on TOL, a 91 day weaning and 126 days from weaning to next joining
+8Jun22: Change the range of the LW for the initial animals.
+18Mar22: Change the default r2_inc to False now that a pickled feed supply is working.
+20May21: Make the extra nut_spread_g1 = 0.1
+1Apr19: Blank worksheet</t>
+  </si>
+  <si>
+    <t>cfat</t>
+  </si>
+  <si>
+    <t>26Sep24: Add cfat (carcase fat depth) trait
+6Sep24: Alter order of age stages so that whole of life is [0] - which is the default in the code.
 5Sep24: Altered descriptions for the age stages to include a value because the stage needs to be defined by a number
 4Sep24: Added wbec as a REV trait (#16). Add age stage information
 28Aug24: Improve commenting on the weaning period wrt user defined periods
@@ -3962,16 +4000,6 @@
                    Moved FVP &amp; N inputs from Stock
 1: 1Apr19-Created the version control table</t>
   </si>
-  <si>
-    <t>22Sep24: Change the yearling End Age to 425 days (so that ewe lambs mated at 9mo can be altered by the yearling ERA)
-9May24: Change Offs sale method to 0 so that pkl_fs for the NFS would work (temporary change)
-27May23: Alter FVP6 to be beginning of the PregTox period rather than end of joining
-30Sep22: Alter the inputs for the user defined FVP dates, changed to a calculation based on TOL, a 91 day weaning and 126 days from weaning to next joining
-8Jun22: Change the range of the LW for the initial animals.
-18Mar22: Change the default r2_inc to False now that a pickled feed supply is working.
-20May21: Make the extra nut_spread_g1 = 0.1
-1Apr19: Blank worksheet</t>
-  </si>
 </sst>
 </file>
 
@@ -3983,7 +4011,7 @@
     <numFmt numFmtId="166" formatCode="0.00_)"/>
     <numFmt numFmtId="167" formatCode="[$-C09]dd\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4202,6 +4230,19 @@
       <color rgb="FF0000CC"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="40">
@@ -27115,14 +27156,14 @@
   <sheetPr codeName="Sheet3">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AE217"/>
+  <dimension ref="A1:AE218"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J151" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="10" topLeftCell="J139" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="J14" sqref="J14:T14"/>
+      <selection pane="bottomRight" activeCell="J13" sqref="J13:T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -27653,10 +27694,10 @@
         <v>16</v>
       </c>
       <c r="I13" s="126">
-        <v>45541.344751273202</v>
+        <v>45561.574224305601</v>
       </c>
       <c r="J13" s="222" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="K13" s="223"/>
       <c r="L13" s="223"/>
@@ -27698,7 +27739,7 @@
         <v>45557.353121412001</v>
       </c>
       <c r="J14" s="225" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="K14" s="226"/>
       <c r="L14" s="226"/>
@@ -32940,7 +32981,7 @@
       <c r="A139" s="1"/>
       <c r="B139" s="33"/>
       <c r="C139" s="73">
-        <f>INT(MAX($C$147:$C$181))+1</f>
+        <f>INT(MAX($C$147:$C$182))+1</f>
         <v>5</v>
       </c>
       <c r="D139" s="3"/>
@@ -34019,7 +34060,7 @@
       <c r="A163" s="1"/>
       <c r="B163" s="33"/>
       <c r="C163" s="73">
-        <f t="shared" ref="C163:C178" si="17">INT(C$140+3)</f>
+        <f t="shared" ref="C163:C179" si="17">INT(C$140+3)</f>
         <v>4</v>
       </c>
       <c r="D163" s="4"/>
@@ -34760,39 +34801,39 @@
       <c r="K178" s="148"/>
       <c r="L178" s="148"/>
       <c r="M178" s="148"/>
-      <c r="N178" s="218" t="s">
+      <c r="N178" s="56" t="s">
         <v>430</v>
       </c>
-      <c r="O178" s="217"/>
-      <c r="P178" s="217"/>
-      <c r="Q178" s="218" t="s">
+      <c r="O178" s="148"/>
+      <c r="P178" s="148"/>
+      <c r="Q178" s="56" t="s">
         <v>430</v>
       </c>
-      <c r="R178" s="218" t="s">
+      <c r="R178" s="56" t="s">
         <v>430</v>
       </c>
-      <c r="S178" s="218" t="s">
+      <c r="S178" s="56" t="s">
         <v>430</v>
       </c>
-      <c r="T178" s="218" t="s">
+      <c r="T178" s="56" t="s">
         <v>430</v>
       </c>
-      <c r="U178" s="218" t="s">
+      <c r="U178" s="56" t="s">
         <v>430</v>
       </c>
-      <c r="V178" s="218" t="s">
+      <c r="V178" s="56" t="s">
         <v>430</v>
       </c>
-      <c r="W178" s="218" t="s">
+      <c r="W178" s="56" t="s">
         <v>430</v>
       </c>
-      <c r="X178" s="218" t="s">
+      <c r="X178" s="56" t="s">
         <v>430</v>
       </c>
-      <c r="Y178" s="218" t="s">
+      <c r="Y178" s="56" t="s">
         <v>430</v>
       </c>
-      <c r="Z178" s="218"/>
+      <c r="Z178" s="56"/>
       <c r="AA178" s="4"/>
       <c r="AB178" s="16"/>
       <c r="AC178" s="1"/>
@@ -34803,32 +34844,58 @@
       <c r="A179" s="1"/>
       <c r="B179" s="33"/>
       <c r="C179" s="73">
-        <f>INT(C$140+3)</f>
+        <f t="shared" si="17"/>
         <v>4</v>
       </c>
       <c r="D179" s="4"/>
-      <c r="E179" s="5"/>
+      <c r="E179" s="5">
+        <v>17</v>
+      </c>
       <c r="F179" s="5"/>
       <c r="G179" s="4"/>
-      <c r="H179" s="148"/>
-      <c r="I179" s="148"/>
+      <c r="H179" s="31" t="s">
+        <v>447</v>
+      </c>
+      <c r="I179" s="31">
+        <v>0</v>
+      </c>
       <c r="J179" s="148"/>
       <c r="K179" s="148"/>
       <c r="L179" s="148"/>
       <c r="M179" s="148"/>
-      <c r="N179" s="216"/>
-      <c r="O179" s="216"/>
-      <c r="P179" s="216"/>
-      <c r="Q179" s="216"/>
-      <c r="R179" s="216"/>
-      <c r="S179" s="53"/>
-      <c r="T179" s="53"/>
-      <c r="U179" s="53"/>
-      <c r="V179" s="53"/>
-      <c r="W179" s="53"/>
-      <c r="X179" s="53"/>
-      <c r="Y179" s="53"/>
-      <c r="Z179" s="53"/>
+      <c r="N179" s="218" t="s">
+        <v>430</v>
+      </c>
+      <c r="O179" s="217"/>
+      <c r="P179" s="217"/>
+      <c r="Q179" s="218" t="s">
+        <v>430</v>
+      </c>
+      <c r="R179" s="218" t="s">
+        <v>430</v>
+      </c>
+      <c r="S179" s="218" t="s">
+        <v>430</v>
+      </c>
+      <c r="T179" s="218" t="s">
+        <v>430</v>
+      </c>
+      <c r="U179" s="218" t="s">
+        <v>430</v>
+      </c>
+      <c r="V179" s="218" t="s">
+        <v>430</v>
+      </c>
+      <c r="W179" s="218" t="s">
+        <v>430</v>
+      </c>
+      <c r="X179" s="218" t="s">
+        <v>430</v>
+      </c>
+      <c r="Y179" s="218" t="s">
+        <v>430</v>
+      </c>
+      <c r="Z179" s="218"/>
       <c r="AA179" s="4"/>
       <c r="AB179" s="16"/>
       <c r="AC179" s="1"/>
@@ -34852,69 +34919,67 @@
       <c r="K180" s="148"/>
       <c r="L180" s="148"/>
       <c r="M180" s="148"/>
-      <c r="N180" s="148"/>
-      <c r="O180" s="148"/>
-      <c r="P180" s="148"/>
-      <c r="Q180" s="148"/>
-      <c r="R180" s="148"/>
-      <c r="S180" s="2"/>
-      <c r="T180" s="2"/>
-      <c r="U180" s="2"/>
-      <c r="V180" s="2"/>
-      <c r="W180" s="2"/>
-      <c r="X180" s="2"/>
-      <c r="Y180" s="2"/>
-      <c r="Z180" s="2"/>
+      <c r="N180" s="216"/>
+      <c r="O180" s="216"/>
+      <c r="P180" s="216"/>
+      <c r="Q180" s="216"/>
+      <c r="R180" s="216"/>
+      <c r="S180" s="53"/>
+      <c r="T180" s="53"/>
+      <c r="U180" s="53"/>
+      <c r="V180" s="53"/>
+      <c r="W180" s="53"/>
+      <c r="X180" s="53"/>
+      <c r="Y180" s="53"/>
+      <c r="Z180" s="53"/>
       <c r="AA180" s="4"/>
       <c r="AB180" s="16"/>
       <c r="AC180" s="1"/>
       <c r="AD180" s="1"/>
       <c r="AE180" s="1"/>
     </row>
-    <row r="181" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:31" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181" s="33"/>
       <c r="C181" s="73">
-        <f>INT($C$140)+3.005</f>
-        <v>4.0049999999999999</v>
+        <f>INT(C$140+3)</f>
+        <v>4</v>
       </c>
       <c r="D181" s="4"/>
-      <c r="E181" s="4"/>
-      <c r="F181" s="4"/>
+      <c r="E181" s="5"/>
+      <c r="F181" s="5"/>
       <c r="G181" s="4"/>
-      <c r="H181" s="4"/>
-      <c r="I181" s="4"/>
-      <c r="J181" s="4"/>
-      <c r="K181" s="4"/>
-      <c r="L181" s="4"/>
-      <c r="M181" s="4"/>
-      <c r="N181" s="4"/>
-      <c r="O181" s="4"/>
-      <c r="P181" s="4"/>
-      <c r="Q181" s="4"/>
-      <c r="R181" s="4"/>
-      <c r="S181" s="4"/>
-      <c r="T181" s="4"/>
-      <c r="U181" s="4"/>
-      <c r="V181" s="4"/>
-      <c r="W181" s="4"/>
-      <c r="X181" s="4"/>
-      <c r="Y181" s="4"/>
-      <c r="Z181" s="4"/>
-      <c r="AA181" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="H181" s="148"/>
+      <c r="I181" s="148"/>
+      <c r="J181" s="148"/>
+      <c r="K181" s="148"/>
+      <c r="L181" s="148"/>
+      <c r="M181" s="148"/>
+      <c r="N181" s="148"/>
+      <c r="O181" s="148"/>
+      <c r="P181" s="148"/>
+      <c r="Q181" s="148"/>
+      <c r="R181" s="148"/>
+      <c r="S181" s="2"/>
+      <c r="T181" s="2"/>
+      <c r="U181" s="2"/>
+      <c r="V181" s="2"/>
+      <c r="W181" s="2"/>
+      <c r="X181" s="2"/>
+      <c r="Y181" s="2"/>
+      <c r="Z181" s="2"/>
+      <c r="AA181" s="4"/>
       <c r="AB181" s="16"/>
       <c r="AC181" s="1"/>
       <c r="AD181" s="1"/>
       <c r="AE181" s="1"/>
     </row>
-    <row r="182" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182" s="33"/>
       <c r="C182" s="73">
-        <f>INT($C$140)+2.005</f>
-        <v>3.0049999999999999</v>
+        <f>INT($C$140)+3.005</f>
+        <v>4.0049999999999999</v>
       </c>
       <c r="D182" s="4"/>
       <c r="E182" s="4"/>
@@ -34939,118 +35004,120 @@
       <c r="X182" s="4"/>
       <c r="Y182" s="4"/>
       <c r="Z182" s="4"/>
-      <c r="AA182" s="4"/>
+      <c r="AA182" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="AB182" s="16"/>
       <c r="AC182" s="1"/>
       <c r="AD182" s="1"/>
       <c r="AE182" s="1"/>
     </row>
-    <row r="183" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
-      <c r="B183" s="35"/>
-      <c r="C183" s="76">
-        <f>INT($C$140)+1.005</f>
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="D183" s="17"/>
-      <c r="E183" s="17"/>
-      <c r="F183" s="17"/>
-      <c r="G183" s="17"/>
-      <c r="H183" s="17"/>
-      <c r="I183" s="17"/>
-      <c r="J183" s="17"/>
-      <c r="K183" s="17"/>
-      <c r="L183" s="17"/>
-      <c r="M183" s="17"/>
-      <c r="N183" s="17"/>
-      <c r="O183" s="17"/>
-      <c r="P183" s="17"/>
-      <c r="Q183" s="17"/>
-      <c r="R183" s="17"/>
-      <c r="S183" s="17"/>
-      <c r="T183" s="17"/>
-      <c r="U183" s="17"/>
-      <c r="V183" s="17"/>
-      <c r="W183" s="17"/>
-      <c r="X183" s="17"/>
-      <c r="Y183" s="17"/>
-      <c r="Z183" s="17"/>
-      <c r="AA183" s="17"/>
-      <c r="AB183" s="18" t="s">
-        <v>1</v>
-      </c>
+      <c r="B183" s="33"/>
+      <c r="C183" s="73">
+        <f>INT($C$140)+2.005</f>
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="D183" s="4"/>
+      <c r="E183" s="4"/>
+      <c r="F183" s="4"/>
+      <c r="G183" s="4"/>
+      <c r="H183" s="4"/>
+      <c r="I183" s="4"/>
+      <c r="J183" s="4"/>
+      <c r="K183" s="4"/>
+      <c r="L183" s="4"/>
+      <c r="M183" s="4"/>
+      <c r="N183" s="4"/>
+      <c r="O183" s="4"/>
+      <c r="P183" s="4"/>
+      <c r="Q183" s="4"/>
+      <c r="R183" s="4"/>
+      <c r="S183" s="4"/>
+      <c r="T183" s="4"/>
+      <c r="U183" s="4"/>
+      <c r="V183" s="4"/>
+      <c r="W183" s="4"/>
+      <c r="X183" s="4"/>
+      <c r="Y183" s="4"/>
+      <c r="Z183" s="4"/>
+      <c r="AA183" s="4"/>
+      <c r="AB183" s="16"/>
       <c r="AC183" s="1"/>
       <c r="AD183" s="1"/>
       <c r="AE183" s="1"/>
     </row>
-    <row r="184" spans="1:31" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
-      <c r="B184" s="19"/>
-      <c r="C184" s="77">
-        <f>INT($C$140)+0.005</f>
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="D184" s="19"/>
-      <c r="E184" s="19"/>
-      <c r="F184" s="19"/>
-      <c r="G184" s="19"/>
-      <c r="H184" s="19"/>
-      <c r="I184" s="19"/>
-      <c r="J184" s="19"/>
-      <c r="K184" s="19"/>
-      <c r="L184" s="19"/>
-      <c r="M184" s="19"/>
-      <c r="N184" s="19"/>
-      <c r="O184" s="19"/>
-      <c r="P184" s="19"/>
-      <c r="Q184" s="19"/>
-      <c r="R184" s="19"/>
-      <c r="S184" s="19"/>
-      <c r="T184" s="19"/>
-      <c r="U184" s="19"/>
-      <c r="V184" s="19"/>
-      <c r="W184" s="19"/>
-      <c r="X184" s="19"/>
-      <c r="Y184" s="19"/>
-      <c r="Z184" s="19"/>
-      <c r="AA184" s="19"/>
-      <c r="AB184" s="19"/>
+      <c r="B184" s="35"/>
+      <c r="C184" s="76">
+        <f>INT($C$140)+1.005</f>
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="D184" s="17"/>
+      <c r="E184" s="17"/>
+      <c r="F184" s="17"/>
+      <c r="G184" s="17"/>
+      <c r="H184" s="17"/>
+      <c r="I184" s="17"/>
+      <c r="J184" s="17"/>
+      <c r="K184" s="17"/>
+      <c r="L184" s="17"/>
+      <c r="M184" s="17"/>
+      <c r="N184" s="17"/>
+      <c r="O184" s="17"/>
+      <c r="P184" s="17"/>
+      <c r="Q184" s="17"/>
+      <c r="R184" s="17"/>
+      <c r="S184" s="17"/>
+      <c r="T184" s="17"/>
+      <c r="U184" s="17"/>
+      <c r="V184" s="17"/>
+      <c r="W184" s="17"/>
+      <c r="X184" s="17"/>
+      <c r="Y184" s="17"/>
+      <c r="Z184" s="17"/>
+      <c r="AA184" s="17"/>
+      <c r="AB184" s="18" t="s">
+        <v>1</v>
+      </c>
       <c r="AC184" s="1"/>
       <c r="AD184" s="1"/>
       <c r="AE184" s="1"/>
     </row>
-    <row r="185" spans="1:31" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:31" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
-      <c r="B185" s="1"/>
-      <c r="C185" s="73">
-        <f>INT($C$140)+2</f>
-        <v>3</v>
-      </c>
-      <c r="D185" s="1"/>
-      <c r="E185" s="1"/>
-      <c r="F185" s="1"/>
-      <c r="G185" s="1"/>
-      <c r="H185" s="1"/>
-      <c r="I185" s="1"/>
-      <c r="J185" s="1"/>
-      <c r="K185" s="1"/>
-      <c r="L185" s="1"/>
-      <c r="M185" s="1"/>
-      <c r="N185" s="1"/>
-      <c r="O185" s="1"/>
-      <c r="P185" s="1"/>
-      <c r="Q185" s="1"/>
-      <c r="R185" s="1"/>
-      <c r="S185" s="1"/>
-      <c r="T185" s="1"/>
-      <c r="U185" s="1"/>
-      <c r="V185" s="1"/>
-      <c r="W185" s="1"/>
-      <c r="X185" s="1"/>
-      <c r="Y185" s="1"/>
-      <c r="Z185" s="1"/>
-      <c r="AA185" s="1"/>
-      <c r="AB185" s="1"/>
+      <c r="B185" s="19"/>
+      <c r="C185" s="77">
+        <f>INT($C$140)+0.005</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D185" s="19"/>
+      <c r="E185" s="19"/>
+      <c r="F185" s="19"/>
+      <c r="G185" s="19"/>
+      <c r="H185" s="19"/>
+      <c r="I185" s="19"/>
+      <c r="J185" s="19"/>
+      <c r="K185" s="19"/>
+      <c r="L185" s="19"/>
+      <c r="M185" s="19"/>
+      <c r="N185" s="19"/>
+      <c r="O185" s="19"/>
+      <c r="P185" s="19"/>
+      <c r="Q185" s="19"/>
+      <c r="R185" s="19"/>
+      <c r="S185" s="19"/>
+      <c r="T185" s="19"/>
+      <c r="U185" s="19"/>
+      <c r="V185" s="19"/>
+      <c r="W185" s="19"/>
+      <c r="X185" s="19"/>
+      <c r="Y185" s="19"/>
+      <c r="Z185" s="19"/>
+      <c r="AA185" s="19"/>
+      <c r="AB185" s="19"/>
       <c r="AC185" s="1"/>
       <c r="AD185" s="1"/>
       <c r="AE185" s="1"/>
@@ -35059,7 +35126,7 @@
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="73">
-        <f>INT($C$190)+2</f>
+        <f>INT($C$140)+2</f>
         <v>3</v>
       </c>
       <c r="D186" s="1"/>
@@ -35091,266 +35158,264 @@
       <c r="AD186" s="1"/>
       <c r="AE186" s="1"/>
     </row>
-    <row r="187" spans="1:31" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:31" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
-      <c r="B187" s="20"/>
-      <c r="C187" s="74">
-        <f>INT($C$190)+0.005</f>
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="D187" s="20"/>
-      <c r="E187" s="20"/>
-      <c r="F187" s="20"/>
-      <c r="G187" s="20"/>
-      <c r="H187" s="20"/>
-      <c r="I187" s="20"/>
-      <c r="J187" s="20"/>
-      <c r="K187" s="20"/>
-      <c r="L187" s="20"/>
-      <c r="M187" s="20"/>
-      <c r="N187" s="20"/>
-      <c r="O187" s="20"/>
-      <c r="P187" s="20"/>
-      <c r="Q187" s="20"/>
-      <c r="R187" s="20"/>
-      <c r="S187" s="20"/>
-      <c r="T187" s="20"/>
-      <c r="U187" s="20"/>
-      <c r="V187" s="20"/>
-      <c r="W187" s="20"/>
-      <c r="X187" s="20"/>
-      <c r="Y187" s="20"/>
-      <c r="Z187" s="20"/>
-      <c r="AA187" s="20"/>
-      <c r="AB187" s="20"/>
+      <c r="B187" s="1"/>
+      <c r="C187" s="73">
+        <f>INT($C$191)+2</f>
+        <v>3</v>
+      </c>
+      <c r="D187" s="1"/>
+      <c r="E187" s="1"/>
+      <c r="F187" s="1"/>
+      <c r="G187" s="1"/>
+      <c r="H187" s="1"/>
+      <c r="I187" s="1"/>
+      <c r="J187" s="1"/>
+      <c r="K187" s="1"/>
+      <c r="L187" s="1"/>
+      <c r="M187" s="1"/>
+      <c r="N187" s="1"/>
+      <c r="O187" s="1"/>
+      <c r="P187" s="1"/>
+      <c r="Q187" s="1"/>
+      <c r="R187" s="1"/>
+      <c r="S187" s="1"/>
+      <c r="T187" s="1"/>
+      <c r="U187" s="1"/>
+      <c r="V187" s="1"/>
+      <c r="W187" s="1"/>
+      <c r="X187" s="1"/>
+      <c r="Y187" s="1"/>
+      <c r="Z187" s="1"/>
+      <c r="AA187" s="1"/>
+      <c r="AB187" s="1"/>
       <c r="AC187" s="1"/>
       <c r="AD187" s="1"/>
       <c r="AE187" s="1"/>
     </row>
-    <row r="188" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:31" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="1"/>
-      <c r="B188" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="C188" s="75">
-        <f>INT($C$190)+1.005</f>
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="D188" s="14"/>
-      <c r="E188" s="14"/>
-      <c r="F188" s="14"/>
-      <c r="G188" s="14"/>
-      <c r="H188" s="14"/>
-      <c r="I188" s="14"/>
-      <c r="J188" s="14"/>
-      <c r="K188" s="14"/>
-      <c r="L188" s="14"/>
-      <c r="M188" s="14"/>
-      <c r="N188" s="14"/>
-      <c r="O188" s="14"/>
-      <c r="P188" s="14"/>
-      <c r="Q188" s="14"/>
-      <c r="R188" s="14"/>
-      <c r="S188" s="14"/>
-      <c r="T188" s="14"/>
-      <c r="U188" s="14"/>
-      <c r="V188" s="14"/>
-      <c r="W188" s="14"/>
-      <c r="X188" s="14"/>
-      <c r="Y188" s="14"/>
-      <c r="Z188" s="14"/>
-      <c r="AA188" s="14"/>
-      <c r="AB188" s="15"/>
+      <c r="B188" s="20"/>
+      <c r="C188" s="74">
+        <f>INT($C$191)+0.005</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D188" s="20"/>
+      <c r="E188" s="20"/>
+      <c r="F188" s="20"/>
+      <c r="G188" s="20"/>
+      <c r="H188" s="20"/>
+      <c r="I188" s="20"/>
+      <c r="J188" s="20"/>
+      <c r="K188" s="20"/>
+      <c r="L188" s="20"/>
+      <c r="M188" s="20"/>
+      <c r="N188" s="20"/>
+      <c r="O188" s="20"/>
+      <c r="P188" s="20"/>
+      <c r="Q188" s="20"/>
+      <c r="R188" s="20"/>
+      <c r="S188" s="20"/>
+      <c r="T188" s="20"/>
+      <c r="U188" s="20"/>
+      <c r="V188" s="20"/>
+      <c r="W188" s="20"/>
+      <c r="X188" s="20"/>
+      <c r="Y188" s="20"/>
+      <c r="Z188" s="20"/>
+      <c r="AA188" s="20"/>
+      <c r="AB188" s="20"/>
       <c r="AC188" s="1"/>
       <c r="AD188" s="1"/>
       <c r="AE188" s="1"/>
     </row>
-    <row r="189" spans="1:31" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
-      <c r="B189" s="33"/>
-      <c r="C189" s="73">
-        <f>INT(MAX($C$198:$C$206))+1</f>
-        <v>5</v>
-      </c>
-      <c r="D189" s="3"/>
-      <c r="E189" s="3"/>
-      <c r="F189" s="3"/>
-      <c r="G189" s="3"/>
-      <c r="H189" s="27"/>
-      <c r="I189" s="27"/>
-      <c r="J189" s="27"/>
-      <c r="K189" s="27"/>
-      <c r="L189" s="27"/>
-      <c r="M189" s="27"/>
-      <c r="N189" s="27"/>
-      <c r="O189" s="27"/>
-      <c r="P189" s="27"/>
-      <c r="Q189" s="27"/>
-      <c r="R189" s="27"/>
-      <c r="S189" s="27"/>
-      <c r="T189" s="27"/>
-      <c r="U189" s="27"/>
-      <c r="V189" s="27"/>
-      <c r="W189" s="27"/>
-      <c r="X189" s="27"/>
-      <c r="Y189" s="27"/>
-      <c r="Z189" s="27"/>
-      <c r="AA189" s="3"/>
-      <c r="AB189" s="16"/>
+      <c r="B189" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C189" s="75">
+        <f>INT($C$191)+1.005</f>
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="D189" s="14"/>
+      <c r="E189" s="14"/>
+      <c r="F189" s="14"/>
+      <c r="G189" s="14"/>
+      <c r="H189" s="14"/>
+      <c r="I189" s="14"/>
+      <c r="J189" s="14"/>
+      <c r="K189" s="14"/>
+      <c r="L189" s="14"/>
+      <c r="M189" s="14"/>
+      <c r="N189" s="14"/>
+      <c r="O189" s="14"/>
+      <c r="P189" s="14"/>
+      <c r="Q189" s="14"/>
+      <c r="R189" s="14"/>
+      <c r="S189" s="14"/>
+      <c r="T189" s="14"/>
+      <c r="U189" s="14"/>
+      <c r="V189" s="14"/>
+      <c r="W189" s="14"/>
+      <c r="X189" s="14"/>
+      <c r="Y189" s="14"/>
+      <c r="Z189" s="14"/>
+      <c r="AA189" s="14"/>
+      <c r="AB189" s="15"/>
       <c r="AC189" s="1"/>
       <c r="AD189" s="1"/>
       <c r="AE189" s="1"/>
     </row>
-    <row r="190" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:31" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
       <c r="B190" s="33"/>
       <c r="C190" s="73">
-        <v>1.02</v>
-      </c>
-      <c r="D190" s="21"/>
-      <c r="E190" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="F190" s="25"/>
-      <c r="G190" s="12"/>
-      <c r="H190" s="147" t="str">
-        <f>COUNTIFS($B$1:$B190, "«")&amp;" Feed Pool definitions"</f>
-        <v>6 Feed Pool definitions</v>
-      </c>
-      <c r="I190" s="6"/>
-      <c r="J190" s="6"/>
-      <c r="K190" s="6"/>
-      <c r="L190" s="6"/>
-      <c r="M190" s="6"/>
-      <c r="N190" s="6"/>
-      <c r="O190" s="6"/>
-      <c r="P190" s="6"/>
-      <c r="Q190" s="6"/>
-      <c r="R190" s="6"/>
-      <c r="S190" s="6"/>
-      <c r="T190" s="6"/>
-      <c r="U190" s="6"/>
-      <c r="V190" s="6"/>
-      <c r="W190" s="6"/>
-      <c r="X190" s="6"/>
-      <c r="Y190" s="6"/>
-      <c r="Z190" s="6"/>
-      <c r="AA190" s="10"/>
+        <f>INT(MAX($C$199:$C$207))+1</f>
+        <v>5</v>
+      </c>
+      <c r="D190" s="3"/>
+      <c r="E190" s="3"/>
+      <c r="F190" s="3"/>
+      <c r="G190" s="3"/>
+      <c r="H190" s="27"/>
+      <c r="I190" s="27"/>
+      <c r="J190" s="27"/>
+      <c r="K190" s="27"/>
+      <c r="L190" s="27"/>
+      <c r="M190" s="27"/>
+      <c r="N190" s="27"/>
+      <c r="O190" s="27"/>
+      <c r="P190" s="27"/>
+      <c r="Q190" s="27"/>
+      <c r="R190" s="27"/>
+      <c r="S190" s="27"/>
+      <c r="T190" s="27"/>
+      <c r="U190" s="27"/>
+      <c r="V190" s="27"/>
+      <c r="W190" s="27"/>
+      <c r="X190" s="27"/>
+      <c r="Y190" s="27"/>
+      <c r="Z190" s="27"/>
+      <c r="AA190" s="3"/>
       <c r="AB190" s="16"/>
       <c r="AC190" s="1"/>
       <c r="AD190" s="1"/>
       <c r="AE190" s="1"/>
     </row>
-    <row r="191" spans="1:31" ht="18.75" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="B191" s="33"/>
       <c r="C191" s="73">
-        <f>INT($C$190)+1.02</f>
-        <v>2.02</v>
+        <v>1.02</v>
       </c>
       <c r="D191" s="21"/>
       <c r="E191" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F191" s="28">
-        <v>1</v>
-      </c>
-      <c r="G191" s="13"/>
-      <c r="H191" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="I191" s="7"/>
-      <c r="J191" s="7"/>
-      <c r="K191" s="7"/>
-      <c r="L191" s="7"/>
-      <c r="M191" s="7"/>
-      <c r="N191" s="7"/>
-      <c r="O191" s="7"/>
-      <c r="P191" s="7"/>
-      <c r="Q191" s="7"/>
-      <c r="R191" s="7"/>
-      <c r="S191" s="7"/>
-      <c r="T191" s="7"/>
-      <c r="U191" s="7"/>
-      <c r="V191" s="7"/>
-      <c r="W191" s="7"/>
-      <c r="X191" s="7"/>
-      <c r="Y191" s="7"/>
-      <c r="Z191" s="7"/>
-      <c r="AA191" s="11"/>
+        <v>6</v>
+      </c>
+      <c r="F191" s="25"/>
+      <c r="G191" s="12"/>
+      <c r="H191" s="147" t="str">
+        <f>COUNTIFS($B$1:$B191, "«")&amp;" Feed Pool definitions"</f>
+        <v>6 Feed Pool definitions</v>
+      </c>
+      <c r="I191" s="6"/>
+      <c r="J191" s="6"/>
+      <c r="K191" s="6"/>
+      <c r="L191" s="6"/>
+      <c r="M191" s="6"/>
+      <c r="N191" s="6"/>
+      <c r="O191" s="6"/>
+      <c r="P191" s="6"/>
+      <c r="Q191" s="6"/>
+      <c r="R191" s="6"/>
+      <c r="S191" s="6"/>
+      <c r="T191" s="6"/>
+      <c r="U191" s="6"/>
+      <c r="V191" s="6"/>
+      <c r="W191" s="6"/>
+      <c r="X191" s="6"/>
+      <c r="Y191" s="6"/>
+      <c r="Z191" s="6"/>
+      <c r="AA191" s="10"/>
       <c r="AB191" s="16"/>
       <c r="AC191" s="1"/>
       <c r="AD191" s="1"/>
       <c r="AE191" s="1"/>
     </row>
-    <row r="192" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:31" ht="18.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
       <c r="B192" s="33"/>
       <c r="C192" s="73">
-        <f>INT($C$190)+2.005</f>
-        <v>3.0049999999999999</v>
-      </c>
-      <c r="D192" s="3"/>
-      <c r="E192" s="3"/>
-      <c r="F192" s="3"/>
-      <c r="G192" s="3"/>
-      <c r="H192" s="3"/>
-      <c r="I192" s="3"/>
-      <c r="J192" s="3"/>
-      <c r="K192" s="3"/>
-      <c r="L192" s="3"/>
-      <c r="M192" s="3"/>
-      <c r="N192" s="3"/>
-      <c r="O192" s="3"/>
-      <c r="P192" s="3"/>
-      <c r="Q192" s="3"/>
-      <c r="R192" s="3"/>
-      <c r="S192" s="3"/>
-      <c r="T192" s="3"/>
-      <c r="U192" s="3"/>
-      <c r="V192" s="3"/>
-      <c r="W192" s="3"/>
-      <c r="X192" s="3"/>
-      <c r="Y192" s="3"/>
-      <c r="Z192" s="3"/>
-      <c r="AA192" s="3"/>
+        <f>INT($C$191)+1.02</f>
+        <v>2.02</v>
+      </c>
+      <c r="D192" s="21"/>
+      <c r="E192" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F192" s="28">
+        <v>1</v>
+      </c>
+      <c r="G192" s="13"/>
+      <c r="H192" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="I192" s="7"/>
+      <c r="J192" s="7"/>
+      <c r="K192" s="7"/>
+      <c r="L192" s="7"/>
+      <c r="M192" s="7"/>
+      <c r="N192" s="7"/>
+      <c r="O192" s="7"/>
+      <c r="P192" s="7"/>
+      <c r="Q192" s="7"/>
+      <c r="R192" s="7"/>
+      <c r="S192" s="7"/>
+      <c r="T192" s="7"/>
+      <c r="U192" s="7"/>
+      <c r="V192" s="7"/>
+      <c r="W192" s="7"/>
+      <c r="X192" s="7"/>
+      <c r="Y192" s="7"/>
+      <c r="Z192" s="7"/>
+      <c r="AA192" s="11"/>
       <c r="AB192" s="16"/>
       <c r="AC192" s="1"/>
       <c r="AD192" s="1"/>
       <c r="AE192" s="1"/>
     </row>
-    <row r="193" spans="1:31" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
       <c r="B193" s="33"/>
       <c r="C193" s="73">
-        <f>INT($C$190)+2</f>
-        <v>3</v>
+        <f>INT($C$191)+2.005</f>
+        <v>3.0049999999999999</v>
       </c>
       <c r="D193" s="3"/>
-      <c r="E193" s="5"/>
-      <c r="F193" s="5"/>
+      <c r="E193" s="3"/>
+      <c r="F193" s="3"/>
       <c r="G193" s="3"/>
-      <c r="H193" s="29"/>
-      <c r="I193" s="29"/>
-      <c r="J193" s="65" t="s">
-        <v>293</v>
-      </c>
-      <c r="K193" s="65"/>
-      <c r="L193" s="65"/>
-      <c r="M193" s="65"/>
-      <c r="N193" s="65"/>
-      <c r="O193" s="65"/>
-      <c r="P193" s="65"/>
-      <c r="Q193" s="65"/>
-      <c r="R193" s="65"/>
-      <c r="S193" s="65"/>
-      <c r="T193" s="29"/>
-      <c r="U193" s="29"/>
-      <c r="V193" s="29"/>
-      <c r="W193" s="29"/>
-      <c r="X193" s="29"/>
-      <c r="Y193" s="29"/>
-      <c r="Z193" s="29"/>
+      <c r="H193" s="3"/>
+      <c r="I193" s="3"/>
+      <c r="J193" s="3"/>
+      <c r="K193" s="3"/>
+      <c r="L193" s="3"/>
+      <c r="M193" s="3"/>
+      <c r="N193" s="3"/>
+      <c r="O193" s="3"/>
+      <c r="P193" s="3"/>
+      <c r="Q193" s="3"/>
+      <c r="R193" s="3"/>
+      <c r="S193" s="3"/>
+      <c r="T193" s="3"/>
+      <c r="U193" s="3"/>
+      <c r="V193" s="3"/>
+      <c r="W193" s="3"/>
+      <c r="X193" s="3"/>
+      <c r="Y193" s="3"/>
+      <c r="Z193" s="3"/>
       <c r="AA193" s="3"/>
       <c r="AB193" s="16"/>
       <c r="AC193" s="1"/>
@@ -35361,7 +35426,7 @@
       <c r="A194" s="1"/>
       <c r="B194" s="33"/>
       <c r="C194" s="73">
-        <f>INT($C$190)+2</f>
+        <f>INT($C$191)+2</f>
         <v>3</v>
       </c>
       <c r="D194" s="3"/>
@@ -35370,36 +35435,18 @@
       <c r="G194" s="3"/>
       <c r="H194" s="29"/>
       <c r="I194" s="29"/>
-      <c r="J194" s="29">
-        <v>0</v>
-      </c>
-      <c r="K194" s="29">
-        <v>1</v>
-      </c>
-      <c r="L194" s="29">
-        <v>2</v>
-      </c>
-      <c r="M194" s="29">
-        <v>3</v>
-      </c>
-      <c r="N194" s="29">
-        <v>4</v>
-      </c>
-      <c r="O194" s="29">
-        <v>5</v>
-      </c>
-      <c r="P194" s="29">
-        <v>6</v>
-      </c>
-      <c r="Q194" s="29">
-        <v>7</v>
-      </c>
-      <c r="R194" s="29">
-        <v>8</v>
-      </c>
-      <c r="S194" s="29">
-        <v>9</v>
-      </c>
+      <c r="J194" s="65" t="s">
+        <v>293</v>
+      </c>
+      <c r="K194" s="65"/>
+      <c r="L194" s="65"/>
+      <c r="M194" s="65"/>
+      <c r="N194" s="65"/>
+      <c r="O194" s="65"/>
+      <c r="P194" s="65"/>
+      <c r="Q194" s="65"/>
+      <c r="R194" s="65"/>
+      <c r="S194" s="65"/>
       <c r="T194" s="29"/>
       <c r="U194" s="29"/>
       <c r="V194" s="29"/>
@@ -35413,31 +35460,49 @@
       <c r="AD194" s="1"/>
       <c r="AE194" s="1"/>
     </row>
-    <row r="195" spans="1:31" ht="9.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:31" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
-      <c r="B195" s="33" t="s">
-        <v>20</v>
-      </c>
+      <c r="B195" s="33"/>
       <c r="C195" s="73">
-        <f>INT($C$190)+2.01</f>
-        <v>3.01</v>
+        <f>INT($C$191)+2</f>
+        <v>3</v>
       </c>
       <c r="D195" s="3"/>
-      <c r="E195" s="3"/>
-      <c r="F195" s="3"/>
+      <c r="E195" s="5"/>
+      <c r="F195" s="5"/>
       <c r="G195" s="3"/>
       <c r="H195" s="29"/>
       <c r="I195" s="29"/>
-      <c r="J195" s="29"/>
-      <c r="K195" s="29"/>
-      <c r="L195" s="29"/>
-      <c r="M195" s="29"/>
-      <c r="N195" s="29"/>
-      <c r="O195" s="29"/>
-      <c r="P195" s="29"/>
-      <c r="Q195" s="29"/>
-      <c r="R195" s="29"/>
-      <c r="S195" s="29"/>
+      <c r="J195" s="29">
+        <v>0</v>
+      </c>
+      <c r="K195" s="29">
+        <v>1</v>
+      </c>
+      <c r="L195" s="29">
+        <v>2</v>
+      </c>
+      <c r="M195" s="29">
+        <v>3</v>
+      </c>
+      <c r="N195" s="29">
+        <v>4</v>
+      </c>
+      <c r="O195" s="29">
+        <v>5</v>
+      </c>
+      <c r="P195" s="29">
+        <v>6</v>
+      </c>
+      <c r="Q195" s="29">
+        <v>7</v>
+      </c>
+      <c r="R195" s="29">
+        <v>8</v>
+      </c>
+      <c r="S195" s="29">
+        <v>9</v>
+      </c>
       <c r="T195" s="29"/>
       <c r="U195" s="29"/>
       <c r="V195" s="29"/>
@@ -35451,37 +35516,39 @@
       <c r="AD195" s="1"/>
       <c r="AE195" s="1"/>
     </row>
-    <row r="196" spans="1:31" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:31" ht="9.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
-      <c r="B196" s="33"/>
+      <c r="B196" s="33" t="s">
+        <v>20</v>
+      </c>
       <c r="C196" s="73">
-        <f>C$189</f>
-        <v>5</v>
-      </c>
-      <c r="D196" s="4"/>
-      <c r="E196" s="5"/>
-      <c r="F196" s="5"/>
-      <c r="G196" s="4"/>
-      <c r="H196" s="5"/>
-      <c r="I196" s="5"/>
-      <c r="J196" s="5"/>
-      <c r="K196" s="5"/>
-      <c r="L196" s="5"/>
-      <c r="M196" s="5"/>
-      <c r="N196" s="5"/>
-      <c r="O196" s="5"/>
-      <c r="P196" s="5"/>
-      <c r="Q196" s="5"/>
-      <c r="R196" s="5"/>
-      <c r="S196" s="5"/>
-      <c r="T196" s="5"/>
-      <c r="U196" s="5"/>
-      <c r="V196" s="5"/>
-      <c r="W196" s="5"/>
-      <c r="X196" s="5"/>
-      <c r="Y196" s="5"/>
-      <c r="Z196" s="5"/>
-      <c r="AA196" s="4"/>
+        <f>INT($C$191)+2.01</f>
+        <v>3.01</v>
+      </c>
+      <c r="D196" s="3"/>
+      <c r="E196" s="3"/>
+      <c r="F196" s="3"/>
+      <c r="G196" s="3"/>
+      <c r="H196" s="29"/>
+      <c r="I196" s="29"/>
+      <c r="J196" s="29"/>
+      <c r="K196" s="29"/>
+      <c r="L196" s="29"/>
+      <c r="M196" s="29"/>
+      <c r="N196" s="29"/>
+      <c r="O196" s="29"/>
+      <c r="P196" s="29"/>
+      <c r="Q196" s="29"/>
+      <c r="R196" s="29"/>
+      <c r="S196" s="29"/>
+      <c r="T196" s="29"/>
+      <c r="U196" s="29"/>
+      <c r="V196" s="29"/>
+      <c r="W196" s="29"/>
+      <c r="X196" s="29"/>
+      <c r="Y196" s="29"/>
+      <c r="Z196" s="29"/>
+      <c r="AA196" s="3"/>
       <c r="AB196" s="16"/>
       <c r="AC196" s="1"/>
       <c r="AD196" s="1"/>
@@ -35489,16 +35556,12 @@
     </row>
     <row r="197" spans="1:31" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
-      <c r="B197" s="33" t="s">
-        <v>19</v>
-      </c>
+      <c r="B197" s="33"/>
       <c r="C197" s="73">
-        <f>C$189</f>
+        <f>C$190</f>
         <v>5</v>
       </c>
-      <c r="D197" s="4" t="s">
-        <v>44</v>
-      </c>
+      <c r="D197" s="4"/>
       <c r="E197" s="5"/>
       <c r="F197" s="5"/>
       <c r="G197" s="4"/>
@@ -35527,100 +35590,104 @@
       <c r="AD197" s="1"/>
       <c r="AE197" s="1"/>
     </row>
-    <row r="198" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:31" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
-      <c r="B198" s="33"/>
+      <c r="B198" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="C198" s="73">
-        <f>INT($C$190)+2.005</f>
-        <v>3.0049999999999999</v>
+        <f>C$190</f>
+        <v>5</v>
       </c>
       <c r="D198" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E198" s="4"/>
-      <c r="F198" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="E198" s="5"/>
+      <c r="F198" s="5"/>
       <c r="G198" s="4"/>
-      <c r="H198" s="58"/>
-      <c r="I198" s="58"/>
-      <c r="J198" s="58"/>
-      <c r="K198" s="58"/>
-      <c r="L198" s="58"/>
-      <c r="M198" s="58"/>
-      <c r="N198" s="58"/>
-      <c r="O198" s="58"/>
-      <c r="P198" s="58"/>
-      <c r="Q198" s="58"/>
-      <c r="R198" s="58"/>
-      <c r="S198" s="58"/>
-      <c r="T198" s="58"/>
-      <c r="U198" s="58"/>
-      <c r="V198" s="58"/>
-      <c r="W198" s="58"/>
-      <c r="X198" s="82"/>
-      <c r="Y198" s="82"/>
-      <c r="Z198" s="82"/>
+      <c r="H198" s="5"/>
+      <c r="I198" s="5"/>
+      <c r="J198" s="5"/>
+      <c r="K198" s="5"/>
+      <c r="L198" s="5"/>
+      <c r="M198" s="5"/>
+      <c r="N198" s="5"/>
+      <c r="O198" s="5"/>
+      <c r="P198" s="5"/>
+      <c r="Q198" s="5"/>
+      <c r="R198" s="5"/>
+      <c r="S198" s="5"/>
+      <c r="T198" s="5"/>
+      <c r="U198" s="5"/>
+      <c r="V198" s="5"/>
+      <c r="W198" s="5"/>
+      <c r="X198" s="5"/>
+      <c r="Y198" s="5"/>
+      <c r="Z198" s="5"/>
       <c r="AA198" s="4"/>
       <c r="AB198" s="16"/>
       <c r="AC198" s="1"/>
       <c r="AD198" s="1"/>
       <c r="AE198" s="1"/>
     </row>
-    <row r="199" spans="1:31" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
       <c r="B199" s="33"/>
       <c r="C199" s="73">
-        <f>INT($C$190)+2</f>
-        <v>3</v>
-      </c>
-      <c r="D199" s="4"/>
-      <c r="E199" s="5"/>
-      <c r="F199" s="5"/>
+        <f>INT($C$191)+2.005</f>
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="D199" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E199" s="4"/>
+      <c r="F199" s="4"/>
       <c r="G199" s="4"/>
-      <c r="H199" s="64" t="s">
-        <v>287</v>
-      </c>
-      <c r="I199" s="31">
-        <v>4</v>
-      </c>
-      <c r="J199" s="158" t="s">
-        <v>291</v>
-      </c>
-      <c r="K199" s="2"/>
-      <c r="L199" s="2"/>
-      <c r="M199" s="2"/>
-      <c r="N199" s="2"/>
-      <c r="O199" s="2"/>
-      <c r="P199" s="2"/>
-      <c r="Q199" s="2"/>
-      <c r="R199" s="2"/>
-      <c r="S199" s="2"/>
-      <c r="T199" s="2"/>
-      <c r="U199" s="2"/>
-      <c r="V199" s="2"/>
-      <c r="W199" s="2"/>
-      <c r="X199" s="2"/>
-      <c r="Y199" s="2"/>
-      <c r="Z199" s="2"/>
+      <c r="H199" s="58"/>
+      <c r="I199" s="58"/>
+      <c r="J199" s="58"/>
+      <c r="K199" s="58"/>
+      <c r="L199" s="58"/>
+      <c r="M199" s="58"/>
+      <c r="N199" s="58"/>
+      <c r="O199" s="58"/>
+      <c r="P199" s="58"/>
+      <c r="Q199" s="58"/>
+      <c r="R199" s="58"/>
+      <c r="S199" s="58"/>
+      <c r="T199" s="58"/>
+      <c r="U199" s="58"/>
+      <c r="V199" s="58"/>
+      <c r="W199" s="58"/>
+      <c r="X199" s="82"/>
+      <c r="Y199" s="82"/>
+      <c r="Z199" s="82"/>
       <c r="AA199" s="4"/>
       <c r="AB199" s="16"/>
       <c r="AC199" s="1"/>
       <c r="AD199" s="1"/>
       <c r="AE199" s="1"/>
     </row>
-    <row r="200" spans="1:31" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:31" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
       <c r="B200" s="33"/>
       <c r="C200" s="73">
-        <f>INT($C$190)+3</f>
-        <v>4</v>
+        <f>INT($C$191)+2</f>
+        <v>3</v>
       </c>
       <c r="D200" s="4"/>
       <c r="E200" s="5"/>
       <c r="F200" s="5"/>
       <c r="G200" s="4"/>
-      <c r="H200" s="157"/>
-      <c r="I200" s="2"/>
-      <c r="J200" s="2"/>
+      <c r="H200" s="64" t="s">
+        <v>287</v>
+      </c>
+      <c r="I200" s="31">
+        <v>4</v>
+      </c>
+      <c r="J200" s="158" t="s">
+        <v>291</v>
+      </c>
       <c r="K200" s="2"/>
       <c r="L200" s="2"/>
       <c r="M200" s="2"/>
@@ -35643,20 +35710,18 @@
       <c r="AD200" s="1"/>
       <c r="AE200" s="1"/>
     </row>
-    <row r="201" spans="1:31" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:31" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A201" s="1"/>
       <c r="B201" s="33"/>
       <c r="C201" s="73">
-        <f>INT($C$190)+2</f>
-        <v>3</v>
+        <f>INT($C$191)+3</f>
+        <v>4</v>
       </c>
       <c r="D201" s="4"/>
       <c r="E201" s="5"/>
       <c r="F201" s="5"/>
       <c r="G201" s="4"/>
-      <c r="H201" s="64" t="s">
-        <v>292</v>
-      </c>
+      <c r="H201" s="157"/>
       <c r="I201" s="2"/>
       <c r="J201" s="2"/>
       <c r="K201" s="2"/>
@@ -35681,51 +35746,31 @@
       <c r="AD201" s="1"/>
       <c r="AE201" s="1"/>
     </row>
-    <row r="202" spans="1:31" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:31" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A202" s="1"/>
       <c r="B202" s="33"/>
       <c r="C202" s="73">
-        <f>INT($C$190)+3</f>
-        <v>4</v>
+        <f>INT($C$191)+2</f>
+        <v>3</v>
       </c>
       <c r="D202" s="4"/>
       <c r="E202" s="5"/>
       <c r="F202" s="5"/>
       <c r="G202" s="4"/>
-      <c r="H202" s="159" t="s">
-        <v>298</v>
+      <c r="H202" s="64" t="s">
+        <v>292</v>
       </c>
       <c r="I202" s="2"/>
-      <c r="J202" s="31">
-        <v>3</v>
-      </c>
-      <c r="K202" s="31">
-        <v>4</v>
-      </c>
-      <c r="L202" s="31">
-        <v>6</v>
-      </c>
-      <c r="M202" s="31">
-        <v>8</v>
-      </c>
-      <c r="N202" s="31">
-        <v>9</v>
-      </c>
-      <c r="O202" s="31">
-        <v>6</v>
-      </c>
-      <c r="P202" s="31">
-        <v>5</v>
-      </c>
-      <c r="Q202" s="31">
-        <v>4</v>
-      </c>
-      <c r="R202" s="31">
-        <v>3.5</v>
-      </c>
-      <c r="S202" s="31">
-        <v>3</v>
-      </c>
+      <c r="J202" s="2"/>
+      <c r="K202" s="2"/>
+      <c r="L202" s="2"/>
+      <c r="M202" s="2"/>
+      <c r="N202" s="2"/>
+      <c r="O202" s="2"/>
+      <c r="P202" s="2"/>
+      <c r="Q202" s="2"/>
+      <c r="R202" s="2"/>
+      <c r="S202" s="2"/>
       <c r="T202" s="2"/>
       <c r="U202" s="2"/>
       <c r="V202" s="2"/>
@@ -35739,11 +35784,11 @@
       <c r="AD202" s="1"/>
       <c r="AE202" s="1"/>
     </row>
-    <row r="203" spans="1:31" outlineLevel="3" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:31" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A203" s="1"/>
       <c r="B203" s="33"/>
       <c r="C203" s="73">
-        <f>INT($C$190)+3</f>
+        <f>INT($C$191)+3</f>
         <v>4</v>
       </c>
       <c r="D203" s="4"/>
@@ -35751,38 +35796,38 @@
       <c r="F203" s="5"/>
       <c r="G203" s="4"/>
       <c r="H203" s="159" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="I203" s="2"/>
       <c r="J203" s="31">
-        <v>13.3</v>
+        <v>3</v>
       </c>
       <c r="K203" s="31">
-        <v>13.3</v>
+        <v>4</v>
       </c>
       <c r="L203" s="31">
-        <v>13.3</v>
+        <v>6</v>
       </c>
       <c r="M203" s="31">
-        <v>13.3</v>
+        <v>8</v>
       </c>
       <c r="N203" s="31">
-        <v>13.3</v>
+        <v>9</v>
       </c>
       <c r="O203" s="31">
-        <v>13.3</v>
+        <v>6</v>
       </c>
       <c r="P203" s="31">
-        <v>13.3</v>
+        <v>5</v>
       </c>
       <c r="Q203" s="31">
-        <v>13.3</v>
+        <v>4</v>
       </c>
       <c r="R203" s="31">
-        <v>13.3</v>
+        <v>3.5</v>
       </c>
       <c r="S203" s="31">
-        <v>13.3</v>
+        <v>3</v>
       </c>
       <c r="T203" s="2"/>
       <c r="U203" s="2"/>
@@ -35797,29 +35842,51 @@
       <c r="AD203" s="1"/>
       <c r="AE203" s="1"/>
     </row>
-    <row r="204" spans="1:31" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:31" outlineLevel="3" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A204" s="1"/>
       <c r="B204" s="33"/>
       <c r="C204" s="73">
-        <f>INT(C$190+3)</f>
+        <f>INT($C$191)+3</f>
         <v>4</v>
       </c>
       <c r="D204" s="4"/>
       <c r="E204" s="5"/>
       <c r="F204" s="5"/>
       <c r="G204" s="4"/>
-      <c r="H204" s="148"/>
-      <c r="I204" s="148"/>
-      <c r="J204" s="148"/>
-      <c r="K204" s="148"/>
-      <c r="L204" s="148"/>
-      <c r="M204" s="148"/>
-      <c r="N204" s="148"/>
-      <c r="O204" s="148"/>
-      <c r="P204" s="148"/>
-      <c r="Q204" s="148"/>
-      <c r="R204" s="148"/>
-      <c r="S204" s="148"/>
+      <c r="H204" s="159" t="s">
+        <v>294</v>
+      </c>
+      <c r="I204" s="2"/>
+      <c r="J204" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="K204" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="L204" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="M204" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="N204" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="O204" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="P204" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="Q204" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="R204" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="S204" s="31">
+        <v>13.3</v>
+      </c>
       <c r="T204" s="2"/>
       <c r="U204" s="2"/>
       <c r="V204" s="2"/>
@@ -35837,7 +35904,7 @@
       <c r="A205" s="1"/>
       <c r="B205" s="33"/>
       <c r="C205" s="73">
-        <f>INT(C$190+3)</f>
+        <f>INT(C$191+3)</f>
         <v>4</v>
       </c>
       <c r="D205" s="4"/>
@@ -35855,7 +35922,7 @@
       <c r="P205" s="148"/>
       <c r="Q205" s="148"/>
       <c r="R205" s="148"/>
-      <c r="S205" s="2"/>
+      <c r="S205" s="148"/>
       <c r="T205" s="2"/>
       <c r="U205" s="2"/>
       <c r="V205" s="2"/>
@@ -35869,50 +35936,48 @@
       <c r="AD205" s="1"/>
       <c r="AE205" s="1"/>
     </row>
-    <row r="206" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:31" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A206" s="1"/>
       <c r="B206" s="33"/>
       <c r="C206" s="73">
-        <f>INT($C$190)+3.005</f>
-        <v>4.0049999999999999</v>
+        <f>INT(C$191+3)</f>
+        <v>4</v>
       </c>
       <c r="D206" s="4"/>
-      <c r="E206" s="4"/>
-      <c r="F206" s="4"/>
+      <c r="E206" s="5"/>
+      <c r="F206" s="5"/>
       <c r="G206" s="4"/>
-      <c r="H206" s="4"/>
-      <c r="I206" s="4"/>
-      <c r="J206" s="4"/>
-      <c r="K206" s="4"/>
-      <c r="L206" s="4"/>
-      <c r="M206" s="4"/>
-      <c r="N206" s="4"/>
-      <c r="O206" s="4"/>
-      <c r="P206" s="4"/>
-      <c r="Q206" s="4"/>
-      <c r="R206" s="4"/>
-      <c r="S206" s="4"/>
-      <c r="T206" s="4"/>
-      <c r="U206" s="4"/>
-      <c r="V206" s="4"/>
-      <c r="W206" s="4"/>
-      <c r="X206" s="4"/>
-      <c r="Y206" s="4"/>
-      <c r="Z206" s="4"/>
-      <c r="AA206" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="H206" s="148"/>
+      <c r="I206" s="148"/>
+      <c r="J206" s="148"/>
+      <c r="K206" s="148"/>
+      <c r="L206" s="148"/>
+      <c r="M206" s="148"/>
+      <c r="N206" s="148"/>
+      <c r="O206" s="148"/>
+      <c r="P206" s="148"/>
+      <c r="Q206" s="148"/>
+      <c r="R206" s="148"/>
+      <c r="S206" s="2"/>
+      <c r="T206" s="2"/>
+      <c r="U206" s="2"/>
+      <c r="V206" s="2"/>
+      <c r="W206" s="2"/>
+      <c r="X206" s="2"/>
+      <c r="Y206" s="2"/>
+      <c r="Z206" s="2"/>
+      <c r="AA206" s="4"/>
       <c r="AB206" s="16"/>
       <c r="AC206" s="1"/>
       <c r="AD206" s="1"/>
       <c r="AE206" s="1"/>
     </row>
-    <row r="207" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A207" s="1"/>
       <c r="B207" s="33"/>
       <c r="C207" s="73">
-        <f>INT($C$190)+2.005</f>
-        <v>3.0049999999999999</v>
+        <f>INT($C$191)+3.005</f>
+        <v>4.0049999999999999</v>
       </c>
       <c r="D207" s="4"/>
       <c r="E207" s="4"/>
@@ -35937,126 +36002,131 @@
       <c r="X207" s="4"/>
       <c r="Y207" s="4"/>
       <c r="Z207" s="4"/>
-      <c r="AA207" s="4"/>
+      <c r="AA207" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="AB207" s="16"/>
       <c r="AC207" s="1"/>
       <c r="AD207" s="1"/>
       <c r="AE207" s="1"/>
     </row>
-    <row r="208" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A208" s="1"/>
-      <c r="B208" s="35"/>
-      <c r="C208" s="76">
-        <f>INT($C$190)+1.005</f>
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="D208" s="17"/>
-      <c r="E208" s="17"/>
-      <c r="F208" s="17"/>
-      <c r="G208" s="17"/>
-      <c r="H208" s="17"/>
-      <c r="I208" s="17"/>
-      <c r="J208" s="17"/>
-      <c r="K208" s="17"/>
-      <c r="L208" s="17"/>
-      <c r="M208" s="17"/>
-      <c r="N208" s="17"/>
-      <c r="O208" s="17"/>
-      <c r="P208" s="17"/>
-      <c r="Q208" s="17"/>
-      <c r="R208" s="17"/>
-      <c r="S208" s="17"/>
-      <c r="T208" s="17"/>
-      <c r="U208" s="17"/>
-      <c r="V208" s="17"/>
-      <c r="W208" s="17"/>
-      <c r="X208" s="17"/>
-      <c r="Y208" s="17"/>
-      <c r="Z208" s="17"/>
-      <c r="AA208" s="17"/>
-      <c r="AB208" s="18" t="s">
-        <v>1</v>
-      </c>
+      <c r="B208" s="33"/>
+      <c r="C208" s="73">
+        <f>INT($C$191)+2.005</f>
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="D208" s="4"/>
+      <c r="E208" s="4"/>
+      <c r="F208" s="4"/>
+      <c r="G208" s="4"/>
+      <c r="H208" s="4"/>
+      <c r="I208" s="4"/>
+      <c r="J208" s="4"/>
+      <c r="K208" s="4"/>
+      <c r="L208" s="4"/>
+      <c r="M208" s="4"/>
+      <c r="N208" s="4"/>
+      <c r="O208" s="4"/>
+      <c r="P208" s="4"/>
+      <c r="Q208" s="4"/>
+      <c r="R208" s="4"/>
+      <c r="S208" s="4"/>
+      <c r="T208" s="4"/>
+      <c r="U208" s="4"/>
+      <c r="V208" s="4"/>
+      <c r="W208" s="4"/>
+      <c r="X208" s="4"/>
+      <c r="Y208" s="4"/>
+      <c r="Z208" s="4"/>
+      <c r="AA208" s="4"/>
+      <c r="AB208" s="16"/>
       <c r="AC208" s="1"/>
       <c r="AD208" s="1"/>
       <c r="AE208" s="1"/>
     </row>
-    <row r="209" spans="1:31" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:31" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A209" s="1"/>
-      <c r="B209" s="19"/>
-      <c r="C209" s="77">
-        <f>INT($C$190)+0.005</f>
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="D209" s="19"/>
-      <c r="E209" s="19"/>
-      <c r="F209" s="19"/>
-      <c r="G209" s="19"/>
-      <c r="H209" s="19"/>
-      <c r="I209" s="19"/>
-      <c r="J209" s="19"/>
-      <c r="K209" s="19"/>
-      <c r="L209" s="19"/>
-      <c r="M209" s="19"/>
-      <c r="N209" s="19"/>
-      <c r="O209" s="19"/>
-      <c r="P209" s="19"/>
-      <c r="Q209" s="19"/>
-      <c r="R209" s="19"/>
-      <c r="S209" s="19"/>
-      <c r="T209" s="19"/>
-      <c r="U209" s="19"/>
-      <c r="V209" s="19"/>
-      <c r="W209" s="19"/>
-      <c r="X209" s="19"/>
-      <c r="Y209" s="19"/>
-      <c r="Z209" s="19"/>
-      <c r="AA209" s="19"/>
-      <c r="AB209" s="19"/>
+      <c r="B209" s="35"/>
+      <c r="C209" s="76">
+        <f>INT($C$191)+1.005</f>
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="D209" s="17"/>
+      <c r="E209" s="17"/>
+      <c r="F209" s="17"/>
+      <c r="G209" s="17"/>
+      <c r="H209" s="17"/>
+      <c r="I209" s="17"/>
+      <c r="J209" s="17"/>
+      <c r="K209" s="17"/>
+      <c r="L209" s="17"/>
+      <c r="M209" s="17"/>
+      <c r="N209" s="17"/>
+      <c r="O209" s="17"/>
+      <c r="P209" s="17"/>
+      <c r="Q209" s="17"/>
+      <c r="R209" s="17"/>
+      <c r="S209" s="17"/>
+      <c r="T209" s="17"/>
+      <c r="U209" s="17"/>
+      <c r="V209" s="17"/>
+      <c r="W209" s="17"/>
+      <c r="X209" s="17"/>
+      <c r="Y209" s="17"/>
+      <c r="Z209" s="17"/>
+      <c r="AA209" s="17"/>
+      <c r="AB209" s="18" t="s">
+        <v>1</v>
+      </c>
       <c r="AC209" s="1"/>
       <c r="AD209" s="1"/>
       <c r="AE209" s="1"/>
     </row>
-    <row r="210" spans="1:31" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:31" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="1"/>
-      <c r="B210" s="1"/>
-      <c r="C210" s="73">
-        <f>INT($C$190)+2</f>
-        <v>3</v>
-      </c>
-      <c r="D210" s="1"/>
-      <c r="E210" s="1"/>
-      <c r="F210" s="1"/>
-      <c r="G210" s="1"/>
-      <c r="H210" s="1"/>
-      <c r="I210" s="1"/>
-      <c r="J210" s="1"/>
-      <c r="K210" s="1"/>
-      <c r="L210" s="1"/>
-      <c r="M210" s="1"/>
-      <c r="N210" s="1"/>
-      <c r="O210" s="1"/>
-      <c r="P210" s="1"/>
-      <c r="Q210" s="1"/>
-      <c r="R210" s="1"/>
-      <c r="S210" s="1"/>
-      <c r="T210" s="1"/>
-      <c r="U210" s="1"/>
-      <c r="V210" s="1"/>
-      <c r="W210" s="1"/>
-      <c r="X210" s="1"/>
-      <c r="Y210" s="1"/>
-      <c r="Z210" s="1"/>
-      <c r="AA210" s="1"/>
-      <c r="AB210" s="1"/>
+      <c r="B210" s="19"/>
+      <c r="C210" s="77">
+        <f>INT($C$191)+0.005</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D210" s="19"/>
+      <c r="E210" s="19"/>
+      <c r="F210" s="19"/>
+      <c r="G210" s="19"/>
+      <c r="H210" s="19"/>
+      <c r="I210" s="19"/>
+      <c r="J210" s="19"/>
+      <c r="K210" s="19"/>
+      <c r="L210" s="19"/>
+      <c r="M210" s="19"/>
+      <c r="N210" s="19"/>
+      <c r="O210" s="19"/>
+      <c r="P210" s="19"/>
+      <c r="Q210" s="19"/>
+      <c r="R210" s="19"/>
+      <c r="S210" s="19"/>
+      <c r="T210" s="19"/>
+      <c r="U210" s="19"/>
+      <c r="V210" s="19"/>
+      <c r="W210" s="19"/>
+      <c r="X210" s="19"/>
+      <c r="Y210" s="19"/>
+      <c r="Z210" s="19"/>
+      <c r="AA210" s="19"/>
+      <c r="AB210" s="19"/>
       <c r="AC210" s="1"/>
       <c r="AD210" s="1"/>
       <c r="AE210" s="1"/>
     </row>
-    <row r="211" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:31" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A211" s="1"/>
       <c r="B211" s="1"/>
-      <c r="C211" s="66"/>
+      <c r="C211" s="73">
+        <f>INT($C$191)+2</f>
+        <v>3</v>
+      </c>
       <c r="D211" s="1"/>
       <c r="E211" s="1"/>
       <c r="F211" s="1"/>
@@ -36252,7 +36322,40 @@
       <c r="AE216" s="1"/>
     </row>
     <row r="217" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="C217" s="72" t="s">
+      <c r="A217" s="1"/>
+      <c r="B217" s="1"/>
+      <c r="C217" s="66"/>
+      <c r="D217" s="1"/>
+      <c r="E217" s="1"/>
+      <c r="F217" s="1"/>
+      <c r="G217" s="1"/>
+      <c r="H217" s="1"/>
+      <c r="I217" s="1"/>
+      <c r="J217" s="1"/>
+      <c r="K217" s="1"/>
+      <c r="L217" s="1"/>
+      <c r="M217" s="1"/>
+      <c r="N217" s="1"/>
+      <c r="O217" s="1"/>
+      <c r="P217" s="1"/>
+      <c r="Q217" s="1"/>
+      <c r="R217" s="1"/>
+      <c r="S217" s="1"/>
+      <c r="T217" s="1"/>
+      <c r="U217" s="1"/>
+      <c r="V217" s="1"/>
+      <c r="W217" s="1"/>
+      <c r="X217" s="1"/>
+      <c r="Y217" s="1"/>
+      <c r="Z217" s="1"/>
+      <c r="AA217" s="1"/>
+      <c r="AB217" s="1"/>
+      <c r="AC217" s="1"/>
+      <c r="AD217" s="1"/>
+      <c r="AE217" s="1"/>
+    </row>
+    <row r="218" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="C218" s="72" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
increase planning horizon for MP model so that MP model give same answer as SE.
</commit_message>
<xml_diff>
--- a/ExcelInputs/Structural.xlsx
+++ b/ExcelInputs/Structural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\Work-Uni-Coding\Models\AFO\ExcelInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D848917-76CA-4296-8FDA-EA5E85042601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684672CD-3FCA-464B-9A49-9FC8BF9F1401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28650" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="-10935" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -11476,7 +11476,7 @@
   </sheetPr>
   <dimension ref="A1:AB334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
       <pane xSplit="9" ySplit="10" topLeftCell="J146" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
@@ -27305,12 +27305,12 @@
   </sheetPr>
   <dimension ref="A1:AE218"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="9" ySplit="10" topLeftCell="J23" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="M47" sqref="M47"/>
+      <selection pane="bottomRight" activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
@@ -29135,7 +29135,7 @@
         <v>449</v>
       </c>
       <c r="M46" s="222">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="N46" s="2" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
add note about MP planning horizon.
</commit_message>
<xml_diff>
--- a/ExcelInputs/Structural.xlsx
+++ b/ExcelInputs/Structural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\Work-Uni-Coding\Models\AFO\ExcelInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED38BFF5-A4E4-47E8-BB30-0598BFE89993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCF3236-7018-45D4-A32D-99ABD8AEE677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28650" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="678" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="150" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -739,7 +739,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Michael:</t>
         </r>
@@ -748,7 +748,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 At prejoining all numbers get allocated to the NM slice. They then get allocated to the other b slices at mating.</t>
@@ -1321,7 +1321,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Michael:</t>
         </r>
@@ -1330,10 +1330,11 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-What is the planning horizon. This is used for the discount rate calculation and the MP model (q gets weighted to represent the planning horizon).</t>
+This is used for the discount rate calculation and the MP model (q gets weighted to represent the planning horizon).
+The standard version of AFO MP includes 7 discrete years for which the management is optimised. The final year is structured as an equilibrium so that the end of the 7th year must be equal to the start of that year. This final year is weighted in the discounted objective function to represent a 100 year planning horizon. The very long horizon was required to ensure that the flock structure was optimised correctly. Using a shorter calculation horizon resulted in extra sheep being sold in the penultimate year because the discounted cashflow was greater from selling than retaining even though the return on assets for the animals if they had been retained was greater than the discount rate. The maths is related to the implied minimum ROA required to retain animals for the final year. In the earlier years the future return must be greater than the discount rate, whereas for the decision to retain for the final year the ROA is the discount factor for the penultimate year divided by the cumulative factor for the final year. The shorter the period that the animals are retained the higher the implied ROA.</t>
         </r>
       </text>
     </comment>
@@ -1345,7 +1346,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Michael:</t>
         </r>
@@ -1354,7 +1355,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Time value of money</t>
@@ -2470,7 +2471,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>John:</t>
         </r>
@@ -2479,7 +2480,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Carcase fat depth</t>
@@ -4104,7 +4105,7 @@
     <numFmt numFmtId="166" formatCode="0.00_)"/>
     <numFmt numFmtId="167" formatCode="[$-C09]dd\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4323,19 +4324,6 @@
       <color rgb="FF0000CC"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="40">
@@ -6793,7 +6781,7 @@
   </sheetPr>
   <dimension ref="A1:AT127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <pane xSplit="9" ySplit="10" topLeftCell="J79" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
@@ -27319,12 +27307,12 @@
   </sheetPr>
   <dimension ref="A1:AE218"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J60" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="9" ySplit="10" topLeftCell="J31" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="J14" sqref="J14:T14"/>
+      <selection pane="bottomRight" activeCell="S48" sqref="S48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
temp: code changes for tactics
</commit_message>
<xml_diff>
--- a/ExcelInputs/Structural.xlsx
+++ b/ExcelInputs/Structural.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\Work-Uni-Coding\Models\AFO\ExcelInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7CE2F7-D461-448F-B7A0-FBF88BD003B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA9D6A2-98B6-4F8B-86A2-2965A459F412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="-28920" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="678" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <definedName name="dry_groups" localSheetId="0">General!$I$47:$J$47</definedName>
     <definedName name="foo_levels" localSheetId="0">General!$I$49:$K$49</definedName>
     <definedName name="grain_pools" localSheetId="0">General!$I$44:$J$44</definedName>
-    <definedName name="grazing_int" localSheetId="0">General!$I$48:$L$48</definedName>
+    <definedName name="grazing_int" localSheetId="0">General!$I$48:$U$48</definedName>
     <definedName name="i_a0_pos">Stock!$I$43</definedName>
     <definedName name="i_a1_pos">Stock!$I$44</definedName>
     <definedName name="i_a2_idx" localSheetId="0">General!$N$79</definedName>
@@ -184,7 +184,7 @@
     <definedName name="ZA.WidthCol" localSheetId="4">Admin!$L$26</definedName>
     <definedName name="ZA.ZoomSheet" localSheetId="4">Admin!$O$26</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2551,7 +2551,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="461">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -4039,6 +4039,33 @@
   </si>
   <si>
     <t>lf</t>
+  </si>
+  <si>
+    <t>Graz5</t>
+  </si>
+  <si>
+    <t>Graz10</t>
+  </si>
+  <si>
+    <t>Graz15</t>
+  </si>
+  <si>
+    <t>Graz20</t>
+  </si>
+  <si>
+    <t>Graz30</t>
+  </si>
+  <si>
+    <t>Graz35</t>
+  </si>
+  <si>
+    <t>Graz40</t>
+  </si>
+  <si>
+    <t>Graz45</t>
+  </si>
+  <si>
+    <t>Graz60</t>
   </si>
 </sst>
 </file>
@@ -6727,12 +6754,12 @@
   </sheetPr>
   <dimension ref="A1:AT127"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J79" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <pane xSplit="9" ySplit="10" topLeftCell="J31" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="J85" sqref="J85:J86"/>
+      <selection pane="bottomRight" activeCell="T48" sqref="T48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
@@ -8480,23 +8507,41 @@
         <v>179</v>
       </c>
       <c r="J48" s="97" t="s">
+        <v>452</v>
+      </c>
+      <c r="K48" s="97" t="s">
+        <v>453</v>
+      </c>
+      <c r="L48" s="97" t="s">
+        <v>454</v>
+      </c>
+      <c r="M48" s="97" t="s">
+        <v>455</v>
+      </c>
+      <c r="N48" s="97" t="s">
         <v>180</v>
       </c>
-      <c r="K48" s="97" t="s">
+      <c r="O48" s="97" t="s">
+        <v>456</v>
+      </c>
+      <c r="P48" s="97" t="s">
+        <v>457</v>
+      </c>
+      <c r="Q48" s="97" t="s">
+        <v>458</v>
+      </c>
+      <c r="R48" s="97" t="s">
+        <v>459</v>
+      </c>
+      <c r="S48" s="97" t="s">
         <v>264</v>
       </c>
-      <c r="L48" s="97" t="s">
+      <c r="T48" s="97" t="s">
+        <v>460</v>
+      </c>
+      <c r="U48" s="97" t="s">
         <v>181</v>
       </c>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
-      <c r="O48" s="2"/>
-      <c r="P48" s="2"/>
-      <c r="Q48" s="2"/>
-      <c r="R48" s="2"/>
-      <c r="S48" s="2"/>
-      <c r="T48" s="2"/>
-      <c r="U48" s="2"/>
       <c r="V48" s="2"/>
       <c r="W48" s="2"/>
       <c r="X48" s="4"/>
@@ -11424,7 +11469,7 @@
   </sheetPr>
   <dimension ref="A1:AB333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
       <pane xSplit="9" ySplit="10" topLeftCell="J146" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>

</xml_diff>

<commit_message>
Temp: increase nv slices offs and turn off confinement nv pool
</commit_message>
<xml_diff>
--- a/ExcelInputs/Structural.xlsx
+++ b/ExcelInputs/Structural.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\Work-Uni-Coding\Models\AFO\ExcelInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2BFF323-42CA-4DEB-8BAA-6495699E53CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4135A1-F31C-442A-8519-6FF2DB3349FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28950" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
@@ -27127,11 +27127,11 @@
   <dimension ref="A1:AE214"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="10" topLeftCell="J190" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="R43" sqref="R43"/>
+      <selection pane="bottomRight" activeCell="I200" sqref="I200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
@@ -35697,7 +35697,7 @@
         <v>287</v>
       </c>
       <c r="I200" s="31">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J200" s="158" t="s">
         <v>291</v>

</xml_diff>

<commit_message>
Temp: reset nv pools to 4 and use SAV to adjust
</commit_message>
<xml_diff>
--- a/ExcelInputs/Structural.xlsx
+++ b/ExcelInputs/Structural.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\Work-Uni-Coding\Models\AFO\ExcelInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4135A1-F31C-442A-8519-6FF2DB3349FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E604769-CDC2-4F18-9508-6FF493FEDC0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28950" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
@@ -182,7 +182,7 @@
     <definedName name="ZA.WidthCol" localSheetId="4">Admin!$L$26</definedName>
     <definedName name="ZA.ZoomSheet" localSheetId="4">Admin!$O$26</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35697,7 +35697,7 @@
         <v>287</v>
       </c>
       <c r="I200" s="31">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J200" s="158" t="s">
         <v>291</v>

</xml_diff>